<commit_message>
changed master csv file
</commit_message>
<xml_diff>
--- a/data_25_01_14.xlsx
+++ b/data_25_01_14.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="all data" sheetId="1" r:id="rId1"/>
     <sheet name="data for model comparison" sheetId="2" r:id="rId2"/>
     <sheet name="misalignment" sheetId="3" r:id="rId3"/>
-    <sheet name="dynamic" sheetId="4" r:id="rId4"/>
-    <sheet name="MinMax Accuracy Data " sheetId="5" r:id="rId5"/>
+    <sheet name=" dynamic autobending" sheetId="4" r:id="rId4"/>
+    <sheet name="all_data_accuracy" sheetId="5" r:id="rId5"/>
     <sheet name="reapplication" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
@@ -28931,8 +28931,8 @@
   </sheetPr>
   <dimension ref="A1:AM2"/>
   <sheetViews>
-    <sheetView topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -29121,8 +29121,8 @@
   </sheetPr>
   <dimension ref="A1:AM12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="L19" sqref="L19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -30163,7 +30163,7 @@
     <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" ht="15.75">
+    <row r="1" spans="1:39">
       <c r="A1" s="132" t="s">
         <v>198</v>
       </c>
@@ -30248,7 +30248,7 @@
       <c r="AL1" s="135"/>
       <c r="AM1" s="135"/>
     </row>
-    <row r="2" spans="1:39" ht="15.75">
+    <row r="2" spans="1:39">
       <c r="A2" s="122" t="s">
         <v>198</v>
       </c>
@@ -30331,7 +30331,7 @@
       <c r="AL2" s="137"/>
       <c r="AM2" s="137"/>
     </row>
-    <row r="3" spans="1:39" ht="15.75">
+    <row r="3" spans="1:39">
       <c r="A3" s="122" t="s">
         <v>198</v>
       </c>
@@ -30414,7 +30414,7 @@
       <c r="AL3" s="137"/>
       <c r="AM3" s="137"/>
     </row>
-    <row r="4" spans="1:39" ht="15.75">
+    <row r="4" spans="1:39">
       <c r="A4" s="122" t="s">
         <v>198</v>
       </c>

</xml_diff>

<commit_message>
Sensor Fab and Mis Data
Collected new misalignment data on two additional samples.   Also created cad files and png image for sensor fabrication image for future paper
</commit_message>
<xml_diff>
--- a/data_25_01_14.xlsx
+++ b/data_25_01_14.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2158" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2291" uniqueCount="349">
   <si>
     <t>Sample Name</t>
   </si>
@@ -985,6 +985,93 @@
   </si>
   <si>
     <t>CSV Data/2_6_2025/third test/Bending_data_abs_1p7_4th_reapply_2_6_25.csv</t>
+  </si>
+  <si>
+    <t>2_11_25</t>
+  </si>
+  <si>
+    <t>1.685 in</t>
+  </si>
+  <si>
+    <t>Misalignement</t>
+  </si>
+  <si>
+    <t>0 degrees</t>
+  </si>
+  <si>
+    <t>abs_1p685_0deg</t>
+  </si>
+  <si>
+    <t>67.8 F</t>
+  </si>
+  <si>
+    <t>CSV Data/2_11_2025/0 deg/Bending_data_abs_1p685_0deg_2_11_25.csv</t>
+  </si>
+  <si>
+    <t>CSV Data/2_11_2025/0 deg/Bending_data_abs_1p685_0deg_2_11_25.png</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>abs_1p732_0deg</t>
+  </si>
+  <si>
+    <t>1.732 in</t>
+  </si>
+  <si>
+    <t>70.9 F</t>
+  </si>
+  <si>
+    <t>CSV Data/2_11_2025/0 deg/1p732/Bending_data_abs_1p732_0deg_2_11_25.csv</t>
+  </si>
+  <si>
+    <t>abs_1p732_8deg</t>
+  </si>
+  <si>
+    <t>8 degrees</t>
+  </si>
+  <si>
+    <t>CSV Data/2_11_2025/8 deg/1p732/Bending_data_abs_1p732_8deg_2_11_25.csv</t>
+  </si>
+  <si>
+    <t>Failed ?  When sample peeled off and measured resistance, very high</t>
+  </si>
+  <si>
+    <t>CSV Data/2_11_2025/8 deg/Bending_data_abs_1p732_8deg_2_11_25.jpg</t>
+  </si>
+  <si>
+    <t>abs_1p732_20deg</t>
+  </si>
+  <si>
+    <t>20 degrees</t>
+  </si>
+  <si>
+    <t>CSV Data/2_11_2025/20 deg/1p732/Bending_data_abs_1p732_20deg_2_11_25.csv</t>
+  </si>
+  <si>
+    <t>CSV Data/2_11_2025/20 deg/Bending_data_abs_1p732_20deg_2_11_25.jpg</t>
+  </si>
+  <si>
+    <t>74.5 F</t>
+  </si>
+  <si>
+    <t>CSV Data/2_11_2025/8 deg/1p758/Bending_data_abs_1p758_8deg_2_11_25.csv</t>
+  </si>
+  <si>
+    <t>CSV Data/2_11_2025/0 deg/1p758/Bending_data_abs_1p7_abs_1p758_1st_reapply_2_6_25.csv</t>
+  </si>
+  <si>
+    <t>abs_1p758_1st_reapply_0deg</t>
+  </si>
+  <si>
+    <t>abs_1p758_1st_reapply_8deg</t>
+  </si>
+  <si>
+    <t>abs_1p758_1st_reapply_20deg</t>
+  </si>
+  <si>
+    <t>CSV Data/2_11_2025/20 deg/1p758/Bending_data_abs_1p758_20deg_2_11_25.csv</t>
   </si>
 </sst>
 </file>
@@ -1055,7 +1142,7 @@
       <name val="JetBrains Mono"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1101,6 +1188,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF23B947"/>
+        <bgColor rgb="FF93C47D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor rgb="FF93C47D"/>
       </patternFill>
     </fill>
@@ -1234,7 +1333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="146">
+  <cellXfs count="153">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1561,6 +1660,25 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1784,16 +1902,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AM988"/>
+  <dimension ref="A1:AM989"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B94" sqref="B94"/>
+      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A100" sqref="A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="46.140625" customWidth="1"/>
     <col min="5" max="6" width="14.5703125" customWidth="1"/>
@@ -7863,7 +7981,9 @@
       <c r="T86" s="143" t="s">
         <v>236</v>
       </c>
-      <c r="U86" s="139"/>
+      <c r="U86" s="12" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="87" spans="1:39" s="144" customFormat="1">
       <c r="A87" s="139" t="s">
@@ -7922,7 +8042,9 @@
       <c r="T87" s="143" t="s">
         <v>236</v>
       </c>
-      <c r="U87" s="139"/>
+      <c r="U87" s="12" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="88" spans="1:39" s="144" customFormat="1">
       <c r="A88" s="139" t="s">
@@ -7981,7 +8103,9 @@
       <c r="T88" s="143" t="s">
         <v>236</v>
       </c>
-      <c r="U88" s="139"/>
+      <c r="U88" s="12" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="89" spans="1:39" s="144" customFormat="1">
       <c r="A89" s="139" t="s">
@@ -8040,7 +8164,9 @@
       <c r="T89" s="143" t="s">
         <v>236</v>
       </c>
-      <c r="U89" s="139"/>
+      <c r="U89" s="12" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="90" spans="1:39">
       <c r="A90" s="4" t="s">
@@ -8142,7 +8268,9 @@
       <c r="T91" s="143" t="s">
         <v>236</v>
       </c>
-      <c r="U91" s="3"/>
+      <c r="U91" s="12" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="92" spans="1:39">
       <c r="A92" s="139" t="s">
@@ -8201,7 +8329,9 @@
       <c r="T92" s="143" t="s">
         <v>236</v>
       </c>
-      <c r="U92" s="3"/>
+      <c r="U92" s="12" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="93" spans="1:39">
       <c r="A93" s="139" t="s">
@@ -8260,7 +8390,9 @@
       <c r="T93" s="143" t="s">
         <v>236</v>
       </c>
-      <c r="U93" s="3"/>
+      <c r="U93" s="12" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="94" spans="1:39">
       <c r="A94" s="139" t="s">
@@ -8319,186 +8451,479 @@
       <c r="T94" s="143" t="s">
         <v>236</v>
       </c>
-      <c r="U94" s="3"/>
+      <c r="U94" s="3" t="s">
+        <v>328</v>
+      </c>
     </row>
     <row r="95" spans="1:39">
-      <c r="A95" s="12"/>
-      <c r="B95" s="3"/>
-      <c r="C95" s="3"/>
-      <c r="D95" s="3"/>
-      <c r="E95" s="3"/>
-      <c r="F95" s="3"/>
-      <c r="G95" s="3"/>
-      <c r="H95" s="3"/>
-      <c r="I95" s="3"/>
-      <c r="J95" s="3"/>
-      <c r="K95" s="3"/>
-      <c r="L95" s="3"/>
-      <c r="M95" s="3"/>
-      <c r="N95" s="3"/>
-      <c r="O95" s="3"/>
-      <c r="P95" s="3"/>
-      <c r="Q95" s="3"/>
-      <c r="R95" s="3"/>
-      <c r="S95" s="3"/>
-      <c r="U95" s="3"/>
-    </row>
-    <row r="96" spans="1:39">
-      <c r="A96" s="12"/>
-      <c r="B96" s="3"/>
-      <c r="C96" s="3"/>
-      <c r="D96" s="3"/>
-      <c r="E96" s="3"/>
-      <c r="F96" s="3"/>
-      <c r="G96" s="3"/>
-      <c r="H96" s="3"/>
-      <c r="I96" s="3"/>
-      <c r="J96" s="3"/>
-      <c r="K96" s="3"/>
-      <c r="L96" s="3"/>
-      <c r="M96" s="3"/>
-      <c r="N96" s="3"/>
-      <c r="O96" s="3"/>
-      <c r="P96" s="3"/>
-      <c r="Q96" s="3"/>
-      <c r="R96" s="3"/>
-      <c r="S96" s="3"/>
-      <c r="U96" s="3"/>
-    </row>
-    <row r="97" spans="1:21">
-      <c r="A97" s="12"/>
-      <c r="B97" s="3"/>
-      <c r="C97" s="3"/>
-      <c r="D97" s="3"/>
-      <c r="E97" s="3"/>
-      <c r="F97" s="3"/>
-      <c r="G97" s="3"/>
-      <c r="H97" s="3"/>
-      <c r="I97" s="3"/>
-      <c r="J97" s="3"/>
-      <c r="K97" s="3"/>
-      <c r="L97" s="3"/>
-      <c r="M97" s="3"/>
-      <c r="N97" s="3"/>
-      <c r="O97" s="3"/>
-      <c r="P97" s="3"/>
-      <c r="Q97" s="3"/>
-      <c r="R97" s="3"/>
-      <c r="S97" s="3"/>
-      <c r="U97" s="3"/>
-    </row>
-    <row r="98" spans="1:21">
-      <c r="A98" s="12"/>
-      <c r="B98" s="3"/>
-      <c r="C98" s="3"/>
-      <c r="D98" s="3"/>
-      <c r="E98" s="3"/>
-      <c r="F98" s="3"/>
-      <c r="G98" s="3"/>
-      <c r="H98" s="3"/>
-      <c r="I98" s="3"/>
-      <c r="J98" s="3"/>
-      <c r="K98" s="3"/>
-      <c r="L98" s="3"/>
-      <c r="M98" s="3"/>
-      <c r="N98" s="3"/>
-      <c r="O98" s="3"/>
-      <c r="P98" s="3"/>
-      <c r="Q98" s="3"/>
-      <c r="R98" s="3"/>
-      <c r="S98" s="3"/>
-      <c r="U98" s="3"/>
-    </row>
-    <row r="99" spans="1:21">
-      <c r="A99" s="3"/>
-      <c r="B99" s="3"/>
-      <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
-      <c r="E99" s="3"/>
-      <c r="F99" s="3"/>
-      <c r="G99" s="3"/>
-      <c r="H99" s="3"/>
-      <c r="I99" s="3"/>
-      <c r="J99" s="3"/>
-      <c r="K99" s="3"/>
-      <c r="L99" s="3"/>
-      <c r="M99" s="3"/>
-      <c r="N99" s="3"/>
-      <c r="O99" s="3"/>
-      <c r="P99" s="3"/>
-      <c r="Q99" s="3"/>
-      <c r="R99" s="3"/>
-      <c r="S99" s="3"/>
-      <c r="U99" s="3"/>
-    </row>
-    <row r="100" spans="1:21">
-      <c r="A100" s="3"/>
-      <c r="B100" s="3"/>
-      <c r="C100" s="3"/>
-      <c r="D100" s="3"/>
-      <c r="E100" s="3"/>
-      <c r="F100" s="3"/>
-      <c r="G100" s="3"/>
-      <c r="H100" s="3"/>
-      <c r="I100" s="3"/>
-      <c r="J100" s="3"/>
-      <c r="K100" s="3"/>
-      <c r="L100" s="3"/>
-      <c r="M100" s="3"/>
-      <c r="N100" s="3"/>
-      <c r="O100" s="3"/>
-      <c r="P100" s="3"/>
-      <c r="Q100" s="3"/>
-      <c r="R100" s="3"/>
-      <c r="S100" s="3"/>
-      <c r="U100" s="3"/>
+      <c r="A95" s="4" t="s">
+        <v>320</v>
+      </c>
+      <c r="B95" s="51"/>
+      <c r="C95" s="51"/>
+      <c r="D95" s="51"/>
+      <c r="E95" s="51"/>
+      <c r="F95" s="51"/>
+      <c r="G95" s="51"/>
+      <c r="H95" s="51"/>
+      <c r="I95" s="51"/>
+      <c r="J95" s="51"/>
+      <c r="K95" s="51"/>
+      <c r="L95" s="51"/>
+      <c r="M95" s="51"/>
+      <c r="N95" s="51"/>
+      <c r="O95" s="51"/>
+      <c r="P95" s="51"/>
+      <c r="Q95" s="51"/>
+      <c r="R95" s="51"/>
+      <c r="S95" s="51"/>
+      <c r="T95" s="8"/>
+      <c r="U95" s="51"/>
+      <c r="V95" s="8"/>
+      <c r="W95" s="8"/>
+      <c r="X95" s="8"/>
+      <c r="Y95" s="8"/>
+      <c r="Z95" s="8"/>
+      <c r="AA95" s="8"/>
+      <c r="AB95" s="8"/>
+      <c r="AC95" s="8"/>
+      <c r="AD95" s="8"/>
+      <c r="AE95" s="8"/>
+      <c r="AF95" s="8"/>
+      <c r="AG95" s="8"/>
+      <c r="AH95" s="8"/>
+      <c r="AI95" s="8"/>
+      <c r="AJ95" s="8"/>
+      <c r="AK95" s="8"/>
+      <c r="AL95" s="8"/>
+      <c r="AM95" s="8"/>
+    </row>
+    <row r="96" spans="1:39" s="152" customFormat="1">
+      <c r="A96" s="146" t="s">
+        <v>324</v>
+      </c>
+      <c r="B96" s="146"/>
+      <c r="C96" s="146" t="s">
+        <v>323</v>
+      </c>
+      <c r="D96" s="146" t="s">
+        <v>322</v>
+      </c>
+      <c r="E96" s="147" t="s">
+        <v>232</v>
+      </c>
+      <c r="F96" s="146" t="s">
+        <v>293</v>
+      </c>
+      <c r="G96" s="146" t="s">
+        <v>292</v>
+      </c>
+      <c r="H96" s="146" t="s">
+        <v>290</v>
+      </c>
+      <c r="I96" s="146" t="s">
+        <v>321</v>
+      </c>
+      <c r="J96" s="146" t="s">
+        <v>288</v>
+      </c>
+      <c r="K96" s="146" t="s">
+        <v>325</v>
+      </c>
+      <c r="L96" s="148">
+        <v>0.35</v>
+      </c>
+      <c r="M96" s="146"/>
+      <c r="N96" s="146" t="s">
+        <v>32</v>
+      </c>
+      <c r="O96" s="146" t="s">
+        <v>326</v>
+      </c>
+      <c r="P96" s="146" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q96" s="147" t="s">
+        <v>143</v>
+      </c>
+      <c r="R96" s="147" t="s">
+        <v>36</v>
+      </c>
+      <c r="S96" s="149" t="s">
+        <v>132</v>
+      </c>
+      <c r="T96" s="150" t="s">
+        <v>236</v>
+      </c>
+      <c r="U96" s="146" t="s">
+        <v>327</v>
+      </c>
+      <c r="V96" s="151" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="97" spans="1:21" s="152" customFormat="1">
+      <c r="A97" s="146" t="s">
+        <v>329</v>
+      </c>
+      <c r="B97" s="146"/>
+      <c r="C97" s="146" t="s">
+        <v>323</v>
+      </c>
+      <c r="D97" s="146" t="s">
+        <v>322</v>
+      </c>
+      <c r="E97" s="147" t="s">
+        <v>232</v>
+      </c>
+      <c r="F97" s="146" t="s">
+        <v>293</v>
+      </c>
+      <c r="G97" s="146" t="s">
+        <v>292</v>
+      </c>
+      <c r="H97" s="146" t="s">
+        <v>290</v>
+      </c>
+      <c r="I97" s="146" t="s">
+        <v>330</v>
+      </c>
+      <c r="J97" s="146" t="s">
+        <v>288</v>
+      </c>
+      <c r="K97" s="146" t="s">
+        <v>331</v>
+      </c>
+      <c r="L97" s="148">
+        <v>0.33</v>
+      </c>
+      <c r="M97" s="146"/>
+      <c r="N97" s="146" t="s">
+        <v>32</v>
+      </c>
+      <c r="O97" s="146" t="s">
+        <v>332</v>
+      </c>
+      <c r="P97" s="146" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q97" s="147" t="s">
+        <v>143</v>
+      </c>
+      <c r="R97" s="147" t="s">
+        <v>36</v>
+      </c>
+      <c r="S97" s="149" t="s">
+        <v>132</v>
+      </c>
+      <c r="T97" s="150" t="s">
+        <v>236</v>
+      </c>
+      <c r="U97" s="146" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="98" spans="1:21" s="152" customFormat="1">
+      <c r="A98" s="146" t="s">
+        <v>333</v>
+      </c>
+      <c r="B98" s="146"/>
+      <c r="C98" s="146" t="s">
+        <v>334</v>
+      </c>
+      <c r="D98" s="146" t="s">
+        <v>322</v>
+      </c>
+      <c r="E98" s="147" t="s">
+        <v>232</v>
+      </c>
+      <c r="F98" s="146" t="s">
+        <v>293</v>
+      </c>
+      <c r="G98" s="146" t="s">
+        <v>292</v>
+      </c>
+      <c r="H98" s="146" t="s">
+        <v>290</v>
+      </c>
+      <c r="I98" s="146" t="s">
+        <v>330</v>
+      </c>
+      <c r="J98" s="146" t="s">
+        <v>288</v>
+      </c>
+      <c r="K98" s="146" t="s">
+        <v>308</v>
+      </c>
+      <c r="L98" s="148">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M98" s="146"/>
+      <c r="N98" s="146" t="s">
+        <v>32</v>
+      </c>
+      <c r="O98" s="146" t="s">
+        <v>335</v>
+      </c>
+      <c r="P98" s="146" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q98" s="147" t="s">
+        <v>143</v>
+      </c>
+      <c r="R98" s="147" t="s">
+        <v>36</v>
+      </c>
+      <c r="S98" s="149" t="s">
+        <v>132</v>
+      </c>
+      <c r="T98" s="150" t="s">
+        <v>236</v>
+      </c>
+      <c r="U98" s="146" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="99" spans="1:21" s="152" customFormat="1">
+      <c r="A99" s="146" t="s">
+        <v>338</v>
+      </c>
+      <c r="B99" s="146"/>
+      <c r="C99" s="146" t="s">
+        <v>339</v>
+      </c>
+      <c r="D99" s="146" t="s">
+        <v>322</v>
+      </c>
+      <c r="E99" s="147" t="s">
+        <v>232</v>
+      </c>
+      <c r="F99" s="146" t="s">
+        <v>137</v>
+      </c>
+      <c r="G99" s="146" t="s">
+        <v>292</v>
+      </c>
+      <c r="H99" s="146" t="s">
+        <v>290</v>
+      </c>
+      <c r="I99" s="146" t="s">
+        <v>330</v>
+      </c>
+      <c r="J99" s="146" t="s">
+        <v>288</v>
+      </c>
+      <c r="K99" s="146" t="s">
+        <v>308</v>
+      </c>
+      <c r="L99" s="148">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="M99" s="146"/>
+      <c r="N99" s="146" t="s">
+        <v>32</v>
+      </c>
+      <c r="O99" s="146" t="s">
+        <v>340</v>
+      </c>
+      <c r="P99" s="146" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q99" s="147" t="s">
+        <v>143</v>
+      </c>
+      <c r="R99" s="147" t="s">
+        <v>36</v>
+      </c>
+      <c r="S99" s="149" t="s">
+        <v>132</v>
+      </c>
+      <c r="T99" s="150" t="s">
+        <v>236</v>
+      </c>
+      <c r="U99" s="146" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="100" spans="1:21" s="152" customFormat="1">
+      <c r="A100" s="139" t="s">
+        <v>345</v>
+      </c>
+      <c r="B100" s="146"/>
+      <c r="C100" s="146" t="s">
+        <v>323</v>
+      </c>
+      <c r="D100" s="146" t="s">
+        <v>322</v>
+      </c>
+      <c r="E100" s="147" t="s">
+        <v>232</v>
+      </c>
+      <c r="F100" s="146" t="s">
+        <v>293</v>
+      </c>
+      <c r="G100" s="146" t="s">
+        <v>292</v>
+      </c>
+      <c r="H100" s="146" t="s">
+        <v>290</v>
+      </c>
+      <c r="I100" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="J100" s="146" t="s">
+        <v>288</v>
+      </c>
+      <c r="K100" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="L100" s="145">
+        <v>0.27</v>
+      </c>
+      <c r="M100" s="146"/>
+      <c r="N100" s="146" t="s">
+        <v>32</v>
+      </c>
+      <c r="O100" s="146" t="s">
+        <v>344</v>
+      </c>
+      <c r="P100" s="146" t="s">
+        <v>303</v>
+      </c>
+      <c r="Q100" s="147" t="s">
+        <v>143</v>
+      </c>
+      <c r="R100" s="147" t="s">
+        <v>36</v>
+      </c>
+      <c r="S100" s="149" t="s">
+        <v>132</v>
+      </c>
+      <c r="T100" s="150" t="s">
+        <v>236</v>
+      </c>
+      <c r="U100" s="146"/>
     </row>
     <row r="101" spans="1:21">
-      <c r="A101" s="3"/>
+      <c r="A101" s="139" t="s">
+        <v>346</v>
+      </c>
       <c r="B101" s="3"/>
-      <c r="C101" s="3"/>
-      <c r="D101" s="3"/>
-      <c r="E101" s="3"/>
-      <c r="F101" s="3"/>
-      <c r="G101" s="3"/>
-      <c r="H101" s="3"/>
-      <c r="I101" s="3"/>
-      <c r="J101" s="3"/>
-      <c r="K101" s="3"/>
-      <c r="L101" s="3"/>
+      <c r="C101" s="146" t="s">
+        <v>334</v>
+      </c>
+      <c r="D101" s="146" t="s">
+        <v>322</v>
+      </c>
+      <c r="E101" s="147" t="s">
+        <v>232</v>
+      </c>
+      <c r="F101" s="146" t="s">
+        <v>293</v>
+      </c>
+      <c r="G101" s="146" t="s">
+        <v>292</v>
+      </c>
+      <c r="H101" s="146" t="s">
+        <v>290</v>
+      </c>
+      <c r="I101" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="J101" s="146" t="s">
+        <v>288</v>
+      </c>
+      <c r="K101" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="L101" s="145">
+        <v>0.27</v>
+      </c>
       <c r="M101" s="3"/>
-      <c r="N101" s="3"/>
-      <c r="O101" s="3"/>
-      <c r="P101" s="3"/>
-      <c r="Q101" s="3"/>
-      <c r="R101" s="3"/>
-      <c r="S101" s="3"/>
+      <c r="N101" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O101" s="146" t="s">
+        <v>343</v>
+      </c>
+      <c r="P101" s="146" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q101" s="147" t="s">
+        <v>143</v>
+      </c>
+      <c r="R101" s="147" t="s">
+        <v>36</v>
+      </c>
+      <c r="S101" s="149" t="s">
+        <v>132</v>
+      </c>
+      <c r="T101" s="150" t="s">
+        <v>236</v>
+      </c>
       <c r="U101" s="3"/>
     </row>
     <row r="102" spans="1:21">
-      <c r="A102" s="12"/>
+      <c r="A102" s="139" t="s">
+        <v>347</v>
+      </c>
       <c r="B102" s="3"/>
-      <c r="C102" s="3"/>
-      <c r="D102" s="3"/>
-      <c r="E102" s="3"/>
-      <c r="F102" s="3"/>
-      <c r="G102" s="3"/>
-      <c r="H102" s="3"/>
-      <c r="I102" s="3"/>
-      <c r="J102" s="3"/>
-      <c r="K102" s="3"/>
-      <c r="L102" s="3"/>
+      <c r="C102" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="D102" s="146" t="s">
+        <v>322</v>
+      </c>
+      <c r="E102" s="147" t="s">
+        <v>232</v>
+      </c>
+      <c r="F102" s="146" t="s">
+        <v>293</v>
+      </c>
+      <c r="G102" s="146" t="s">
+        <v>292</v>
+      </c>
+      <c r="H102" s="146" t="s">
+        <v>290</v>
+      </c>
+      <c r="I102" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="J102" s="146" t="s">
+        <v>288</v>
+      </c>
+      <c r="K102" s="12" t="s">
+        <v>342</v>
+      </c>
+      <c r="L102" s="145">
+        <v>0.27</v>
+      </c>
       <c r="M102" s="3"/>
-      <c r="N102" s="3"/>
-      <c r="O102" s="3"/>
-      <c r="P102" s="3"/>
-      <c r="Q102" s="3"/>
-      <c r="R102" s="3"/>
-      <c r="S102" s="3"/>
+      <c r="N102" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O102" s="146" t="s">
+        <v>348</v>
+      </c>
+      <c r="P102" s="146" t="s">
+        <v>320</v>
+      </c>
+      <c r="Q102" s="147" t="s">
+        <v>143</v>
+      </c>
+      <c r="R102" s="147" t="s">
+        <v>36</v>
+      </c>
+      <c r="S102" s="149" t="s">
+        <v>132</v>
+      </c>
+      <c r="T102" s="150" t="s">
+        <v>236</v>
+      </c>
       <c r="U102" s="3"/>
     </row>
     <row r="103" spans="1:21">
-      <c r="A103" s="12"/>
+      <c r="A103" s="139"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
       <c r="D103" s="3"/>
@@ -8564,7 +8989,7 @@
       <c r="U105" s="3"/>
     </row>
     <row r="106" spans="1:21">
-      <c r="A106" s="3"/>
+      <c r="A106" s="12"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
       <c r="D106" s="3"/>
@@ -8586,7 +9011,7 @@
       <c r="U106" s="3"/>
     </row>
     <row r="107" spans="1:21">
-      <c r="A107" s="12"/>
+      <c r="A107" s="3"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
       <c r="D107" s="3"/>
@@ -8608,7 +9033,7 @@
       <c r="U107" s="3"/>
     </row>
     <row r="108" spans="1:21">
-      <c r="A108" s="3"/>
+      <c r="A108" s="12"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
       <c r="D108" s="3"/>
@@ -8630,7 +9055,7 @@
       <c r="U108" s="3"/>
     </row>
     <row r="109" spans="1:21">
-      <c r="A109" s="12"/>
+      <c r="A109" s="3"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
       <c r="D109" s="3"/>
@@ -8652,7 +9077,7 @@
       <c r="U109" s="3"/>
     </row>
     <row r="110" spans="1:21">
-      <c r="A110" s="3"/>
+      <c r="A110" s="12"/>
       <c r="B110" s="3"/>
       <c r="C110" s="3"/>
       <c r="D110" s="3"/>
@@ -8674,7 +9099,7 @@
       <c r="U110" s="3"/>
     </row>
     <row r="111" spans="1:21">
-      <c r="A111" s="12"/>
+      <c r="A111" s="3"/>
       <c r="B111" s="3"/>
       <c r="C111" s="3"/>
       <c r="D111" s="3"/>
@@ -8718,7 +9143,7 @@
       <c r="U112" s="3"/>
     </row>
     <row r="113" spans="1:21">
-      <c r="A113" s="119"/>
+      <c r="A113" s="12"/>
       <c r="B113" s="3"/>
       <c r="C113" s="3"/>
       <c r="D113" s="3"/>
@@ -8740,7 +9165,7 @@
       <c r="U113" s="3"/>
     </row>
     <row r="114" spans="1:21">
-      <c r="A114" s="12"/>
+      <c r="A114" s="119"/>
       <c r="B114" s="3"/>
       <c r="C114" s="3"/>
       <c r="D114" s="3"/>
@@ -8762,7 +9187,7 @@
       <c r="U114" s="3"/>
     </row>
     <row r="115" spans="1:21">
-      <c r="A115" s="3"/>
+      <c r="A115" s="12"/>
       <c r="B115" s="3"/>
       <c r="C115" s="3"/>
       <c r="D115" s="3"/>
@@ -27988,6 +28413,28 @@
       <c r="R988" s="3"/>
       <c r="S988" s="3"/>
       <c r="U988" s="3"/>
+    </row>
+    <row r="989" spans="1:21">
+      <c r="A989" s="3"/>
+      <c r="B989" s="3"/>
+      <c r="C989" s="3"/>
+      <c r="D989" s="3"/>
+      <c r="E989" s="3"/>
+      <c r="F989" s="3"/>
+      <c r="G989" s="3"/>
+      <c r="H989" s="3"/>
+      <c r="I989" s="3"/>
+      <c r="J989" s="3"/>
+      <c r="K989" s="3"/>
+      <c r="L989" s="3"/>
+      <c r="M989" s="3"/>
+      <c r="N989" s="3"/>
+      <c r="O989" s="3"/>
+      <c r="P989" s="3"/>
+      <c r="Q989" s="3"/>
+      <c r="R989" s="3"/>
+      <c r="S989" s="3"/>
+      <c r="U989" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated bender_class and added analysis code
updated bender_class , added analysis code, and created prelim fig 1
</commit_message>
<xml_diff>
--- a/data_25_01_14.xlsx
+++ b/data_25_01_14.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320" firstSheet="2" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7320"/>
   </bookViews>
   <sheets>
     <sheet name="all data" sheetId="1" r:id="rId1"/>
@@ -783,9 +783,6 @@
     <t>1.897 in</t>
   </si>
   <si>
-    <t>...CSV Data/12_2_24/fourth/Bending_data_abs_1p897_s4_12_9_24.csv</t>
-  </si>
-  <si>
     <t xml:space="preserve">0.28" width, 0.083" thick, </t>
   </si>
   <si>
@@ -1072,6 +1069,9 @@
   </si>
   <si>
     <t>CSV Data/2_11_2025/20 deg/1p758/Bending_data_abs_1p758_20deg_2_11_25.csv</t>
+  </si>
+  <si>
+    <t>...CSV Data/12_9_24/fourth/Bending_data_abs_1p897_s4_12_9_24.csv</t>
   </si>
 </sst>
 </file>
@@ -1904,9 +1904,9 @@
   </sheetPr>
   <dimension ref="A1:AM989"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A85" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A95" sqref="A95:XFD102"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A89" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A101" sqref="A101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1949,7 +1949,7 @@
         <v>5</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>6</v>
@@ -7167,7 +7167,7 @@
         <v>32</v>
       </c>
       <c r="O75" s="109" t="s">
-        <v>244</v>
+        <v>275</v>
       </c>
       <c r="P75" s="83" t="s">
         <v>229</v>
@@ -7252,7 +7252,7 @@
         <v>32</v>
       </c>
       <c r="O76" s="109" t="s">
-        <v>247</v>
+        <v>276</v>
       </c>
       <c r="P76" s="83" t="s">
         <v>229</v>
@@ -7337,7 +7337,7 @@
         <v>32</v>
       </c>
       <c r="O77" s="102" t="s">
-        <v>252</v>
+        <v>348</v>
       </c>
       <c r="P77" s="100" t="s">
         <v>229</v>
@@ -7358,7 +7358,7 @@
         <v>158</v>
       </c>
       <c r="V77" s="103" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="W77" s="104"/>
       <c r="X77" s="104"/>
@@ -7380,7 +7380,7 @@
     </row>
     <row r="78" spans="1:39">
       <c r="A78" s="4" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B78" s="51"/>
       <c r="C78" s="51"/>
@@ -7423,13 +7423,13 @@
     </row>
     <row r="79" spans="1:39">
       <c r="A79" s="83" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B79" s="83" t="s">
         <v>179</v>
       </c>
       <c r="C79" s="83" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D79" s="83" t="s">
         <v>213</v>
@@ -7441,13 +7441,13 @@
         <v>137</v>
       </c>
       <c r="G79" s="83" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H79" s="82" t="s">
         <v>181</v>
       </c>
       <c r="I79" s="83" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J79" s="83" t="s">
         <v>234</v>
@@ -7465,10 +7465,10 @@
         <v>32</v>
       </c>
       <c r="O79" s="109" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P79" s="83" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Q79" s="83" t="s">
         <v>143</v>
@@ -7483,7 +7483,7 @@
         <v>236</v>
       </c>
       <c r="U79" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="V79" s="110"/>
       <c r="W79" s="110"/>
@@ -7506,13 +7506,13 @@
     </row>
     <row r="80" spans="1:39">
       <c r="A80" s="83" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B80" s="83" t="s">
         <v>179</v>
       </c>
       <c r="C80" s="83" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D80" s="83" t="s">
         <v>213</v>
@@ -7524,13 +7524,13 @@
         <v>137</v>
       </c>
       <c r="G80" s="83" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H80" s="82" t="s">
         <v>181</v>
       </c>
       <c r="I80" s="83" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J80" s="83" t="s">
         <v>234</v>
@@ -7548,10 +7548,10 @@
         <v>32</v>
       </c>
       <c r="O80" s="109" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="P80" s="83" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Q80" s="83" t="s">
         <v>143</v>
@@ -7566,7 +7566,7 @@
         <v>236</v>
       </c>
       <c r="U80" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="V80" s="110"/>
       <c r="W80" s="110"/>
@@ -7589,7 +7589,7 @@
     </row>
     <row r="81" spans="1:39">
       <c r="A81" s="4" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B81" s="51"/>
       <c r="C81" s="51"/>
@@ -7632,16 +7632,16 @@
     </row>
     <row r="82" spans="1:39">
       <c r="A82" s="83" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B82" s="83">
         <v>111</v>
       </c>
       <c r="C82" s="83" t="s">
+        <v>264</v>
+      </c>
+      <c r="D82" s="83" t="s">
         <v>265</v>
-      </c>
-      <c r="D82" s="83" t="s">
-        <v>266</v>
       </c>
       <c r="E82" s="83" t="s">
         <v>232</v>
@@ -7650,13 +7650,13 @@
         <v>137</v>
       </c>
       <c r="G82" s="83" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H82" s="82" t="s">
         <v>181</v>
       </c>
       <c r="I82" s="83" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J82" s="83" t="s">
         <v>234</v>
@@ -7674,10 +7674,10 @@
         <v>32</v>
       </c>
       <c r="O82" s="109" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="P82" s="83" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q82" s="83" t="s">
         <v>143</v>
@@ -7695,7 +7695,7 @@
         <v>158</v>
       </c>
       <c r="V82" s="118" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="W82" s="110"/>
       <c r="X82" s="110"/>
@@ -7717,13 +7717,13 @@
     </row>
     <row r="83" spans="1:39">
       <c r="A83" s="83" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B83" s="83" t="s">
         <v>179</v>
       </c>
       <c r="C83" s="83" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D83" s="83" t="s">
         <v>213</v>
@@ -7735,13 +7735,13 @@
         <v>137</v>
       </c>
       <c r="G83" s="83" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H83" s="82" t="s">
         <v>181</v>
       </c>
       <c r="I83" s="83" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J83" s="83" t="s">
         <v>234</v>
@@ -7759,10 +7759,10 @@
         <v>32</v>
       </c>
       <c r="O83" s="109" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P83" s="83" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q83" s="83" t="s">
         <v>143</v>
@@ -7800,16 +7800,16 @@
     </row>
     <row r="84" spans="1:39">
       <c r="A84" s="83" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B84" s="83">
         <v>121</v>
       </c>
       <c r="C84" s="83" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D84" s="83" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E84" s="83" t="s">
         <v>232</v>
@@ -7818,13 +7818,13 @@
         <v>137</v>
       </c>
       <c r="G84" s="83" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H84" s="82" t="s">
         <v>181</v>
       </c>
       <c r="I84" s="83" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J84" s="83" t="s">
         <v>234</v>
@@ -7842,10 +7842,10 @@
         <v>32</v>
       </c>
       <c r="O84" s="109" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P84" s="83" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q84" s="83" t="s">
         <v>143</v>
@@ -7883,7 +7883,7 @@
     </row>
     <row r="85" spans="1:39">
       <c r="A85" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B85" s="51"/>
       <c r="C85" s="51"/>
@@ -7926,11 +7926,11 @@
     </row>
     <row r="86" spans="1:39" s="144" customFormat="1">
       <c r="A86" s="139" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B86" s="139"/>
       <c r="C86" s="139" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D86" s="139" t="s">
         <v>188</v>
@@ -7939,19 +7939,19 @@
         <v>232</v>
       </c>
       <c r="F86" s="139" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G86" s="139" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H86" s="139" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I86" s="139" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J86" s="139" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K86" s="139" t="s">
         <v>171</v>
@@ -7964,10 +7964,10 @@
         <v>32</v>
       </c>
       <c r="O86" s="139" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P86" s="139" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="Q86" s="140" t="s">
         <v>143</v>
@@ -7982,16 +7982,16 @@
         <v>236</v>
       </c>
       <c r="U86" s="12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="87" spans="1:39" s="144" customFormat="1">
       <c r="A87" s="139" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B87" s="139"/>
       <c r="C87" s="139" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D87" s="139" t="s">
         <v>188</v>
@@ -8000,22 +8000,22 @@
         <v>232</v>
       </c>
       <c r="F87" s="139" t="s">
+        <v>292</v>
+      </c>
+      <c r="G87" s="139" t="s">
+        <v>291</v>
+      </c>
+      <c r="H87" s="139" t="s">
+        <v>289</v>
+      </c>
+      <c r="I87" s="139" t="s">
+        <v>288</v>
+      </c>
+      <c r="J87" s="139" t="s">
+        <v>287</v>
+      </c>
+      <c r="K87" s="139" t="s">
         <v>293</v>
-      </c>
-      <c r="G87" s="139" t="s">
-        <v>292</v>
-      </c>
-      <c r="H87" s="139" t="s">
-        <v>290</v>
-      </c>
-      <c r="I87" s="139" t="s">
-        <v>289</v>
-      </c>
-      <c r="J87" s="139" t="s">
-        <v>288</v>
-      </c>
-      <c r="K87" s="139" t="s">
-        <v>294</v>
       </c>
       <c r="L87" s="141">
         <v>0.41</v>
@@ -8025,10 +8025,10 @@
         <v>32</v>
       </c>
       <c r="O87" s="139" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P87" s="139" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="Q87" s="140" t="s">
         <v>143</v>
@@ -8043,16 +8043,16 @@
         <v>236</v>
       </c>
       <c r="U87" s="12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="88" spans="1:39" s="144" customFormat="1">
       <c r="A88" s="139" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B88" s="139"/>
       <c r="C88" s="139" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D88" s="139" t="s">
         <v>188</v>
@@ -8061,22 +8061,22 @@
         <v>232</v>
       </c>
       <c r="F88" s="139" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G88" s="139" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H88" s="139" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I88" s="139" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J88" s="139" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K88" s="139" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L88" s="141">
         <v>0.41</v>
@@ -8086,10 +8086,10 @@
         <v>32</v>
       </c>
       <c r="O88" s="139" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="P88" s="139" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="Q88" s="140" t="s">
         <v>143</v>
@@ -8104,16 +8104,16 @@
         <v>236</v>
       </c>
       <c r="U88" s="12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="89" spans="1:39" s="144" customFormat="1">
       <c r="A89" s="139" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B89" s="139"/>
       <c r="C89" s="139" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D89" s="139" t="s">
         <v>188</v>
@@ -8122,22 +8122,22 @@
         <v>232</v>
       </c>
       <c r="F89" s="139" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G89" s="139" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H89" s="139" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I89" s="139" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J89" s="139" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K89" s="139" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L89" s="141">
         <v>0.42</v>
@@ -8147,10 +8147,10 @@
         <v>32</v>
       </c>
       <c r="O89" s="139" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="P89" s="139" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="Q89" s="140" t="s">
         <v>143</v>
@@ -8165,12 +8165,12 @@
         <v>236</v>
       </c>
       <c r="U89" s="12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="90" spans="1:39">
       <c r="A90" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B90" s="51"/>
       <c r="C90" s="51"/>
@@ -8213,11 +8213,11 @@
     </row>
     <row r="91" spans="1:39">
       <c r="A91" s="139" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B91" s="3"/>
       <c r="C91" s="139" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D91" s="139" t="s">
         <v>188</v>
@@ -8226,22 +8226,22 @@
         <v>232</v>
       </c>
       <c r="F91" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G91" s="139" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H91" s="139" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I91" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="J91" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="K91" s="3" t="s">
         <v>304</v>
-      </c>
-      <c r="J91" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="K91" s="3" t="s">
-        <v>305</v>
       </c>
       <c r="L91" s="145">
         <v>0.37</v>
@@ -8251,10 +8251,10 @@
         <v>32</v>
       </c>
       <c r="O91" s="139" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="P91" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="Q91" s="140" t="s">
         <v>143</v>
@@ -8269,16 +8269,16 @@
         <v>236</v>
       </c>
       <c r="U91" s="12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="92" spans="1:39">
       <c r="A92" s="139" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B92" s="3"/>
       <c r="C92" s="139" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D92" s="139" t="s">
         <v>188</v>
@@ -8287,22 +8287,22 @@
         <v>232</v>
       </c>
       <c r="F92" s="12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G92" s="139" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H92" s="139" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I92" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J92" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K92" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L92" s="145">
         <v>0.35</v>
@@ -8312,10 +8312,10 @@
         <v>32</v>
       </c>
       <c r="O92" s="139" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="P92" s="12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="Q92" s="140" t="s">
         <v>143</v>
@@ -8330,16 +8330,16 @@
         <v>236</v>
       </c>
       <c r="U92" s="12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="93" spans="1:39">
       <c r="A93" s="139" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B93" s="3"/>
       <c r="C93" s="139" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D93" s="139" t="s">
         <v>188</v>
@@ -8348,22 +8348,22 @@
         <v>232</v>
       </c>
       <c r="F93" s="12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G93" s="139" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H93" s="139" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I93" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J93" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K93" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L93" s="145">
         <v>0.41</v>
@@ -8373,10 +8373,10 @@
         <v>32</v>
       </c>
       <c r="O93" s="139" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="P93" s="12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="Q93" s="140" t="s">
         <v>143</v>
@@ -8391,16 +8391,16 @@
         <v>236</v>
       </c>
       <c r="U93" s="12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="94" spans="1:39">
       <c r="A94" s="139" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B94" s="3"/>
       <c r="C94" s="139" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D94" s="139" t="s">
         <v>188</v>
@@ -8409,22 +8409,22 @@
         <v>232</v>
       </c>
       <c r="F94" s="12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G94" s="139" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H94" s="139" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I94" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J94" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K94" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L94" s="145">
         <v>0.41</v>
@@ -8434,10 +8434,10 @@
         <v>32</v>
       </c>
       <c r="O94" s="139" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="P94" s="12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="Q94" s="140" t="s">
         <v>143</v>
@@ -8452,12 +8452,12 @@
         <v>236</v>
       </c>
       <c r="U94" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="95" spans="1:39">
       <c r="A95" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B95" s="51"/>
       <c r="C95" s="51"/>
@@ -8500,35 +8500,35 @@
     </row>
     <row r="96" spans="1:39" s="152" customFormat="1">
       <c r="A96" s="146" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B96" s="146"/>
       <c r="C96" s="146" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D96" s="146" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E96" s="147" t="s">
         <v>232</v>
       </c>
       <c r="F96" s="146" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G96" s="146" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H96" s="146" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I96" s="146" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J96" s="146" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K96" s="146" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="L96" s="148">
         <v>0.35</v>
@@ -8538,10 +8538,10 @@
         <v>32</v>
       </c>
       <c r="O96" s="146" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P96" s="146" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q96" s="147" t="s">
         <v>143</v>
@@ -8556,43 +8556,43 @@
         <v>236</v>
       </c>
       <c r="U96" s="146" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="V96" s="151" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="97" spans="1:21" s="152" customFormat="1">
       <c r="A97" s="146" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B97" s="146"/>
       <c r="C97" s="146" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D97" s="146" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E97" s="147" t="s">
         <v>232</v>
       </c>
       <c r="F97" s="146" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G97" s="146" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H97" s="146" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I97" s="146" t="s">
+        <v>329</v>
+      </c>
+      <c r="J97" s="146" t="s">
+        <v>287</v>
+      </c>
+      <c r="K97" s="146" t="s">
         <v>330</v>
-      </c>
-      <c r="J97" s="146" t="s">
-        <v>288</v>
-      </c>
-      <c r="K97" s="146" t="s">
-        <v>331</v>
       </c>
       <c r="L97" s="148">
         <v>0.33</v>
@@ -8602,10 +8602,10 @@
         <v>32</v>
       </c>
       <c r="O97" s="146" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="P97" s="146" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q97" s="147" t="s">
         <v>143</v>
@@ -8620,40 +8620,40 @@
         <v>236</v>
       </c>
       <c r="U97" s="146" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="98" spans="1:21" s="152" customFormat="1">
       <c r="A98" s="146" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B98" s="146"/>
       <c r="C98" s="146" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D98" s="146" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E98" s="147" t="s">
         <v>232</v>
       </c>
       <c r="F98" s="146" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G98" s="146" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H98" s="146" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I98" s="146" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="J98" s="146" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K98" s="146" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L98" s="148">
         <v>0.28999999999999998</v>
@@ -8663,10 +8663,10 @@
         <v>32</v>
       </c>
       <c r="O98" s="146" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="P98" s="146" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q98" s="147" t="s">
         <v>143</v>
@@ -8681,19 +8681,19 @@
         <v>236</v>
       </c>
       <c r="U98" s="146" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="99" spans="1:21" s="152" customFormat="1">
       <c r="A99" s="146" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B99" s="146"/>
       <c r="C99" s="146" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D99" s="146" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E99" s="147" t="s">
         <v>232</v>
@@ -8702,19 +8702,19 @@
         <v>137</v>
       </c>
       <c r="G99" s="146" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H99" s="146" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I99" s="146" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="J99" s="146" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K99" s="146" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L99" s="148">
         <v>0.28999999999999998</v>
@@ -8724,10 +8724,10 @@
         <v>32</v>
       </c>
       <c r="O99" s="146" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="P99" s="146" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q99" s="147" t="s">
         <v>143</v>
@@ -8742,40 +8742,40 @@
         <v>236</v>
       </c>
       <c r="U99" s="146" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="100" spans="1:21" s="152" customFormat="1">
       <c r="A100" s="139" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B100" s="146"/>
       <c r="C100" s="146" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D100" s="146" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E100" s="147" t="s">
         <v>232</v>
       </c>
       <c r="F100" s="146" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G100" s="146" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H100" s="146" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I100" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J100" s="146" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K100" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L100" s="145">
         <v>0.27</v>
@@ -8785,10 +8785,10 @@
         <v>32</v>
       </c>
       <c r="O100" s="146" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="P100" s="146" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="Q100" s="147" t="s">
         <v>143</v>
@@ -8806,35 +8806,35 @@
     </row>
     <row r="101" spans="1:21">
       <c r="A101" s="139" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B101" s="3"/>
       <c r="C101" s="146" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D101" s="146" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E101" s="147" t="s">
         <v>232</v>
       </c>
       <c r="F101" s="146" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G101" s="146" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H101" s="146" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I101" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J101" s="146" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K101" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L101" s="145">
         <v>0.27</v>
@@ -8844,10 +8844,10 @@
         <v>32</v>
       </c>
       <c r="O101" s="146" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="P101" s="146" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q101" s="147" t="s">
         <v>143</v>
@@ -8865,35 +8865,35 @@
     </row>
     <row r="102" spans="1:21">
       <c r="A102" s="139" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B102" s="3"/>
       <c r="C102" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D102" s="146" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E102" s="147" t="s">
         <v>232</v>
       </c>
       <c r="F102" s="146" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G102" s="146" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H102" s="146" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I102" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J102" s="146" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K102" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L102" s="145">
         <v>0.27</v>
@@ -8903,10 +8903,10 @@
         <v>32</v>
       </c>
       <c r="O102" s="146" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="P102" s="146" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q102" s="147" t="s">
         <v>143</v>
@@ -29219,13 +29219,13 @@
     </row>
     <row r="10" spans="1:39">
       <c r="A10" s="122" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B10" s="122" t="s">
         <v>179</v>
       </c>
       <c r="C10" s="122" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D10" s="122" t="s">
         <v>213</v>
@@ -29237,13 +29237,13 @@
         <v>137</v>
       </c>
       <c r="G10" s="122" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H10" s="121" t="s">
         <v>181</v>
       </c>
       <c r="I10" s="122" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J10" s="122" t="s">
         <v>234</v>
@@ -29261,10 +29261,10 @@
         <v>32</v>
       </c>
       <c r="O10" s="136" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P10" s="122" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Q10" s="122" t="s">
         <v>143</v>
@@ -29279,7 +29279,7 @@
         <v>236</v>
       </c>
       <c r="U10" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="V10" s="137"/>
       <c r="W10" s="137"/>
@@ -29302,13 +29302,13 @@
     </row>
     <row r="11" spans="1:39">
       <c r="A11" s="122" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B11" s="122" t="s">
         <v>179</v>
       </c>
       <c r="C11" s="122" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D11" s="122" t="s">
         <v>213</v>
@@ -29320,13 +29320,13 @@
         <v>137</v>
       </c>
       <c r="G11" s="122" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H11" s="121" t="s">
         <v>181</v>
       </c>
       <c r="I11" s="122" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J11" s="122" t="s">
         <v>234</v>
@@ -29344,10 +29344,10 @@
         <v>32</v>
       </c>
       <c r="O11" s="136" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="P11" s="122" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Q11" s="122" t="s">
         <v>143</v>
@@ -29362,7 +29362,7 @@
         <v>236</v>
       </c>
       <c r="U11" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="V11" s="137"/>
       <c r="W11" s="137"/>
@@ -29385,13 +29385,13 @@
     </row>
     <row r="12" spans="1:39">
       <c r="A12" s="122" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B12" s="122" t="s">
         <v>179</v>
       </c>
       <c r="C12" s="122" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D12" s="122" t="s">
         <v>213</v>
@@ -29403,13 +29403,13 @@
         <v>137</v>
       </c>
       <c r="G12" s="122" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H12" s="121" t="s">
         <v>181</v>
       </c>
       <c r="I12" s="122" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J12" s="122" t="s">
         <v>234</v>
@@ -29427,10 +29427,10 @@
         <v>32</v>
       </c>
       <c r="O12" s="136" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P12" s="122" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q12" s="122" t="s">
         <v>143</v>
@@ -29475,7 +29475,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -29483,15 +29483,15 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" spans="1:11">
       <c r="E2" t="s">
+        <v>282</v>
+      </c>
+      <c r="F2" t="s">
         <v>283</v>
-      </c>
-      <c r="F2" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -29570,18 +29570,18 @@
     </row>
     <row r="10" spans="1:11">
       <c r="A10" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:11">
       <c r="E11" t="s">
+        <v>282</v>
+      </c>
+      <c r="F11" t="s">
         <v>283</v>
       </c>
-      <c r="F11" t="s">
+      <c r="I11" t="s">
         <v>284</v>
-      </c>
-      <c r="I11" t="s">
-        <v>285</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -29643,10 +29643,10 @@
         <v>0.03</v>
       </c>
       <c r="J14" t="s">
+        <v>282</v>
+      </c>
+      <c r="K14" t="s">
         <v>283</v>
-      </c>
-      <c r="K14" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -29692,18 +29692,18 @@
     </row>
     <row r="19" spans="1:6">
       <c r="A19" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="20" spans="1:6">
       <c r="C20" t="s">
+        <v>281</v>
+      </c>
+      <c r="E20" t="s">
         <v>282</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>283</v>
-      </c>
-      <c r="F20" t="s">
-        <v>284</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -29810,13 +29810,13 @@
   <sheetData>
     <row r="1" spans="1:39">
       <c r="A1" s="122" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B1" s="122" t="s">
         <v>179</v>
       </c>
       <c r="C1" s="122" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D1" s="122" t="s">
         <v>213</v>
@@ -29828,13 +29828,13 @@
         <v>137</v>
       </c>
       <c r="G1" s="122" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H1" s="121" t="s">
         <v>181</v>
       </c>
       <c r="I1" s="122" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J1" s="122" t="s">
         <v>234</v>
@@ -29852,10 +29852,10 @@
         <v>32</v>
       </c>
       <c r="O1" s="136" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P1" s="122" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Q1" s="122" t="s">
         <v>143</v>
@@ -29870,7 +29870,7 @@
         <v>236</v>
       </c>
       <c r="U1" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="V1" s="137"/>
       <c r="W1" s="137"/>
@@ -29893,13 +29893,13 @@
     </row>
     <row r="2" spans="1:39">
       <c r="A2" s="122" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B2" s="122" t="s">
         <v>179</v>
       </c>
       <c r="C2" s="122" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D2" s="122" t="s">
         <v>213</v>
@@ -29911,13 +29911,13 @@
         <v>137</v>
       </c>
       <c r="G2" s="122" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H2" s="121" t="s">
         <v>181</v>
       </c>
       <c r="I2" s="122" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J2" s="122" t="s">
         <v>234</v>
@@ -29935,10 +29935,10 @@
         <v>32</v>
       </c>
       <c r="O2" s="136" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="P2" s="122" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Q2" s="122" t="s">
         <v>143</v>
@@ -29953,7 +29953,7 @@
         <v>236</v>
       </c>
       <c r="U2" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="V2" s="137"/>
       <c r="W2" s="137"/>
@@ -29976,13 +29976,13 @@
     </row>
     <row r="3" spans="1:39">
       <c r="A3" s="122" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B3" s="122" t="s">
         <v>179</v>
       </c>
       <c r="C3" s="122" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D3" s="122" t="s">
         <v>213</v>
@@ -29994,13 +29994,13 @@
         <v>137</v>
       </c>
       <c r="G3" s="122" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H3" s="121" t="s">
         <v>181</v>
       </c>
       <c r="I3" s="122" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J3" s="122" t="s">
         <v>234</v>
@@ -30018,10 +30018,10 @@
         <v>32</v>
       </c>
       <c r="O3" s="136" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P3" s="122" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q3" s="122" t="s">
         <v>143</v>
@@ -30059,7 +30059,7 @@
     </row>
     <row r="4" spans="1:39">
       <c r="A4" s="4" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B4" s="51"/>
       <c r="C4" s="51"/>
@@ -30102,35 +30102,35 @@
     </row>
     <row r="5" spans="1:39" s="152" customFormat="1">
       <c r="A5" s="146" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B5" s="146"/>
       <c r="C5" s="146" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D5" s="146" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E5" s="147" t="s">
         <v>232</v>
       </c>
       <c r="F5" s="146" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G5" s="146" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H5" s="146" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I5" s="146" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="J5" s="146" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K5" s="146" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="L5" s="148">
         <v>0.35</v>
@@ -30140,10 +30140,10 @@
         <v>32</v>
       </c>
       <c r="O5" s="146" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="P5" s="146" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q5" s="147" t="s">
         <v>143</v>
@@ -30158,43 +30158,43 @@
         <v>236</v>
       </c>
       <c r="U5" s="146" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="V5" s="151" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="6" spans="1:39" s="152" customFormat="1">
       <c r="A6" s="146" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B6" s="146"/>
       <c r="C6" s="146" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D6" s="146" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E6" s="147" t="s">
         <v>232</v>
       </c>
       <c r="F6" s="146" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G6" s="146" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H6" s="146" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I6" s="146" t="s">
+        <v>329</v>
+      </c>
+      <c r="J6" s="146" t="s">
+        <v>287</v>
+      </c>
+      <c r="K6" s="146" t="s">
         <v>330</v>
-      </c>
-      <c r="J6" s="146" t="s">
-        <v>288</v>
-      </c>
-      <c r="K6" s="146" t="s">
-        <v>331</v>
       </c>
       <c r="L6" s="148">
         <v>0.33</v>
@@ -30204,10 +30204,10 @@
         <v>32</v>
       </c>
       <c r="O6" s="146" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="P6" s="146" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q6" s="147" t="s">
         <v>143</v>
@@ -30222,40 +30222,40 @@
         <v>236</v>
       </c>
       <c r="U6" s="146" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="7" spans="1:39" s="152" customFormat="1">
       <c r="A7" s="146" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B7" s="146"/>
       <c r="C7" s="146" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D7" s="146" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E7" s="147" t="s">
         <v>232</v>
       </c>
       <c r="F7" s="146" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G7" s="146" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H7" s="146" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I7" s="146" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="J7" s="146" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K7" s="146" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L7" s="148">
         <v>0.28999999999999998</v>
@@ -30265,10 +30265,10 @@
         <v>32</v>
       </c>
       <c r="O7" s="146" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="P7" s="146" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q7" s="147" t="s">
         <v>143</v>
@@ -30283,19 +30283,19 @@
         <v>236</v>
       </c>
       <c r="U7" s="146" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="8" spans="1:39" s="152" customFormat="1">
       <c r="A8" s="146" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B8" s="146"/>
       <c r="C8" s="146" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D8" s="146" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E8" s="147" t="s">
         <v>232</v>
@@ -30304,19 +30304,19 @@
         <v>137</v>
       </c>
       <c r="G8" s="146" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H8" s="146" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I8" s="146" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="J8" s="146" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K8" s="146" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L8" s="148">
         <v>0.28999999999999998</v>
@@ -30326,10 +30326,10 @@
         <v>32</v>
       </c>
       <c r="O8" s="146" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="P8" s="146" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q8" s="147" t="s">
         <v>143</v>
@@ -30344,40 +30344,40 @@
         <v>236</v>
       </c>
       <c r="U8" s="146" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="9" spans="1:39" s="152" customFormat="1">
       <c r="A9" s="139" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B9" s="146"/>
       <c r="C9" s="146" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D9" s="146" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E9" s="147" t="s">
         <v>232</v>
       </c>
       <c r="F9" s="146" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G9" s="146" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H9" s="146" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I9" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J9" s="146" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K9" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L9" s="145">
         <v>0.27</v>
@@ -30387,10 +30387,10 @@
         <v>32</v>
       </c>
       <c r="O9" s="146" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="P9" s="146" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="Q9" s="147" t="s">
         <v>143</v>
@@ -30408,35 +30408,35 @@
     </row>
     <row r="10" spans="1:39">
       <c r="A10" s="139" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B10" s="12"/>
       <c r="C10" s="146" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D10" s="146" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E10" s="147" t="s">
         <v>232</v>
       </c>
       <c r="F10" s="146" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G10" s="146" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H10" s="146" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I10" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J10" s="146" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K10" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L10" s="145">
         <v>0.27</v>
@@ -30446,10 +30446,10 @@
         <v>32</v>
       </c>
       <c r="O10" s="146" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="P10" s="146" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q10" s="147" t="s">
         <v>143</v>
@@ -30467,35 +30467,35 @@
     </row>
     <row r="11" spans="1:39">
       <c r="A11" s="139" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="12" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D11" s="146" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="E11" s="147" t="s">
         <v>232</v>
       </c>
       <c r="F11" s="146" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G11" s="146" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H11" s="146" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I11" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J11" s="146" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K11" s="12" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="L11" s="145">
         <v>0.27</v>
@@ -30505,10 +30505,10 @@
         <v>32</v>
       </c>
       <c r="O11" s="146" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="P11" s="146" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="Q11" s="147" t="s">
         <v>143</v>
@@ -30548,16 +30548,16 @@
   <sheetData>
     <row r="1" spans="1:39">
       <c r="A1" s="122" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B1" s="122">
         <v>111</v>
       </c>
       <c r="C1" s="122" t="s">
+        <v>264</v>
+      </c>
+      <c r="D1" s="122" t="s">
         <v>265</v>
-      </c>
-      <c r="D1" s="122" t="s">
-        <v>266</v>
       </c>
       <c r="E1" s="122" t="s">
         <v>232</v>
@@ -30566,13 +30566,13 @@
         <v>137</v>
       </c>
       <c r="G1" s="122" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H1" s="121" t="s">
         <v>181</v>
       </c>
       <c r="I1" s="122" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J1" s="122" t="s">
         <v>234</v>
@@ -30590,10 +30590,10 @@
         <v>32</v>
       </c>
       <c r="O1" s="136" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="P1" s="122" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q1" s="122" t="s">
         <v>143</v>
@@ -30611,7 +30611,7 @@
         <v>158</v>
       </c>
       <c r="V1" s="137" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="W1" s="137"/>
       <c r="X1" s="137"/>
@@ -30633,16 +30633,16 @@
     </row>
     <row r="2" spans="1:39">
       <c r="A2" s="122" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B2" s="122">
         <v>121</v>
       </c>
       <c r="C2" s="122" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D2" s="122" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E2" s="122" t="s">
         <v>232</v>
@@ -30651,13 +30651,13 @@
         <v>137</v>
       </c>
       <c r="G2" s="122" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H2" s="121" t="s">
         <v>181</v>
       </c>
       <c r="I2" s="122" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J2" s="122" t="s">
         <v>234</v>
@@ -30675,10 +30675,10 @@
         <v>32</v>
       </c>
       <c r="O2" s="136" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="P2" s="122" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q2" s="122" t="s">
         <v>143</v>
@@ -30866,7 +30866,7 @@
         <v>32</v>
       </c>
       <c r="O2" s="129" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="P2" s="87" t="s">
         <v>168</v>
@@ -31370,7 +31370,7 @@
         <v>32</v>
       </c>
       <c r="O8" s="136" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="P8" s="122" t="s">
         <v>229</v>
@@ -31455,7 +31455,7 @@
         <v>32</v>
       </c>
       <c r="O9" s="136" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="P9" s="122" t="s">
         <v>229</v>
@@ -31498,13 +31498,13 @@
     </row>
     <row r="10" spans="1:39">
       <c r="A10" s="122" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B10" s="122" t="s">
         <v>179</v>
       </c>
       <c r="C10" s="122" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D10" s="122" t="s">
         <v>213</v>
@@ -31516,13 +31516,13 @@
         <v>137</v>
       </c>
       <c r="G10" s="122" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H10" s="121" t="s">
         <v>181</v>
       </c>
       <c r="I10" s="122" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J10" s="122" t="s">
         <v>234</v>
@@ -31540,10 +31540,10 @@
         <v>32</v>
       </c>
       <c r="O10" s="136" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="P10" s="122" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Q10" s="122" t="s">
         <v>143</v>
@@ -31558,7 +31558,7 @@
         <v>236</v>
       </c>
       <c r="U10" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="V10" s="137"/>
       <c r="W10" s="137"/>
@@ -31581,13 +31581,13 @@
     </row>
     <row r="11" spans="1:39">
       <c r="A11" s="122" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B11" s="122" t="s">
         <v>179</v>
       </c>
       <c r="C11" s="122" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D11" s="122" t="s">
         <v>213</v>
@@ -31599,13 +31599,13 @@
         <v>137</v>
       </c>
       <c r="G11" s="122" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H11" s="121" t="s">
         <v>181</v>
       </c>
       <c r="I11" s="122" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="J11" s="122" t="s">
         <v>234</v>
@@ -31623,10 +31623,10 @@
         <v>32</v>
       </c>
       <c r="O11" s="136" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="P11" s="122" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="Q11" s="122" t="s">
         <v>143</v>
@@ -31641,7 +31641,7 @@
         <v>236</v>
       </c>
       <c r="U11" s="11" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="V11" s="137"/>
       <c r="W11" s="137"/>
@@ -31664,13 +31664,13 @@
     </row>
     <row r="12" spans="1:39">
       <c r="A12" s="122" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B12" s="122" t="s">
         <v>179</v>
       </c>
       <c r="C12" s="122" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="D12" s="122" t="s">
         <v>213</v>
@@ -31682,13 +31682,13 @@
         <v>137</v>
       </c>
       <c r="G12" s="122" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="H12" s="121" t="s">
         <v>181</v>
       </c>
       <c r="I12" s="122" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="J12" s="122" t="s">
         <v>234</v>
@@ -31706,10 +31706,10 @@
         <v>32</v>
       </c>
       <c r="O12" s="136" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="P12" s="122" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="Q12" s="122" t="s">
         <v>143</v>
@@ -32102,9 +32102,9 @@
       <c r="AL4" s="137"/>
       <c r="AM4" s="137"/>
     </row>
-    <row r="5" spans="1:39" ht="15.75">
+    <row r="5" spans="1:39">
       <c r="A5" s="4" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B5" s="51"/>
       <c r="C5" s="51"/>
@@ -32145,13 +32145,13 @@
       <c r="AL5" s="8"/>
       <c r="AM5" s="8"/>
     </row>
-    <row r="6" spans="1:39" s="144" customFormat="1" ht="15.75">
+    <row r="6" spans="1:39" s="144" customFormat="1">
       <c r="A6" s="139" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B6" s="139"/>
       <c r="C6" s="139" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D6" s="139" t="s">
         <v>188</v>
@@ -32160,19 +32160,19 @@
         <v>232</v>
       </c>
       <c r="F6" s="139" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G6" s="139" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H6" s="139" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I6" s="139" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J6" s="139" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K6" s="139" t="s">
         <v>171</v>
@@ -32185,10 +32185,10 @@
         <v>32</v>
       </c>
       <c r="O6" s="139" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="P6" s="139" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="Q6" s="140" t="s">
         <v>143</v>
@@ -32203,16 +32203,16 @@
         <v>236</v>
       </c>
       <c r="U6" s="12" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="7" spans="1:39" s="144" customFormat="1" ht="15.75">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="7" spans="1:39" s="144" customFormat="1">
       <c r="A7" s="139" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B7" s="139"/>
       <c r="C7" s="139" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D7" s="139" t="s">
         <v>188</v>
@@ -32221,22 +32221,22 @@
         <v>232</v>
       </c>
       <c r="F7" s="139" t="s">
+        <v>292</v>
+      </c>
+      <c r="G7" s="139" t="s">
+        <v>291</v>
+      </c>
+      <c r="H7" s="139" t="s">
+        <v>289</v>
+      </c>
+      <c r="I7" s="139" t="s">
+        <v>288</v>
+      </c>
+      <c r="J7" s="139" t="s">
+        <v>287</v>
+      </c>
+      <c r="K7" s="139" t="s">
         <v>293</v>
-      </c>
-      <c r="G7" s="139" t="s">
-        <v>292</v>
-      </c>
-      <c r="H7" s="139" t="s">
-        <v>290</v>
-      </c>
-      <c r="I7" s="139" t="s">
-        <v>289</v>
-      </c>
-      <c r="J7" s="139" t="s">
-        <v>288</v>
-      </c>
-      <c r="K7" s="139" t="s">
-        <v>294</v>
       </c>
       <c r="L7" s="141">
         <v>0.41</v>
@@ -32246,10 +32246,10 @@
         <v>32</v>
       </c>
       <c r="O7" s="139" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="P7" s="139" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="Q7" s="140" t="s">
         <v>143</v>
@@ -32264,16 +32264,16 @@
         <v>236</v>
       </c>
       <c r="U7" s="12" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="8" spans="1:39" s="144" customFormat="1" ht="15.75">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="8" spans="1:39" s="144" customFormat="1">
       <c r="A8" s="139" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="B8" s="139"/>
       <c r="C8" s="139" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D8" s="139" t="s">
         <v>188</v>
@@ -32282,22 +32282,22 @@
         <v>232</v>
       </c>
       <c r="F8" s="139" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G8" s="139" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H8" s="139" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I8" s="139" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J8" s="139" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K8" s="139" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="L8" s="141">
         <v>0.41</v>
@@ -32307,10 +32307,10 @@
         <v>32</v>
       </c>
       <c r="O8" s="139" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="P8" s="139" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="Q8" s="140" t="s">
         <v>143</v>
@@ -32325,16 +32325,16 @@
         <v>236</v>
       </c>
       <c r="U8" s="12" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="9" spans="1:39" s="144" customFormat="1" ht="15.75">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="9" spans="1:39" s="144" customFormat="1">
       <c r="A9" s="139" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B9" s="139"/>
       <c r="C9" s="139" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D9" s="139" t="s">
         <v>188</v>
@@ -32343,22 +32343,22 @@
         <v>232</v>
       </c>
       <c r="F9" s="139" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G9" s="139" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H9" s="139" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I9" s="139" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="J9" s="139" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K9" s="139" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="L9" s="141">
         <v>0.42</v>
@@ -32368,10 +32368,10 @@
         <v>32</v>
       </c>
       <c r="O9" s="139" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="P9" s="139" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="Q9" s="140" t="s">
         <v>143</v>
@@ -32386,12 +32386,12 @@
         <v>236</v>
       </c>
       <c r="U9" s="12" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="10" spans="1:39" ht="15.75">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39">
       <c r="A10" s="4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B10" s="51"/>
       <c r="C10" s="51"/>
@@ -32432,13 +32432,13 @@
       <c r="AL10" s="8"/>
       <c r="AM10" s="8"/>
     </row>
-    <row r="11" spans="1:39" ht="15.75">
+    <row r="11" spans="1:39">
       <c r="A11" s="139" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B11" s="12"/>
       <c r="C11" s="139" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D11" s="139" t="s">
         <v>188</v>
@@ -32447,22 +32447,22 @@
         <v>232</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G11" s="139" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H11" s="139" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I11" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="J11" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="K11" s="12" t="s">
         <v>304</v>
-      </c>
-      <c r="J11" s="12" t="s">
-        <v>288</v>
-      </c>
-      <c r="K11" s="12" t="s">
-        <v>305</v>
       </c>
       <c r="L11" s="145">
         <v>0.37</v>
@@ -32472,10 +32472,10 @@
         <v>32</v>
       </c>
       <c r="O11" s="139" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="P11" s="12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="Q11" s="140" t="s">
         <v>143</v>
@@ -32490,16 +32490,16 @@
         <v>236</v>
       </c>
       <c r="U11" s="12" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="12" spans="1:39" ht="15.75">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39">
       <c r="A12" s="139" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B12" s="12"/>
       <c r="C12" s="139" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D12" s="139" t="s">
         <v>188</v>
@@ -32508,22 +32508,22 @@
         <v>232</v>
       </c>
       <c r="F12" s="12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G12" s="139" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H12" s="139" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I12" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J12" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K12" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L12" s="145">
         <v>0.35</v>
@@ -32533,10 +32533,10 @@
         <v>32</v>
       </c>
       <c r="O12" s="139" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="P12" s="12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="Q12" s="140" t="s">
         <v>143</v>
@@ -32551,16 +32551,16 @@
         <v>236</v>
       </c>
       <c r="U12" s="12" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="13" spans="1:39" ht="15.75">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="13" spans="1:39">
       <c r="A13" s="139" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B13" s="12"/>
       <c r="C13" s="139" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D13" s="139" t="s">
         <v>188</v>
@@ -32569,22 +32569,22 @@
         <v>232</v>
       </c>
       <c r="F13" s="12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G13" s="139" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H13" s="139" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I13" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K13" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L13" s="145">
         <v>0.41</v>
@@ -32594,10 +32594,10 @@
         <v>32</v>
       </c>
       <c r="O13" s="139" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="P13" s="12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="Q13" s="140" t="s">
         <v>143</v>
@@ -32612,16 +32612,16 @@
         <v>236</v>
       </c>
       <c r="U13" s="12" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="14" spans="1:39" ht="15.75">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="14" spans="1:39">
       <c r="A14" s="139" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B14" s="12"/>
       <c r="C14" s="139" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="D14" s="139" t="s">
         <v>188</v>
@@ -32630,22 +32630,22 @@
         <v>232</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G14" s="139" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H14" s="139" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="I14" s="12" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="J14" s="12" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="K14" s="12" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="L14" s="145">
         <v>0.41</v>
@@ -32655,10 +32655,10 @@
         <v>32</v>
       </c>
       <c r="O14" s="139" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="P14" s="12" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="Q14" s="140" t="s">
         <v>143</v>
@@ -32673,7 +32673,7 @@
         <v>236</v>
       </c>
       <c r="U14" s="12" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
data updates to PK tab
</commit_message>
<xml_diff>
--- a/data_25_01_14.xlsx
+++ b/data_25_01_14.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/preeyakhanna/code_khannalab/Strain-Sensor-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06D3E42-5B17-7143-AE76-68B895C59C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{239D2CDE-BC71-8942-AE20-2B3540D437C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="22240" windowWidth="30240" windowHeight="19000" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2840" yWindow="640" windowWidth="27400" windowHeight="19000" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all data" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2774" uniqueCount="349">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2793" uniqueCount="349">
   <si>
     <t>Sample Name</t>
   </si>
@@ -1907,8 +1907,8 @@
   <dimension ref="A1:AM989"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A64" sqref="A64:XFD64"/>
+      <pane ySplit="1" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A48" sqref="A48:XFD48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -30730,7 +30730,7 @@
   <dimension ref="A1:AM12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -31758,14 +31758,15 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C6FF399-B898-9B4D-9BEA-88752D6153C6}">
-  <dimension ref="A1:AM15"/>
+  <dimension ref="A1:AM17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
+    <col min="1" max="1" width="30.5" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" customWidth="1"/>
     <col min="15" max="15" width="51" customWidth="1"/>
   </cols>
@@ -32609,6 +32610,89 @@
       <c r="U15" s="129" t="s">
         <v>327</v>
       </c>
+    </row>
+    <row r="17" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A17" s="72" t="s">
+        <v>270</v>
+      </c>
+      <c r="B17" s="72" t="s">
+        <v>179</v>
+      </c>
+      <c r="C17" s="72" t="s">
+        <v>271</v>
+      </c>
+      <c r="D17" s="72" t="s">
+        <v>213</v>
+      </c>
+      <c r="E17" s="72" t="s">
+        <v>232</v>
+      </c>
+      <c r="F17" s="72" t="s">
+        <v>137</v>
+      </c>
+      <c r="G17" s="72" t="s">
+        <v>266</v>
+      </c>
+      <c r="H17" s="71" t="s">
+        <v>181</v>
+      </c>
+      <c r="I17" s="72" t="s">
+        <v>267</v>
+      </c>
+      <c r="J17" s="72" t="s">
+        <v>234</v>
+      </c>
+      <c r="K17" s="72" t="s">
+        <v>171</v>
+      </c>
+      <c r="L17" s="73">
+        <v>0.39</v>
+      </c>
+      <c r="M17" s="72">
+        <v>1</v>
+      </c>
+      <c r="N17" s="94" t="s">
+        <v>32</v>
+      </c>
+      <c r="O17" s="94" t="s">
+        <v>272</v>
+      </c>
+      <c r="P17" s="72" t="s">
+        <v>262</v>
+      </c>
+      <c r="Q17" s="72" t="s">
+        <v>143</v>
+      </c>
+      <c r="R17" s="72" t="s">
+        <v>36</v>
+      </c>
+      <c r="S17" s="76" t="s">
+        <v>132</v>
+      </c>
+      <c r="T17" s="10" t="s">
+        <v>236</v>
+      </c>
+      <c r="U17" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="V17" s="95"/>
+      <c r="W17" s="95"/>
+      <c r="X17" s="95"/>
+      <c r="Y17" s="95"/>
+      <c r="Z17" s="95"/>
+      <c r="AA17" s="95"/>
+      <c r="AB17" s="95"/>
+      <c r="AC17" s="95"/>
+      <c r="AD17" s="95"/>
+      <c r="AE17" s="95"/>
+      <c r="AF17" s="95"/>
+      <c r="AG17" s="95"/>
+      <c r="AH17" s="95"/>
+      <c r="AI17" s="95"/>
+      <c r="AJ17" s="95"/>
+      <c r="AK17" s="95"/>
+      <c r="AL17" s="95"/>
+      <c r="AM17" s="95"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
New voltage divider circuit and retests
</commit_message>
<xml_diff>
--- a/data_25_01_14.xlsx
+++ b/data_25_01_14.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csuma-my.sharepoint.com/personal/toppenheim_csum_edu/Documents/Documents/GitHub/Strain-Sensor-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="322" documentId="13_ncr:1_{C06D3E42-5B17-7143-AE76-68B895C59C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{704E279C-AB48-4AE3-83E2-85EDBEDC80E8}"/>
+  <xr:revisionPtr revIDLastSave="464" documentId="13_ncr:1_{C06D3E42-5B17-7143-AE76-68B895C59C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60C961E0-77BE-46B5-94A1-45984602831C}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2970" uniqueCount="393">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3061" uniqueCount="415">
   <si>
     <t>Sample Name</t>
   </si>
@@ -1218,7 +1218,73 @@
     <t>CSV Data/3_18_25/Bending_data_abs_1p758_retest_v4_3_18_25.csv</t>
   </si>
   <si>
-    <t>data noise looks good but looks like sample not mounted correctly? ?</t>
+    <t>data noise looks good but looks like sample not mounted correctly? ? Slack</t>
+  </si>
+  <si>
+    <t>3_20_25</t>
+  </si>
+  <si>
+    <t>abs_1p758_retest_v5</t>
+  </si>
+  <si>
+    <t>retest</t>
+  </si>
+  <si>
+    <t>71.8F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volt Div:  8x amp with 16 bit encoding, 3.3V exc (not Vref) and 50 ohm (not 100 ohm) divider </t>
+  </si>
+  <si>
+    <t>CSV Data/3_20_25/Bending_data_abs_1p758_retest_v5_3_20_25.csv</t>
+  </si>
+  <si>
+    <t>very low noise/variance, slack in sample</t>
+  </si>
+  <si>
+    <t>CSV Data/3_20_25/Bending_data_abs_1p758_retest_v5_3_20_25.jpg</t>
+  </si>
+  <si>
+    <t>abs_1p758_retest_v6</t>
+  </si>
+  <si>
+    <t>68F</t>
+  </si>
+  <si>
+    <t>CSV Data/3_20_25/Bending_data_abs_1p758_retest_v6_3_20_25.csv</t>
+  </si>
+  <si>
+    <t>abs_1p758_retest_v7</t>
+  </si>
+  <si>
+    <t>CSV Data/3_20_25/Bending_data_abs_1p758_retest_7_3_20_25.csv</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Volt Div:  8x amp with 16 bit encoding, 3.3V exc (not Vref) and 50 ohm (not 100 ohm) divider, inst. Amp (ad620) makes &gt;10000 ADC starting </t>
+  </si>
+  <si>
+    <t>lots of hysteresis.  I think because lots of variation coming from instr. Amplifier gain pot, not sample slipping etc. sample looks totally fine</t>
+  </si>
+  <si>
+    <t>abs_1p758_retest_v8</t>
+  </si>
+  <si>
+    <t>CSV Data/3_20_25/Bending_data_abs_1p758_retest_8_3_20_25.csv</t>
+  </si>
+  <si>
+    <t>Volt Div:  8x amp with 16 bit encoding, 3.3V exc (not Vref) and 50 ohm (not 100 ohm) divider</t>
+  </si>
+  <si>
+    <t>1,987 in</t>
+  </si>
+  <si>
+    <t>CSV Data/3_20_25/Bending_data_abs_1p987_retest_4_18_25.csv</t>
+  </si>
+  <si>
+    <t>abs_1p987_retest_v3</t>
+  </si>
+  <si>
+    <t>hysteresis?  Slipping ?  I will re-test Tuesday</t>
   </si>
 </sst>
 </file>
@@ -1529,7 +1595,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="195">
+  <cellXfs count="194">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2001,14 +2067,11 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2239,8 +2302,8 @@
   <dimension ref="A1:AM988"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A86" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="V114" sqref="V114"/>
+      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -2259,8 +2322,9 @@
     <col min="15" max="15" width="103" customWidth="1"/>
     <col min="17" max="17" width="38.6640625" customWidth="1"/>
     <col min="18" max="18" width="17.5" customWidth="1"/>
-    <col min="19" max="21" width="73.5" customWidth="1"/>
-    <col min="22" max="22" width="95.6640625" customWidth="1"/>
+    <col min="19" max="19" width="113.6640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="21" width="73.5" customWidth="1"/>
+    <col min="22" max="22" width="190.27734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:39" ht="15.75" customHeight="1">
@@ -9812,258 +9876,477 @@
         <v>384</v>
       </c>
     </row>
-    <row r="113" spans="1:22" s="176" customFormat="1" ht="12.3">
-      <c r="A113" s="171" t="s">
+    <row r="113" spans="1:39" s="140" customFormat="1" ht="12.3">
+      <c r="A113" s="135" t="s">
         <v>385</v>
       </c>
-      <c r="B113" s="171"/>
-      <c r="C113" s="171" t="s">
+      <c r="B113" s="135"/>
+      <c r="C113" s="135" t="s">
         <v>355</v>
       </c>
-      <c r="D113" s="171" t="s">
+      <c r="D113" s="135" t="s">
         <v>388</v>
       </c>
-      <c r="E113" s="172" t="s">
+      <c r="E113" s="136" t="s">
         <v>232</v>
       </c>
-      <c r="F113" s="171" t="s">
+      <c r="F113" s="135" t="s">
         <v>137</v>
       </c>
-      <c r="G113" s="171" t="s">
+      <c r="G113" s="135" t="s">
         <v>291</v>
       </c>
-      <c r="H113" s="171" t="s">
+      <c r="H113" s="135" t="s">
         <v>289</v>
       </c>
-      <c r="J113" s="186" t="s">
+      <c r="J113" s="183" t="s">
         <v>287</v>
       </c>
-      <c r="K113" s="186" t="s">
+      <c r="K113" s="183" t="s">
         <v>386</v>
       </c>
-      <c r="L113" s="173">
+      <c r="L113" s="137">
         <v>0.28000000000000003</v>
       </c>
-      <c r="M113" s="171"/>
-      <c r="N113" s="171" t="s">
+      <c r="M113" s="135"/>
+      <c r="N113" s="135" t="s">
         <v>32</v>
       </c>
-      <c r="O113" s="171" t="s">
+      <c r="O113" s="135" t="s">
         <v>387</v>
       </c>
-      <c r="P113" s="171" t="s">
+      <c r="P113" s="135" t="s">
         <v>349</v>
       </c>
-      <c r="Q113" s="172" t="s">
+      <c r="Q113" s="136" t="s">
         <v>143</v>
       </c>
-      <c r="R113" s="172" t="s">
+      <c r="R113" s="136" t="s">
         <v>36</v>
       </c>
-      <c r="S113" s="174" t="s">
+      <c r="S113" s="138" t="s">
         <v>382</v>
       </c>
-      <c r="T113" s="175" t="s">
+      <c r="T113" s="139" t="s">
         <v>236</v>
       </c>
-      <c r="U113" s="171"/>
-      <c r="V113" s="192" t="s">
+      <c r="U113" s="135"/>
+      <c r="V113" s="193" t="s">
         <v>389</v>
       </c>
     </row>
-    <row r="114" spans="1:22" s="146" customFormat="1" ht="12.3">
-      <c r="A114" s="141" t="s">
+    <row r="114" spans="1:39" s="140" customFormat="1" ht="12.3">
+      <c r="A114" s="135" t="s">
         <v>390</v>
       </c>
-      <c r="B114" s="141"/>
-      <c r="C114" s="141" t="s">
+      <c r="B114" s="135"/>
+      <c r="C114" s="135" t="s">
         <v>355</v>
       </c>
-      <c r="D114" s="141" t="s">
+      <c r="D114" s="135" t="s">
         <v>388</v>
       </c>
-      <c r="E114" s="142" t="s">
+      <c r="E114" s="136" t="s">
         <v>232</v>
       </c>
-      <c r="F114" s="141" t="s">
+      <c r="F114" s="135" t="s">
         <v>137</v>
       </c>
-      <c r="G114" s="141" t="s">
+      <c r="G114" s="135" t="s">
         <v>291</v>
       </c>
-      <c r="H114" s="141" t="s">
+      <c r="H114" s="135" t="s">
         <v>289</v>
       </c>
-      <c r="I114" s="141" t="s">
+      <c r="I114" s="135" t="s">
         <v>371</v>
       </c>
-      <c r="J114" s="193" t="s">
+      <c r="J114" s="183" t="s">
         <v>287</v>
       </c>
-      <c r="K114" s="193" t="s">
+      <c r="K114" s="183" t="s">
         <v>386</v>
       </c>
-      <c r="L114" s="143">
+      <c r="L114" s="137">
         <v>0.28000000000000003</v>
       </c>
-      <c r="M114" s="141"/>
-      <c r="N114" s="141"/>
-      <c r="O114" s="141" t="s">
+      <c r="M114" s="135"/>
+      <c r="N114" s="135" t="s">
+        <v>32</v>
+      </c>
+      <c r="O114" s="135" t="s">
         <v>391</v>
       </c>
-      <c r="P114" s="141" t="s">
+      <c r="P114" s="135" t="s">
         <v>349</v>
       </c>
-      <c r="Q114" s="142" t="s">
+      <c r="Q114" s="136" t="s">
         <v>143</v>
       </c>
-      <c r="R114" s="142" t="s">
+      <c r="R114" s="136" t="s">
         <v>36</v>
       </c>
-      <c r="S114" s="144" t="s">
+      <c r="S114" s="138" t="s">
         <v>382</v>
       </c>
-      <c r="T114" s="145" t="s">
+      <c r="T114" s="139" t="s">
         <v>236</v>
       </c>
-      <c r="U114" s="141"/>
-      <c r="V114" s="194" t="s">
+      <c r="U114" s="135"/>
+      <c r="V114" s="193" t="s">
         <v>392</v>
       </c>
     </row>
-    <row r="115" spans="1:22" ht="12.3">
-      <c r="A115" s="3"/>
-      <c r="B115" s="3"/>
-      <c r="C115" s="3"/>
-      <c r="D115" s="3"/>
-      <c r="E115" s="3"/>
-      <c r="F115" s="3"/>
-      <c r="G115" s="3"/>
-      <c r="H115" s="3"/>
-      <c r="I115" s="3"/>
-      <c r="J115" s="28"/>
-      <c r="K115" s="28"/>
-      <c r="L115" s="3"/>
-      <c r="M115" s="3"/>
-      <c r="N115" s="3"/>
-      <c r="O115" s="3"/>
-      <c r="P115" s="3"/>
-      <c r="Q115" s="3"/>
-      <c r="R115" s="3"/>
-      <c r="S115" s="3"/>
-      <c r="U115" s="3"/>
-    </row>
-    <row r="116" spans="1:22" ht="12.3">
-      <c r="A116" s="3"/>
-      <c r="B116" s="3"/>
-      <c r="C116" s="3"/>
-      <c r="D116" s="3"/>
-      <c r="E116" s="3"/>
-      <c r="F116" s="3"/>
-      <c r="G116" s="3"/>
-      <c r="H116" s="3"/>
-      <c r="I116" s="3"/>
-      <c r="J116" s="28"/>
-      <c r="K116" s="28"/>
-      <c r="L116" s="3"/>
-      <c r="M116" s="3"/>
-      <c r="N116" s="3"/>
-      <c r="O116" s="3"/>
-      <c r="P116" s="3"/>
-      <c r="Q116" s="3"/>
-      <c r="R116" s="3"/>
-      <c r="S116" s="3"/>
-      <c r="U116" s="3"/>
-    </row>
-    <row r="117" spans="1:22" ht="12.3">
-      <c r="A117" s="3"/>
-      <c r="B117" s="3"/>
-      <c r="C117" s="3"/>
-      <c r="D117" s="3"/>
-      <c r="E117" s="3"/>
-      <c r="F117" s="3"/>
-      <c r="G117" s="3"/>
-      <c r="H117" s="3"/>
-      <c r="I117" s="3"/>
-      <c r="J117" s="28"/>
-      <c r="K117" s="28"/>
-      <c r="L117" s="3"/>
-      <c r="M117" s="3"/>
-      <c r="N117" s="3"/>
-      <c r="O117" s="3"/>
-      <c r="P117" s="3"/>
-      <c r="Q117" s="3"/>
-      <c r="R117" s="3"/>
-      <c r="S117" s="3"/>
-      <c r="U117" s="3"/>
-    </row>
-    <row r="118" spans="1:22" ht="12.3">
-      <c r="A118" s="3"/>
-      <c r="B118" s="3"/>
-      <c r="C118" s="3"/>
-      <c r="D118" s="3"/>
-      <c r="E118" s="3"/>
-      <c r="F118" s="3"/>
-      <c r="G118" s="3"/>
-      <c r="H118" s="3"/>
-      <c r="I118" s="3"/>
-      <c r="J118" s="28"/>
-      <c r="K118" s="28"/>
-      <c r="L118" s="3"/>
-      <c r="M118" s="3"/>
-      <c r="N118" s="3"/>
-      <c r="O118" s="3"/>
-      <c r="P118" s="3"/>
-      <c r="Q118" s="3"/>
-      <c r="R118" s="3"/>
-      <c r="S118" s="3"/>
-      <c r="U118" s="3"/>
-    </row>
-    <row r="119" spans="1:22" ht="12.3">
-      <c r="A119" s="3"/>
-      <c r="B119" s="3"/>
-      <c r="C119" s="3"/>
-      <c r="D119" s="3"/>
-      <c r="E119" s="3"/>
-      <c r="F119" s="3"/>
-      <c r="G119" s="3"/>
-      <c r="H119" s="3"/>
-      <c r="I119" s="3"/>
-      <c r="J119" s="28"/>
-      <c r="K119" s="28"/>
-      <c r="L119" s="3"/>
-      <c r="M119" s="3"/>
-      <c r="N119" s="3"/>
-      <c r="O119" s="3"/>
-      <c r="P119" s="3"/>
-      <c r="Q119" s="3"/>
-      <c r="R119" s="3"/>
-      <c r="S119" s="3"/>
-      <c r="U119" s="3"/>
-    </row>
-    <row r="120" spans="1:22" ht="12.3">
-      <c r="A120" s="3"/>
-      <c r="B120" s="3"/>
-      <c r="C120" s="3"/>
-      <c r="D120" s="3"/>
-      <c r="E120" s="3"/>
-      <c r="F120" s="3"/>
-      <c r="G120" s="3"/>
-      <c r="H120" s="3"/>
-      <c r="I120" s="3"/>
-      <c r="J120" s="28"/>
-      <c r="K120" s="28"/>
-      <c r="L120" s="3"/>
-      <c r="M120" s="3"/>
-      <c r="N120" s="3"/>
-      <c r="O120" s="3"/>
-      <c r="P120" s="3"/>
-      <c r="Q120" s="3"/>
-      <c r="R120" s="3"/>
-      <c r="S120" s="3"/>
-      <c r="U120" s="3"/>
-    </row>
-    <row r="121" spans="1:22" ht="12.3">
+    <row r="115" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A115" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="B115" s="6"/>
+      <c r="C115" s="6"/>
+      <c r="D115" s="6"/>
+      <c r="E115" s="6"/>
+      <c r="F115" s="6"/>
+      <c r="G115" s="6"/>
+      <c r="H115" s="6"/>
+      <c r="I115" s="6"/>
+      <c r="J115" s="5"/>
+      <c r="K115" s="5"/>
+      <c r="L115" s="6"/>
+      <c r="M115" s="6"/>
+      <c r="N115" s="6"/>
+      <c r="O115" s="6"/>
+      <c r="P115" s="6"/>
+      <c r="Q115" s="6"/>
+      <c r="R115" s="6"/>
+      <c r="S115" s="6"/>
+      <c r="T115" s="7"/>
+      <c r="U115" s="6"/>
+      <c r="V115" s="7"/>
+      <c r="W115" s="7"/>
+      <c r="X115" s="7"/>
+      <c r="Y115" s="7"/>
+      <c r="Z115" s="7"/>
+      <c r="AA115" s="7"/>
+      <c r="AB115" s="7"/>
+      <c r="AC115" s="7"/>
+      <c r="AD115" s="7"/>
+      <c r="AE115" s="7"/>
+      <c r="AF115" s="7"/>
+      <c r="AG115" s="7"/>
+      <c r="AH115" s="7"/>
+      <c r="AI115" s="7"/>
+      <c r="AJ115" s="7"/>
+      <c r="AK115" s="7"/>
+      <c r="AL115" s="7"/>
+      <c r="AM115" s="7"/>
+    </row>
+    <row r="116" spans="1:39" s="140" customFormat="1" ht="12.3">
+      <c r="A116" s="135" t="s">
+        <v>394</v>
+      </c>
+      <c r="B116" s="135"/>
+      <c r="C116" s="135" t="s">
+        <v>395</v>
+      </c>
+      <c r="D116" s="135" t="s">
+        <v>388</v>
+      </c>
+      <c r="E116" s="136" t="s">
+        <v>232</v>
+      </c>
+      <c r="F116" s="135" t="s">
+        <v>137</v>
+      </c>
+      <c r="G116" s="135" t="s">
+        <v>291</v>
+      </c>
+      <c r="H116" s="135" t="s">
+        <v>289</v>
+      </c>
+      <c r="I116" s="135" t="s">
+        <v>371</v>
+      </c>
+      <c r="J116" s="183" t="s">
+        <v>287</v>
+      </c>
+      <c r="K116" s="183" t="s">
+        <v>396</v>
+      </c>
+      <c r="L116" s="137">
+        <v>0.35</v>
+      </c>
+      <c r="M116" s="135"/>
+      <c r="N116" s="135" t="s">
+        <v>32</v>
+      </c>
+      <c r="O116" s="135" t="s">
+        <v>398</v>
+      </c>
+      <c r="P116" s="135" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q116" s="136" t="s">
+        <v>143</v>
+      </c>
+      <c r="R116" s="136" t="s">
+        <v>36</v>
+      </c>
+      <c r="S116" s="138" t="s">
+        <v>397</v>
+      </c>
+      <c r="T116" s="139" t="s">
+        <v>236</v>
+      </c>
+      <c r="U116" s="135" t="s">
+        <v>400</v>
+      </c>
+      <c r="V116" s="140" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="117" spans="1:39" s="176" customFormat="1" ht="12.3">
+      <c r="A117" s="171" t="s">
+        <v>401</v>
+      </c>
+      <c r="B117" s="171"/>
+      <c r="C117" s="171" t="s">
+        <v>395</v>
+      </c>
+      <c r="D117" s="171" t="s">
+        <v>388</v>
+      </c>
+      <c r="E117" s="172" t="s">
+        <v>232</v>
+      </c>
+      <c r="F117" s="171" t="s">
+        <v>137</v>
+      </c>
+      <c r="G117" s="171" t="s">
+        <v>291</v>
+      </c>
+      <c r="H117" s="171" t="s">
+        <v>289</v>
+      </c>
+      <c r="I117" s="171" t="s">
+        <v>371</v>
+      </c>
+      <c r="J117" s="186" t="s">
+        <v>287</v>
+      </c>
+      <c r="K117" s="186" t="s">
+        <v>402</v>
+      </c>
+      <c r="L117" s="173">
+        <v>0.36</v>
+      </c>
+      <c r="M117" s="171"/>
+      <c r="N117" s="171" t="s">
+        <v>32</v>
+      </c>
+      <c r="O117" s="171" t="s">
+        <v>403</v>
+      </c>
+      <c r="P117" s="171" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q117" s="172" t="s">
+        <v>143</v>
+      </c>
+      <c r="R117" s="172" t="s">
+        <v>36</v>
+      </c>
+      <c r="S117" s="174" t="s">
+        <v>397</v>
+      </c>
+      <c r="T117" s="175" t="s">
+        <v>236</v>
+      </c>
+      <c r="U117" s="171"/>
+    </row>
+    <row r="118" spans="1:39" s="169" customFormat="1" ht="12.3">
+      <c r="A118" s="164" t="s">
+        <v>404</v>
+      </c>
+      <c r="B118" s="164"/>
+      <c r="C118" s="164" t="s">
+        <v>395</v>
+      </c>
+      <c r="D118" s="164" t="s">
+        <v>388</v>
+      </c>
+      <c r="E118" s="165" t="s">
+        <v>232</v>
+      </c>
+      <c r="F118" s="164" t="s">
+        <v>137</v>
+      </c>
+      <c r="G118" s="164" t="s">
+        <v>291</v>
+      </c>
+      <c r="H118" s="164" t="s">
+        <v>289</v>
+      </c>
+      <c r="I118" s="164" t="s">
+        <v>371</v>
+      </c>
+      <c r="J118" s="187" t="s">
+        <v>287</v>
+      </c>
+      <c r="K118" s="187" t="s">
+        <v>361</v>
+      </c>
+      <c r="L118" s="166">
+        <v>0.33</v>
+      </c>
+      <c r="M118" s="164"/>
+      <c r="N118" s="164" t="s">
+        <v>155</v>
+      </c>
+      <c r="O118" s="164" t="s">
+        <v>405</v>
+      </c>
+      <c r="P118" s="164" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q118" s="165" t="s">
+        <v>143</v>
+      </c>
+      <c r="R118" s="165" t="s">
+        <v>36</v>
+      </c>
+      <c r="S118" s="167" t="s">
+        <v>406</v>
+      </c>
+      <c r="T118" s="168" t="s">
+        <v>236</v>
+      </c>
+      <c r="U118" s="164"/>
+      <c r="V118" s="169" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="119" spans="1:39" s="176" customFormat="1" ht="12.3">
+      <c r="A119" s="171" t="s">
+        <v>408</v>
+      </c>
+      <c r="B119" s="171"/>
+      <c r="C119" s="171" t="s">
+        <v>395</v>
+      </c>
+      <c r="D119" s="171" t="s">
+        <v>388</v>
+      </c>
+      <c r="E119" s="172" t="s">
+        <v>232</v>
+      </c>
+      <c r="F119" s="171" t="s">
+        <v>137</v>
+      </c>
+      <c r="G119" s="171" t="s">
+        <v>291</v>
+      </c>
+      <c r="H119" s="171" t="s">
+        <v>289</v>
+      </c>
+      <c r="I119" s="171" t="s">
+        <v>371</v>
+      </c>
+      <c r="J119" s="186" t="s">
+        <v>287</v>
+      </c>
+      <c r="K119" s="186" t="s">
+        <v>365</v>
+      </c>
+      <c r="L119" s="173">
+        <v>0.31</v>
+      </c>
+      <c r="M119" s="171"/>
+      <c r="N119" s="171" t="s">
+        <v>32</v>
+      </c>
+      <c r="O119" s="171" t="s">
+        <v>409</v>
+      </c>
+      <c r="P119" s="171" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q119" s="172" t="s">
+        <v>143</v>
+      </c>
+      <c r="R119" s="172" t="s">
+        <v>36</v>
+      </c>
+      <c r="S119" s="174" t="s">
+        <v>410</v>
+      </c>
+      <c r="T119" s="175" t="s">
+        <v>236</v>
+      </c>
+      <c r="U119" s="171"/>
+    </row>
+    <row r="120" spans="1:39" s="176" customFormat="1" ht="12.3">
+      <c r="A120" s="170" t="s">
+        <v>413</v>
+      </c>
+      <c r="B120" s="171"/>
+      <c r="C120" s="171" t="s">
+        <v>395</v>
+      </c>
+      <c r="D120" s="171" t="s">
+        <v>388</v>
+      </c>
+      <c r="E120" s="172" t="s">
+        <v>232</v>
+      </c>
+      <c r="F120" s="171" t="s">
+        <v>137</v>
+      </c>
+      <c r="G120" s="171" t="s">
+        <v>291</v>
+      </c>
+      <c r="H120" s="171" t="s">
+        <v>289</v>
+      </c>
+      <c r="I120" s="171" t="s">
+        <v>411</v>
+      </c>
+      <c r="J120" s="186" t="s">
+        <v>287</v>
+      </c>
+      <c r="K120" s="186" t="s">
+        <v>361</v>
+      </c>
+      <c r="L120" s="173">
+        <v>0.33</v>
+      </c>
+      <c r="M120" s="171"/>
+      <c r="N120" s="171" t="s">
+        <v>32</v>
+      </c>
+      <c r="O120" s="171" t="s">
+        <v>412</v>
+      </c>
+      <c r="P120" s="171" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q120" s="172" t="s">
+        <v>143</v>
+      </c>
+      <c r="R120" s="172" t="s">
+        <v>36</v>
+      </c>
+      <c r="S120" s="174" t="s">
+        <v>410</v>
+      </c>
+      <c r="T120" s="175" t="s">
+        <v>236</v>
+      </c>
+      <c r="U120" s="171"/>
+      <c r="V120" s="176" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="121" spans="1:39" ht="12.3">
       <c r="A121" s="3"/>
       <c r="B121" s="3"/>
       <c r="C121" s="3"/>
@@ -10085,7 +10368,7 @@
       <c r="S121" s="3"/>
       <c r="U121" s="3"/>
     </row>
-    <row r="122" spans="1:22" ht="12.3">
+    <row r="122" spans="1:39" ht="12.3">
       <c r="A122" s="3"/>
       <c r="B122" s="3"/>
       <c r="C122" s="3"/>
@@ -10107,7 +10390,7 @@
       <c r="S122" s="3"/>
       <c r="U122" s="3"/>
     </row>
-    <row r="123" spans="1:22" ht="12.3">
+    <row r="123" spans="1:39" ht="12.3">
       <c r="A123" s="3"/>
       <c r="B123" s="3"/>
       <c r="C123" s="3"/>
@@ -10129,7 +10412,7 @@
       <c r="S123" s="3"/>
       <c r="U123" s="3"/>
     </row>
-    <row r="124" spans="1:22" ht="12.3">
+    <row r="124" spans="1:39" ht="12.3">
       <c r="A124" s="3"/>
       <c r="B124" s="3"/>
       <c r="C124" s="3"/>
@@ -10151,7 +10434,7 @@
       <c r="S124" s="3"/>
       <c r="U124" s="3"/>
     </row>
-    <row r="125" spans="1:22" ht="12.3">
+    <row r="125" spans="1:39" ht="12.3">
       <c r="A125" s="3"/>
       <c r="B125" s="3"/>
       <c r="C125" s="3"/>
@@ -10173,7 +10456,7 @@
       <c r="S125" s="3"/>
       <c r="U125" s="3"/>
     </row>
-    <row r="126" spans="1:22" ht="12.3">
+    <row r="126" spans="1:39" ht="12.3">
       <c r="A126" s="3"/>
       <c r="B126" s="3"/>
       <c r="C126" s="3"/>
@@ -10195,7 +10478,7 @@
       <c r="S126" s="3"/>
       <c r="U126" s="3"/>
     </row>
-    <row r="127" spans="1:22" ht="12.3">
+    <row r="127" spans="1:39" ht="12.3">
       <c r="A127" s="3"/>
       <c r="B127" s="3"/>
       <c r="C127" s="3"/>
@@ -10217,7 +10500,7 @@
       <c r="S127" s="3"/>
       <c r="U127" s="3"/>
     </row>
-    <row r="128" spans="1:22" ht="12.3">
+    <row r="128" spans="1:39" ht="12.3">
       <c r="A128" s="3"/>
       <c r="B128" s="3"/>
       <c r="C128" s="3"/>
@@ -29161,7 +29444,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added data, daq code, and modified analysis
added data, daq code, and modified analysis delta norm to take into account negative and pos adc values
</commit_message>
<xml_diff>
--- a/data_25_01_14.xlsx
+++ b/data_25_01_14.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csuma-my.sharepoint.com/personal/toppenheim_csum_edu/Documents/Documents/GitHub/Strain-Sensor-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="464" documentId="13_ncr:1_{C06D3E42-5B17-7143-AE76-68B895C59C70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{60C961E0-77BE-46B5-94A1-45984602831C}"/>
+  <xr:revisionPtr revIDLastSave="156" documentId="13_ncr:1_{C7A043D2-2238-4A3A-B3B1-D197D0E45859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08AD170A-1FE6-4FAF-93ED-FC2DE685D0E1}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3061" uniqueCount="415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3216" uniqueCount="455">
   <si>
     <t>Sample Name</t>
   </si>
@@ -1278,20 +1278,140 @@
     <t>1,987 in</t>
   </si>
   <si>
-    <t>CSV Data/3_20_25/Bending_data_abs_1p987_retest_4_18_25.csv</t>
-  </si>
-  <si>
     <t>abs_1p987_retest_v3</t>
   </si>
   <si>
     <t>hysteresis?  Slipping ?  I will re-test Tuesday</t>
+  </si>
+  <si>
+    <t>3_25_25</t>
+  </si>
+  <si>
+    <t>abs_1p987_retest_v4</t>
+  </si>
+  <si>
+    <t>70.7F</t>
+  </si>
+  <si>
+    <t>CSV Data/3_20_25/Bending_data_abs_1p987_retest_v3_3_20_25.csv</t>
+  </si>
+  <si>
+    <t>CSV Data/3_25_25/Bending_data_abs_1p987_retest_v4_3_25_25.csv</t>
+  </si>
+  <si>
+    <t>Volt Div:  8x amp with 16 bit encoding, 3.3V exc - LVR with 10uF cap in in/out (not Vref) and 50 ohm (not 100 ohm) divider</t>
+  </si>
+  <si>
+    <t>abs_1p987_retest_v5</t>
+  </si>
+  <si>
+    <t>CSV Data/3_25_25/Bending_data_abs_1p987_retest_v5_3_27_25.csv</t>
+  </si>
+  <si>
+    <t>3_27_25</t>
+  </si>
+  <si>
+    <t>Volt Div:  8x amp with 16 bit encoding, 3.3V exc - LVR with 10uF cap in in/out (not Vref) and 50 ohm (not 100 ohm) divider,0.1 uF cer cap on inst. Amp out</t>
+  </si>
+  <si>
+    <t>DID NOT CONDUCT TEST</t>
+  </si>
+  <si>
+    <t>when looking at arduino uno serial monitor, adc values slowly drift up…..issue with inst amplifier despite adding cap?</t>
+  </si>
+  <si>
+    <t>Volt Div:  8x amp with 16 bit encoding, 3.3V exc - LVR with 10uF cap in in/out (not Vref) and 40 ohm (not 100 ohm) divider</t>
+  </si>
+  <si>
+    <t>3_31_25</t>
+  </si>
+  <si>
+    <t>abs_1p987_retest_v6</t>
+  </si>
+  <si>
+    <t>CSV Data/3_25_25/Bending_data_abs_1p987_retest_v6_3_31_25.csv</t>
+  </si>
+  <si>
+    <t>Volt Div:  8x amp with 16 bit encoding, 3.3V exc - LVR with 10uF cap in in/out (not Vref) and 1K ohm (not 100 ohm) divider</t>
+  </si>
+  <si>
+    <t>slightly more noisy than previous green because using smaller range of adc…more noise…</t>
+  </si>
+  <si>
+    <t>4_8_25</t>
+  </si>
+  <si>
+    <t>abs_1pxxx_gains_4_8_25</t>
+  </si>
+  <si>
+    <t>ad620 2.5x gain + LMC648 120x gain</t>
+  </si>
+  <si>
+    <t>Volt. Div. 100, 100, 0.4; 120 x volt across 0.4 ohm to ad620 in+, 2.048 ref to in-, Vref to GND, ad620 2.5x gain, adc 1x 16 bit res.</t>
+  </si>
+  <si>
+    <t>(in+ x LMC gain - in- volt ref ad620) x G of ad620 makes data exponential!!</t>
+  </si>
+  <si>
+    <t>abs_1pxxx_gains_unity_gain_v2_4_8_25</t>
+  </si>
+  <si>
+    <t>ad620 1x gain + LMC648 120x gain</t>
+  </si>
+  <si>
+    <t>4_9_25</t>
+  </si>
+  <si>
+    <t>LMC648 49x gain + MCP34212x gain</t>
+  </si>
+  <si>
+    <t>CSV Data/4_8_25/Bending_data_abs_1pxxx_gains_4_8_25.csv</t>
+  </si>
+  <si>
+    <t>Volt. Div. 2 parallel 100 and 0.4 gauge; LMC648 49x out strian gauge in+ (~1.9V), 2.048 ref to in-;  adc 2x 16 bit res.</t>
+  </si>
+  <si>
+    <t>CSV Data/4_9_25/Bending_data_abs_1pxxx_gains_unity_gain_v34_9_25.csv</t>
+  </si>
+  <si>
+    <t>abs_2p25_gains_2xp49x_gain_v3_4_9_25</t>
+  </si>
+  <si>
+    <t>abs_2p25_gains_2xp75x_gain_v4_4_9_25</t>
+  </si>
+  <si>
+    <t>LMC648 75x gain + MCP34212x gain</t>
+  </si>
+  <si>
+    <t>CSV Data/4_9_25/Bending_data_abs_2p25_gains_2xp75x_gain_v4_4_9_25.csv</t>
+  </si>
+  <si>
+    <t>Volt. Div. 2 parallel 100 and 0.4 gauge; LMC648 75x out strian gauge in+ (~1.9V), 2.048 ref to in-;  adc 2x 16 bit res.</t>
+  </si>
+  <si>
+    <t>LMC648 75x gain + MCP34212x gain + 1k res and 1uF cap</t>
+  </si>
+  <si>
+    <t>Maybe</t>
+  </si>
+  <si>
+    <t>Volt. Div. 2 parallel 100 and 0.4 gauge; LMC648 75x out strian gauge in+ (~1.9V), 2.048 ref to in-;  adc 2x 16 bit res., 1k + 1uF cap for filter</t>
+  </si>
+  <si>
+    <t>abs_2p25_gains_2xp75x_gain_v5_4_9_25_1k_1uF_0p1uF</t>
+  </si>
+  <si>
+    <t>CSV Data/4_9_25/Bending_data_abs_2p25_gains_2xp75x_gain_v5_4_9_25_1k_1uF_0p1uF.csv</t>
+  </si>
+  <si>
+    <t>2.25 in</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1354,6 +1474,13 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="JetBrains Mono"/>
+    </font>
+    <font>
+      <sz val="9.8000000000000007"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="major"/>
     </font>
   </fonts>
   <fills count="19">
@@ -1595,7 +1722,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="194">
+  <cellXfs count="202">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2072,6 +2199,26 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2299,18 +2446,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AM988"/>
+  <dimension ref="A1:AM989"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A91" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A120" sqref="A120"/>
+      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T134" sqref="T134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="46.1640625" customWidth="1"/>
+    <col min="3" max="3" width="49.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="46.1640625" customWidth="1"/>
     <col min="5" max="6" width="14.5" customWidth="1"/>
     <col min="7" max="7" width="15.5" customWidth="1"/>
     <col min="8" max="8" width="34.5" bestFit="1" customWidth="1"/>
@@ -2322,7 +2470,7 @@
     <col min="15" max="15" width="103" customWidth="1"/>
     <col min="17" max="17" width="38.6640625" customWidth="1"/>
     <col min="18" max="18" width="17.5" customWidth="1"/>
-    <col min="19" max="19" width="113.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="124.0546875" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="73.5" customWidth="1"/>
     <col min="22" max="22" width="190.27734375" bestFit="1" customWidth="1"/>
   </cols>
@@ -10286,7 +10434,7 @@
     </row>
     <row r="120" spans="1:39" s="176" customFormat="1" ht="12.3">
       <c r="A120" s="170" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B120" s="171"/>
       <c r="C120" s="171" t="s">
@@ -10324,7 +10472,7 @@
         <v>32</v>
       </c>
       <c r="O120" s="171" t="s">
-        <v>412</v>
+        <v>417</v>
       </c>
       <c r="P120" s="171" t="s">
         <v>393</v>
@@ -10343,220 +10491,521 @@
       </c>
       <c r="U120" s="171"/>
       <c r="V120" s="176" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="121" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A121" s="4" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="121" spans="1:39" ht="12.3">
-      <c r="A121" s="3"/>
-      <c r="B121" s="3"/>
-      <c r="C121" s="3"/>
-      <c r="D121" s="3"/>
-      <c r="E121" s="3"/>
-      <c r="F121" s="3"/>
-      <c r="G121" s="3"/>
-      <c r="H121" s="3"/>
-      <c r="I121" s="3"/>
-      <c r="J121" s="28"/>
-      <c r="K121" s="28"/>
-      <c r="L121" s="3"/>
-      <c r="M121" s="3"/>
-      <c r="N121" s="3"/>
-      <c r="O121" s="3"/>
-      <c r="P121" s="3"/>
-      <c r="Q121" s="3"/>
-      <c r="R121" s="3"/>
-      <c r="S121" s="3"/>
-      <c r="U121" s="3"/>
-    </row>
-    <row r="122" spans="1:39" ht="12.3">
-      <c r="A122" s="3"/>
-      <c r="B122" s="3"/>
-      <c r="C122" s="3"/>
-      <c r="D122" s="3"/>
-      <c r="E122" s="3"/>
-      <c r="F122" s="3"/>
-      <c r="G122" s="3"/>
-      <c r="H122" s="3"/>
-      <c r="I122" s="3"/>
-      <c r="J122" s="28"/>
-      <c r="K122" s="28"/>
-      <c r="L122" s="3"/>
-      <c r="M122" s="3"/>
-      <c r="N122" s="3"/>
-      <c r="O122" s="3"/>
-      <c r="P122" s="3"/>
-      <c r="Q122" s="3"/>
-      <c r="R122" s="3"/>
-      <c r="S122" s="3"/>
-      <c r="U122" s="3"/>
-    </row>
-    <row r="123" spans="1:39" ht="12.3">
-      <c r="A123" s="3"/>
-      <c r="B123" s="3"/>
-      <c r="C123" s="3"/>
-      <c r="D123" s="3"/>
-      <c r="E123" s="3"/>
-      <c r="F123" s="3"/>
-      <c r="G123" s="3"/>
-      <c r="H123" s="3"/>
-      <c r="I123" s="3"/>
-      <c r="J123" s="28"/>
-      <c r="K123" s="28"/>
-      <c r="L123" s="3"/>
-      <c r="M123" s="3"/>
-      <c r="N123" s="3"/>
-      <c r="O123" s="3"/>
-      <c r="P123" s="3"/>
-      <c r="Q123" s="3"/>
-      <c r="R123" s="3"/>
-      <c r="S123" s="3"/>
-      <c r="U123" s="3"/>
-    </row>
-    <row r="124" spans="1:39" ht="12.3">
-      <c r="A124" s="3"/>
-      <c r="B124" s="3"/>
-      <c r="C124" s="3"/>
-      <c r="D124" s="3"/>
-      <c r="E124" s="3"/>
-      <c r="F124" s="3"/>
-      <c r="G124" s="3"/>
-      <c r="H124" s="3"/>
-      <c r="I124" s="3"/>
-      <c r="J124" s="28"/>
-      <c r="K124" s="28"/>
-      <c r="L124" s="3"/>
-      <c r="M124" s="3"/>
-      <c r="N124" s="3"/>
-      <c r="O124" s="3"/>
-      <c r="P124" s="3"/>
-      <c r="Q124" s="3"/>
-      <c r="R124" s="3"/>
-      <c r="S124" s="3"/>
-      <c r="U124" s="3"/>
-    </row>
-    <row r="125" spans="1:39" ht="12.3">
-      <c r="A125" s="3"/>
-      <c r="B125" s="3"/>
-      <c r="C125" s="3"/>
-      <c r="D125" s="3"/>
-      <c r="E125" s="3"/>
-      <c r="F125" s="3"/>
-      <c r="G125" s="3"/>
-      <c r="H125" s="3"/>
-      <c r="I125" s="3"/>
-      <c r="J125" s="28"/>
-      <c r="K125" s="28"/>
-      <c r="L125" s="3"/>
-      <c r="M125" s="3"/>
-      <c r="N125" s="3"/>
-      <c r="O125" s="3"/>
-      <c r="P125" s="3"/>
-      <c r="Q125" s="3"/>
-      <c r="R125" s="3"/>
-      <c r="S125" s="3"/>
-      <c r="U125" s="3"/>
-    </row>
-    <row r="126" spans="1:39" ht="12.3">
-      <c r="A126" s="3"/>
-      <c r="B126" s="3"/>
-      <c r="C126" s="3"/>
-      <c r="D126" s="3"/>
-      <c r="E126" s="3"/>
-      <c r="F126" s="3"/>
-      <c r="G126" s="3"/>
-      <c r="H126" s="3"/>
-      <c r="I126" s="3"/>
-      <c r="J126" s="28"/>
-      <c r="K126" s="28"/>
-      <c r="L126" s="3"/>
-      <c r="M126" s="3"/>
-      <c r="N126" s="3"/>
-      <c r="O126" s="3"/>
-      <c r="P126" s="3"/>
-      <c r="Q126" s="3"/>
-      <c r="R126" s="3"/>
-      <c r="S126" s="3"/>
-      <c r="U126" s="3"/>
-    </row>
-    <row r="127" spans="1:39" ht="12.3">
-      <c r="A127" s="3"/>
-      <c r="B127" s="3"/>
-      <c r="C127" s="3"/>
-      <c r="D127" s="3"/>
-      <c r="E127" s="3"/>
-      <c r="F127" s="3"/>
-      <c r="G127" s="3"/>
-      <c r="H127" s="3"/>
-      <c r="I127" s="3"/>
-      <c r="J127" s="28"/>
-      <c r="K127" s="28"/>
-      <c r="L127" s="3"/>
-      <c r="M127" s="3"/>
-      <c r="N127" s="3"/>
-      <c r="O127" s="3"/>
-      <c r="P127" s="3"/>
-      <c r="Q127" s="3"/>
-      <c r="R127" s="3"/>
-      <c r="S127" s="3"/>
-      <c r="U127" s="3"/>
-    </row>
-    <row r="128" spans="1:39" ht="12.3">
-      <c r="A128" s="3"/>
-      <c r="B128" s="3"/>
-      <c r="C128" s="3"/>
-      <c r="D128" s="3"/>
-      <c r="E128" s="3"/>
-      <c r="F128" s="3"/>
-      <c r="G128" s="3"/>
-      <c r="H128" s="3"/>
-      <c r="I128" s="3"/>
-      <c r="J128" s="28"/>
-      <c r="K128" s="28"/>
-      <c r="L128" s="3"/>
-      <c r="M128" s="3"/>
-      <c r="N128" s="3"/>
-      <c r="O128" s="3"/>
-      <c r="P128" s="3"/>
-      <c r="Q128" s="3"/>
-      <c r="R128" s="3"/>
-      <c r="S128" s="3"/>
-      <c r="U128" s="3"/>
-    </row>
-    <row r="129" spans="1:21" ht="12.3">
-      <c r="A129" s="3"/>
+      <c r="B121" s="6"/>
+      <c r="C121" s="6"/>
+      <c r="D121" s="6"/>
+      <c r="E121" s="6"/>
+      <c r="F121" s="6"/>
+      <c r="G121" s="6"/>
+      <c r="H121" s="6"/>
+      <c r="I121" s="6"/>
+      <c r="J121" s="5"/>
+      <c r="K121" s="5"/>
+      <c r="L121" s="6"/>
+      <c r="M121" s="6"/>
+      <c r="N121" s="6"/>
+      <c r="O121" s="6"/>
+      <c r="P121" s="6"/>
+      <c r="Q121" s="6"/>
+      <c r="R121" s="6"/>
+      <c r="S121" s="6"/>
+      <c r="T121" s="7"/>
+      <c r="U121" s="6"/>
+      <c r="V121" s="7"/>
+      <c r="W121" s="7"/>
+      <c r="X121" s="7"/>
+      <c r="Y121" s="7"/>
+      <c r="Z121" s="7"/>
+      <c r="AA121" s="7"/>
+      <c r="AB121" s="7"/>
+      <c r="AC121" s="7"/>
+      <c r="AD121" s="7"/>
+      <c r="AE121" s="7"/>
+      <c r="AF121" s="7"/>
+      <c r="AG121" s="7"/>
+      <c r="AH121" s="7"/>
+      <c r="AI121" s="7"/>
+      <c r="AJ121" s="7"/>
+      <c r="AK121" s="7"/>
+      <c r="AL121" s="7"/>
+      <c r="AM121" s="7"/>
+    </row>
+    <row r="122" spans="1:39" s="134" customFormat="1" ht="12.3">
+      <c r="A122" s="194" t="s">
+        <v>415</v>
+      </c>
+      <c r="B122" s="128"/>
+      <c r="C122" s="128" t="s">
+        <v>395</v>
+      </c>
+      <c r="D122" s="128" t="s">
+        <v>388</v>
+      </c>
+      <c r="E122" s="129" t="s">
+        <v>232</v>
+      </c>
+      <c r="F122" s="128" t="s">
+        <v>137</v>
+      </c>
+      <c r="G122" s="128" t="s">
+        <v>291</v>
+      </c>
+      <c r="H122" s="128" t="s">
+        <v>289</v>
+      </c>
+      <c r="I122" s="128" t="s">
+        <v>267</v>
+      </c>
+      <c r="J122" s="185" t="s">
+        <v>287</v>
+      </c>
+      <c r="K122" s="185" t="s">
+        <v>416</v>
+      </c>
+      <c r="L122" s="130">
+        <v>0.5</v>
+      </c>
+      <c r="M122" s="128"/>
+      <c r="N122" s="128" t="s">
+        <v>32</v>
+      </c>
+      <c r="O122" s="128" t="s">
+        <v>418</v>
+      </c>
+      <c r="P122" s="128" t="s">
+        <v>414</v>
+      </c>
+      <c r="Q122" s="129" t="s">
+        <v>143</v>
+      </c>
+      <c r="R122" s="129" t="s">
+        <v>36</v>
+      </c>
+      <c r="S122" s="131" t="s">
+        <v>419</v>
+      </c>
+      <c r="T122" s="132" t="s">
+        <v>236</v>
+      </c>
+      <c r="U122" s="128"/>
+    </row>
+    <row r="123" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A123" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="B123" s="6"/>
+      <c r="C123" s="6"/>
+      <c r="D123" s="6"/>
+      <c r="E123" s="6"/>
+      <c r="F123" s="6"/>
+      <c r="G123" s="6"/>
+      <c r="H123" s="6"/>
+      <c r="I123" s="6"/>
+      <c r="J123" s="5"/>
+      <c r="K123" s="5"/>
+      <c r="L123" s="6"/>
+      <c r="M123" s="6"/>
+      <c r="N123" s="6"/>
+      <c r="O123" s="6"/>
+      <c r="P123" s="6"/>
+      <c r="Q123" s="6"/>
+      <c r="R123" s="6"/>
+      <c r="S123" s="6"/>
+      <c r="T123" s="7"/>
+      <c r="U123" s="6"/>
+      <c r="V123" s="7"/>
+      <c r="W123" s="7"/>
+      <c r="X123" s="7"/>
+      <c r="Y123" s="7"/>
+      <c r="Z123" s="7"/>
+      <c r="AA123" s="7"/>
+      <c r="AB123" s="7"/>
+      <c r="AC123" s="7"/>
+      <c r="AD123" s="7"/>
+      <c r="AE123" s="7"/>
+      <c r="AF123" s="7"/>
+      <c r="AG123" s="7"/>
+      <c r="AH123" s="7"/>
+      <c r="AI123" s="7"/>
+      <c r="AJ123" s="7"/>
+      <c r="AK123" s="7"/>
+      <c r="AL123" s="7"/>
+      <c r="AM123" s="7"/>
+    </row>
+    <row r="124" spans="1:39" s="169" customFormat="1" ht="12.3">
+      <c r="A124" s="163" t="s">
+        <v>420</v>
+      </c>
+      <c r="B124" s="164"/>
+      <c r="C124" s="164" t="s">
+        <v>395</v>
+      </c>
+      <c r="D124" s="164" t="s">
+        <v>388</v>
+      </c>
+      <c r="E124" s="165" t="s">
+        <v>232</v>
+      </c>
+      <c r="F124" s="164" t="s">
+        <v>137</v>
+      </c>
+      <c r="G124" s="164" t="s">
+        <v>291</v>
+      </c>
+      <c r="H124" s="164" t="s">
+        <v>289</v>
+      </c>
+      <c r="I124" s="164" t="s">
+        <v>267</v>
+      </c>
+      <c r="J124" s="187" t="s">
+        <v>287</v>
+      </c>
+      <c r="K124" s="187" t="s">
+        <v>416</v>
+      </c>
+      <c r="L124" s="166">
+        <v>0.5</v>
+      </c>
+      <c r="M124" s="164"/>
+      <c r="N124" s="164" t="s">
+        <v>155</v>
+      </c>
+      <c r="O124" s="164" t="s">
+        <v>424</v>
+      </c>
+      <c r="P124" s="164" t="s">
+        <v>422</v>
+      </c>
+      <c r="Q124" s="165" t="s">
+        <v>143</v>
+      </c>
+      <c r="R124" s="165" t="s">
+        <v>36</v>
+      </c>
+      <c r="S124" s="167" t="s">
+        <v>423</v>
+      </c>
+      <c r="T124" s="168" t="s">
+        <v>236</v>
+      </c>
+      <c r="U124" s="164"/>
+      <c r="V124" s="190" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="125" spans="1:39" s="126" customFormat="1" ht="12.3">
+      <c r="A125" s="195" t="s">
+        <v>420</v>
+      </c>
+      <c r="B125" s="121"/>
+      <c r="C125" s="121" t="s">
+        <v>395</v>
+      </c>
+      <c r="D125" s="121" t="s">
+        <v>388</v>
+      </c>
+      <c r="E125" s="122" t="s">
+        <v>232</v>
+      </c>
+      <c r="F125" s="121" t="s">
+        <v>137</v>
+      </c>
+      <c r="G125" s="121" t="s">
+        <v>291</v>
+      </c>
+      <c r="H125" s="121" t="s">
+        <v>289</v>
+      </c>
+      <c r="I125" s="121" t="s">
+        <v>267</v>
+      </c>
+      <c r="J125" s="184" t="s">
+        <v>287</v>
+      </c>
+      <c r="K125" s="184" t="s">
+        <v>416</v>
+      </c>
+      <c r="L125" s="123">
+        <v>0.5</v>
+      </c>
+      <c r="M125" s="121"/>
+      <c r="N125" s="121" t="s">
+        <v>32</v>
+      </c>
+      <c r="O125" s="121" t="s">
+        <v>421</v>
+      </c>
+      <c r="P125" s="121" t="s">
+        <v>422</v>
+      </c>
+      <c r="Q125" s="122" t="s">
+        <v>143</v>
+      </c>
+      <c r="R125" s="122" t="s">
+        <v>36</v>
+      </c>
+      <c r="S125" s="124" t="s">
+        <v>426</v>
+      </c>
+      <c r="T125" s="125" t="s">
+        <v>236</v>
+      </c>
+      <c r="U125" s="121"/>
+      <c r="V125" s="196"/>
+    </row>
+    <row r="126" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A126" s="4" t="s">
+        <v>427</v>
+      </c>
+      <c r="B126" s="6"/>
+      <c r="C126" s="6"/>
+      <c r="D126" s="6"/>
+      <c r="E126" s="6"/>
+      <c r="F126" s="6"/>
+      <c r="G126" s="6"/>
+      <c r="H126" s="6"/>
+      <c r="I126" s="6"/>
+      <c r="J126" s="5"/>
+      <c r="K126" s="5"/>
+      <c r="L126" s="6"/>
+      <c r="M126" s="6"/>
+      <c r="N126" s="6"/>
+      <c r="O126" s="6"/>
+      <c r="P126" s="6"/>
+      <c r="Q126" s="6"/>
+      <c r="R126" s="6"/>
+      <c r="S126" s="6"/>
+      <c r="T126" s="7"/>
+      <c r="U126" s="6"/>
+      <c r="V126" s="7"/>
+      <c r="W126" s="7"/>
+      <c r="X126" s="7"/>
+      <c r="Y126" s="7"/>
+      <c r="Z126" s="7"/>
+      <c r="AA126" s="7"/>
+      <c r="AB126" s="7"/>
+      <c r="AC126" s="7"/>
+      <c r="AD126" s="7"/>
+      <c r="AE126" s="7"/>
+      <c r="AF126" s="7"/>
+      <c r="AG126" s="7"/>
+      <c r="AH126" s="7"/>
+      <c r="AI126" s="7"/>
+      <c r="AJ126" s="7"/>
+      <c r="AK126" s="7"/>
+      <c r="AL126" s="7"/>
+      <c r="AM126" s="7"/>
+    </row>
+    <row r="127" spans="1:39" s="176" customFormat="1" ht="12.3">
+      <c r="A127" s="170" t="s">
+        <v>428</v>
+      </c>
+      <c r="B127" s="171"/>
+      <c r="C127" s="171" t="s">
+        <v>395</v>
+      </c>
+      <c r="D127" s="171" t="s">
+        <v>388</v>
+      </c>
+      <c r="E127" s="172" t="s">
+        <v>232</v>
+      </c>
+      <c r="F127" s="171" t="s">
+        <v>137</v>
+      </c>
+      <c r="G127" s="171" t="s">
+        <v>291</v>
+      </c>
+      <c r="H127" s="171" t="s">
+        <v>289</v>
+      </c>
+      <c r="I127" s="171" t="s">
+        <v>267</v>
+      </c>
+      <c r="J127" s="186" t="s">
+        <v>287</v>
+      </c>
+      <c r="K127" s="186" t="s">
+        <v>361</v>
+      </c>
+      <c r="L127" s="173">
+        <v>0.43</v>
+      </c>
+      <c r="M127" s="171"/>
+      <c r="N127" s="171" t="s">
+        <v>32</v>
+      </c>
+      <c r="O127" s="171" t="s">
+        <v>429</v>
+      </c>
+      <c r="P127" s="171" t="s">
+        <v>427</v>
+      </c>
+      <c r="Q127" s="172" t="s">
+        <v>143</v>
+      </c>
+      <c r="R127" s="172" t="s">
+        <v>36</v>
+      </c>
+      <c r="S127" s="174" t="s">
+        <v>430</v>
+      </c>
+      <c r="T127" s="175" t="s">
+        <v>236</v>
+      </c>
+      <c r="U127" s="171"/>
+      <c r="V127" s="176" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="128" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A128" s="4" t="s">
+        <v>432</v>
+      </c>
+      <c r="B128" s="6"/>
+      <c r="C128" s="6"/>
+      <c r="D128" s="6"/>
+      <c r="E128" s="6"/>
+      <c r="F128" s="6"/>
+      <c r="G128" s="6"/>
+      <c r="H128" s="6"/>
+      <c r="I128" s="6"/>
+      <c r="J128" s="5"/>
+      <c r="K128" s="5"/>
+      <c r="L128" s="6"/>
+      <c r="M128" s="6"/>
+      <c r="N128" s="6"/>
+      <c r="O128" s="6"/>
+      <c r="P128" s="6"/>
+      <c r="Q128" s="6"/>
+      <c r="R128" s="6"/>
+      <c r="S128" s="6"/>
+      <c r="T128" s="7"/>
+      <c r="U128" s="6"/>
+      <c r="V128" s="7"/>
+      <c r="W128" s="7"/>
+      <c r="X128" s="7"/>
+      <c r="Y128" s="7"/>
+      <c r="Z128" s="7"/>
+      <c r="AA128" s="7"/>
+      <c r="AB128" s="7"/>
+      <c r="AC128" s="7"/>
+      <c r="AD128" s="7"/>
+      <c r="AE128" s="7"/>
+      <c r="AF128" s="7"/>
+      <c r="AG128" s="7"/>
+      <c r="AH128" s="7"/>
+      <c r="AI128" s="7"/>
+      <c r="AJ128" s="7"/>
+      <c r="AK128" s="7"/>
+      <c r="AL128" s="7"/>
+      <c r="AM128" s="7"/>
+    </row>
+    <row r="129" spans="1:39" ht="12.3">
+      <c r="A129" s="197" t="s">
+        <v>433</v>
+      </c>
       <c r="B129" s="3"/>
-      <c r="C129" s="3"/>
-      <c r="D129" s="3"/>
-      <c r="E129" s="3"/>
-      <c r="F129" s="3"/>
-      <c r="G129" s="3"/>
-      <c r="H129" s="3"/>
-      <c r="I129" s="3"/>
-      <c r="J129" s="28"/>
-      <c r="K129" s="28"/>
-      <c r="L129" s="3"/>
+      <c r="C129" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="E129" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F129" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="G129" s="171" t="s">
+        <v>291</v>
+      </c>
+      <c r="H129" s="171" t="s">
+        <v>289</v>
+      </c>
+      <c r="I129" s="171" t="s">
+        <v>267</v>
+      </c>
+      <c r="J129" s="186" t="s">
+        <v>287</v>
+      </c>
+      <c r="K129" s="186" t="s">
+        <v>368</v>
+      </c>
+      <c r="L129" s="127">
+        <v>0.37</v>
+      </c>
       <c r="M129" s="3"/>
-      <c r="N129" s="3"/>
-      <c r="O129" s="3"/>
-      <c r="P129" s="3"/>
-      <c r="Q129" s="3"/>
-      <c r="R129" s="3"/>
-      <c r="S129" s="3"/>
+      <c r="N129" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="O129" s="171" t="s">
+        <v>441</v>
+      </c>
+      <c r="P129" s="198" t="s">
+        <v>432</v>
+      </c>
+      <c r="Q129" s="172" t="s">
+        <v>143</v>
+      </c>
+      <c r="R129" s="172" t="s">
+        <v>36</v>
+      </c>
+      <c r="S129" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="T129" s="175" t="s">
+        <v>236</v>
+      </c>
       <c r="U129" s="3"/>
-    </row>
-    <row r="130" spans="1:21" ht="12.3">
-      <c r="A130" s="3"/>
+      <c r="V129" s="199" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="130" spans="1:39" ht="12.3">
+      <c r="A130" s="197" t="s">
+        <v>437</v>
+      </c>
       <c r="B130" s="3"/>
-      <c r="C130" s="3"/>
-      <c r="D130" s="3"/>
-      <c r="E130" s="3"/>
-      <c r="F130" s="3"/>
-      <c r="G130" s="3"/>
-      <c r="H130" s="3"/>
-      <c r="I130" s="3"/>
-      <c r="J130" s="28"/>
-      <c r="K130" s="28"/>
-      <c r="L130" s="3"/>
+      <c r="C130" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F130" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="G130" s="171" t="s">
+        <v>291</v>
+      </c>
+      <c r="H130" s="171" t="s">
+        <v>289</v>
+      </c>
+      <c r="I130" s="171" t="s">
+        <v>267</v>
+      </c>
+      <c r="J130" s="186" t="s">
+        <v>287</v>
+      </c>
+      <c r="K130" s="186" t="s">
+        <v>368</v>
+      </c>
+      <c r="L130" s="127">
+        <v>0.37</v>
+      </c>
       <c r="M130" s="3"/>
       <c r="N130" s="3"/>
       <c r="O130" s="3"/>
@@ -10564,97 +11013,232 @@
       <c r="Q130" s="3"/>
       <c r="R130" s="3"/>
       <c r="S130" s="3"/>
+      <c r="T130" s="175" t="s">
+        <v>236</v>
+      </c>
       <c r="U130" s="3"/>
     </row>
-    <row r="131" spans="1:21" ht="12.3">
-      <c r="A131" s="3"/>
-      <c r="B131" s="3"/>
-      <c r="C131" s="3"/>
-      <c r="D131" s="3"/>
-      <c r="E131" s="3"/>
-      <c r="F131" s="3"/>
-      <c r="G131" s="3"/>
-      <c r="H131" s="3"/>
-      <c r="I131" s="3"/>
-      <c r="J131" s="28"/>
-      <c r="K131" s="28"/>
-      <c r="L131" s="3"/>
-      <c r="M131" s="3"/>
-      <c r="N131" s="3"/>
-      <c r="O131" s="3"/>
-      <c r="P131" s="3"/>
-      <c r="Q131" s="3"/>
-      <c r="R131" s="3"/>
-      <c r="S131" s="3"/>
-      <c r="U131" s="3"/>
-    </row>
-    <row r="132" spans="1:21" ht="12.3">
-      <c r="A132" s="3"/>
-      <c r="B132" s="3"/>
-      <c r="C132" s="3"/>
-      <c r="D132" s="3"/>
-      <c r="E132" s="3"/>
-      <c r="F132" s="3"/>
-      <c r="G132" s="3"/>
-      <c r="H132" s="3"/>
-      <c r="I132" s="3"/>
-      <c r="J132" s="28"/>
-      <c r="K132" s="28"/>
-      <c r="L132" s="3"/>
-      <c r="M132" s="3"/>
-      <c r="N132" s="3"/>
-      <c r="O132" s="3"/>
-      <c r="P132" s="3"/>
-      <c r="Q132" s="3"/>
-      <c r="R132" s="3"/>
-      <c r="S132" s="3"/>
-      <c r="U132" s="3"/>
-    </row>
-    <row r="133" spans="1:21" ht="12.3">
-      <c r="A133" s="3"/>
-      <c r="B133" s="3"/>
-      <c r="C133" s="3"/>
-      <c r="D133" s="3"/>
-      <c r="E133" s="3"/>
-      <c r="F133" s="3"/>
-      <c r="G133" s="3"/>
-      <c r="H133" s="3"/>
-      <c r="I133" s="3"/>
-      <c r="J133" s="28"/>
-      <c r="K133" s="28"/>
-      <c r="L133" s="3"/>
-      <c r="M133" s="3"/>
-      <c r="N133" s="3"/>
-      <c r="O133" s="3"/>
-      <c r="P133" s="3"/>
-      <c r="Q133" s="3"/>
-      <c r="R133" s="3"/>
-      <c r="S133" s="3"/>
-      <c r="U133" s="3"/>
-    </row>
-    <row r="134" spans="1:21" ht="12.3">
-      <c r="A134" s="3"/>
-      <c r="B134" s="3"/>
-      <c r="C134" s="3"/>
-      <c r="D134" s="3"/>
-      <c r="E134" s="3"/>
-      <c r="F134" s="3"/>
-      <c r="G134" s="3"/>
-      <c r="H134" s="3"/>
-      <c r="I134" s="3"/>
-      <c r="J134" s="28"/>
-      <c r="K134" s="28"/>
-      <c r="L134" s="3"/>
-      <c r="M134" s="3"/>
-      <c r="N134" s="3"/>
-      <c r="O134" s="3"/>
-      <c r="P134" s="3"/>
-      <c r="Q134" s="3"/>
-      <c r="R134" s="3"/>
-      <c r="S134" s="3"/>
-      <c r="U134" s="3"/>
-    </row>
-    <row r="135" spans="1:21" ht="12.3">
+    <row r="131" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A131" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="B131" s="6"/>
+      <c r="C131" s="6"/>
+      <c r="D131" s="6"/>
+      <c r="E131" s="6"/>
+      <c r="F131" s="6"/>
+      <c r="G131" s="6"/>
+      <c r="H131" s="6"/>
+      <c r="I131" s="6"/>
+      <c r="J131" s="5"/>
+      <c r="K131" s="5"/>
+      <c r="L131" s="6"/>
+      <c r="M131" s="6"/>
+      <c r="N131" s="6"/>
+      <c r="O131" s="6"/>
+      <c r="P131" s="6"/>
+      <c r="Q131" s="6"/>
+      <c r="R131" s="6"/>
+      <c r="S131" s="6"/>
+      <c r="T131" s="7"/>
+      <c r="U131" s="6"/>
+      <c r="V131" s="7"/>
+      <c r="W131" s="7"/>
+      <c r="X131" s="7"/>
+      <c r="Y131" s="7"/>
+      <c r="Z131" s="7"/>
+      <c r="AA131" s="7"/>
+      <c r="AB131" s="7"/>
+      <c r="AC131" s="7"/>
+      <c r="AD131" s="7"/>
+      <c r="AE131" s="7"/>
+      <c r="AF131" s="7"/>
+      <c r="AG131" s="7"/>
+      <c r="AH131" s="7"/>
+      <c r="AI131" s="7"/>
+      <c r="AJ131" s="7"/>
+      <c r="AK131" s="7"/>
+      <c r="AL131" s="7"/>
+      <c r="AM131" s="7"/>
+    </row>
+    <row r="132" spans="1:39" s="176" customFormat="1" ht="12.3">
+      <c r="A132" s="200" t="s">
+        <v>444</v>
+      </c>
+      <c r="B132" s="171"/>
+      <c r="C132" s="171" t="s">
+        <v>440</v>
+      </c>
+      <c r="D132" s="171" t="s">
+        <v>351</v>
+      </c>
+      <c r="E132" s="171" t="s">
+        <v>232</v>
+      </c>
+      <c r="F132" s="171" t="s">
+        <v>292</v>
+      </c>
+      <c r="G132" s="171" t="s">
+        <v>291</v>
+      </c>
+      <c r="H132" s="171" t="s">
+        <v>289</v>
+      </c>
+      <c r="I132" s="171" t="s">
+        <v>454</v>
+      </c>
+      <c r="J132" s="186" t="s">
+        <v>287</v>
+      </c>
+      <c r="K132" s="186" t="s">
+        <v>368</v>
+      </c>
+      <c r="L132" s="173">
+        <v>0.37</v>
+      </c>
+      <c r="M132" s="171"/>
+      <c r="N132" s="171" t="s">
+        <v>32</v>
+      </c>
+      <c r="O132" s="171" t="s">
+        <v>443</v>
+      </c>
+      <c r="P132" s="171" t="s">
+        <v>439</v>
+      </c>
+      <c r="Q132" s="172" t="s">
+        <v>143</v>
+      </c>
+      <c r="R132" s="172" t="s">
+        <v>36</v>
+      </c>
+      <c r="S132" s="171" t="s">
+        <v>442</v>
+      </c>
+      <c r="T132" s="175" t="s">
+        <v>236</v>
+      </c>
+      <c r="U132" s="171"/>
+    </row>
+    <row r="133" spans="1:39" s="140" customFormat="1" ht="12" customHeight="1">
+      <c r="A133" s="201" t="s">
+        <v>445</v>
+      </c>
+      <c r="B133" s="135"/>
+      <c r="C133" s="135" t="s">
+        <v>446</v>
+      </c>
+      <c r="D133" s="135" t="s">
+        <v>351</v>
+      </c>
+      <c r="E133" s="135" t="s">
+        <v>232</v>
+      </c>
+      <c r="F133" s="135" t="s">
+        <v>292</v>
+      </c>
+      <c r="G133" s="135" t="s">
+        <v>291</v>
+      </c>
+      <c r="H133" s="135" t="s">
+        <v>289</v>
+      </c>
+      <c r="I133" s="171" t="s">
+        <v>454</v>
+      </c>
+      <c r="J133" s="186" t="s">
+        <v>287</v>
+      </c>
+      <c r="K133" s="183" t="s">
+        <v>368</v>
+      </c>
+      <c r="L133" s="137">
+        <v>0.37</v>
+      </c>
+      <c r="M133" s="135"/>
+      <c r="N133" s="135" t="s">
+        <v>450</v>
+      </c>
+      <c r="O133" s="135" t="s">
+        <v>447</v>
+      </c>
+      <c r="P133" s="135" t="s">
+        <v>439</v>
+      </c>
+      <c r="Q133" s="136" t="s">
+        <v>143</v>
+      </c>
+      <c r="R133" s="136" t="s">
+        <v>36</v>
+      </c>
+      <c r="S133" s="135" t="s">
+        <v>448</v>
+      </c>
+      <c r="T133" s="175" t="s">
+        <v>236</v>
+      </c>
+      <c r="U133" s="135"/>
+    </row>
+    <row r="134" spans="1:39" s="176" customFormat="1" ht="12.3">
+      <c r="A134" s="200" t="s">
+        <v>452</v>
+      </c>
+      <c r="B134" s="171"/>
+      <c r="C134" s="171" t="s">
+        <v>449</v>
+      </c>
+      <c r="D134" s="171" t="s">
+        <v>351</v>
+      </c>
+      <c r="E134" s="171" t="s">
+        <v>232</v>
+      </c>
+      <c r="F134" s="171" t="s">
+        <v>292</v>
+      </c>
+      <c r="G134" s="171" t="s">
+        <v>291</v>
+      </c>
+      <c r="H134" s="171" t="s">
+        <v>289</v>
+      </c>
+      <c r="I134" s="171" t="s">
+        <v>454</v>
+      </c>
+      <c r="J134" s="186" t="s">
+        <v>287</v>
+      </c>
+      <c r="K134" s="186" t="s">
+        <v>368</v>
+      </c>
+      <c r="L134" s="173">
+        <v>0.37</v>
+      </c>
+      <c r="M134" s="171"/>
+      <c r="N134" s="171" t="s">
+        <v>32</v>
+      </c>
+      <c r="O134" s="171" t="s">
+        <v>453</v>
+      </c>
+      <c r="P134" s="171" t="s">
+        <v>439</v>
+      </c>
+      <c r="Q134" s="172" t="s">
+        <v>143</v>
+      </c>
+      <c r="R134" s="172" t="s">
+        <v>36</v>
+      </c>
+      <c r="S134" s="171" t="s">
+        <v>451</v>
+      </c>
+      <c r="T134" s="175" t="s">
+        <v>236</v>
+      </c>
+      <c r="U134" s="171"/>
+    </row>
+    <row r="135" spans="1:39" ht="12.3">
       <c r="A135" s="3"/>
       <c r="B135" s="3"/>
       <c r="C135" s="3"/>
@@ -10676,7 +11260,7 @@
       <c r="S135" s="3"/>
       <c r="U135" s="3"/>
     </row>
-    <row r="136" spans="1:21" ht="12.3">
+    <row r="136" spans="1:39" ht="12.3">
       <c r="A136" s="3"/>
       <c r="B136" s="3"/>
       <c r="C136" s="3"/>
@@ -10698,7 +11282,7 @@
       <c r="S136" s="3"/>
       <c r="U136" s="3"/>
     </row>
-    <row r="137" spans="1:21" ht="12.3">
+    <row r="137" spans="1:39" ht="12.3">
       <c r="A137" s="3"/>
       <c r="B137" s="3"/>
       <c r="C137" s="3"/>
@@ -10720,7 +11304,7 @@
       <c r="S137" s="3"/>
       <c r="U137" s="3"/>
     </row>
-    <row r="138" spans="1:21" ht="12.3">
+    <row r="138" spans="1:39" ht="12.3">
       <c r="A138" s="3"/>
       <c r="B138" s="3"/>
       <c r="C138" s="3"/>
@@ -10742,7 +11326,7 @@
       <c r="S138" s="3"/>
       <c r="U138" s="3"/>
     </row>
-    <row r="139" spans="1:21" ht="12.3">
+    <row r="139" spans="1:39" ht="12.3">
       <c r="A139" s="3"/>
       <c r="B139" s="3"/>
       <c r="C139" s="3"/>
@@ -10764,7 +11348,7 @@
       <c r="S139" s="3"/>
       <c r="U139" s="3"/>
     </row>
-    <row r="140" spans="1:21" ht="12.3">
+    <row r="140" spans="1:39" ht="12.3">
       <c r="A140" s="3"/>
       <c r="B140" s="3"/>
       <c r="C140" s="3"/>
@@ -10786,7 +11370,7 @@
       <c r="S140" s="3"/>
       <c r="U140" s="3"/>
     </row>
-    <row r="141" spans="1:21" ht="12.3">
+    <row r="141" spans="1:39" ht="12.3">
       <c r="A141" s="3"/>
       <c r="B141" s="3"/>
       <c r="C141" s="3"/>
@@ -10808,7 +11392,7 @@
       <c r="S141" s="3"/>
       <c r="U141" s="3"/>
     </row>
-    <row r="142" spans="1:21" ht="12.3">
+    <row r="142" spans="1:39" ht="12.3">
       <c r="A142" s="3"/>
       <c r="B142" s="3"/>
       <c r="C142" s="3"/>
@@ -10830,7 +11414,7 @@
       <c r="S142" s="3"/>
       <c r="U142" s="3"/>
     </row>
-    <row r="143" spans="1:21" ht="12.3">
+    <row r="143" spans="1:39" ht="12.3">
       <c r="A143" s="3"/>
       <c r="B143" s="3"/>
       <c r="C143" s="3"/>
@@ -10852,7 +11436,7 @@
       <c r="S143" s="3"/>
       <c r="U143" s="3"/>
     </row>
-    <row r="144" spans="1:21" ht="12.3">
+    <row r="144" spans="1:39" ht="12.3">
       <c r="A144" s="3"/>
       <c r="B144" s="3"/>
       <c r="C144" s="3"/>
@@ -29441,6 +30025,28 @@
       <c r="R988" s="3"/>
       <c r="S988" s="3"/>
       <c r="U988" s="3"/>
+    </row>
+    <row r="989" spans="1:21" ht="12.3">
+      <c r="A989" s="3"/>
+      <c r="B989" s="3"/>
+      <c r="C989" s="3"/>
+      <c r="D989" s="3"/>
+      <c r="E989" s="3"/>
+      <c r="F989" s="3"/>
+      <c r="G989" s="3"/>
+      <c r="H989" s="3"/>
+      <c r="I989" s="3"/>
+      <c r="J989" s="28"/>
+      <c r="K989" s="28"/>
+      <c r="L989" s="3"/>
+      <c r="M989" s="3"/>
+      <c r="N989" s="3"/>
+      <c r="O989" s="3"/>
+      <c r="P989" s="3"/>
+      <c r="Q989" s="3"/>
+      <c r="R989" s="3"/>
+      <c r="S989" s="3"/>
+      <c r="U989" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Acquired More Data, Changed analysis.py to include quadratic fitting
</commit_message>
<xml_diff>
--- a/data_25_01_14.xlsx
+++ b/data_25_01_14.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csuma-my.sharepoint.com/personal/toppenheim_csum_edu/Documents/Documents/GitHub/Strain-Sensor-/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toppe\OneDrive - CSU Maritime Academy\Documents\GitHub\Strain-Sensor-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="380" documentId="13_ncr:1_{C7A043D2-2238-4A3A-B3B1-D197D0E45859}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54950038-1706-46D6-8292-B44215A2A348}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B456EFE-629F-46DB-BDAD-2277034A9104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3400" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3556" uniqueCount="525">
   <si>
     <t>Sample Name</t>
   </si>
@@ -1455,9 +1455,6 @@
     <t>1.86_static_vs2v2_4_11_25</t>
   </si>
   <si>
-    <t>CSV Data/4_11_25/1.86_static_vs2v2_4_11_25</t>
-  </si>
-  <si>
     <t>data improved from yesterday.  Also use a shielded cable from sample to breadboard, and turned OFF flourescent light above sample during testing.  Sample had overnight for glue to cure further.  Data significantly.  improved, but still a touch noisy.  Bad sample? also moved as many gnd pins to one side as possible (avoid GND loops)</t>
   </si>
   <si>
@@ -1467,18 +1464,12 @@
     <t xml:space="preserve"> MCP3421 8x gain</t>
   </si>
   <si>
-    <t>CSV Data/4_11_25/1.86_static_vs3_v1_4_11_25</t>
-  </si>
-  <si>
     <t>Volt. Div.  2 parallel 100 ohm and 0.4 gauge;   adc 8x 16 bit res. (single ended)</t>
   </si>
   <si>
     <t>1.86_static_vs3_v2_4_11_25</t>
   </si>
   <si>
-    <t>CSV Data/4_11_25/1.86_static_vs3_v2_4_11_25</t>
-  </si>
-  <si>
     <t>just wanted to compare circuit with no amplification for same sample as previous line.  Some error/noise but somewhat comparable accuracy.  Amplication so far seems to produce more consistent accuracies</t>
   </si>
   <si>
@@ -1491,15 +1482,9 @@
     <t>didn’t wait long engough for glue to settle before testing!</t>
   </si>
   <si>
-    <t>CSV Data/4_11_25/1.86_static_vs4_v1_4_11_25</t>
-  </si>
-  <si>
     <t>1.86_static_vs5_v1_4_11_25</t>
   </si>
   <si>
-    <t>CSV Data/4_11_25/1.86_static_vs5_v1_4_11_25</t>
-  </si>
-  <si>
     <t>Volt. Div.  2 parallel 100 ohm and 0.4 gauge; LMC648 75x out strian gauge in+ (~1.9V), 2.048 ref to in-;  adc 2x 16 bit res.</t>
   </si>
   <si>
@@ -1507,6 +1492,129 @@
   </si>
   <si>
     <t>sample slipping and slack…I also think these samples, the way they were made, not good. Add silicone first to cover LM holes then the silpoxy.  JUST ADD SILPOXY!!!</t>
+  </si>
+  <si>
+    <t>4_15_25</t>
+  </si>
+  <si>
+    <t>1.85 in</t>
+  </si>
+  <si>
+    <t>75 F</t>
+  </si>
+  <si>
+    <t>1.85_static_v1_4_15_25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data looks good but looks like more quadratic towards 90 degrees?  </t>
+  </si>
+  <si>
+    <t>1.85_static_v2_4_15_25</t>
+  </si>
+  <si>
+    <t>0.123 in</t>
+  </si>
+  <si>
+    <t>2.2 in</t>
+  </si>
+  <si>
+    <t>Data looks good but looks like more quadratic towards 90 degrees?  Waiting 30+ min before testing to allow enough time for silicone glue to cure!!!</t>
+  </si>
+  <si>
+    <t>2.2_static_v1_4_15_25</t>
+  </si>
+  <si>
+    <t>CSV Data/4_15_25/2.2_static_v1_4_15_25.csv</t>
+  </si>
+  <si>
+    <t>CSV Data/4_15_25/1.85_static_v2_4_15_25.csv</t>
+  </si>
+  <si>
+    <t>CSV Data/4_15_25/1.85_static_v1_4_15_25.csv</t>
+  </si>
+  <si>
+    <t>CSV Data/4_11_25/1.86_static_vs5_v1_4_11_25.csv</t>
+  </si>
+  <si>
+    <t>CSV Data/4_11_25/1.86_static_vs4_v1_4_11_25.csv</t>
+  </si>
+  <si>
+    <t>CSV Data/4_11_25/1.86_static_vs3_v2_4_11_25.csv</t>
+  </si>
+  <si>
+    <t>CSV Data/4_11_25/1.86_static_vs3_v1_4_11_25.csv</t>
+  </si>
+  <si>
+    <t>CSV Data/4_11_25/1.86_static_vs2v2_4_11_25.csv</t>
+  </si>
+  <si>
+    <t>noisy closer to 90 deg</t>
+  </si>
+  <si>
+    <t>much better than previous!!!</t>
+  </si>
+  <si>
+    <t>2.2_static_v2_4_15_25</t>
+  </si>
+  <si>
+    <t>CSV Data/4_15_25/2.2_static_v2_4_15_25.csv</t>
+  </si>
+  <si>
+    <t>2.2_static_v3_4_15_25</t>
+  </si>
+  <si>
+    <t>CSV Data/4_15_25/2.2_static_v3_4_15_25.csv</t>
+  </si>
+  <si>
+    <t>static re-test</t>
+  </si>
+  <si>
+    <t>good..clearly quadratic</t>
+  </si>
+  <si>
+    <t>data looks good but maybe slack in sample at rest?  Re-test</t>
+  </si>
+  <si>
+    <t>1.98_static_v2_4_15_25</t>
+  </si>
+  <si>
+    <t>1.98_static_v1_4_15_25</t>
+  </si>
+  <si>
+    <t>1.98 in</t>
+  </si>
+  <si>
+    <t>CSV Data/4_15_25/1.98_static_v1_4_15_25</t>
+  </si>
+  <si>
+    <t>CSV Data/4_15_25/1.98_static_v2_4_15_25</t>
+  </si>
+  <si>
+    <t>looks good!</t>
+  </si>
+  <si>
+    <t>LMC648 75x gain + MCP3421 1x gain</t>
+  </si>
+  <si>
+    <t>1.875 in</t>
+  </si>
+  <si>
+    <t>CSV Data/4_15_25/1.875_static_v1_4_15_25</t>
+  </si>
+  <si>
+    <t>Volt. Div.  100 ohm and 0.4 gauge; LMC648 75x out strian gauge in+ (~1.9V), 2.048 ref to in-;  adc 1x 16 bit res.</t>
+  </si>
+  <si>
+    <t>1.875_static_v1_4_15_25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">static re-test </t>
+  </si>
+  <si>
+    <t>staticre-test</t>
+  </si>
+  <si>
+    <t>clipping and wonky….reapply sample to double check</t>
   </si>
 </sst>
 </file>
@@ -2371,10 +2479,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -2579,8 +2683,8 @@
   <dimension ref="A1:AL990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A151" sqref="A151"/>
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A160" sqref="A160"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -11149,7 +11253,7 @@
         <v>444</v>
       </c>
       <c r="C136" s="152" t="s">
-        <v>340</v>
+        <v>508</v>
       </c>
       <c r="D136" s="152" t="s">
         <v>221</v>
@@ -11207,7 +11311,7 @@
         <v>448</v>
       </c>
       <c r="C137" s="152" t="s">
-        <v>340</v>
+        <v>508</v>
       </c>
       <c r="D137" s="152" t="s">
         <v>221</v>
@@ -11323,7 +11427,7 @@
         <v>448</v>
       </c>
       <c r="C139" s="152" t="s">
-        <v>340</v>
+        <v>523</v>
       </c>
       <c r="D139" s="152" t="s">
         <v>221</v>
@@ -11337,8 +11441,8 @@
       <c r="G139" s="152" t="s">
         <v>278</v>
       </c>
-      <c r="H139" s="152">
-        <v>1.86</v>
+      <c r="H139" s="152" t="s">
+        <v>232</v>
       </c>
       <c r="I139" s="174" t="s">
         <v>276</v>
@@ -11384,7 +11488,7 @@
         <v>448</v>
       </c>
       <c r="C140" s="152" t="s">
-        <v>340</v>
+        <v>508</v>
       </c>
       <c r="D140" s="152" t="s">
         <v>221</v>
@@ -11398,8 +11502,8 @@
       <c r="G140" s="152" t="s">
         <v>278</v>
       </c>
-      <c r="H140" s="152">
-        <v>1.86</v>
+      <c r="H140" s="152" t="s">
+        <v>232</v>
       </c>
       <c r="I140" s="174" t="s">
         <v>276</v>
@@ -11445,7 +11549,7 @@
         <v>448</v>
       </c>
       <c r="C141" s="152" t="s">
-        <v>340</v>
+        <v>508</v>
       </c>
       <c r="D141" s="152" t="s">
         <v>221</v>
@@ -11459,8 +11563,8 @@
       <c r="G141" s="152" t="s">
         <v>278</v>
       </c>
-      <c r="H141" s="152">
-        <v>1.86</v>
+      <c r="H141" s="152" t="s">
+        <v>232</v>
       </c>
       <c r="I141" s="174" t="s">
         <v>276</v>
@@ -11506,7 +11610,7 @@
         <v>448</v>
       </c>
       <c r="C142" s="152" t="s">
-        <v>340</v>
+        <v>508</v>
       </c>
       <c r="D142" s="152" t="s">
         <v>221</v>
@@ -11520,8 +11624,8 @@
       <c r="G142" s="152" t="s">
         <v>278</v>
       </c>
-      <c r="H142" s="152">
-        <v>1.86</v>
+      <c r="H142" s="152" t="s">
+        <v>232</v>
       </c>
       <c r="I142" s="174" t="s">
         <v>276</v>
@@ -11567,7 +11671,7 @@
         <v>448</v>
       </c>
       <c r="C143" s="152" t="s">
-        <v>340</v>
+        <v>508</v>
       </c>
       <c r="D143" s="152" t="s">
         <v>221</v>
@@ -11581,8 +11685,8 @@
       <c r="G143" s="152" t="s">
         <v>278</v>
       </c>
-      <c r="H143" s="152">
-        <v>1.86</v>
+      <c r="H143" s="152" t="s">
+        <v>232</v>
       </c>
       <c r="I143" s="174" t="s">
         <v>276</v>
@@ -11617,7 +11721,7 @@
       </c>
       <c r="T143" s="3"/>
       <c r="U143" s="152" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
     </row>
     <row r="144" spans="1:38" ht="15.75" customHeight="1">
@@ -11662,7 +11766,7 @@
       <c r="AK144" s="7"/>
       <c r="AL144" s="7"/>
     </row>
-    <row r="145" spans="1:21" ht="12.3">
+    <row r="145" spans="1:38" ht="12.3">
       <c r="A145" s="24" t="s">
         <v>470</v>
       </c>
@@ -11670,7 +11774,7 @@
         <v>448</v>
       </c>
       <c r="C145" s="152" t="s">
-        <v>340</v>
+        <v>508</v>
       </c>
       <c r="D145" s="152" t="s">
         <v>221</v>
@@ -11684,8 +11788,8 @@
       <c r="G145" s="152" t="s">
         <v>278</v>
       </c>
-      <c r="H145" s="152">
-        <v>1.86</v>
+      <c r="H145" s="152" t="s">
+        <v>232</v>
       </c>
       <c r="I145" s="174" t="s">
         <v>276</v>
@@ -11701,7 +11805,7 @@
         <v>148</v>
       </c>
       <c r="N145" s="152" t="s">
-        <v>471</v>
+        <v>501</v>
       </c>
       <c r="O145" s="152" t="s">
         <v>469</v>
@@ -11720,18 +11824,18 @@
       </c>
       <c r="T145" s="3"/>
       <c r="U145" s="177" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="146" spans="1:38" s="123" customFormat="1" ht="12.3">
+      <c r="A146" s="172" t="s">
         <v>472</v>
-      </c>
-    </row>
-    <row r="146" spans="1:21" s="123" customFormat="1" ht="12.3">
-      <c r="A146" s="172" t="s">
-        <v>473</v>
       </c>
       <c r="B146" s="117" t="s">
         <v>448</v>
       </c>
       <c r="C146" s="117" t="s">
-        <v>340</v>
+        <v>508</v>
       </c>
       <c r="D146" s="117" t="s">
         <v>221</v>
@@ -11745,8 +11849,8 @@
       <c r="G146" s="117" t="s">
         <v>278</v>
       </c>
-      <c r="H146" s="117">
-        <v>1.86</v>
+      <c r="H146" s="117" t="s">
+        <v>232</v>
       </c>
       <c r="I146" s="172" t="s">
         <v>276</v>
@@ -11762,7 +11866,7 @@
         <v>30</v>
       </c>
       <c r="N146" s="117" t="s">
-        <v>475</v>
+        <v>500</v>
       </c>
       <c r="O146" s="117" t="s">
         <v>469</v>
@@ -11781,15 +11885,15 @@
       </c>
       <c r="T146" s="117"/>
     </row>
-    <row r="147" spans="1:21" s="129" customFormat="1" ht="12.3">
+    <row r="147" spans="1:38" s="129" customFormat="1" ht="12.3">
       <c r="A147" s="170" t="s">
-        <v>477</v>
+        <v>475</v>
       </c>
       <c r="B147" s="124" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C147" s="124" t="s">
-        <v>340</v>
+        <v>508</v>
       </c>
       <c r="D147" s="124" t="s">
         <v>221</v>
@@ -11803,8 +11907,8 @@
       <c r="G147" s="124" t="s">
         <v>278</v>
       </c>
-      <c r="H147" s="124">
-        <v>1.86</v>
+      <c r="H147" s="124" t="s">
+        <v>232</v>
       </c>
       <c r="I147" s="170" t="s">
         <v>276</v>
@@ -11820,7 +11924,7 @@
         <v>437</v>
       </c>
       <c r="N147" s="124" t="s">
-        <v>478</v>
+        <v>499</v>
       </c>
       <c r="O147" s="124" t="s">
         <v>469</v>
@@ -11832,25 +11936,25 @@
         <v>34</v>
       </c>
       <c r="R147" s="124" t="s">
-        <v>476</v>
+        <v>474</v>
       </c>
       <c r="S147" s="128" t="s">
         <v>225</v>
       </c>
       <c r="T147" s="124"/>
       <c r="U147" s="129" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="148" spans="1:21" ht="12.3">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="148" spans="1:38" ht="12.3">
       <c r="A148" s="24" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="B148" s="152" t="s">
         <v>448</v>
       </c>
       <c r="C148" s="152" t="s">
-        <v>340</v>
+        <v>508</v>
       </c>
       <c r="D148" s="152" t="s">
         <v>221</v>
@@ -11864,8 +11968,8 @@
       <c r="G148" s="152" t="s">
         <v>278</v>
       </c>
-      <c r="H148" s="152">
-        <v>1.86</v>
+      <c r="H148" s="152" t="s">
+        <v>232</v>
       </c>
       <c r="I148" s="174" t="s">
         <v>276</v>
@@ -11881,7 +11985,7 @@
         <v>148</v>
       </c>
       <c r="N148" s="3" t="s">
-        <v>483</v>
+        <v>498</v>
       </c>
       <c r="O148" s="152" t="s">
         <v>469</v>
@@ -11900,18 +12004,18 @@
       </c>
       <c r="T148" s="3"/>
       <c r="U148" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="149" spans="1:21" ht="12.3">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="149" spans="1:38" ht="12.3">
       <c r="A149" s="24" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="B149" s="152" t="s">
         <v>448</v>
       </c>
       <c r="C149" s="152" t="s">
-        <v>340</v>
+        <v>522</v>
       </c>
       <c r="D149" s="152" t="s">
         <v>221</v>
@@ -11925,8 +12029,8 @@
       <c r="G149" s="152" t="s">
         <v>278</v>
       </c>
-      <c r="H149" s="152">
-        <v>1.86</v>
+      <c r="H149" s="152" t="s">
+        <v>232</v>
       </c>
       <c r="I149" s="174" t="s">
         <v>276</v>
@@ -11942,7 +12046,7 @@
         <v>148</v>
       </c>
       <c r="N149" s="3" t="s">
-        <v>485</v>
+        <v>497</v>
       </c>
       <c r="O149" s="152" t="s">
         <v>469</v>
@@ -11961,12 +12065,12 @@
       </c>
       <c r="T149" s="3"/>
       <c r="U149" t="s">
-        <v>488</v>
-      </c>
-    </row>
-    <row r="150" spans="1:21" s="123" customFormat="1" ht="12.3">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="150" spans="1:38" s="123" customFormat="1" ht="12.3">
       <c r="A150" s="172" t="s">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="B150" s="117" t="s">
         <v>448</v>
@@ -11986,8 +12090,8 @@
       <c r="G150" s="117" t="s">
         <v>278</v>
       </c>
-      <c r="H150" s="117">
-        <v>1.758</v>
+      <c r="H150" s="117" t="s">
+        <v>360</v>
       </c>
       <c r="I150" s="172" t="s">
         <v>276</v>
@@ -12011,203 +12115,544 @@
         <v>34</v>
       </c>
       <c r="R150" s="117" t="s">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="S150" s="121" t="s">
         <v>225</v>
       </c>
       <c r="T150" s="117"/>
     </row>
-    <row r="151" spans="1:21" ht="12.3">
-      <c r="A151" s="24"/>
-      <c r="B151" s="3"/>
-      <c r="C151" s="3"/>
-      <c r="D151" s="3"/>
-      <c r="E151" s="3"/>
-      <c r="F151" s="3"/>
-      <c r="G151" s="3"/>
-      <c r="H151" s="3"/>
-      <c r="I151" s="24"/>
-      <c r="J151" s="24"/>
-      <c r="K151" s="3"/>
-      <c r="L151" s="3"/>
-      <c r="M151" s="3"/>
-      <c r="N151" s="3"/>
-      <c r="O151" s="3"/>
-      <c r="P151" s="3"/>
-      <c r="Q151" s="3"/>
-      <c r="R151" s="3"/>
-      <c r="T151" s="3"/>
-    </row>
-    <row r="152" spans="1:21" ht="12.3">
-      <c r="A152" s="24"/>
-      <c r="B152" s="3"/>
-      <c r="C152" s="3"/>
-      <c r="D152" s="3"/>
-      <c r="E152" s="3"/>
-      <c r="F152" s="3"/>
-      <c r="G152" s="3"/>
-      <c r="H152" s="3"/>
-      <c r="I152" s="24"/>
-      <c r="J152" s="24"/>
-      <c r="K152" s="3"/>
-      <c r="L152" s="3"/>
-      <c r="M152" s="3"/>
-      <c r="N152" s="3"/>
-      <c r="O152" s="3"/>
-      <c r="P152" s="3"/>
-      <c r="Q152" s="3"/>
-      <c r="R152" s="3"/>
-      <c r="T152" s="3"/>
-    </row>
-    <row r="153" spans="1:21" ht="12.3">
-      <c r="A153" s="24"/>
-      <c r="B153" s="3"/>
-      <c r="C153" s="3"/>
-      <c r="D153" s="3"/>
-      <c r="E153" s="3"/>
-      <c r="F153" s="3"/>
-      <c r="G153" s="3"/>
-      <c r="H153" s="3"/>
-      <c r="I153" s="24"/>
-      <c r="J153" s="24"/>
-      <c r="K153" s="3"/>
-      <c r="L153" s="3"/>
-      <c r="M153" s="3"/>
-      <c r="N153" s="3"/>
-      <c r="O153" s="3"/>
-      <c r="P153" s="3"/>
-      <c r="Q153" s="3"/>
-      <c r="R153" s="3"/>
-      <c r="T153" s="3"/>
-    </row>
-    <row r="154" spans="1:21" ht="12.3">
-      <c r="A154" s="24"/>
-      <c r="B154" s="3"/>
-      <c r="C154" s="3"/>
-      <c r="D154" s="3"/>
-      <c r="E154" s="3"/>
-      <c r="F154" s="3"/>
-      <c r="G154" s="3"/>
-      <c r="H154" s="3"/>
-      <c r="I154" s="24"/>
-      <c r="J154" s="24"/>
-      <c r="K154" s="3"/>
-      <c r="L154" s="3"/>
-      <c r="M154" s="3"/>
-      <c r="N154" s="3"/>
-      <c r="O154" s="3"/>
-      <c r="P154" s="3"/>
-      <c r="Q154" s="3"/>
-      <c r="R154" s="3"/>
-      <c r="T154" s="3"/>
-    </row>
-    <row r="155" spans="1:21" ht="12.3">
-      <c r="A155" s="24"/>
-      <c r="B155" s="3"/>
-      <c r="C155" s="3"/>
-      <c r="D155" s="3"/>
-      <c r="E155" s="3"/>
-      <c r="F155" s="3"/>
-      <c r="G155" s="3"/>
-      <c r="H155" s="3"/>
-      <c r="I155" s="24"/>
-      <c r="J155" s="24"/>
-      <c r="K155" s="3"/>
-      <c r="L155" s="3"/>
-      <c r="M155" s="3"/>
-      <c r="N155" s="3"/>
-      <c r="O155" s="3"/>
-      <c r="P155" s="3"/>
-      <c r="Q155" s="3"/>
-      <c r="R155" s="3"/>
-      <c r="T155" s="3"/>
-    </row>
-    <row r="156" spans="1:21" ht="12.3">
-      <c r="A156" s="24"/>
-      <c r="B156" s="3"/>
-      <c r="C156" s="3"/>
-      <c r="D156" s="3"/>
-      <c r="E156" s="3"/>
-      <c r="F156" s="3"/>
-      <c r="G156" s="3"/>
-      <c r="H156" s="3"/>
-      <c r="I156" s="24"/>
-      <c r="J156" s="24"/>
-      <c r="K156" s="3"/>
-      <c r="L156" s="3"/>
-      <c r="M156" s="3"/>
-      <c r="N156" s="3"/>
-      <c r="O156" s="3"/>
-      <c r="P156" s="3"/>
-      <c r="Q156" s="3"/>
-      <c r="R156" s="3"/>
-      <c r="T156" s="3"/>
-    </row>
-    <row r="157" spans="1:21" ht="12.3">
-      <c r="A157" s="24"/>
-      <c r="B157" s="3"/>
-      <c r="C157" s="3"/>
-      <c r="D157" s="3"/>
-      <c r="E157" s="3"/>
-      <c r="F157" s="3"/>
-      <c r="G157" s="3"/>
-      <c r="H157" s="3"/>
-      <c r="I157" s="24"/>
-      <c r="J157" s="24"/>
-      <c r="K157" s="3"/>
-      <c r="L157" s="3"/>
-      <c r="M157" s="3"/>
-      <c r="N157" s="3"/>
-      <c r="O157" s="3"/>
-      <c r="P157" s="3"/>
-      <c r="Q157" s="3"/>
-      <c r="R157" s="3"/>
-      <c r="T157" s="3"/>
-    </row>
-    <row r="158" spans="1:21" ht="12.3">
-      <c r="A158" s="24"/>
-      <c r="B158" s="3"/>
-      <c r="C158" s="3"/>
-      <c r="D158" s="3"/>
-      <c r="E158" s="3"/>
-      <c r="F158" s="3"/>
-      <c r="G158" s="3"/>
-      <c r="H158" s="3"/>
-      <c r="I158" s="24"/>
-      <c r="J158" s="24"/>
-      <c r="K158" s="3"/>
-      <c r="L158" s="3"/>
-      <c r="M158" s="3"/>
-      <c r="N158" s="3"/>
-      <c r="O158" s="3"/>
-      <c r="P158" s="3"/>
-      <c r="Q158" s="3"/>
-      <c r="R158" s="3"/>
-      <c r="T158" s="3"/>
-    </row>
-    <row r="159" spans="1:21" ht="12.3">
-      <c r="A159" s="24"/>
-      <c r="B159" s="3"/>
-      <c r="C159" s="3"/>
-      <c r="D159" s="3"/>
-      <c r="E159" s="3"/>
-      <c r="F159" s="3"/>
-      <c r="G159" s="3"/>
-      <c r="H159" s="3"/>
-      <c r="I159" s="24"/>
-      <c r="J159" s="24"/>
-      <c r="K159" s="3"/>
-      <c r="L159" s="3"/>
-      <c r="M159" s="3"/>
-      <c r="N159" s="3"/>
-      <c r="O159" s="3"/>
-      <c r="P159" s="3"/>
-      <c r="Q159" s="3"/>
-      <c r="R159" s="3"/>
-      <c r="T159" s="3"/>
-    </row>
-    <row r="160" spans="1:21" ht="12.3">
+    <row r="151" spans="1:38" ht="15.75" customHeight="1">
+      <c r="A151" s="184" t="s">
+        <v>484</v>
+      </c>
+      <c r="B151" s="6"/>
+      <c r="C151" s="6"/>
+      <c r="D151" s="6"/>
+      <c r="E151" s="6"/>
+      <c r="F151" s="6"/>
+      <c r="G151" s="6"/>
+      <c r="H151" s="6"/>
+      <c r="I151" s="5"/>
+      <c r="J151" s="5"/>
+      <c r="K151" s="6"/>
+      <c r="L151" s="6"/>
+      <c r="M151" s="6"/>
+      <c r="N151" s="207"/>
+      <c r="O151" s="6"/>
+      <c r="P151" s="6"/>
+      <c r="Q151" s="6"/>
+      <c r="R151" s="6"/>
+      <c r="S151" s="7"/>
+      <c r="T151" s="6"/>
+      <c r="U151" s="7"/>
+      <c r="V151" s="7"/>
+      <c r="W151" s="7"/>
+      <c r="X151" s="7"/>
+      <c r="Y151" s="7"/>
+      <c r="Z151" s="7"/>
+      <c r="AA151" s="7"/>
+      <c r="AB151" s="7"/>
+      <c r="AC151" s="7"/>
+      <c r="AD151" s="7"/>
+      <c r="AE151" s="7"/>
+      <c r="AF151" s="7"/>
+      <c r="AG151" s="7"/>
+      <c r="AH151" s="7"/>
+      <c r="AI151" s="7"/>
+      <c r="AJ151" s="7"/>
+      <c r="AK151" s="7"/>
+      <c r="AL151" s="7"/>
+    </row>
+    <row r="152" spans="1:38" s="129" customFormat="1" ht="12.3">
+      <c r="A152" s="170" t="s">
+        <v>487</v>
+      </c>
+      <c r="B152" s="124" t="s">
+        <v>448</v>
+      </c>
+      <c r="C152" s="124" t="s">
+        <v>340</v>
+      </c>
+      <c r="D152" s="124" t="s">
+        <v>221</v>
+      </c>
+      <c r="E152" s="124" t="s">
+        <v>281</v>
+      </c>
+      <c r="F152" s="124" t="s">
+        <v>280</v>
+      </c>
+      <c r="G152" s="124" t="s">
+        <v>278</v>
+      </c>
+      <c r="H152" s="124" t="s">
+        <v>485</v>
+      </c>
+      <c r="I152" s="170" t="s">
+        <v>276</v>
+      </c>
+      <c r="J152" s="170" t="s">
+        <v>486</v>
+      </c>
+      <c r="K152" s="126">
+        <v>0.38</v>
+      </c>
+      <c r="L152" s="124"/>
+      <c r="M152" s="124" t="s">
+        <v>30</v>
+      </c>
+      <c r="N152" s="124" t="s">
+        <v>496</v>
+      </c>
+      <c r="O152" s="124" t="s">
+        <v>484</v>
+      </c>
+      <c r="P152" s="125" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q152" s="125" t="s">
+        <v>34</v>
+      </c>
+      <c r="R152" s="124" t="s">
+        <v>481</v>
+      </c>
+      <c r="S152" s="128" t="s">
+        <v>225</v>
+      </c>
+      <c r="T152" s="124"/>
+      <c r="U152" s="129" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="153" spans="1:38" s="163" customFormat="1" ht="12.3">
+      <c r="A153" s="173" t="s">
+        <v>489</v>
+      </c>
+      <c r="B153" s="158" t="s">
+        <v>448</v>
+      </c>
+      <c r="C153" s="158" t="s">
+        <v>508</v>
+      </c>
+      <c r="D153" s="158" t="s">
+        <v>221</v>
+      </c>
+      <c r="E153" s="158" t="s">
+        <v>281</v>
+      </c>
+      <c r="F153" s="158" t="s">
+        <v>280</v>
+      </c>
+      <c r="G153" s="158" t="s">
+        <v>278</v>
+      </c>
+      <c r="H153" s="158" t="s">
+        <v>485</v>
+      </c>
+      <c r="I153" s="173" t="s">
+        <v>276</v>
+      </c>
+      <c r="J153" s="173" t="s">
+        <v>486</v>
+      </c>
+      <c r="K153" s="160">
+        <v>0.38</v>
+      </c>
+      <c r="L153" s="158"/>
+      <c r="M153" s="158" t="s">
+        <v>30</v>
+      </c>
+      <c r="N153" s="158" t="s">
+        <v>495</v>
+      </c>
+      <c r="O153" s="158" t="s">
+        <v>484</v>
+      </c>
+      <c r="P153" s="159" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q153" s="159" t="s">
+        <v>34</v>
+      </c>
+      <c r="R153" s="158" t="s">
+        <v>481</v>
+      </c>
+      <c r="S153" s="162" t="s">
+        <v>225</v>
+      </c>
+      <c r="T153" s="158"/>
+      <c r="U153" s="163" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="154" spans="1:38" s="129" customFormat="1" ht="12.3">
+      <c r="A154" s="170" t="s">
+        <v>493</v>
+      </c>
+      <c r="B154" s="124" t="s">
+        <v>448</v>
+      </c>
+      <c r="C154" s="124" t="s">
+        <v>340</v>
+      </c>
+      <c r="D154" s="124" t="s">
+        <v>221</v>
+      </c>
+      <c r="E154" s="124" t="s">
+        <v>281</v>
+      </c>
+      <c r="F154" s="124" t="s">
+        <v>490</v>
+      </c>
+      <c r="G154" s="124" t="s">
+        <v>278</v>
+      </c>
+      <c r="H154" s="124" t="s">
+        <v>491</v>
+      </c>
+      <c r="I154" s="170" t="s">
+        <v>276</v>
+      </c>
+      <c r="J154" s="170" t="s">
+        <v>486</v>
+      </c>
+      <c r="K154" s="126">
+        <v>0.38</v>
+      </c>
+      <c r="L154" s="124"/>
+      <c r="M154" s="124" t="s">
+        <v>437</v>
+      </c>
+      <c r="N154" s="124" t="s">
+        <v>494</v>
+      </c>
+      <c r="O154" s="124" t="s">
+        <v>484</v>
+      </c>
+      <c r="P154" s="124" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q154" s="124" t="s">
+        <v>34</v>
+      </c>
+      <c r="R154" s="124" t="s">
+        <v>481</v>
+      </c>
+      <c r="S154" s="128" t="s">
+        <v>225</v>
+      </c>
+      <c r="T154" s="124"/>
+      <c r="U154" s="129" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="155" spans="1:38" s="129" customFormat="1" ht="12.3">
+      <c r="A155" s="170" t="s">
+        <v>504</v>
+      </c>
+      <c r="B155" s="124" t="s">
+        <v>448</v>
+      </c>
+      <c r="C155" s="124" t="s">
+        <v>508</v>
+      </c>
+      <c r="D155" s="124" t="s">
+        <v>221</v>
+      </c>
+      <c r="E155" s="124" t="s">
+        <v>281</v>
+      </c>
+      <c r="F155" s="124" t="s">
+        <v>490</v>
+      </c>
+      <c r="G155" s="124" t="s">
+        <v>278</v>
+      </c>
+      <c r="H155" s="124" t="s">
+        <v>491</v>
+      </c>
+      <c r="I155" s="170" t="s">
+        <v>276</v>
+      </c>
+      <c r="J155" s="170" t="s">
+        <v>486</v>
+      </c>
+      <c r="K155" s="126">
+        <v>0.38</v>
+      </c>
+      <c r="L155" s="124"/>
+      <c r="M155" s="124" t="s">
+        <v>437</v>
+      </c>
+      <c r="N155" s="124" t="s">
+        <v>505</v>
+      </c>
+      <c r="O155" s="124" t="s">
+        <v>484</v>
+      </c>
+      <c r="P155" s="124" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q155" s="124" t="s">
+        <v>34</v>
+      </c>
+      <c r="R155" s="124" t="s">
+        <v>481</v>
+      </c>
+      <c r="S155" s="128" t="s">
+        <v>225</v>
+      </c>
+      <c r="T155" s="124"/>
+      <c r="U155" s="129" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="156" spans="1:38" s="163" customFormat="1" ht="12.3">
+      <c r="A156" s="173" t="s">
+        <v>506</v>
+      </c>
+      <c r="B156" s="158" t="s">
+        <v>448</v>
+      </c>
+      <c r="C156" s="158" t="s">
+        <v>508</v>
+      </c>
+      <c r="D156" s="158" t="s">
+        <v>221</v>
+      </c>
+      <c r="E156" s="158" t="s">
+        <v>281</v>
+      </c>
+      <c r="F156" s="158" t="s">
+        <v>490</v>
+      </c>
+      <c r="G156" s="158" t="s">
+        <v>278</v>
+      </c>
+      <c r="H156" s="158" t="s">
+        <v>491</v>
+      </c>
+      <c r="I156" s="173" t="s">
+        <v>276</v>
+      </c>
+      <c r="J156" s="173" t="s">
+        <v>486</v>
+      </c>
+      <c r="K156" s="160">
+        <v>0.38</v>
+      </c>
+      <c r="L156" s="158"/>
+      <c r="M156" s="158" t="s">
+        <v>30</v>
+      </c>
+      <c r="N156" s="158" t="s">
+        <v>507</v>
+      </c>
+      <c r="O156" s="158" t="s">
+        <v>484</v>
+      </c>
+      <c r="P156" s="158" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q156" s="158" t="s">
+        <v>34</v>
+      </c>
+      <c r="R156" s="158" t="s">
+        <v>481</v>
+      </c>
+      <c r="S156" s="162" t="s">
+        <v>225</v>
+      </c>
+      <c r="T156" s="158"/>
+      <c r="U156" s="163" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="157" spans="1:38" s="129" customFormat="1" ht="12.3">
+      <c r="A157" s="170" t="s">
+        <v>512</v>
+      </c>
+      <c r="B157" s="124" t="s">
+        <v>448</v>
+      </c>
+      <c r="C157" s="124" t="s">
+        <v>340</v>
+      </c>
+      <c r="D157" s="124" t="s">
+        <v>221</v>
+      </c>
+      <c r="E157" s="124" t="s">
+        <v>281</v>
+      </c>
+      <c r="F157" s="124" t="s">
+        <v>490</v>
+      </c>
+      <c r="G157" s="124" t="s">
+        <v>278</v>
+      </c>
+      <c r="H157" s="124" t="s">
+        <v>513</v>
+      </c>
+      <c r="I157" s="170" t="s">
+        <v>276</v>
+      </c>
+      <c r="J157" s="170" t="s">
+        <v>486</v>
+      </c>
+      <c r="K157" s="126">
+        <v>0.38</v>
+      </c>
+      <c r="L157" s="124"/>
+      <c r="M157" s="124" t="s">
+        <v>437</v>
+      </c>
+      <c r="N157" s="124" t="s">
+        <v>514</v>
+      </c>
+      <c r="O157" s="124" t="s">
+        <v>484</v>
+      </c>
+      <c r="P157" s="124" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q157" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="R157" s="124" t="s">
+        <v>481</v>
+      </c>
+      <c r="S157" s="128" t="s">
+        <v>225</v>
+      </c>
+      <c r="T157" s="124"/>
+      <c r="U157" s="129" t="s">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="158" spans="1:38" s="123" customFormat="1" ht="12.3">
+      <c r="A158" s="172" t="s">
+        <v>511</v>
+      </c>
+      <c r="B158" s="117" t="s">
+        <v>448</v>
+      </c>
+      <c r="C158" s="117" t="s">
+        <v>508</v>
+      </c>
+      <c r="D158" s="117" t="s">
+        <v>221</v>
+      </c>
+      <c r="E158" s="117" t="s">
+        <v>281</v>
+      </c>
+      <c r="F158" s="117" t="s">
+        <v>490</v>
+      </c>
+      <c r="G158" s="117" t="s">
+        <v>278</v>
+      </c>
+      <c r="H158" s="117" t="s">
+        <v>513</v>
+      </c>
+      <c r="I158" s="172" t="s">
+        <v>276</v>
+      </c>
+      <c r="J158" s="172" t="s">
+        <v>486</v>
+      </c>
+      <c r="K158" s="119">
+        <v>0.38</v>
+      </c>
+      <c r="L158" s="117"/>
+      <c r="M158" s="117" t="s">
+        <v>30</v>
+      </c>
+      <c r="N158" s="117" t="s">
+        <v>515</v>
+      </c>
+      <c r="O158" s="117" t="s">
+        <v>484</v>
+      </c>
+      <c r="P158" s="117" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q158" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="R158" s="117" t="s">
+        <v>481</v>
+      </c>
+      <c r="S158" s="121" t="s">
+        <v>225</v>
+      </c>
+      <c r="T158" s="117"/>
+      <c r="U158" s="123" t="s">
+        <v>516</v>
+      </c>
+    </row>
+    <row r="159" spans="1:38" s="157" customFormat="1" ht="12.3">
+      <c r="A159" s="174" t="s">
+        <v>521</v>
+      </c>
+      <c r="B159" s="152" t="s">
+        <v>517</v>
+      </c>
+      <c r="C159" s="152" t="s">
+        <v>340</v>
+      </c>
+      <c r="D159" s="152" t="s">
+        <v>221</v>
+      </c>
+      <c r="E159" s="152" t="s">
+        <v>281</v>
+      </c>
+      <c r="F159" s="152" t="s">
+        <v>490</v>
+      </c>
+      <c r="G159" s="152" t="s">
+        <v>278</v>
+      </c>
+      <c r="H159" s="152" t="s">
+        <v>518</v>
+      </c>
+      <c r="I159" s="174" t="s">
+        <v>276</v>
+      </c>
+      <c r="J159" s="174" t="s">
+        <v>486</v>
+      </c>
+      <c r="K159" s="154">
+        <v>0.38</v>
+      </c>
+      <c r="L159" s="152"/>
+      <c r="M159" s="152" t="s">
+        <v>148</v>
+      </c>
+      <c r="N159" s="152" t="s">
+        <v>519</v>
+      </c>
+      <c r="O159" s="152" t="s">
+        <v>484</v>
+      </c>
+      <c r="P159" s="152" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q159" s="152" t="s">
+        <v>34</v>
+      </c>
+      <c r="R159" s="152" t="s">
+        <v>520</v>
+      </c>
+      <c r="S159" s="156" t="s">
+        <v>225</v>
+      </c>
+      <c r="T159" s="152"/>
+      <c r="U159" s="157" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="160" spans="1:38" ht="12.3">
       <c r="A160" s="24"/>
       <c r="B160" s="3"/>
       <c r="C160" s="3"/>

</xml_diff>

<commit_message>
1 sample of reapplicaton and misalignment with Velcro...updated presentation
</commit_message>
<xml_diff>
--- a/data_25_01_14.xlsx
+++ b/data_25_01_14.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toppe\OneDrive - CSU Maritime Academy\Documents\GitHub\Strain-Sensor-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csuma-my.sharepoint.com/personal/toppenheim_csum_edu/Documents/Documents/GitHub/Strain-Sensor-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B456EFE-629F-46DB-BDAD-2277034A9104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="199" documentId="13_ncr:1_{8B456EFE-629F-46DB-BDAD-2277034A9104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90B54E48-1048-4C20-8019-AEFA531FA849}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3556" uniqueCount="525">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3720" uniqueCount="569">
   <si>
     <t>Sample Name</t>
   </si>
@@ -1584,12 +1584,6 @@
     <t>1.98 in</t>
   </si>
   <si>
-    <t>CSV Data/4_15_25/1.98_static_v1_4_15_25</t>
-  </si>
-  <si>
-    <t>CSV Data/4_15_25/1.98_static_v2_4_15_25</t>
-  </si>
-  <si>
     <t>looks good!</t>
   </si>
   <si>
@@ -1599,9 +1593,6 @@
     <t>1.875 in</t>
   </si>
   <si>
-    <t>CSV Data/4_15_25/1.875_static_v1_4_15_25</t>
-  </si>
-  <si>
     <t>Volt. Div.  100 ohm and 0.4 gauge; LMC648 75x out strian gauge in+ (~1.9V), 2.048 ref to in-;  adc 1x 16 bit res.</t>
   </si>
   <si>
@@ -1614,7 +1605,148 @@
     <t>staticre-test</t>
   </si>
   <si>
-    <t>clipping and wonky….reapply sample to double check</t>
+    <t>clipping  with 1 and 2x gain via adc.  ….reapply sample to double check….gain on amplifier needs to be adjusted so ALL samples can work</t>
+  </si>
+  <si>
+    <t>4_17_25</t>
+  </si>
+  <si>
+    <t>2.185 in</t>
+  </si>
+  <si>
+    <t>72.9 F</t>
+  </si>
+  <si>
+    <t>2.185_static_v1_4_17_25</t>
+  </si>
+  <si>
+    <t>CSV Data/4_17_25/2.185_static_v1_4_17_25.csv</t>
+  </si>
+  <si>
+    <t>CSV Data/4_15_25/1.875_static_v1_4_15_25.csv</t>
+  </si>
+  <si>
+    <t>CSV Data/4_15_25/1.98_static_v2_4_15_25.csv</t>
+  </si>
+  <si>
+    <t>CSV Data/4_15_25/1.98_static_v1_4_15_25.csv</t>
+  </si>
+  <si>
+    <t>sample slipping..need to wait longer than 10-15 min</t>
+  </si>
+  <si>
+    <t>2.185_static_v2_4_17_25</t>
+  </si>
+  <si>
+    <t>74.1 F</t>
+  </si>
+  <si>
+    <t>CSV Data/4_17_25/2.185_static_v2_4_17_25.csv</t>
+  </si>
+  <si>
+    <t>sample not glued on properly….</t>
+  </si>
+  <si>
+    <t>2.24 in</t>
+  </si>
+  <si>
+    <t>Volt. Div.  100 ohm and 0.5 gauge; LMC648 75x out strian gauge in+ (~1.9V), 2.048 ref to in-;  adc 2x 16 bit res.</t>
+  </si>
+  <si>
+    <t>LMC648 75x gain + MCP3421 2x gain+velcro</t>
+  </si>
+  <si>
+    <t>1 ohm</t>
+  </si>
+  <si>
+    <t>2.24_static_v1_4_17_25</t>
+  </si>
+  <si>
+    <t>CSV Data/4_17_25/2.24_static_v1_4_17_25</t>
+  </si>
+  <si>
+    <t>Good test</t>
+  </si>
+  <si>
+    <t>Volt. Div.  2 x 100 ohm in series and pre-stretched to 1 ohm gauge; LMC648 75x out strian gauge in+ (~1.9V), 2.048 ref to in-;  adc 2x 16 bit res.</t>
+  </si>
+  <si>
+    <t>2.24_reapplication_v1_4_17_25</t>
+  </si>
+  <si>
+    <t>2.24_reapplication_v2_4_17_25</t>
+  </si>
+  <si>
+    <t>CSV Data/4_17_25/2.24_reapplication_v1_4_17_25</t>
+  </si>
+  <si>
+    <t>linear appearing….velcro came off sample hence the data drift but if secure perhaps could work…cable connecting to strain gauge lifting gauge off test bed….need better strain relief</t>
+  </si>
+  <si>
+    <t>1.1 ohm</t>
+  </si>
+  <si>
+    <t>CSV Data/4_17_25/2.24_reapplication_v2_4_17_25</t>
+  </si>
+  <si>
+    <t>data good.  Added strain relief by placing bottle on top of a strain sensor wire to keep top of strain sensor stuck onto velcro</t>
+  </si>
+  <si>
+    <t>CSV Data/4_17_25/cable strain relief for velcro.jpg</t>
+  </si>
+  <si>
+    <t>LMC648 75x gain + MCP3421 2x gain + silicone glue</t>
+  </si>
+  <si>
+    <t>2.24_reapplication_v3_4_17_25</t>
+  </si>
+  <si>
+    <t>LMC648 75x gain + MCP3421 2x gain+velcro 3nd  reapply</t>
+  </si>
+  <si>
+    <t>0.9 ohm</t>
+  </si>
+  <si>
+    <t>CSV Data/4_17_25/2.24_reapplication_v3_4_17_25</t>
+  </si>
+  <si>
+    <t>data looks good but there appears to be more variability in error data than previous test</t>
+  </si>
+  <si>
+    <t>2.24_reapplication_v4_4_17_25</t>
+  </si>
+  <si>
+    <t>LMC648 75x gain + MCP3421 2x gain+velcro 4th  reapply</t>
+  </si>
+  <si>
+    <t>CSV Data/4_17_25/2.24_reapplication_v4_4_17_25</t>
+  </si>
+  <si>
+    <t>CSV Data/4_17_25/2.24 8 degree.jpg</t>
+  </si>
+  <si>
+    <t>2.24_misalignment_v10_4_17_25</t>
+  </si>
+  <si>
+    <t>LMC648 75x gain + MCP3421 2x gain+velcro 5th  reapply 10 degree</t>
+  </si>
+  <si>
+    <t>CSV Data/4_17_25/2.24 20 deg.jpg</t>
+  </si>
+  <si>
+    <t>CSV Data/4_17_25/2.24_misalignment_v10_4_17_25</t>
+  </si>
+  <si>
+    <t>2.24_misalignment_v20_4_17_25</t>
+  </si>
+  <si>
+    <t>LMC648 75x gain + MCP3421 2x gain+velcro 5th  reapply 20 degree</t>
+  </si>
+  <si>
+    <t>CSV Data/4_17_25/2.24_misalignment_v20_4_17_25</t>
+  </si>
+  <si>
+    <t>LMC648 75x gain + MCP3421 2x gain+velcro 2nd reapply (same sample as row 163)</t>
   </si>
 </sst>
 </file>
@@ -1699,7 +1831,7 @@
       <scheme val="major"/>
     </font>
   </fonts>
-  <fills count="20">
+  <fills count="21">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1811,6 +1943,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1944,7 +2082,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="208">
+  <cellXfs count="214">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2457,6 +2595,24 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2683,14 +2839,14 @@
   <dimension ref="A1:AL990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A160" sqref="A160"/>
+      <pane ySplit="1" topLeftCell="A141" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A168" sqref="A168"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="48.33203125" style="176" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="68.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="46.1640625" customWidth="1"/>
     <col min="4" max="5" width="14.5" customWidth="1"/>
     <col min="6" max="6" width="15.5" customWidth="1"/>
@@ -11427,7 +11583,7 @@
         <v>448</v>
       </c>
       <c r="C139" s="152" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="D139" s="152" t="s">
         <v>221</v>
@@ -12015,7 +12171,7 @@
         <v>448</v>
       </c>
       <c r="C149" s="152" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="D149" s="152" t="s">
         <v>221</v>
@@ -12508,7 +12664,7 @@
         <v>437</v>
       </c>
       <c r="N157" s="124" t="s">
-        <v>514</v>
+        <v>529</v>
       </c>
       <c r="O157" s="124" t="s">
         <v>484</v>
@@ -12569,7 +12725,7 @@
         <v>30</v>
       </c>
       <c r="N158" s="117" t="s">
-        <v>515</v>
+        <v>528</v>
       </c>
       <c r="O158" s="117" t="s">
         <v>484</v>
@@ -12588,15 +12744,15 @@
       </c>
       <c r="T158" s="117"/>
       <c r="U158" s="123" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
     </row>
     <row r="159" spans="1:38" s="157" customFormat="1" ht="12.3">
       <c r="A159" s="174" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="B159" s="152" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="C159" s="152" t="s">
         <v>340</v>
@@ -12614,7 +12770,7 @@
         <v>278</v>
       </c>
       <c r="H159" s="152" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="I159" s="174" t="s">
         <v>276</v>
@@ -12630,7 +12786,7 @@
         <v>148</v>
       </c>
       <c r="N159" s="152" t="s">
-        <v>519</v>
+        <v>527</v>
       </c>
       <c r="O159" s="152" t="s">
         <v>484</v>
@@ -12642,227 +12798,605 @@
         <v>34</v>
       </c>
       <c r="R159" s="152" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="S159" s="156" t="s">
         <v>225</v>
       </c>
       <c r="T159" s="152"/>
       <c r="U159" s="157" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="160" spans="1:38" ht="15.75" customHeight="1">
+      <c r="A160" s="184" t="s">
+        <v>522</v>
+      </c>
+      <c r="B160" s="6"/>
+      <c r="C160" s="6"/>
+      <c r="D160" s="6"/>
+      <c r="E160" s="6"/>
+      <c r="F160" s="6"/>
+      <c r="G160" s="6"/>
+      <c r="H160" s="6"/>
+      <c r="I160" s="5"/>
+      <c r="J160" s="5"/>
+      <c r="K160" s="6"/>
+      <c r="L160" s="6"/>
+      <c r="M160" s="6"/>
+      <c r="N160" s="207"/>
+      <c r="O160" s="6"/>
+      <c r="P160" s="6"/>
+      <c r="Q160" s="6"/>
+      <c r="R160" s="6"/>
+      <c r="S160" s="7"/>
+      <c r="T160" s="6"/>
+      <c r="U160" s="7"/>
+      <c r="V160" s="7"/>
+      <c r="W160" s="7"/>
+      <c r="X160" s="7"/>
+      <c r="Y160" s="7"/>
+      <c r="Z160" s="7"/>
+      <c r="AA160" s="7"/>
+      <c r="AB160" s="7"/>
+      <c r="AC160" s="7"/>
+      <c r="AD160" s="7"/>
+      <c r="AE160" s="7"/>
+      <c r="AF160" s="7"/>
+      <c r="AG160" s="7"/>
+      <c r="AH160" s="7"/>
+      <c r="AI160" s="7"/>
+      <c r="AJ160" s="7"/>
+      <c r="AK160" s="7"/>
+      <c r="AL160" s="7"/>
+    </row>
+    <row r="161" spans="1:21" ht="12.3">
+      <c r="A161" s="24" t="s">
+        <v>525</v>
+      </c>
+      <c r="B161" s="152" t="s">
+        <v>448</v>
+      </c>
+      <c r="C161" s="152" t="s">
+        <v>340</v>
+      </c>
+      <c r="D161" s="152" t="s">
+        <v>221</v>
+      </c>
+      <c r="E161" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F161" s="152" t="s">
+        <v>490</v>
+      </c>
+      <c r="G161" s="152" t="s">
+        <v>278</v>
+      </c>
+      <c r="H161" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="I161" s="174" t="s">
+        <v>276</v>
+      </c>
+      <c r="J161" s="24" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="160" spans="1:38" ht="12.3">
-      <c r="A160" s="24"/>
-      <c r="B160" s="3"/>
-      <c r="C160" s="3"/>
-      <c r="D160" s="3"/>
-      <c r="E160" s="3"/>
-      <c r="F160" s="3"/>
-      <c r="G160" s="3"/>
-      <c r="H160" s="3"/>
-      <c r="I160" s="24"/>
-      <c r="J160" s="24"/>
-      <c r="K160" s="3"/>
-      <c r="L160" s="3"/>
-      <c r="M160" s="3"/>
-      <c r="N160" s="3"/>
-      <c r="O160" s="3"/>
-      <c r="P160" s="3"/>
-      <c r="Q160" s="3"/>
-      <c r="R160" s="3"/>
-      <c r="T160" s="3"/>
-    </row>
-    <row r="161" spans="1:20" ht="12.3">
-      <c r="A161" s="24"/>
-      <c r="B161" s="3"/>
-      <c r="C161" s="3"/>
-      <c r="D161" s="3"/>
-      <c r="E161" s="3"/>
-      <c r="F161" s="3"/>
-      <c r="G161" s="3"/>
-      <c r="H161" s="3"/>
-      <c r="I161" s="24"/>
-      <c r="J161" s="24"/>
-      <c r="K161" s="3"/>
+      <c r="K161" s="116">
+        <v>0.39</v>
+      </c>
       <c r="L161" s="3"/>
-      <c r="M161" s="3"/>
-      <c r="N161" s="3"/>
-      <c r="O161" s="3"/>
-      <c r="P161" s="3"/>
-      <c r="Q161" s="3"/>
-      <c r="R161" s="3"/>
+      <c r="M161" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="N161" s="152" t="s">
+        <v>526</v>
+      </c>
+      <c r="O161" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="P161" s="152" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q161" s="152" t="s">
+        <v>34</v>
+      </c>
+      <c r="R161" s="152" t="s">
+        <v>461</v>
+      </c>
+      <c r="S161" s="156" t="s">
+        <v>225</v>
+      </c>
       <c r="T161" s="3"/>
-    </row>
-    <row r="162" spans="1:20" ht="12.3">
-      <c r="A162" s="24"/>
-      <c r="B162" s="3"/>
-      <c r="C162" s="3"/>
-      <c r="D162" s="3"/>
-      <c r="E162" s="3"/>
-      <c r="F162" s="3"/>
-      <c r="G162" s="3"/>
-      <c r="H162" s="3"/>
-      <c r="I162" s="24"/>
-      <c r="J162" s="24"/>
-      <c r="K162" s="3"/>
+      <c r="U161" s="208" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="162" spans="1:21" ht="12.3">
+      <c r="A162" s="24" t="s">
+        <v>531</v>
+      </c>
+      <c r="B162" s="152" t="s">
+        <v>448</v>
+      </c>
+      <c r="C162" s="152" t="s">
+        <v>508</v>
+      </c>
+      <c r="D162" s="152" t="s">
+        <v>221</v>
+      </c>
+      <c r="E162" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F162" s="152" t="s">
+        <v>490</v>
+      </c>
+      <c r="G162" s="152" t="s">
+        <v>278</v>
+      </c>
+      <c r="H162" s="3" t="s">
+        <v>523</v>
+      </c>
+      <c r="I162" s="174" t="s">
+        <v>276</v>
+      </c>
+      <c r="J162" s="24" t="s">
+        <v>532</v>
+      </c>
+      <c r="K162" s="209">
+        <v>0.39</v>
+      </c>
       <c r="L162" s="3"/>
-      <c r="M162" s="3"/>
-      <c r="N162" s="3"/>
-      <c r="O162" s="3"/>
-      <c r="P162" s="3"/>
-      <c r="Q162" s="3"/>
-      <c r="R162" s="3"/>
+      <c r="M162" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="N162" s="152" t="s">
+        <v>533</v>
+      </c>
+      <c r="O162" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="P162" s="152" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q162" s="152" t="s">
+        <v>34</v>
+      </c>
+      <c r="R162" s="152" t="s">
+        <v>461</v>
+      </c>
+      <c r="S162" s="156" t="s">
+        <v>225</v>
+      </c>
       <c r="T162" s="3"/>
-    </row>
-    <row r="163" spans="1:20" ht="12.3">
-      <c r="A163" s="24"/>
-      <c r="B163" s="3"/>
-      <c r="C163" s="3"/>
-      <c r="D163" s="3"/>
-      <c r="E163" s="3"/>
-      <c r="F163" s="3"/>
-      <c r="G163" s="3"/>
-      <c r="H163" s="3"/>
-      <c r="I163" s="24"/>
-      <c r="J163" s="24"/>
-      <c r="K163" s="3"/>
-      <c r="L163" s="3"/>
-      <c r="M163" s="3"/>
-      <c r="N163" s="3"/>
-      <c r="O163" s="3"/>
-      <c r="P163" s="3"/>
-      <c r="Q163" s="3"/>
-      <c r="R163" s="3"/>
-      <c r="T163" s="3"/>
-    </row>
-    <row r="164" spans="1:20" ht="12.3">
-      <c r="A164" s="24"/>
-      <c r="B164" s="3"/>
-      <c r="C164" s="3"/>
-      <c r="D164" s="3"/>
-      <c r="E164" s="3"/>
-      <c r="F164" s="3"/>
-      <c r="G164" s="3"/>
-      <c r="H164" s="3"/>
-      <c r="I164" s="24"/>
-      <c r="J164" s="24"/>
-      <c r="K164" s="3"/>
+      <c r="U162" s="208" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="163" spans="1:21" s="163" customFormat="1" ht="12.3">
+      <c r="A163" s="173" t="s">
+        <v>539</v>
+      </c>
+      <c r="B163" s="158" t="s">
+        <v>551</v>
+      </c>
+      <c r="C163" s="158" t="s">
+        <v>340</v>
+      </c>
+      <c r="D163" s="158" t="s">
+        <v>221</v>
+      </c>
+      <c r="E163" s="158" t="s">
+        <v>131</v>
+      </c>
+      <c r="F163" s="158" t="s">
+        <v>490</v>
+      </c>
+      <c r="G163" s="158" t="s">
+        <v>278</v>
+      </c>
+      <c r="H163" s="158" t="s">
+        <v>535</v>
+      </c>
+      <c r="I163" s="173" t="s">
+        <v>276</v>
+      </c>
+      <c r="J163" s="173" t="s">
+        <v>532</v>
+      </c>
+      <c r="K163" s="210">
+        <v>0.39</v>
+      </c>
+      <c r="L163" s="158"/>
+      <c r="M163" s="158" t="s">
+        <v>30</v>
+      </c>
+      <c r="N163" s="158" t="s">
+        <v>540</v>
+      </c>
+      <c r="O163" s="158" t="s">
+        <v>522</v>
+      </c>
+      <c r="P163" s="158" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q163" s="158" t="s">
+        <v>34</v>
+      </c>
+      <c r="R163" s="158" t="s">
+        <v>536</v>
+      </c>
+      <c r="S163" s="162" t="s">
+        <v>225</v>
+      </c>
+      <c r="T163" s="158"/>
+      <c r="U163" s="211" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="164" spans="1:21" ht="12.3">
+      <c r="A164" s="24" t="s">
+        <v>543</v>
+      </c>
+      <c r="B164" s="152" t="s">
+        <v>537</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D164" s="152" t="s">
+        <v>221</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>538</v>
+      </c>
+      <c r="F164" s="152" t="s">
+        <v>490</v>
+      </c>
+      <c r="G164" s="152" t="s">
+        <v>278</v>
+      </c>
+      <c r="H164" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="I164" s="174" t="s">
+        <v>276</v>
+      </c>
+      <c r="J164" s="24" t="s">
+        <v>532</v>
+      </c>
+      <c r="K164" s="209">
+        <v>0.39</v>
+      </c>
       <c r="L164" s="3"/>
-      <c r="M164" s="3"/>
-      <c r="N164" s="3"/>
-      <c r="O164" s="3"/>
-      <c r="P164" s="3"/>
-      <c r="Q164" s="3"/>
-      <c r="R164" s="3"/>
+      <c r="M164" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="N164" s="24" t="s">
+        <v>545</v>
+      </c>
+      <c r="O164" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="P164" s="152" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q164" s="152" t="s">
+        <v>34</v>
+      </c>
+      <c r="R164" s="212" t="s">
+        <v>542</v>
+      </c>
+      <c r="S164" s="156" t="s">
+        <v>225</v>
+      </c>
       <c r="T164" s="3"/>
-    </row>
-    <row r="165" spans="1:20" ht="12.3">
-      <c r="A165" s="24"/>
-      <c r="B165" s="3"/>
-      <c r="C165" s="3"/>
-      <c r="D165" s="3"/>
-      <c r="E165" s="3"/>
-      <c r="F165" s="3"/>
-      <c r="G165" s="3"/>
-      <c r="H165" s="3"/>
-      <c r="I165" s="24"/>
-      <c r="J165" s="24"/>
-      <c r="K165" s="3"/>
-      <c r="L165" s="3"/>
-      <c r="M165" s="3"/>
-      <c r="N165" s="3"/>
-      <c r="O165" s="3"/>
-      <c r="P165" s="3"/>
-      <c r="Q165" s="3"/>
-      <c r="R165" s="3"/>
-      <c r="T165" s="3"/>
-    </row>
-    <row r="166" spans="1:20" ht="12.3">
-      <c r="A166" s="24"/>
-      <c r="B166" s="3"/>
-      <c r="C166" s="3"/>
-      <c r="D166" s="3"/>
-      <c r="E166" s="3"/>
-      <c r="F166" s="3"/>
-      <c r="G166" s="3"/>
-      <c r="H166" s="3"/>
-      <c r="I166" s="24"/>
-      <c r="J166" s="24"/>
-      <c r="K166" s="3"/>
-      <c r="L166" s="3"/>
-      <c r="M166" s="3"/>
-      <c r="N166" s="3"/>
-      <c r="O166" s="3"/>
-      <c r="P166" s="3"/>
-      <c r="Q166" s="3"/>
-      <c r="R166" s="3"/>
-      <c r="T166" s="3"/>
-    </row>
-    <row r="167" spans="1:20" ht="12.3">
-      <c r="A167" s="24"/>
-      <c r="B167" s="3"/>
-      <c r="C167" s="3"/>
-      <c r="D167" s="3"/>
-      <c r="E167" s="3"/>
-      <c r="F167" s="3"/>
-      <c r="G167" s="3"/>
-      <c r="H167" s="3"/>
-      <c r="I167" s="24"/>
-      <c r="J167" s="24"/>
-      <c r="K167" s="3"/>
-      <c r="L167" s="3"/>
-      <c r="M167" s="3"/>
-      <c r="N167" s="3"/>
-      <c r="O167" s="3"/>
-      <c r="P167" s="3"/>
-      <c r="Q167" s="3"/>
-      <c r="R167" s="3"/>
-      <c r="T167" s="3"/>
-    </row>
-    <row r="168" spans="1:20" ht="12.3">
-      <c r="A168" s="24"/>
-      <c r="B168" s="3"/>
-      <c r="C168" s="3"/>
-      <c r="D168" s="3"/>
-      <c r="E168" s="3"/>
-      <c r="F168" s="3"/>
-      <c r="G168" s="3"/>
-      <c r="H168" s="3"/>
-      <c r="I168" s="24"/>
-      <c r="J168" s="24"/>
-      <c r="K168" s="3"/>
-      <c r="L168" s="3"/>
-      <c r="M168" s="3"/>
-      <c r="N168" s="3"/>
-      <c r="O168" s="3"/>
-      <c r="P168" s="3"/>
-      <c r="Q168" s="3"/>
-      <c r="R168" s="3"/>
-      <c r="T168" s="3"/>
-    </row>
-    <row r="169" spans="1:20" ht="12.3">
-      <c r="A169" s="24"/>
-      <c r="B169" s="3"/>
-      <c r="C169" s="3"/>
-      <c r="D169" s="3"/>
-      <c r="E169" s="3"/>
-      <c r="F169" s="3"/>
-      <c r="G169" s="3"/>
-      <c r="H169" s="3"/>
-      <c r="I169" s="24"/>
-      <c r="J169" s="24"/>
-      <c r="K169" s="3"/>
-      <c r="L169" s="3"/>
-      <c r="M169" s="3"/>
-      <c r="N169" s="3"/>
-      <c r="O169" s="3"/>
-      <c r="P169" s="3"/>
-      <c r="Q169" s="3"/>
-      <c r="R169" s="3"/>
-      <c r="T169" s="3"/>
-    </row>
-    <row r="170" spans="1:20" ht="12.3">
+      <c r="U164" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="165" spans="1:21" s="163" customFormat="1" ht="12.3">
+      <c r="A165" s="173" t="s">
+        <v>544</v>
+      </c>
+      <c r="B165" s="158" t="s">
+        <v>568</v>
+      </c>
+      <c r="C165" s="158" t="s">
+        <v>47</v>
+      </c>
+      <c r="D165" s="158" t="s">
+        <v>221</v>
+      </c>
+      <c r="E165" s="158" t="s">
+        <v>547</v>
+      </c>
+      <c r="F165" s="158" t="s">
+        <v>490</v>
+      </c>
+      <c r="G165" s="158" t="s">
+        <v>278</v>
+      </c>
+      <c r="H165" s="158" t="s">
+        <v>535</v>
+      </c>
+      <c r="I165" s="173" t="s">
+        <v>276</v>
+      </c>
+      <c r="J165" s="173" t="s">
+        <v>532</v>
+      </c>
+      <c r="K165" s="210">
+        <v>0.39</v>
+      </c>
+      <c r="L165" s="158"/>
+      <c r="M165" s="158" t="s">
+        <v>30</v>
+      </c>
+      <c r="N165" s="173" t="s">
+        <v>548</v>
+      </c>
+      <c r="O165" s="158" t="s">
+        <v>522</v>
+      </c>
+      <c r="P165" s="158" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q165" s="158" t="s">
+        <v>34</v>
+      </c>
+      <c r="R165" s="158" t="s">
+        <v>542</v>
+      </c>
+      <c r="S165" s="162" t="s">
+        <v>225</v>
+      </c>
+      <c r="T165" s="158" t="s">
+        <v>550</v>
+      </c>
+      <c r="U165" s="163" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="166" spans="1:21" s="129" customFormat="1" ht="12.3">
+      <c r="A166" s="170" t="s">
+        <v>552</v>
+      </c>
+      <c r="B166" s="124" t="s">
+        <v>553</v>
+      </c>
+      <c r="C166" s="124" t="s">
+        <v>47</v>
+      </c>
+      <c r="D166" s="124" t="s">
+        <v>221</v>
+      </c>
+      <c r="E166" s="124" t="s">
+        <v>554</v>
+      </c>
+      <c r="F166" s="124" t="s">
+        <v>490</v>
+      </c>
+      <c r="G166" s="124" t="s">
+        <v>278</v>
+      </c>
+      <c r="H166" s="124" t="s">
+        <v>535</v>
+      </c>
+      <c r="I166" s="170" t="s">
+        <v>276</v>
+      </c>
+      <c r="J166" s="170" t="s">
+        <v>532</v>
+      </c>
+      <c r="K166" s="213">
+        <v>0.39</v>
+      </c>
+      <c r="L166" s="124"/>
+      <c r="M166" s="124" t="s">
+        <v>30</v>
+      </c>
+      <c r="N166" s="170" t="s">
+        <v>555</v>
+      </c>
+      <c r="O166" s="124" t="s">
+        <v>522</v>
+      </c>
+      <c r="P166" s="124" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q166" s="124" t="s">
+        <v>34</v>
+      </c>
+      <c r="R166" s="124" t="s">
+        <v>542</v>
+      </c>
+      <c r="S166" s="128" t="s">
+        <v>225</v>
+      </c>
+      <c r="T166" s="124"/>
+      <c r="U166" s="129" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="167" spans="1:21" s="163" customFormat="1" ht="12.3">
+      <c r="A167" s="173" t="s">
+        <v>557</v>
+      </c>
+      <c r="B167" s="158" t="s">
+        <v>558</v>
+      </c>
+      <c r="C167" s="158" t="s">
+        <v>47</v>
+      </c>
+      <c r="D167" s="158" t="s">
+        <v>221</v>
+      </c>
+      <c r="E167" s="158" t="s">
+        <v>538</v>
+      </c>
+      <c r="F167" s="158" t="s">
+        <v>490</v>
+      </c>
+      <c r="G167" s="158" t="s">
+        <v>278</v>
+      </c>
+      <c r="H167" s="158" t="s">
+        <v>535</v>
+      </c>
+      <c r="I167" s="173" t="s">
+        <v>276</v>
+      </c>
+      <c r="J167" s="173" t="s">
+        <v>532</v>
+      </c>
+      <c r="K167" s="210">
+        <v>0.39</v>
+      </c>
+      <c r="L167" s="158"/>
+      <c r="M167" s="158" t="s">
+        <v>30</v>
+      </c>
+      <c r="N167" s="173" t="s">
+        <v>559</v>
+      </c>
+      <c r="O167" s="158" t="s">
+        <v>522</v>
+      </c>
+      <c r="P167" s="158" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q167" s="158" t="s">
+        <v>34</v>
+      </c>
+      <c r="R167" s="158" t="s">
+        <v>542</v>
+      </c>
+      <c r="S167" s="162" t="s">
+        <v>225</v>
+      </c>
+      <c r="T167" s="158"/>
+    </row>
+    <row r="168" spans="1:21" s="163" customFormat="1" ht="12.3">
+      <c r="A168" s="173" t="s">
+        <v>561</v>
+      </c>
+      <c r="B168" s="158" t="s">
+        <v>562</v>
+      </c>
+      <c r="C168" s="158" t="s">
+        <v>203</v>
+      </c>
+      <c r="D168" s="158" t="s">
+        <v>221</v>
+      </c>
+      <c r="E168" s="158" t="s">
+        <v>538</v>
+      </c>
+      <c r="F168" s="158" t="s">
+        <v>490</v>
+      </c>
+      <c r="G168" s="158" t="s">
+        <v>278</v>
+      </c>
+      <c r="H168" s="158" t="s">
+        <v>535</v>
+      </c>
+      <c r="I168" s="173" t="s">
+        <v>276</v>
+      </c>
+      <c r="J168" s="173" t="s">
+        <v>532</v>
+      </c>
+      <c r="K168" s="210">
+        <v>0.39</v>
+      </c>
+      <c r="L168" s="158"/>
+      <c r="M168" s="158" t="s">
+        <v>30</v>
+      </c>
+      <c r="N168" s="158" t="s">
+        <v>564</v>
+      </c>
+      <c r="O168" s="158" t="s">
+        <v>522</v>
+      </c>
+      <c r="P168" s="158" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q168" s="158" t="s">
+        <v>34</v>
+      </c>
+      <c r="R168" s="158" t="s">
+        <v>542</v>
+      </c>
+      <c r="S168" s="162" t="s">
+        <v>225</v>
+      </c>
+      <c r="T168" s="158" t="s">
+        <v>560</v>
+      </c>
+      <c r="U168" s="163" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="169" spans="1:21" s="163" customFormat="1" ht="12.3">
+      <c r="A169" s="173" t="s">
+        <v>565</v>
+      </c>
+      <c r="B169" s="158" t="s">
+        <v>566</v>
+      </c>
+      <c r="C169" s="158" t="s">
+        <v>203</v>
+      </c>
+      <c r="D169" s="158" t="s">
+        <v>221</v>
+      </c>
+      <c r="E169" s="158" t="s">
+        <v>538</v>
+      </c>
+      <c r="F169" s="158" t="s">
+        <v>490</v>
+      </c>
+      <c r="G169" s="158" t="s">
+        <v>278</v>
+      </c>
+      <c r="H169" s="158" t="s">
+        <v>535</v>
+      </c>
+      <c r="I169" s="173" t="s">
+        <v>276</v>
+      </c>
+      <c r="J169" s="173" t="s">
+        <v>532</v>
+      </c>
+      <c r="K169" s="160">
+        <v>0.39</v>
+      </c>
+      <c r="L169" s="158"/>
+      <c r="M169" s="158" t="s">
+        <v>30</v>
+      </c>
+      <c r="N169" s="158" t="s">
+        <v>567</v>
+      </c>
+      <c r="O169" s="158" t="s">
+        <v>522</v>
+      </c>
+      <c r="P169" s="158" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q169" s="158" t="s">
+        <v>34</v>
+      </c>
+      <c r="R169" s="158" t="s">
+        <v>542</v>
+      </c>
+      <c r="S169" s="162" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="170" spans="1:21" ht="12.3">
       <c r="A170" s="24"/>
       <c r="B170" s="3"/>
       <c r="C170" s="3"/>
@@ -12881,9 +13415,11 @@
       <c r="P170" s="3"/>
       <c r="Q170" s="3"/>
       <c r="R170" s="3"/>
-      <c r="T170" s="3"/>
-    </row>
-    <row r="171" spans="1:20" ht="12.3">
+      <c r="T170" s="152" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="171" spans="1:21" ht="12.3">
       <c r="A171" s="24"/>
       <c r="B171" s="3"/>
       <c r="C171" s="3"/>
@@ -12904,7 +13440,7 @@
       <c r="R171" s="3"/>
       <c r="T171" s="3"/>
     </row>
-    <row r="172" spans="1:20" ht="12.3">
+    <row r="172" spans="1:21" ht="12.3">
       <c r="A172" s="24"/>
       <c r="B172" s="3"/>
       <c r="C172" s="3"/>
@@ -12925,7 +13461,7 @@
       <c r="R172" s="3"/>
       <c r="T172" s="3"/>
     </row>
-    <row r="173" spans="1:20" ht="12.3">
+    <row r="173" spans="1:21" ht="12.3">
       <c r="A173" s="24"/>
       <c r="B173" s="3"/>
       <c r="C173" s="3"/>
@@ -12946,7 +13482,7 @@
       <c r="R173" s="3"/>
       <c r="T173" s="3"/>
     </row>
-    <row r="174" spans="1:20" ht="12.3">
+    <row r="174" spans="1:21" ht="12.3">
       <c r="A174" s="24"/>
       <c r="B174" s="3"/>
       <c r="C174" s="3"/>
@@ -12967,7 +13503,7 @@
       <c r="R174" s="3"/>
       <c r="T174" s="3"/>
     </row>
-    <row r="175" spans="1:20" ht="12.3">
+    <row r="175" spans="1:21" ht="12.3">
       <c r="A175" s="24"/>
       <c r="B175" s="3"/>
       <c r="C175" s="3"/>
@@ -12988,7 +13524,7 @@
       <c r="R175" s="3"/>
       <c r="T175" s="3"/>
     </row>
-    <row r="176" spans="1:20" ht="12.3">
+    <row r="176" spans="1:21" ht="12.3">
       <c r="A176" s="24"/>
       <c r="B176" s="3"/>
       <c r="C176" s="3"/>

</xml_diff>

<commit_message>
collected reapplication and misalignment data with velcro
</commit_message>
<xml_diff>
--- a/data_25_01_14.xlsx
+++ b/data_25_01_14.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csuma-my.sharepoint.com/personal/toppenheim_csum_edu/Documents/Documents/GitHub/Strain-Sensor-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="199" documentId="13_ncr:1_{8B456EFE-629F-46DB-BDAD-2277034A9104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{90B54E48-1048-4C20-8019-AEFA531FA849}"/>
+  <xr:revisionPtr revIDLastSave="410" documentId="13_ncr:1_{8B456EFE-629F-46DB-BDAD-2277034A9104}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AD109C3-4516-41C0-A4CA-1B5F1C1A3361}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3720" uniqueCount="569">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3917" uniqueCount="609">
   <si>
     <t>Sample Name</t>
   </si>
@@ -1731,9 +1731,6 @@
     <t>LMC648 75x gain + MCP3421 2x gain+velcro 5th  reapply 10 degree</t>
   </si>
   <si>
-    <t>CSV Data/4_17_25/2.24 20 deg.jpg</t>
-  </si>
-  <si>
     <t>CSV Data/4_17_25/2.24_misalignment_v10_4_17_25</t>
   </si>
   <si>
@@ -1747,6 +1744,129 @@
   </si>
   <si>
     <t>LMC648 75x gain + MCP3421 2x gain+velcro 2nd reapply (same sample as row 163)</t>
+  </si>
+  <si>
+    <t>4_18_25</t>
+  </si>
+  <si>
+    <t>2.27_static_v1_4_18_25</t>
+  </si>
+  <si>
+    <t>slipped after first bend then remained more steady…top part not stuck on velcro need to glue velcro to sample</t>
+  </si>
+  <si>
+    <t>2.27_reapplication_v1_4_18_25</t>
+  </si>
+  <si>
+    <t>CSV Data/4_18_25/2.27_static_v1_4_18_25.csv</t>
+  </si>
+  <si>
+    <t>CSV Data/4_18_25/2.27_reapplication_v1_4_18_25.csv</t>
+  </si>
+  <si>
+    <t>pre-stretched, velcro slipping…really need to glue on top part of silcone</t>
+  </si>
+  <si>
+    <t>2.27_reapplication_v2_4_18_25</t>
+  </si>
+  <si>
+    <t>LMC648 75x gain + MCP3421 2x gain+velcro reapply previous</t>
+  </si>
+  <si>
+    <t>LMC648 75x gain + MCP3421 2x gain+velcro 2nd reapply</t>
+  </si>
+  <si>
+    <t>CSV Data/4_18_25/2.27_reapplication_v2_4_18_25.csv</t>
+  </si>
+  <si>
+    <t>pre-stretched, silicone glued velcro to sample</t>
+  </si>
+  <si>
+    <t>2.27_reapplication_v3_4_18_25</t>
+  </si>
+  <si>
+    <t>LMC648 75x gain + MCP3421 2x gain+velcro 3rd reapply</t>
+  </si>
+  <si>
+    <t>CSV Data/4_18_25/2.27_reapplication_v3_4_18_25.csv</t>
+  </si>
+  <si>
+    <t>added weight to hold down wires to ensure when plate comes back up wires don't try and lift sample</t>
+  </si>
+  <si>
+    <t>2.27_reapplication_v4_4_18_25</t>
+  </si>
+  <si>
+    <t>LMC648 75x gain + MCP3421 2x gain+velcro 4th reapply</t>
+  </si>
+  <si>
+    <t>no weight and very little pre-stretch</t>
+  </si>
+  <si>
+    <t>2.27_reapplication_v5_4_18_25</t>
+  </si>
+  <si>
+    <t>LMC648 75x gain + MCP3421 2x gain+velcro 5th reapply</t>
+  </si>
+  <si>
+    <t>CSV Data/4_18_25/2.27_reapplication_v4_4_18_25.csv</t>
+  </si>
+  <si>
+    <t>CSV Data/4_18_25/2.27_reapplication_v5_4_18_25.csv</t>
+  </si>
+  <si>
+    <t>used stronger bottom velcro piece (mounting oval) on top part of sensor to see if makes a difference</t>
+  </si>
+  <si>
+    <t>CSV Data/4_18_25/2.34_static_v1_4_18_25.csv</t>
+  </si>
+  <si>
+    <t>2.34_static_v1_4_18_25</t>
+  </si>
+  <si>
+    <t>lighter duty velcro glued on both ends of gauge.  Using lighter duty velcro on bender side.  Velcro about 0.75 " long on both side of sample to increase grip area</t>
+  </si>
+  <si>
+    <t>CSV Data/4_18_25/sample 2.34 first static test.jpg</t>
+  </si>
+  <si>
+    <t>2.34_reapplication_v1_4_18_25</t>
+  </si>
+  <si>
+    <t>CSV Data/4_18_25/2.34_reapplication_v1_4_18_25.csv</t>
+  </si>
+  <si>
+    <t>2.34_reapplication_v2_4_18_25</t>
+  </si>
+  <si>
+    <t>LMC648 75x gain + MCP3421 2x gain+velcro reapply third</t>
+  </si>
+  <si>
+    <t>2.34 in</t>
+  </si>
+  <si>
+    <t>CSV Data/4_18_25/2.34_reapplication_v2_4_18_25.csv</t>
+  </si>
+  <si>
+    <t>2.34_misalignment_v10_4_18_25</t>
+  </si>
+  <si>
+    <t>CSV Data/4_18_25/2.34_misalignment_v10_4_18_25</t>
+  </si>
+  <si>
+    <t>2.34_misalignment_v20_4_18_25</t>
+  </si>
+  <si>
+    <t>LMC648 75x gain + MCP3421 2x gain+velcro 6th  reapply 20 degree</t>
+  </si>
+  <si>
+    <t>CSV Data/4_18_25/2.34_misalignment_v20_4_18_25</t>
+  </si>
+  <si>
+    <t>CSV Data/4_18_25/2.34 10 degree misalignment.jpg</t>
+  </si>
+  <si>
+    <t>CSV Data/4_18_25/2.34 20 deg misalignment.jpg</t>
   </si>
 </sst>
 </file>
@@ -2082,7 +2202,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="214">
+  <cellXfs count="219">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2595,23 +2715,38 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="18" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="9" fontId="2" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="16" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2633,6 +2768,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2839,8 +2978,8 @@
   <dimension ref="A1:AL990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A141" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A168" sqref="A168"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B183" sqref="B183"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -12850,7 +12989,7 @@
       <c r="AK160" s="7"/>
       <c r="AL160" s="7"/>
     </row>
-    <row r="161" spans="1:21" ht="12.3">
+    <row r="161" spans="1:38" ht="12.3">
       <c r="A161" s="24" t="s">
         <v>525</v>
       </c>
@@ -12907,11 +13046,11 @@
         <v>225</v>
       </c>
       <c r="T161" s="3"/>
-      <c r="U161" s="208" t="s">
+      <c r="U161" s="152" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="162" spans="1:21" ht="12.3">
+    <row r="162" spans="1:38" ht="12.3">
       <c r="A162" s="24" t="s">
         <v>531</v>
       </c>
@@ -12942,7 +13081,7 @@
       <c r="J162" s="24" t="s">
         <v>532</v>
       </c>
-      <c r="K162" s="209">
+      <c r="K162" s="208">
         <v>0.39</v>
       </c>
       <c r="L162" s="3"/>
@@ -12968,11 +13107,11 @@
         <v>225</v>
       </c>
       <c r="T162" s="3"/>
-      <c r="U162" s="208" t="s">
+      <c r="U162" s="152" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="163" spans="1:21" s="163" customFormat="1" ht="12.3">
+    <row r="163" spans="1:38" s="163" customFormat="1" ht="12.3">
       <c r="A163" s="173" t="s">
         <v>539</v>
       </c>
@@ -13003,7 +13142,7 @@
       <c r="J163" s="173" t="s">
         <v>532</v>
       </c>
-      <c r="K163" s="210">
+      <c r="K163" s="209">
         <v>0.39</v>
       </c>
       <c r="L163" s="158"/>
@@ -13029,11 +13168,11 @@
         <v>225</v>
       </c>
       <c r="T163" s="158"/>
-      <c r="U163" s="211" t="s">
+      <c r="U163" s="158" t="s">
         <v>541</v>
       </c>
     </row>
-    <row r="164" spans="1:21" ht="12.3">
+    <row r="164" spans="1:38" ht="12.3">
       <c r="A164" s="24" t="s">
         <v>543</v>
       </c>
@@ -13064,7 +13203,7 @@
       <c r="J164" s="24" t="s">
         <v>532</v>
       </c>
-      <c r="K164" s="209">
+      <c r="K164" s="208">
         <v>0.39</v>
       </c>
       <c r="L164" s="3"/>
@@ -13083,7 +13222,7 @@
       <c r="Q164" s="152" t="s">
         <v>34</v>
       </c>
-      <c r="R164" s="212" t="s">
+      <c r="R164" s="210" t="s">
         <v>542</v>
       </c>
       <c r="S164" s="156" t="s">
@@ -13094,12 +13233,12 @@
         <v>546</v>
       </c>
     </row>
-    <row r="165" spans="1:21" s="163" customFormat="1" ht="12.3">
+    <row r="165" spans="1:38" s="163" customFormat="1" ht="12.3">
       <c r="A165" s="173" t="s">
         <v>544</v>
       </c>
       <c r="B165" s="158" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="C165" s="158" t="s">
         <v>47</v>
@@ -13125,7 +13264,7 @@
       <c r="J165" s="173" t="s">
         <v>532</v>
       </c>
-      <c r="K165" s="210">
+      <c r="K165" s="209">
         <v>0.39</v>
       </c>
       <c r="L165" s="158"/>
@@ -13157,7 +13296,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="166" spans="1:21" s="129" customFormat="1" ht="12.3">
+    <row r="166" spans="1:38" s="129" customFormat="1" ht="12.3">
       <c r="A166" s="170" t="s">
         <v>552</v>
       </c>
@@ -13188,7 +13327,7 @@
       <c r="J166" s="170" t="s">
         <v>532</v>
       </c>
-      <c r="K166" s="213">
+      <c r="K166" s="211">
         <v>0.39</v>
       </c>
       <c r="L166" s="124"/>
@@ -13218,7 +13357,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="167" spans="1:21" s="163" customFormat="1" ht="12.3">
+    <row r="167" spans="1:38" s="163" customFormat="1" ht="12.3">
       <c r="A167" s="173" t="s">
         <v>557</v>
       </c>
@@ -13249,7 +13388,7 @@
       <c r="J167" s="173" t="s">
         <v>532</v>
       </c>
-      <c r="K167" s="210">
+      <c r="K167" s="209">
         <v>0.39</v>
       </c>
       <c r="L167" s="158"/>
@@ -13276,7 +13415,7 @@
       </c>
       <c r="T167" s="158"/>
     </row>
-    <row r="168" spans="1:21" s="163" customFormat="1" ht="12.3">
+    <row r="168" spans="1:38" s="163" customFormat="1" ht="12.3">
       <c r="A168" s="173" t="s">
         <v>561</v>
       </c>
@@ -13307,7 +13446,7 @@
       <c r="J168" s="173" t="s">
         <v>532</v>
       </c>
-      <c r="K168" s="210">
+      <c r="K168" s="209">
         <v>0.39</v>
       </c>
       <c r="L168" s="158"/>
@@ -13315,7 +13454,7 @@
         <v>30</v>
       </c>
       <c r="N168" s="158" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="O168" s="158" t="s">
         <v>522</v>
@@ -13339,12 +13478,12 @@
         <v>541</v>
       </c>
     </row>
-    <row r="169" spans="1:21" s="163" customFormat="1" ht="12.3">
+    <row r="169" spans="1:38" s="163" customFormat="1" ht="12.3">
       <c r="A169" s="173" t="s">
+        <v>564</v>
+      </c>
+      <c r="B169" s="158" t="s">
         <v>565</v>
-      </c>
-      <c r="B169" s="158" t="s">
-        <v>566</v>
       </c>
       <c r="C169" s="158" t="s">
         <v>203</v>
@@ -13378,7 +13517,7 @@
         <v>30</v>
       </c>
       <c r="N169" s="158" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="O169" s="158" t="s">
         <v>522</v>
@@ -13396,261 +13535,714 @@
         <v>225</v>
       </c>
     </row>
-    <row r="170" spans="1:21" ht="12.3">
-      <c r="A170" s="24"/>
-      <c r="B170" s="3"/>
-      <c r="C170" s="3"/>
-      <c r="D170" s="3"/>
-      <c r="E170" s="3"/>
-      <c r="F170" s="3"/>
-      <c r="G170" s="3"/>
-      <c r="H170" s="3"/>
-      <c r="I170" s="24"/>
-      <c r="J170" s="24"/>
-      <c r="K170" s="3"/>
-      <c r="L170" s="3"/>
-      <c r="M170" s="3"/>
-      <c r="N170" s="3"/>
-      <c r="O170" s="3"/>
-      <c r="P170" s="3"/>
-      <c r="Q170" s="3"/>
-      <c r="R170" s="3"/>
-      <c r="T170" s="152" t="s">
-        <v>563</v>
-      </c>
-    </row>
-    <row r="171" spans="1:21" ht="12.3">
-      <c r="A171" s="24"/>
-      <c r="B171" s="3"/>
-      <c r="C171" s="3"/>
-      <c r="D171" s="3"/>
-      <c r="E171" s="3"/>
-      <c r="F171" s="3"/>
-      <c r="G171" s="3"/>
-      <c r="H171" s="3"/>
-      <c r="I171" s="24"/>
-      <c r="J171" s="24"/>
-      <c r="K171" s="3"/>
-      <c r="L171" s="3"/>
-      <c r="M171" s="3"/>
-      <c r="N171" s="3"/>
-      <c r="O171" s="3"/>
-      <c r="P171" s="3"/>
-      <c r="Q171" s="3"/>
-      <c r="R171" s="3"/>
-      <c r="T171" s="3"/>
-    </row>
-    <row r="172" spans="1:21" ht="12.3">
-      <c r="A172" s="24"/>
-      <c r="B172" s="3"/>
-      <c r="C172" s="3"/>
-      <c r="D172" s="3"/>
-      <c r="E172" s="3"/>
-      <c r="F172" s="3"/>
-      <c r="G172" s="3"/>
-      <c r="H172" s="3"/>
-      <c r="I172" s="24"/>
-      <c r="J172" s="24"/>
-      <c r="K172" s="3"/>
-      <c r="L172" s="3"/>
-      <c r="M172" s="3"/>
-      <c r="N172" s="3"/>
-      <c r="O172" s="3"/>
-      <c r="P172" s="3"/>
-      <c r="Q172" s="3"/>
-      <c r="R172" s="3"/>
-      <c r="T172" s="3"/>
-    </row>
-    <row r="173" spans="1:21" ht="12.3">
-      <c r="A173" s="24"/>
-      <c r="B173" s="3"/>
-      <c r="C173" s="3"/>
-      <c r="D173" s="3"/>
-      <c r="E173" s="3"/>
-      <c r="F173" s="3"/>
-      <c r="G173" s="3"/>
-      <c r="H173" s="3"/>
-      <c r="I173" s="24"/>
-      <c r="J173" s="24"/>
-      <c r="K173" s="3"/>
-      <c r="L173" s="3"/>
-      <c r="M173" s="3"/>
-      <c r="N173" s="3"/>
-      <c r="O173" s="3"/>
-      <c r="P173" s="3"/>
-      <c r="Q173" s="3"/>
-      <c r="R173" s="3"/>
-      <c r="T173" s="3"/>
-    </row>
-    <row r="174" spans="1:21" ht="12.3">
-      <c r="A174" s="24"/>
-      <c r="B174" s="3"/>
-      <c r="C174" s="3"/>
-      <c r="D174" s="3"/>
-      <c r="E174" s="3"/>
-      <c r="F174" s="3"/>
-      <c r="G174" s="3"/>
-      <c r="H174" s="3"/>
-      <c r="I174" s="24"/>
-      <c r="J174" s="24"/>
-      <c r="K174" s="3"/>
-      <c r="L174" s="3"/>
-      <c r="M174" s="3"/>
-      <c r="N174" s="3"/>
-      <c r="O174" s="3"/>
-      <c r="P174" s="3"/>
-      <c r="Q174" s="3"/>
-      <c r="R174" s="3"/>
-      <c r="T174" s="3"/>
-    </row>
-    <row r="175" spans="1:21" ht="12.3">
-      <c r="A175" s="24"/>
-      <c r="B175" s="3"/>
-      <c r="C175" s="3"/>
-      <c r="D175" s="3"/>
-      <c r="E175" s="3"/>
-      <c r="F175" s="3"/>
-      <c r="G175" s="3"/>
-      <c r="H175" s="3"/>
-      <c r="I175" s="24"/>
-      <c r="J175" s="24"/>
-      <c r="K175" s="3"/>
-      <c r="L175" s="3"/>
-      <c r="M175" s="3"/>
-      <c r="N175" s="3"/>
-      <c r="O175" s="3"/>
-      <c r="P175" s="3"/>
-      <c r="Q175" s="3"/>
-      <c r="R175" s="3"/>
-      <c r="T175" s="3"/>
-    </row>
-    <row r="176" spans="1:21" ht="12.3">
-      <c r="A176" s="24"/>
-      <c r="B176" s="3"/>
-      <c r="C176" s="3"/>
-      <c r="D176" s="3"/>
-      <c r="E176" s="3"/>
-      <c r="F176" s="3"/>
-      <c r="G176" s="3"/>
-      <c r="H176" s="3"/>
-      <c r="I176" s="24"/>
-      <c r="J176" s="24"/>
-      <c r="K176" s="3"/>
-      <c r="L176" s="3"/>
-      <c r="M176" s="3"/>
-      <c r="N176" s="3"/>
-      <c r="O176" s="3"/>
-      <c r="P176" s="3"/>
-      <c r="Q176" s="3"/>
-      <c r="R176" s="3"/>
-      <c r="T176" s="3"/>
-    </row>
-    <row r="177" spans="1:20" ht="12.3">
-      <c r="A177" s="24"/>
-      <c r="B177" s="3"/>
-      <c r="C177" s="3"/>
-      <c r="D177" s="3"/>
-      <c r="E177" s="3"/>
-      <c r="F177" s="3"/>
-      <c r="G177" s="3"/>
-      <c r="H177" s="3"/>
-      <c r="I177" s="24"/>
-      <c r="J177" s="24"/>
-      <c r="K177" s="3"/>
-      <c r="L177" s="3"/>
-      <c r="M177" s="3"/>
-      <c r="N177" s="3"/>
-      <c r="O177" s="3"/>
-      <c r="P177" s="3"/>
-      <c r="Q177" s="3"/>
-      <c r="R177" s="3"/>
-      <c r="T177" s="3"/>
-    </row>
-    <row r="178" spans="1:20" ht="12.3">
-      <c r="A178" s="24"/>
-      <c r="B178" s="3"/>
-      <c r="C178" s="3"/>
-      <c r="D178" s="3"/>
-      <c r="E178" s="3"/>
-      <c r="F178" s="3"/>
-      <c r="G178" s="3"/>
-      <c r="H178" s="3"/>
-      <c r="I178" s="24"/>
-      <c r="J178" s="24"/>
-      <c r="K178" s="3"/>
-      <c r="L178" s="3"/>
-      <c r="M178" s="3"/>
-      <c r="N178" s="3"/>
-      <c r="O178" s="3"/>
-      <c r="P178" s="3"/>
-      <c r="Q178" s="3"/>
-      <c r="R178" s="3"/>
-      <c r="T178" s="3"/>
-    </row>
-    <row r="179" spans="1:20" ht="12.3">
-      <c r="A179" s="24"/>
-      <c r="B179" s="3"/>
-      <c r="C179" s="3"/>
-      <c r="D179" s="3"/>
-      <c r="E179" s="3"/>
-      <c r="F179" s="3"/>
-      <c r="G179" s="3"/>
-      <c r="H179" s="3"/>
-      <c r="I179" s="24"/>
-      <c r="J179" s="24"/>
-      <c r="K179" s="3"/>
-      <c r="L179" s="3"/>
-      <c r="M179" s="3"/>
-      <c r="N179" s="3"/>
-      <c r="O179" s="3"/>
-      <c r="P179" s="3"/>
-      <c r="Q179" s="3"/>
-      <c r="R179" s="3"/>
-      <c r="T179" s="3"/>
-    </row>
-    <row r="180" spans="1:20" ht="12.3">
-      <c r="A180" s="24"/>
-      <c r="B180" s="3"/>
-      <c r="C180" s="3"/>
-      <c r="D180" s="3"/>
-      <c r="E180" s="3"/>
-      <c r="F180" s="3"/>
-      <c r="G180" s="3"/>
-      <c r="H180" s="3"/>
-      <c r="I180" s="24"/>
-      <c r="J180" s="24"/>
-      <c r="K180" s="3"/>
-      <c r="L180" s="3"/>
-      <c r="M180" s="3"/>
-      <c r="N180" s="3"/>
-      <c r="O180" s="3"/>
-      <c r="P180" s="3"/>
-      <c r="Q180" s="3"/>
-      <c r="R180" s="3"/>
-      <c r="T180" s="3"/>
-    </row>
-    <row r="181" spans="1:20" ht="12.3">
-      <c r="A181" s="24"/>
-      <c r="B181" s="3"/>
-      <c r="C181" s="3"/>
-      <c r="D181" s="3"/>
-      <c r="E181" s="3"/>
-      <c r="F181" s="3"/>
-      <c r="G181" s="3"/>
-      <c r="H181" s="3"/>
-      <c r="I181" s="24"/>
-      <c r="J181" s="24"/>
-      <c r="K181" s="3"/>
-      <c r="L181" s="3"/>
-      <c r="M181" s="3"/>
-      <c r="N181" s="3"/>
-      <c r="O181" s="3"/>
-      <c r="P181" s="3"/>
-      <c r="Q181" s="3"/>
-      <c r="R181" s="3"/>
-      <c r="T181" s="3"/>
-    </row>
-    <row r="182" spans="1:20" ht="12.3">
+    <row r="170" spans="1:38" ht="15.75" customHeight="1">
+      <c r="A170" s="184" t="s">
+        <v>568</v>
+      </c>
+      <c r="B170" s="6"/>
+      <c r="C170" s="6"/>
+      <c r="D170" s="6"/>
+      <c r="E170" s="6"/>
+      <c r="F170" s="6"/>
+      <c r="G170" s="6"/>
+      <c r="H170" s="6"/>
+      <c r="I170" s="5"/>
+      <c r="J170" s="5"/>
+      <c r="K170" s="6"/>
+      <c r="L170" s="6"/>
+      <c r="M170" s="6"/>
+      <c r="N170" s="207"/>
+      <c r="O170" s="6"/>
+      <c r="P170" s="6"/>
+      <c r="Q170" s="6"/>
+      <c r="R170" s="6"/>
+      <c r="S170" s="7"/>
+      <c r="T170" s="6"/>
+      <c r="U170" s="7"/>
+      <c r="V170" s="7"/>
+      <c r="W170" s="7"/>
+      <c r="X170" s="7"/>
+      <c r="Y170" s="7"/>
+      <c r="Z170" s="7"/>
+      <c r="AA170" s="7"/>
+      <c r="AB170" s="7"/>
+      <c r="AC170" s="7"/>
+      <c r="AD170" s="7"/>
+      <c r="AE170" s="7"/>
+      <c r="AF170" s="7"/>
+      <c r="AG170" s="7"/>
+      <c r="AH170" s="7"/>
+      <c r="AI170" s="7"/>
+      <c r="AJ170" s="7"/>
+      <c r="AK170" s="7"/>
+      <c r="AL170" s="7"/>
+    </row>
+    <row r="171" spans="1:38" s="157" customFormat="1" ht="12.3">
+      <c r="A171" s="174" t="s">
+        <v>569</v>
+      </c>
+      <c r="B171" s="152" t="s">
+        <v>537</v>
+      </c>
+      <c r="C171" s="152" t="s">
+        <v>340</v>
+      </c>
+      <c r="D171" s="152" t="s">
+        <v>221</v>
+      </c>
+      <c r="E171" s="152" t="s">
+        <v>281</v>
+      </c>
+      <c r="F171" s="152" t="s">
+        <v>490</v>
+      </c>
+      <c r="G171" s="152" t="s">
+        <v>278</v>
+      </c>
+      <c r="H171" s="152" t="s">
+        <v>146</v>
+      </c>
+      <c r="I171" s="174" t="s">
+        <v>276</v>
+      </c>
+      <c r="J171" s="174" t="s">
+        <v>293</v>
+      </c>
+      <c r="K171" s="212">
+        <v>0.4</v>
+      </c>
+      <c r="L171" s="152"/>
+      <c r="M171" s="152" t="s">
+        <v>148</v>
+      </c>
+      <c r="N171" s="152" t="s">
+        <v>572</v>
+      </c>
+      <c r="O171" s="152" t="s">
+        <v>568</v>
+      </c>
+      <c r="P171" s="152" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q171" s="152" t="s">
+        <v>34</v>
+      </c>
+      <c r="R171" s="152" t="s">
+        <v>481</v>
+      </c>
+      <c r="S171" s="156" t="s">
+        <v>225</v>
+      </c>
+      <c r="T171" s="152"/>
+      <c r="U171" s="157" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="172" spans="1:38" s="129" customFormat="1" ht="12.3">
+      <c r="A172" s="170" t="s">
+        <v>571</v>
+      </c>
+      <c r="B172" s="124" t="s">
+        <v>576</v>
+      </c>
+      <c r="C172" s="124" t="s">
+        <v>47</v>
+      </c>
+      <c r="D172" s="124" t="s">
+        <v>221</v>
+      </c>
+      <c r="E172" s="124" t="s">
+        <v>281</v>
+      </c>
+      <c r="F172" s="124" t="s">
+        <v>490</v>
+      </c>
+      <c r="G172" s="124" t="s">
+        <v>278</v>
+      </c>
+      <c r="H172" s="124" t="s">
+        <v>146</v>
+      </c>
+      <c r="I172" s="170" t="s">
+        <v>276</v>
+      </c>
+      <c r="J172" s="170" t="s">
+        <v>293</v>
+      </c>
+      <c r="K172" s="211">
+        <v>0.4</v>
+      </c>
+      <c r="L172" s="124"/>
+      <c r="M172" s="124" t="s">
+        <v>437</v>
+      </c>
+      <c r="N172" s="170" t="s">
+        <v>573</v>
+      </c>
+      <c r="O172" s="124" t="s">
+        <v>568</v>
+      </c>
+      <c r="P172" s="124" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q172" s="124" t="s">
+        <v>34</v>
+      </c>
+      <c r="R172" s="124" t="s">
+        <v>481</v>
+      </c>
+      <c r="S172" s="128" t="s">
+        <v>225</v>
+      </c>
+      <c r="T172" s="124"/>
+      <c r="U172" s="129" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="173" spans="1:38" s="123" customFormat="1" ht="12.3">
+      <c r="A173" s="172" t="s">
+        <v>575</v>
+      </c>
+      <c r="B173" s="117" t="s">
+        <v>577</v>
+      </c>
+      <c r="C173" s="117" t="s">
+        <v>47</v>
+      </c>
+      <c r="D173" s="117" t="s">
+        <v>221</v>
+      </c>
+      <c r="E173" s="117" t="s">
+        <v>281</v>
+      </c>
+      <c r="F173" s="117" t="s">
+        <v>490</v>
+      </c>
+      <c r="G173" s="117" t="s">
+        <v>278</v>
+      </c>
+      <c r="H173" s="117" t="s">
+        <v>146</v>
+      </c>
+      <c r="I173" s="172" t="s">
+        <v>276</v>
+      </c>
+      <c r="J173" s="172" t="s">
+        <v>293</v>
+      </c>
+      <c r="K173" s="213">
+        <v>0.4</v>
+      </c>
+      <c r="L173" s="117"/>
+      <c r="M173" s="117" t="s">
+        <v>30</v>
+      </c>
+      <c r="N173" s="172" t="s">
+        <v>578</v>
+      </c>
+      <c r="O173" s="117" t="s">
+        <v>568</v>
+      </c>
+      <c r="P173" s="117" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q173" s="117" t="s">
+        <v>34</v>
+      </c>
+      <c r="R173" s="117" t="s">
+        <v>481</v>
+      </c>
+      <c r="S173" s="121" t="s">
+        <v>225</v>
+      </c>
+      <c r="T173" s="117"/>
+      <c r="U173" s="123" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="174" spans="1:38" s="217" customFormat="1" ht="12.3">
+      <c r="A174" s="170" t="s">
+        <v>580</v>
+      </c>
+      <c r="B174" s="170" t="s">
+        <v>581</v>
+      </c>
+      <c r="C174" s="170" t="s">
+        <v>47</v>
+      </c>
+      <c r="D174" s="170" t="s">
+        <v>221</v>
+      </c>
+      <c r="E174" s="170" t="s">
+        <v>281</v>
+      </c>
+      <c r="F174" s="170" t="s">
+        <v>490</v>
+      </c>
+      <c r="G174" s="170" t="s">
+        <v>278</v>
+      </c>
+      <c r="H174" s="170" t="s">
+        <v>146</v>
+      </c>
+      <c r="I174" s="170" t="s">
+        <v>276</v>
+      </c>
+      <c r="J174" s="170" t="s">
+        <v>293</v>
+      </c>
+      <c r="K174" s="211">
+        <v>0.4</v>
+      </c>
+      <c r="L174" s="170"/>
+      <c r="M174" s="217" t="s">
+        <v>437</v>
+      </c>
+      <c r="N174" s="170" t="s">
+        <v>582</v>
+      </c>
+      <c r="O174" s="170" t="s">
+        <v>568</v>
+      </c>
+      <c r="P174" s="170" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q174" s="170" t="s">
+        <v>34</v>
+      </c>
+      <c r="R174" s="170" t="s">
+        <v>481</v>
+      </c>
+      <c r="S174" s="215" t="s">
+        <v>225</v>
+      </c>
+      <c r="T174" s="170"/>
+      <c r="U174" s="216" t="s">
+        <v>583</v>
+      </c>
+    </row>
+    <row r="175" spans="1:38" s="129" customFormat="1" ht="12.3">
+      <c r="A175" s="170" t="s">
+        <v>584</v>
+      </c>
+      <c r="B175" s="124" t="s">
+        <v>585</v>
+      </c>
+      <c r="C175" s="124" t="s">
+        <v>47</v>
+      </c>
+      <c r="D175" s="124" t="s">
+        <v>221</v>
+      </c>
+      <c r="E175" s="124" t="s">
+        <v>281</v>
+      </c>
+      <c r="F175" s="124" t="s">
+        <v>490</v>
+      </c>
+      <c r="G175" s="124" t="s">
+        <v>278</v>
+      </c>
+      <c r="H175" s="124" t="s">
+        <v>146</v>
+      </c>
+      <c r="I175" s="170" t="s">
+        <v>276</v>
+      </c>
+      <c r="J175" s="170" t="s">
+        <v>293</v>
+      </c>
+      <c r="K175" s="211">
+        <v>0.4</v>
+      </c>
+      <c r="L175" s="124"/>
+      <c r="M175" s="124" t="s">
+        <v>437</v>
+      </c>
+      <c r="N175" s="170" t="s">
+        <v>589</v>
+      </c>
+      <c r="O175" s="124" t="s">
+        <v>568</v>
+      </c>
+      <c r="P175" s="124" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q175" s="124" t="s">
+        <v>34</v>
+      </c>
+      <c r="R175" s="124" t="s">
+        <v>481</v>
+      </c>
+      <c r="S175" s="128" t="s">
+        <v>225</v>
+      </c>
+      <c r="T175" s="124"/>
+      <c r="U175" s="214" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="176" spans="1:38" s="163" customFormat="1" ht="12.3">
+      <c r="A176" s="173" t="s">
+        <v>587</v>
+      </c>
+      <c r="B176" s="158" t="s">
+        <v>588</v>
+      </c>
+      <c r="C176" s="158" t="s">
+        <v>47</v>
+      </c>
+      <c r="D176" s="158" t="s">
+        <v>221</v>
+      </c>
+      <c r="E176" s="158" t="s">
+        <v>281</v>
+      </c>
+      <c r="F176" s="158" t="s">
+        <v>490</v>
+      </c>
+      <c r="G176" s="158" t="s">
+        <v>278</v>
+      </c>
+      <c r="H176" s="158" t="s">
+        <v>146</v>
+      </c>
+      <c r="I176" s="173" t="s">
+        <v>276</v>
+      </c>
+      <c r="J176" s="173" t="s">
+        <v>293</v>
+      </c>
+      <c r="K176" s="209">
+        <v>0.37</v>
+      </c>
+      <c r="L176" s="158"/>
+      <c r="M176" s="158" t="s">
+        <v>30</v>
+      </c>
+      <c r="N176" s="173" t="s">
+        <v>590</v>
+      </c>
+      <c r="O176" s="158" t="s">
+        <v>568</v>
+      </c>
+      <c r="P176" s="158" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q176" s="158" t="s">
+        <v>34</v>
+      </c>
+      <c r="R176" s="158" t="s">
+        <v>481</v>
+      </c>
+      <c r="S176" s="162" t="s">
+        <v>225</v>
+      </c>
+      <c r="T176" s="158"/>
+      <c r="U176" s="218" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="177" spans="1:21" s="163" customFormat="1" ht="12.3">
+      <c r="A177" s="173" t="s">
+        <v>593</v>
+      </c>
+      <c r="B177" s="158" t="s">
+        <v>537</v>
+      </c>
+      <c r="C177" s="158" t="s">
+        <v>340</v>
+      </c>
+      <c r="D177" s="158" t="s">
+        <v>221</v>
+      </c>
+      <c r="E177" s="158" t="s">
+        <v>281</v>
+      </c>
+      <c r="F177" s="158" t="s">
+        <v>490</v>
+      </c>
+      <c r="G177" s="158" t="s">
+        <v>278</v>
+      </c>
+      <c r="H177" s="158" t="s">
+        <v>600</v>
+      </c>
+      <c r="I177" s="173" t="s">
+        <v>276</v>
+      </c>
+      <c r="J177" s="173" t="s">
+        <v>293</v>
+      </c>
+      <c r="K177" s="209">
+        <v>0.4</v>
+      </c>
+      <c r="L177" s="158"/>
+      <c r="M177" s="158" t="s">
+        <v>30</v>
+      </c>
+      <c r="N177" s="158" t="s">
+        <v>592</v>
+      </c>
+      <c r="O177" s="158" t="s">
+        <v>568</v>
+      </c>
+      <c r="P177" s="158" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q177" s="158" t="s">
+        <v>34</v>
+      </c>
+      <c r="R177" s="158" t="s">
+        <v>481</v>
+      </c>
+      <c r="S177" s="162" t="s">
+        <v>225</v>
+      </c>
+      <c r="T177" s="158" t="s">
+        <v>595</v>
+      </c>
+      <c r="U177" s="163" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="178" spans="1:21" s="163" customFormat="1" ht="12.3">
+      <c r="A178" s="173" t="s">
+        <v>596</v>
+      </c>
+      <c r="B178" s="158" t="s">
+        <v>576</v>
+      </c>
+      <c r="C178" s="158" t="s">
+        <v>47</v>
+      </c>
+      <c r="D178" s="158" t="s">
+        <v>221</v>
+      </c>
+      <c r="E178" s="158" t="s">
+        <v>281</v>
+      </c>
+      <c r="F178" s="158" t="s">
+        <v>490</v>
+      </c>
+      <c r="G178" s="158" t="s">
+        <v>278</v>
+      </c>
+      <c r="H178" s="158" t="s">
+        <v>600</v>
+      </c>
+      <c r="I178" s="173" t="s">
+        <v>276</v>
+      </c>
+      <c r="J178" s="173" t="s">
+        <v>293</v>
+      </c>
+      <c r="K178" s="209">
+        <v>0.4</v>
+      </c>
+      <c r="L178" s="158"/>
+      <c r="M178" s="158" t="s">
+        <v>30</v>
+      </c>
+      <c r="N178" s="158" t="s">
+        <v>597</v>
+      </c>
+      <c r="O178" s="158" t="s">
+        <v>568</v>
+      </c>
+      <c r="P178" s="158" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q178" s="158" t="s">
+        <v>34</v>
+      </c>
+      <c r="R178" s="158" t="s">
+        <v>481</v>
+      </c>
+      <c r="S178" s="162" t="s">
+        <v>225</v>
+      </c>
+      <c r="T178" s="158"/>
+    </row>
+    <row r="179" spans="1:21" s="163" customFormat="1" ht="12.3">
+      <c r="A179" s="173" t="s">
+        <v>598</v>
+      </c>
+      <c r="B179" s="158" t="s">
+        <v>599</v>
+      </c>
+      <c r="C179" s="158" t="s">
+        <v>47</v>
+      </c>
+      <c r="D179" s="158" t="s">
+        <v>221</v>
+      </c>
+      <c r="E179" s="158" t="s">
+        <v>281</v>
+      </c>
+      <c r="F179" s="158" t="s">
+        <v>490</v>
+      </c>
+      <c r="G179" s="158" t="s">
+        <v>278</v>
+      </c>
+      <c r="H179" s="158" t="s">
+        <v>600</v>
+      </c>
+      <c r="I179" s="173" t="s">
+        <v>276</v>
+      </c>
+      <c r="J179" s="173" t="s">
+        <v>293</v>
+      </c>
+      <c r="K179" s="209">
+        <v>0.4</v>
+      </c>
+      <c r="L179" s="158"/>
+      <c r="M179" s="158" t="s">
+        <v>30</v>
+      </c>
+      <c r="N179" s="158" t="s">
+        <v>601</v>
+      </c>
+      <c r="O179" s="158" t="s">
+        <v>568</v>
+      </c>
+      <c r="P179" s="158" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q179" s="158" t="s">
+        <v>34</v>
+      </c>
+      <c r="R179" s="158" t="s">
+        <v>481</v>
+      </c>
+      <c r="S179" s="162" t="s">
+        <v>225</v>
+      </c>
+      <c r="T179" s="158"/>
+    </row>
+    <row r="180" spans="1:21" s="163" customFormat="1" ht="12.3">
+      <c r="A180" s="173" t="s">
+        <v>602</v>
+      </c>
+      <c r="B180" s="158" t="s">
+        <v>562</v>
+      </c>
+      <c r="C180" s="158" t="s">
+        <v>203</v>
+      </c>
+      <c r="D180" s="158" t="s">
+        <v>221</v>
+      </c>
+      <c r="E180" s="158" t="s">
+        <v>281</v>
+      </c>
+      <c r="F180" s="158" t="s">
+        <v>490</v>
+      </c>
+      <c r="G180" s="158" t="s">
+        <v>278</v>
+      </c>
+      <c r="H180" s="158" t="s">
+        <v>600</v>
+      </c>
+      <c r="I180" s="173" t="s">
+        <v>276</v>
+      </c>
+      <c r="J180" s="173" t="s">
+        <v>293</v>
+      </c>
+      <c r="K180" s="209">
+        <v>0.4</v>
+      </c>
+      <c r="L180" s="158"/>
+      <c r="M180" s="158" t="s">
+        <v>30</v>
+      </c>
+      <c r="N180" s="158" t="s">
+        <v>603</v>
+      </c>
+      <c r="O180" s="158" t="s">
+        <v>568</v>
+      </c>
+      <c r="P180" s="158" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q180" s="158" t="s">
+        <v>34</v>
+      </c>
+      <c r="R180" s="158" t="s">
+        <v>481</v>
+      </c>
+      <c r="S180" s="162" t="s">
+        <v>225</v>
+      </c>
+      <c r="T180" s="158" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="181" spans="1:21" s="163" customFormat="1" ht="12.3">
+      <c r="A181" s="173" t="s">
+        <v>604</v>
+      </c>
+      <c r="B181" s="158" t="s">
+        <v>605</v>
+      </c>
+      <c r="C181" s="158" t="s">
+        <v>203</v>
+      </c>
+      <c r="D181" s="158" t="s">
+        <v>221</v>
+      </c>
+      <c r="E181" s="158" t="s">
+        <v>281</v>
+      </c>
+      <c r="F181" s="158" t="s">
+        <v>490</v>
+      </c>
+      <c r="G181" s="158" t="s">
+        <v>278</v>
+      </c>
+      <c r="H181" s="158" t="s">
+        <v>600</v>
+      </c>
+      <c r="I181" s="173" t="s">
+        <v>276</v>
+      </c>
+      <c r="J181" s="173" t="s">
+        <v>293</v>
+      </c>
+      <c r="K181" s="209">
+        <v>0.4</v>
+      </c>
+      <c r="L181" s="158"/>
+      <c r="M181" s="158" t="s">
+        <v>30</v>
+      </c>
+      <c r="N181" s="158" t="s">
+        <v>606</v>
+      </c>
+      <c r="O181" s="158" t="s">
+        <v>568</v>
+      </c>
+      <c r="P181" s="158" t="s">
+        <v>137</v>
+      </c>
+      <c r="Q181" s="158" t="s">
+        <v>34</v>
+      </c>
+      <c r="R181" s="158" t="s">
+        <v>481</v>
+      </c>
+      <c r="S181" s="162" t="s">
+        <v>225</v>
+      </c>
+      <c r="T181" s="158" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="182" spans="1:21" ht="12.3">
       <c r="A182" s="24"/>
       <c r="B182" s="3"/>
       <c r="C182" s="3"/>
@@ -13671,7 +14263,7 @@
       <c r="R182" s="3"/>
       <c r="T182" s="3"/>
     </row>
-    <row r="183" spans="1:20" ht="12.3">
+    <row r="183" spans="1:21" ht="12.3">
       <c r="A183" s="24"/>
       <c r="B183" s="3"/>
       <c r="C183" s="3"/>
@@ -13692,7 +14284,7 @@
       <c r="R183" s="3"/>
       <c r="T183" s="3"/>
     </row>
-    <row r="184" spans="1:20" ht="12.3">
+    <row r="184" spans="1:21" ht="12.3">
       <c r="A184" s="24"/>
       <c r="B184" s="3"/>
       <c r="C184" s="3"/>
@@ -13713,7 +14305,7 @@
       <c r="R184" s="3"/>
       <c r="T184" s="3"/>
     </row>
-    <row r="185" spans="1:20" ht="12.3">
+    <row r="185" spans="1:21" ht="12.3">
       <c r="A185" s="24"/>
       <c r="B185" s="3"/>
       <c r="C185" s="3"/>
@@ -13734,7 +14326,7 @@
       <c r="R185" s="3"/>
       <c r="T185" s="3"/>
     </row>
-    <row r="186" spans="1:20" ht="12.3">
+    <row r="186" spans="1:21" ht="12.3">
       <c r="A186" s="24"/>
       <c r="B186" s="3"/>
       <c r="C186" s="3"/>
@@ -13755,7 +14347,7 @@
       <c r="R186" s="3"/>
       <c r="T186" s="3"/>
     </row>
-    <row r="187" spans="1:20" ht="12.3">
+    <row r="187" spans="1:21" ht="12.3">
       <c r="A187" s="24"/>
       <c r="B187" s="3"/>
       <c r="C187" s="3"/>
@@ -13776,7 +14368,7 @@
       <c r="R187" s="3"/>
       <c r="T187" s="3"/>
     </row>
-    <row r="188" spans="1:20" ht="12.3">
+    <row r="188" spans="1:21" ht="12.3">
       <c r="A188" s="24"/>
       <c r="B188" s="3"/>
       <c r="C188" s="3"/>
@@ -13797,7 +14389,7 @@
       <c r="R188" s="3"/>
       <c r="T188" s="3"/>
     </row>
-    <row r="189" spans="1:20" ht="12.3">
+    <row r="189" spans="1:21" ht="12.3">
       <c r="A189" s="24"/>
       <c r="B189" s="3"/>
       <c r="C189" s="3"/>
@@ -13818,7 +14410,7 @@
       <c r="R189" s="3"/>
       <c r="T189" s="3"/>
     </row>
-    <row r="190" spans="1:20" ht="12.3">
+    <row r="190" spans="1:21" ht="12.3">
       <c r="A190" s="24"/>
       <c r="B190" s="3"/>
       <c r="C190" s="3"/>
@@ -13839,7 +14431,7 @@
       <c r="R190" s="3"/>
       <c r="T190" s="3"/>
     </row>
-    <row r="191" spans="1:20" ht="12.3">
+    <row r="191" spans="1:21" ht="12.3">
       <c r="A191" s="24"/>
       <c r="B191" s="3"/>
       <c r="C191" s="3"/>
@@ -13860,7 +14452,7 @@
       <c r="R191" s="3"/>
       <c r="T191" s="3"/>
     </row>
-    <row r="192" spans="1:20" ht="12.3">
+    <row r="192" spans="1:21" ht="12.3">
       <c r="A192" s="24"/>
       <c r="B192" s="3"/>
       <c r="C192" s="3"/>

</xml_diff>

<commit_message>
updated datasheet for clarity one last time
</commit_message>
<xml_diff>
--- a/data_25_01_14.xlsx
+++ b/data_25_01_14.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toppe\OneDrive - CSU Maritime Academy\Documents\GitHub\Strain-Sensor-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csuma-my.sharepoint.com/personal/toppenheim_csum_edu/Documents/Documents/GitHub/Strain-Sensor-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA110EF-9F40-42E9-99F9-1FAEB6C9AEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{CDA110EF-9F40-42E9-99F9-1FAEB6C9AEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{836B6EF5-D359-45F5-831F-F399A457CA70}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all data" sheetId="1" r:id="rId1"/>
@@ -3154,18 +3154,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3215,6 +3203,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3441,9 +3441,9 @@
   </sheetPr>
   <dimension ref="A1:AM1008"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD4"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -3538,13 +3538,13 @@
       </c>
       <c r="W1" s="3"/>
     </row>
-    <row r="2" spans="1:39" s="250" customFormat="1" ht="12.3">
-      <c r="A2" s="249" t="s">
+    <row r="2" spans="1:39" s="272" customFormat="1" ht="12.3">
+      <c r="A2" s="271" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="3" spans="1:39" s="250" customFormat="1" ht="12.3"/>
-    <row r="4" spans="1:39" s="250" customFormat="1" ht="12.3"/>
+    <row r="3" spans="1:39" s="272" customFormat="1" ht="12.3"/>
+    <row r="4" spans="1:39" s="272" customFormat="1" ht="12.3"/>
     <row r="5" spans="1:39" ht="15.75" customHeight="1">
       <c r="A5" s="165" t="s">
         <v>18</v>
@@ -6206,7 +6206,7 @@
       <c r="AM44" s="17"/>
     </row>
     <row r="45" spans="1:39" s="141" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A45" s="253" t="s">
+      <c r="A45" s="249" t="s">
         <v>19</v>
       </c>
       <c r="B45" s="136" t="s">
@@ -6233,7 +6233,7 @@
       <c r="I45" s="140" t="s">
         <v>26</v>
       </c>
-      <c r="J45" s="254" t="s">
+      <c r="J45" s="250" t="s">
         <v>27</v>
       </c>
       <c r="K45" s="156" t="s">
@@ -6245,10 +6245,10 @@
       <c r="M45" s="140">
         <v>1</v>
       </c>
-      <c r="N45" s="255" t="s">
+      <c r="N45" s="251" t="s">
         <v>65</v>
       </c>
-      <c r="O45" s="256" t="s">
+      <c r="O45" s="252" t="s">
         <v>113</v>
       </c>
       <c r="P45" s="136" t="s">
@@ -6269,29 +6269,29 @@
       <c r="U45" s="140" t="s">
         <v>36</v>
       </c>
-      <c r="V45" s="257" t="s">
+      <c r="V45" s="253" t="s">
         <v>114</v>
       </c>
-      <c r="W45" s="257"/>
-      <c r="X45" s="257"/>
-      <c r="Y45" s="257"/>
-      <c r="Z45" s="257"/>
-      <c r="AA45" s="257"/>
-      <c r="AB45" s="257"/>
-      <c r="AC45" s="257"/>
-      <c r="AD45" s="257"/>
-      <c r="AE45" s="257"/>
-      <c r="AF45" s="257"/>
-      <c r="AG45" s="257"/>
-      <c r="AH45" s="257"/>
-      <c r="AI45" s="257"/>
-      <c r="AJ45" s="257"/>
-      <c r="AK45" s="257"/>
-      <c r="AL45" s="257"/>
-      <c r="AM45" s="258"/>
+      <c r="W45" s="253"/>
+      <c r="X45" s="253"/>
+      <c r="Y45" s="253"/>
+      <c r="Z45" s="253"/>
+      <c r="AA45" s="253"/>
+      <c r="AB45" s="253"/>
+      <c r="AC45" s="253"/>
+      <c r="AD45" s="253"/>
+      <c r="AE45" s="253"/>
+      <c r="AF45" s="253"/>
+      <c r="AG45" s="253"/>
+      <c r="AH45" s="253"/>
+      <c r="AI45" s="253"/>
+      <c r="AJ45" s="253"/>
+      <c r="AK45" s="253"/>
+      <c r="AL45" s="253"/>
+      <c r="AM45" s="254"/>
     </row>
     <row r="46" spans="1:39" s="141" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A46" s="259" t="s">
+      <c r="A46" s="255" t="s">
         <v>19</v>
       </c>
       <c r="B46" s="136" t="s">
@@ -6318,7 +6318,7 @@
       <c r="I46" s="136" t="s">
         <v>26</v>
       </c>
-      <c r="J46" s="254" t="s">
+      <c r="J46" s="250" t="s">
         <v>27</v>
       </c>
       <c r="K46" s="156" t="s">
@@ -6330,10 +6330,10 @@
       <c r="M46" s="136">
         <v>2</v>
       </c>
-      <c r="N46" s="260" t="s">
+      <c r="N46" s="256" t="s">
         <v>65</v>
       </c>
-      <c r="O46" s="261" t="s">
+      <c r="O46" s="257" t="s">
         <v>113</v>
       </c>
       <c r="P46" s="136" t="s">
@@ -6354,16 +6354,16 @@
       <c r="U46" s="140" t="s">
         <v>36</v>
       </c>
-      <c r="V46" s="262" t="s">
+      <c r="V46" s="258" t="s">
         <v>115</v>
       </c>
-      <c r="AM46" s="263"/>
+      <c r="AM46" s="259"/>
     </row>
     <row r="47" spans="1:39" s="141" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A47" s="264" t="s">
+      <c r="A47" s="260" t="s">
         <v>19</v>
       </c>
-      <c r="B47" s="265" t="s">
+      <c r="B47" s="261" t="s">
         <v>116</v>
       </c>
       <c r="C47" s="136" t="s">
@@ -6372,22 +6372,22 @@
       <c r="D47" s="136" t="s">
         <v>582</v>
       </c>
-      <c r="E47" s="265" t="s">
+      <c r="E47" s="261" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="265" t="s">
+      <c r="F47" s="261" t="s">
         <v>23</v>
       </c>
-      <c r="G47" s="265" t="s">
+      <c r="G47" s="261" t="s">
         <v>24</v>
       </c>
       <c r="H47" s="140" t="s">
         <v>25</v>
       </c>
-      <c r="I47" s="265" t="s">
+      <c r="I47" s="261" t="s">
         <v>26</v>
       </c>
-      <c r="J47" s="254" t="s">
+      <c r="J47" s="250" t="s">
         <v>27</v>
       </c>
       <c r="K47" s="156" t="s">
@@ -6396,7 +6396,7 @@
       <c r="L47" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="M47" s="265">
+      <c r="M47" s="261">
         <v>1</v>
       </c>
       <c r="N47" s="195" t="s">
@@ -6405,16 +6405,16 @@
       <c r="O47" s="37" t="s">
         <v>117</v>
       </c>
-      <c r="P47" s="265" t="s">
+      <c r="P47" s="261" t="s">
         <v>111</v>
       </c>
-      <c r="Q47" s="265" t="s">
+      <c r="Q47" s="261" t="s">
         <v>32</v>
       </c>
-      <c r="R47" s="265" t="s">
+      <c r="R47" s="261" t="s">
         <v>33</v>
       </c>
-      <c r="S47" s="265" t="s">
+      <c r="S47" s="261" t="s">
         <v>93</v>
       </c>
       <c r="T47" s="140" t="s">
@@ -6423,26 +6423,26 @@
       <c r="U47" s="140" t="s">
         <v>36</v>
       </c>
-      <c r="V47" s="266" t="s">
+      <c r="V47" s="262" t="s">
         <v>118</v>
       </c>
-      <c r="W47" s="266"/>
-      <c r="X47" s="266"/>
-      <c r="Y47" s="266"/>
-      <c r="Z47" s="266"/>
-      <c r="AA47" s="266"/>
-      <c r="AB47" s="266"/>
-      <c r="AC47" s="266"/>
-      <c r="AD47" s="266"/>
-      <c r="AE47" s="266"/>
-      <c r="AF47" s="266"/>
-      <c r="AG47" s="266"/>
-      <c r="AH47" s="266"/>
-      <c r="AI47" s="266"/>
-      <c r="AJ47" s="266"/>
-      <c r="AK47" s="266"/>
-      <c r="AL47" s="266"/>
-      <c r="AM47" s="267"/>
+      <c r="W47" s="262"/>
+      <c r="X47" s="262"/>
+      <c r="Y47" s="262"/>
+      <c r="Z47" s="262"/>
+      <c r="AA47" s="262"/>
+      <c r="AB47" s="262"/>
+      <c r="AC47" s="262"/>
+      <c r="AD47" s="262"/>
+      <c r="AE47" s="262"/>
+      <c r="AF47" s="262"/>
+      <c r="AG47" s="262"/>
+      <c r="AH47" s="262"/>
+      <c r="AI47" s="262"/>
+      <c r="AJ47" s="262"/>
+      <c r="AK47" s="262"/>
+      <c r="AL47" s="262"/>
+      <c r="AM47" s="263"/>
     </row>
     <row r="48" spans="1:39" ht="15">
       <c r="A48" s="168" t="s">
@@ -6488,10 +6488,10 @@
       <c r="AM48" s="29"/>
     </row>
     <row r="49" spans="1:39" s="141" customFormat="1" ht="15">
-      <c r="A49" s="268" t="s">
+      <c r="A49" s="264" t="s">
         <v>19</v>
       </c>
-      <c r="B49" s="265" t="s">
+      <c r="B49" s="261" t="s">
         <v>116</v>
       </c>
       <c r="C49" s="136" t="s">
@@ -6500,22 +6500,22 @@
       <c r="D49" s="136" t="s">
         <v>582</v>
       </c>
-      <c r="E49" s="265" t="s">
+      <c r="E49" s="261" t="s">
         <v>22</v>
       </c>
-      <c r="F49" s="269" t="s">
+      <c r="F49" s="265" t="s">
         <v>23</v>
       </c>
-      <c r="G49" s="269" t="s">
+      <c r="G49" s="265" t="s">
         <v>24</v>
       </c>
       <c r="H49" s="140" t="s">
         <v>25</v>
       </c>
-      <c r="I49" s="269" t="s">
+      <c r="I49" s="265" t="s">
         <v>26</v>
       </c>
-      <c r="J49" s="254" t="s">
+      <c r="J49" s="250" t="s">
         <v>27</v>
       </c>
       <c r="K49" s="156" t="s">
@@ -6524,7 +6524,7 @@
       <c r="L49" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="M49" s="269">
+      <c r="M49" s="265">
         <v>1</v>
       </c>
       <c r="N49" s="197" t="s">
@@ -6533,16 +6533,16 @@
       <c r="O49" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="P49" s="269" t="s">
+      <c r="P49" s="265" t="s">
         <v>119</v>
       </c>
-      <c r="Q49" s="269" t="s">
+      <c r="Q49" s="265" t="s">
         <v>32</v>
       </c>
-      <c r="R49" s="269" t="s">
+      <c r="R49" s="265" t="s">
         <v>33</v>
       </c>
-      <c r="S49" s="269" t="s">
+      <c r="S49" s="265" t="s">
         <v>93</v>
       </c>
       <c r="T49" s="140" t="s">
@@ -6551,34 +6551,34 @@
       <c r="U49" s="140" t="s">
         <v>36</v>
       </c>
-      <c r="V49" s="270" t="s">
+      <c r="V49" s="266" t="s">
         <v>121</v>
       </c>
-      <c r="W49" s="270"/>
-      <c r="X49" s="270"/>
-      <c r="Y49" s="270"/>
-      <c r="Z49" s="270"/>
-      <c r="AA49" s="270"/>
-      <c r="AB49" s="270"/>
-      <c r="AC49" s="270"/>
-      <c r="AD49" s="270"/>
-      <c r="AE49" s="270"/>
-      <c r="AF49" s="270"/>
-      <c r="AG49" s="270"/>
-      <c r="AH49" s="270"/>
-      <c r="AI49" s="270"/>
-      <c r="AJ49" s="270"/>
-      <c r="AK49" s="270"/>
-      <c r="AL49" s="270"/>
-      <c r="AM49" s="271"/>
-    </row>
-    <row r="50" spans="1:39" s="250" customFormat="1" ht="12.3">
-      <c r="A50" s="249" t="s">
+      <c r="W49" s="266"/>
+      <c r="X49" s="266"/>
+      <c r="Y49" s="266"/>
+      <c r="Z49" s="266"/>
+      <c r="AA49" s="266"/>
+      <c r="AB49" s="266"/>
+      <c r="AC49" s="266"/>
+      <c r="AD49" s="266"/>
+      <c r="AE49" s="266"/>
+      <c r="AF49" s="266"/>
+      <c r="AG49" s="266"/>
+      <c r="AH49" s="266"/>
+      <c r="AI49" s="266"/>
+      <c r="AJ49" s="266"/>
+      <c r="AK49" s="266"/>
+      <c r="AL49" s="266"/>
+      <c r="AM49" s="267"/>
+    </row>
+    <row r="50" spans="1:39" s="272" customFormat="1" ht="12.3">
+      <c r="A50" s="271" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="51" spans="1:39" s="250" customFormat="1" ht="12.3"/>
-    <row r="52" spans="1:39" s="250" customFormat="1" ht="12.3"/>
+    <row r="51" spans="1:39" s="272" customFormat="1" ht="12.3"/>
+    <row r="52" spans="1:39" s="272" customFormat="1" ht="12.3"/>
     <row r="53" spans="1:39" ht="15.75" customHeight="1">
       <c r="A53" s="168" t="s">
         <v>122</v>
@@ -6623,7 +6623,7 @@
       <c r="AM53" s="41"/>
     </row>
     <row r="54" spans="1:39" s="141" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A54" s="268" t="s">
+      <c r="A54" s="264" t="s">
         <v>19</v>
       </c>
       <c r="B54" s="136" t="s">
@@ -6638,19 +6638,19 @@
       <c r="E54" s="136" t="s">
         <v>22</v>
       </c>
-      <c r="F54" s="269" t="s">
+      <c r="F54" s="265" t="s">
         <v>23</v>
       </c>
-      <c r="G54" s="269" t="s">
+      <c r="G54" s="265" t="s">
         <v>24</v>
       </c>
       <c r="H54" s="140" t="s">
         <v>25</v>
       </c>
-      <c r="I54" s="269" t="s">
+      <c r="I54" s="265" t="s">
         <v>26</v>
       </c>
-      <c r="J54" s="254" t="s">
+      <c r="J54" s="250" t="s">
         <v>27</v>
       </c>
       <c r="K54" s="156" t="s">
@@ -6659,25 +6659,25 @@
       <c r="L54" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="M54" s="269">
+      <c r="M54" s="265">
         <v>1</v>
       </c>
-      <c r="N54" s="272" t="s">
+      <c r="N54" s="268" t="s">
         <v>29</v>
       </c>
-      <c r="O54" s="269" t="s">
+      <c r="O54" s="265" t="s">
         <v>124</v>
       </c>
-      <c r="P54" s="269" t="s">
+      <c r="P54" s="265" t="s">
         <v>122</v>
       </c>
-      <c r="Q54" s="269" t="s">
+      <c r="Q54" s="265" t="s">
         <v>32</v>
       </c>
-      <c r="R54" s="269" t="s">
+      <c r="R54" s="265" t="s">
         <v>33</v>
       </c>
-      <c r="S54" s="269" t="s">
+      <c r="S54" s="265" t="s">
         <v>657</v>
       </c>
       <c r="T54" s="140" t="s">
@@ -6686,26 +6686,26 @@
       <c r="U54" s="140" t="s">
         <v>36</v>
       </c>
-      <c r="V54" s="270" t="s">
+      <c r="V54" s="266" t="s">
         <v>126</v>
       </c>
-      <c r="W54" s="270"/>
-      <c r="X54" s="270"/>
-      <c r="Y54" s="270"/>
-      <c r="Z54" s="270"/>
-      <c r="AA54" s="270"/>
-      <c r="AB54" s="270"/>
-      <c r="AC54" s="270"/>
-      <c r="AD54" s="270"/>
-      <c r="AE54" s="270"/>
-      <c r="AF54" s="270"/>
-      <c r="AG54" s="270"/>
-      <c r="AH54" s="270"/>
-      <c r="AI54" s="270"/>
-      <c r="AJ54" s="270"/>
-      <c r="AK54" s="270"/>
-      <c r="AL54" s="270"/>
-      <c r="AM54" s="271"/>
+      <c r="W54" s="266"/>
+      <c r="X54" s="266"/>
+      <c r="Y54" s="266"/>
+      <c r="Z54" s="266"/>
+      <c r="AA54" s="266"/>
+      <c r="AB54" s="266"/>
+      <c r="AC54" s="266"/>
+      <c r="AD54" s="266"/>
+      <c r="AE54" s="266"/>
+      <c r="AF54" s="266"/>
+      <c r="AG54" s="266"/>
+      <c r="AH54" s="266"/>
+      <c r="AI54" s="266"/>
+      <c r="AJ54" s="266"/>
+      <c r="AK54" s="266"/>
+      <c r="AL54" s="266"/>
+      <c r="AM54" s="267"/>
     </row>
     <row r="55" spans="1:39" ht="15.75" customHeight="1">
       <c r="A55" s="165" t="s">
@@ -6805,7 +6805,7 @@
       <c r="R56" s="136" t="s">
         <v>33</v>
       </c>
-      <c r="S56" s="269" t="s">
+      <c r="S56" s="265" t="s">
         <v>657</v>
       </c>
       <c r="T56" s="140" t="s">
@@ -6814,7 +6814,7 @@
       <c r="U56" s="140" t="s">
         <v>138</v>
       </c>
-      <c r="V56" s="262" t="s">
+      <c r="V56" s="258" t="s">
         <v>139</v>
       </c>
     </row>
@@ -6873,7 +6873,7 @@
       <c r="R57" s="136" t="s">
         <v>33</v>
       </c>
-      <c r="S57" s="269" t="s">
+      <c r="S57" s="265" t="s">
         <v>657</v>
       </c>
       <c r="T57" s="140" t="s">
@@ -6927,7 +6927,7 @@
       <c r="AM58" s="7"/>
     </row>
     <row r="59" spans="1:39" s="141" customFormat="1" ht="16.8" customHeight="1">
-      <c r="A59" s="253" t="s">
+      <c r="A59" s="249" t="s">
         <v>143</v>
       </c>
       <c r="B59" s="140" t="s">
@@ -6981,7 +6981,7 @@
       <c r="R59" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="S59" s="269" t="s">
+      <c r="S59" s="265" t="s">
         <v>657</v>
       </c>
       <c r="T59" s="140" t="s">
@@ -6990,53 +6990,53 @@
       <c r="U59" s="140" t="s">
         <v>150</v>
       </c>
-      <c r="V59" s="257" t="s">
+      <c r="V59" s="253" t="s">
         <v>151</v>
       </c>
-      <c r="W59" s="257"/>
-      <c r="X59" s="257"/>
-      <c r="Y59" s="257"/>
-      <c r="Z59" s="257"/>
-      <c r="AA59" s="257"/>
-      <c r="AB59" s="257"/>
-      <c r="AC59" s="257"/>
-      <c r="AD59" s="257"/>
-      <c r="AE59" s="257"/>
-      <c r="AF59" s="257"/>
-      <c r="AG59" s="257"/>
-      <c r="AH59" s="257"/>
-      <c r="AI59" s="257"/>
-      <c r="AJ59" s="257"/>
-      <c r="AK59" s="257"/>
-      <c r="AL59" s="257"/>
-      <c r="AM59" s="258"/>
+      <c r="W59" s="253"/>
+      <c r="X59" s="253"/>
+      <c r="Y59" s="253"/>
+      <c r="Z59" s="253"/>
+      <c r="AA59" s="253"/>
+      <c r="AB59" s="253"/>
+      <c r="AC59" s="253"/>
+      <c r="AD59" s="253"/>
+      <c r="AE59" s="253"/>
+      <c r="AF59" s="253"/>
+      <c r="AG59" s="253"/>
+      <c r="AH59" s="253"/>
+      <c r="AI59" s="253"/>
+      <c r="AJ59" s="253"/>
+      <c r="AK59" s="253"/>
+      <c r="AL59" s="253"/>
+      <c r="AM59" s="254"/>
     </row>
     <row r="60" spans="1:39" s="141" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A60" s="264" t="s">
+      <c r="A60" s="260" t="s">
         <v>143</v>
       </c>
-      <c r="B60" s="265" t="s">
+      <c r="B60" s="261" t="s">
         <v>144</v>
       </c>
-      <c r="C60" s="265" t="s">
+      <c r="C60" s="261" t="s">
         <v>38</v>
       </c>
       <c r="D60" s="136" t="s">
         <v>582</v>
       </c>
-      <c r="E60" s="265" t="s">
+      <c r="E60" s="261" t="s">
         <v>22</v>
       </c>
-      <c r="F60" s="265" t="s">
+      <c r="F60" s="261" t="s">
         <v>130</v>
       </c>
-      <c r="G60" s="265" t="s">
+      <c r="G60" s="261" t="s">
         <v>24</v>
       </c>
       <c r="H60" s="136" t="s">
         <v>132</v>
       </c>
-      <c r="I60" s="265" t="s">
+      <c r="I60" s="261" t="s">
         <v>145</v>
       </c>
       <c r="J60" s="156" t="s">
@@ -7048,7 +7048,7 @@
       <c r="L60" s="136" t="s">
         <v>28</v>
       </c>
-      <c r="M60" s="265">
+      <c r="M60" s="261">
         <v>1</v>
       </c>
       <c r="N60" s="195" t="s">
@@ -7057,16 +7057,16 @@
       <c r="O60" s="37" t="s">
         <v>152</v>
       </c>
-      <c r="P60" s="265" t="s">
+      <c r="P60" s="261" t="s">
         <v>142</v>
       </c>
-      <c r="Q60" s="265" t="s">
+      <c r="Q60" s="261" t="s">
         <v>136</v>
       </c>
-      <c r="R60" s="265" t="s">
+      <c r="R60" s="261" t="s">
         <v>33</v>
       </c>
-      <c r="S60" s="269" t="s">
+      <c r="S60" s="265" t="s">
         <v>657</v>
       </c>
       <c r="T60" s="140" t="s">
@@ -7075,24 +7075,24 @@
       <c r="U60" s="140" t="s">
         <v>150</v>
       </c>
-      <c r="V60" s="266"/>
-      <c r="W60" s="266"/>
-      <c r="X60" s="266"/>
-      <c r="Y60" s="266"/>
-      <c r="Z60" s="266"/>
-      <c r="AA60" s="266"/>
-      <c r="AB60" s="266"/>
-      <c r="AC60" s="266"/>
-      <c r="AD60" s="266"/>
-      <c r="AE60" s="266"/>
-      <c r="AF60" s="266"/>
-      <c r="AG60" s="266"/>
-      <c r="AH60" s="266"/>
-      <c r="AI60" s="266"/>
-      <c r="AJ60" s="266"/>
-      <c r="AK60" s="266"/>
-      <c r="AL60" s="266"/>
-      <c r="AM60" s="267"/>
+      <c r="V60" s="262"/>
+      <c r="W60" s="262"/>
+      <c r="X60" s="262"/>
+      <c r="Y60" s="262"/>
+      <c r="Z60" s="262"/>
+      <c r="AA60" s="262"/>
+      <c r="AB60" s="262"/>
+      <c r="AC60" s="262"/>
+      <c r="AD60" s="262"/>
+      <c r="AE60" s="262"/>
+      <c r="AF60" s="262"/>
+      <c r="AG60" s="262"/>
+      <c r="AH60" s="262"/>
+      <c r="AI60" s="262"/>
+      <c r="AJ60" s="262"/>
+      <c r="AK60" s="262"/>
+      <c r="AL60" s="262"/>
+      <c r="AM60" s="263"/>
     </row>
     <row r="61" spans="1:39" s="113" customFormat="1" ht="15.75" customHeight="1">
       <c r="A61" s="240" t="s">
@@ -7308,31 +7308,31 @@
       <c r="AM63" s="51"/>
     </row>
     <row r="64" spans="1:39" s="141" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A64" s="264" t="s">
+      <c r="A64" s="260" t="s">
         <v>153</v>
       </c>
-      <c r="B64" s="265" t="s">
+      <c r="B64" s="261" t="s">
         <v>165</v>
       </c>
-      <c r="C64" s="265" t="s">
+      <c r="C64" s="261" t="s">
         <v>46</v>
       </c>
       <c r="D64" s="136" t="s">
         <v>582</v>
       </c>
-      <c r="E64" s="265" t="s">
+      <c r="E64" s="261" t="s">
         <v>22</v>
       </c>
-      <c r="F64" s="265" t="s">
+      <c r="F64" s="261" t="s">
         <v>130</v>
       </c>
-      <c r="G64" s="265" t="s">
+      <c r="G64" s="261" t="s">
         <v>131</v>
       </c>
       <c r="H64" s="136" t="s">
         <v>132</v>
       </c>
-      <c r="I64" s="265" t="s">
+      <c r="I64" s="261" t="s">
         <v>154</v>
       </c>
       <c r="J64" s="149" t="s">
@@ -7356,13 +7356,13 @@
       <c r="P64" s="52" t="s">
         <v>159</v>
       </c>
-      <c r="Q64" s="265" t="s">
+      <c r="Q64" s="261" t="s">
         <v>136</v>
       </c>
-      <c r="R64" s="265" t="s">
+      <c r="R64" s="261" t="s">
         <v>33</v>
       </c>
-      <c r="S64" s="273" t="s">
+      <c r="S64" s="269" t="s">
         <v>657</v>
       </c>
       <c r="T64" s="140" t="s">
@@ -7371,26 +7371,26 @@
       <c r="U64" s="140" t="s">
         <v>150</v>
       </c>
-      <c r="V64" s="266" t="s">
+      <c r="V64" s="262" t="s">
         <v>167</v>
       </c>
-      <c r="W64" s="266"/>
-      <c r="X64" s="266"/>
-      <c r="Y64" s="266"/>
-      <c r="Z64" s="266"/>
-      <c r="AA64" s="266"/>
-      <c r="AB64" s="266"/>
-      <c r="AC64" s="266"/>
-      <c r="AD64" s="266"/>
-      <c r="AE64" s="266"/>
-      <c r="AF64" s="266"/>
-      <c r="AG64" s="266"/>
-      <c r="AH64" s="266"/>
-      <c r="AI64" s="266"/>
-      <c r="AJ64" s="266"/>
-      <c r="AK64" s="266"/>
-      <c r="AL64" s="266"/>
-      <c r="AM64" s="267"/>
+      <c r="W64" s="262"/>
+      <c r="X64" s="262"/>
+      <c r="Y64" s="262"/>
+      <c r="Z64" s="262"/>
+      <c r="AA64" s="262"/>
+      <c r="AB64" s="262"/>
+      <c r="AC64" s="262"/>
+      <c r="AD64" s="262"/>
+      <c r="AE64" s="262"/>
+      <c r="AF64" s="262"/>
+      <c r="AG64" s="262"/>
+      <c r="AH64" s="262"/>
+      <c r="AI64" s="262"/>
+      <c r="AJ64" s="262"/>
+      <c r="AK64" s="262"/>
+      <c r="AL64" s="262"/>
+      <c r="AM64" s="263"/>
     </row>
     <row r="65" spans="1:39" s="113" customFormat="1" ht="15.75" customHeight="1">
       <c r="A65" s="225" t="s">
@@ -8068,13 +8068,13 @@
       <c r="AM73" s="7"/>
     </row>
     <row r="74" spans="1:39" s="141" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A74" s="268" t="s">
+      <c r="A74" s="264" t="s">
         <v>200</v>
       </c>
-      <c r="B74" s="269" t="s">
+      <c r="B74" s="265" t="s">
         <v>201</v>
       </c>
-      <c r="C74" s="265" t="s">
+      <c r="C74" s="261" t="s">
         <v>202</v>
       </c>
       <c r="D74" s="136" t="s">
@@ -8083,28 +8083,28 @@
       <c r="E74" s="136" t="s">
         <v>22</v>
       </c>
-      <c r="F74" s="269" t="s">
+      <c r="F74" s="265" t="s">
         <v>130</v>
       </c>
-      <c r="G74" s="269" t="s">
+      <c r="G74" s="265" t="s">
         <v>131</v>
       </c>
-      <c r="H74" s="269" t="s">
+      <c r="H74" s="265" t="s">
         <v>171</v>
       </c>
-      <c r="I74" s="269" t="s">
+      <c r="I74" s="265" t="s">
         <v>203</v>
       </c>
-      <c r="J74" s="272" t="s">
+      <c r="J74" s="268" t="s">
         <v>155</v>
       </c>
-      <c r="K74" s="272" t="s">
+      <c r="K74" s="268" t="s">
         <v>161</v>
       </c>
-      <c r="L74" s="269" t="s">
+      <c r="L74" s="265" t="s">
         <v>204</v>
       </c>
-      <c r="M74" s="269">
+      <c r="M74" s="265">
         <v>1</v>
       </c>
       <c r="N74" s="200" t="s">
@@ -8113,16 +8113,16 @@
       <c r="O74" s="70" t="s">
         <v>205</v>
       </c>
-      <c r="P74" s="269" t="s">
+      <c r="P74" s="265" t="s">
         <v>199</v>
       </c>
-      <c r="Q74" s="269" t="s">
+      <c r="Q74" s="265" t="s">
         <v>136</v>
       </c>
-      <c r="R74" s="269" t="s">
+      <c r="R74" s="265" t="s">
         <v>33</v>
       </c>
-      <c r="S74" s="273" t="s">
+      <c r="S74" s="269" t="s">
         <v>657</v>
       </c>
       <c r="T74" s="140" t="s">
@@ -8131,35 +8131,35 @@
       <c r="U74" s="140" t="s">
         <v>150</v>
       </c>
-      <c r="V74" s="270" t="s">
+      <c r="V74" s="266" t="s">
         <v>206</v>
       </c>
-      <c r="W74" s="270"/>
-      <c r="X74" s="270"/>
-      <c r="Y74" s="270"/>
-      <c r="Z74" s="270"/>
-      <c r="AA74" s="270"/>
-      <c r="AB74" s="270"/>
-      <c r="AC74" s="270"/>
-      <c r="AD74" s="270"/>
-      <c r="AE74" s="270"/>
-      <c r="AF74" s="270"/>
-      <c r="AG74" s="270"/>
-      <c r="AH74" s="270"/>
-      <c r="AI74" s="270"/>
-      <c r="AJ74" s="270"/>
-      <c r="AK74" s="270"/>
-      <c r="AL74" s="270"/>
-      <c r="AM74" s="271"/>
+      <c r="W74" s="266"/>
+      <c r="X74" s="266"/>
+      <c r="Y74" s="266"/>
+      <c r="Z74" s="266"/>
+      <c r="AA74" s="266"/>
+      <c r="AB74" s="266"/>
+      <c r="AC74" s="266"/>
+      <c r="AD74" s="266"/>
+      <c r="AE74" s="266"/>
+      <c r="AF74" s="266"/>
+      <c r="AG74" s="266"/>
+      <c r="AH74" s="266"/>
+      <c r="AI74" s="266"/>
+      <c r="AJ74" s="266"/>
+      <c r="AK74" s="266"/>
+      <c r="AL74" s="266"/>
+      <c r="AM74" s="267"/>
     </row>
     <row r="75" spans="1:39" s="141" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A75" s="268" t="s">
+      <c r="A75" s="264" t="s">
         <v>207</v>
       </c>
-      <c r="B75" s="269" t="s">
+      <c r="B75" s="265" t="s">
         <v>208</v>
       </c>
-      <c r="C75" s="265" t="s">
+      <c r="C75" s="261" t="s">
         <v>202</v>
       </c>
       <c r="D75" s="136" t="s">
@@ -8168,28 +8168,28 @@
       <c r="E75" s="136" t="s">
         <v>22</v>
       </c>
-      <c r="F75" s="269" t="s">
+      <c r="F75" s="265" t="s">
         <v>130</v>
       </c>
-      <c r="G75" s="269" t="s">
+      <c r="G75" s="265" t="s">
         <v>131</v>
       </c>
-      <c r="H75" s="269" t="s">
+      <c r="H75" s="265" t="s">
         <v>171</v>
       </c>
-      <c r="I75" s="269" t="s">
+      <c r="I75" s="265" t="s">
         <v>209</v>
       </c>
-      <c r="J75" s="272" t="s">
+      <c r="J75" s="268" t="s">
         <v>155</v>
       </c>
-      <c r="K75" s="272" t="s">
+      <c r="K75" s="268" t="s">
         <v>161</v>
       </c>
-      <c r="L75" s="269" t="s">
+      <c r="L75" s="265" t="s">
         <v>204</v>
       </c>
-      <c r="M75" s="269">
+      <c r="M75" s="265">
         <v>1</v>
       </c>
       <c r="N75" s="200" t="s">
@@ -8198,16 +8198,16 @@
       <c r="O75" s="70" t="s">
         <v>210</v>
       </c>
-      <c r="P75" s="269" t="s">
+      <c r="P75" s="265" t="s">
         <v>199</v>
       </c>
-      <c r="Q75" s="269" t="s">
+      <c r="Q75" s="265" t="s">
         <v>136</v>
       </c>
-      <c r="R75" s="269" t="s">
+      <c r="R75" s="265" t="s">
         <v>33</v>
       </c>
-      <c r="S75" s="273" t="s">
+      <c r="S75" s="269" t="s">
         <v>657</v>
       </c>
       <c r="T75" s="140" t="s">
@@ -8216,33 +8216,33 @@
       <c r="U75" s="140" t="s">
         <v>150</v>
       </c>
-      <c r="V75" s="270"/>
-      <c r="W75" s="270"/>
-      <c r="X75" s="270"/>
-      <c r="Y75" s="270"/>
-      <c r="Z75" s="270"/>
-      <c r="AA75" s="270"/>
-      <c r="AB75" s="270"/>
-      <c r="AC75" s="270"/>
-      <c r="AD75" s="270"/>
-      <c r="AE75" s="270"/>
-      <c r="AF75" s="270"/>
-      <c r="AG75" s="270"/>
-      <c r="AH75" s="270"/>
-      <c r="AI75" s="270"/>
-      <c r="AJ75" s="270"/>
-      <c r="AK75" s="270"/>
-      <c r="AL75" s="270"/>
-      <c r="AM75" s="271"/>
+      <c r="V75" s="266"/>
+      <c r="W75" s="266"/>
+      <c r="X75" s="266"/>
+      <c r="Y75" s="266"/>
+      <c r="Z75" s="266"/>
+      <c r="AA75" s="266"/>
+      <c r="AB75" s="266"/>
+      <c r="AC75" s="266"/>
+      <c r="AD75" s="266"/>
+      <c r="AE75" s="266"/>
+      <c r="AF75" s="266"/>
+      <c r="AG75" s="266"/>
+      <c r="AH75" s="266"/>
+      <c r="AI75" s="266"/>
+      <c r="AJ75" s="266"/>
+      <c r="AK75" s="266"/>
+      <c r="AL75" s="266"/>
+      <c r="AM75" s="267"/>
     </row>
     <row r="76" spans="1:39" s="141" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A76" s="253" t="s">
+      <c r="A76" s="249" t="s">
         <v>211</v>
       </c>
       <c r="B76" s="136" t="s">
         <v>212</v>
       </c>
-      <c r="C76" s="265" t="s">
+      <c r="C76" s="261" t="s">
         <v>202</v>
       </c>
       <c r="D76" s="136" t="s">
@@ -8257,19 +8257,19 @@
       <c r="G76" s="140" t="s">
         <v>131</v>
       </c>
-      <c r="H76" s="269" t="s">
+      <c r="H76" s="265" t="s">
         <v>171</v>
       </c>
       <c r="I76" s="140" t="s">
         <v>154</v>
       </c>
-      <c r="J76" s="254" t="s">
+      <c r="J76" s="250" t="s">
         <v>155</v>
       </c>
-      <c r="K76" s="272" t="s">
+      <c r="K76" s="268" t="s">
         <v>161</v>
       </c>
-      <c r="L76" s="269" t="s">
+      <c r="L76" s="265" t="s">
         <v>204</v>
       </c>
       <c r="M76" s="140">
@@ -8290,7 +8290,7 @@
       <c r="R76" s="140" t="s">
         <v>33</v>
       </c>
-      <c r="S76" s="273" t="s">
+      <c r="S76" s="269" t="s">
         <v>657</v>
       </c>
       <c r="T76" s="140" t="s">
@@ -8299,33 +8299,33 @@
       <c r="U76" s="140" t="s">
         <v>150</v>
       </c>
-      <c r="V76" s="257"/>
-      <c r="W76" s="257"/>
-      <c r="X76" s="257"/>
-      <c r="Y76" s="257"/>
-      <c r="Z76" s="257"/>
-      <c r="AA76" s="257"/>
-      <c r="AB76" s="257"/>
-      <c r="AC76" s="257"/>
-      <c r="AD76" s="257"/>
-      <c r="AE76" s="257"/>
-      <c r="AF76" s="257"/>
-      <c r="AG76" s="257"/>
-      <c r="AH76" s="257"/>
-      <c r="AI76" s="257"/>
-      <c r="AJ76" s="257"/>
-      <c r="AK76" s="257"/>
-      <c r="AL76" s="257"/>
-      <c r="AM76" s="258"/>
+      <c r="V76" s="253"/>
+      <c r="W76" s="253"/>
+      <c r="X76" s="253"/>
+      <c r="Y76" s="253"/>
+      <c r="Z76" s="253"/>
+      <c r="AA76" s="253"/>
+      <c r="AB76" s="253"/>
+      <c r="AC76" s="253"/>
+      <c r="AD76" s="253"/>
+      <c r="AE76" s="253"/>
+      <c r="AF76" s="253"/>
+      <c r="AG76" s="253"/>
+      <c r="AH76" s="253"/>
+      <c r="AI76" s="253"/>
+      <c r="AJ76" s="253"/>
+      <c r="AK76" s="253"/>
+      <c r="AL76" s="253"/>
+      <c r="AM76" s="254"/>
     </row>
     <row r="77" spans="1:39" s="141" customFormat="1" ht="15.75" customHeight="1">
-      <c r="A77" s="264" t="s">
+      <c r="A77" s="260" t="s">
         <v>215</v>
       </c>
-      <c r="B77" s="265" t="s">
+      <c r="B77" s="261" t="s">
         <v>201</v>
       </c>
-      <c r="C77" s="265" t="s">
+      <c r="C77" s="261" t="s">
         <v>202</v>
       </c>
       <c r="D77" s="136" t="s">
@@ -8334,28 +8334,28 @@
       <c r="E77" s="136" t="s">
         <v>22</v>
       </c>
-      <c r="F77" s="265" t="s">
+      <c r="F77" s="261" t="s">
         <v>130</v>
       </c>
-      <c r="G77" s="265" t="s">
+      <c r="G77" s="261" t="s">
         <v>131</v>
       </c>
-      <c r="H77" s="269" t="s">
+      <c r="H77" s="265" t="s">
         <v>171</v>
       </c>
-      <c r="I77" s="265" t="s">
+      <c r="I77" s="261" t="s">
         <v>154</v>
       </c>
-      <c r="J77" s="274" t="s">
+      <c r="J77" s="270" t="s">
         <v>155</v>
       </c>
-      <c r="K77" s="272" t="s">
+      <c r="K77" s="268" t="s">
         <v>161</v>
       </c>
-      <c r="L77" s="269" t="s">
+      <c r="L77" s="265" t="s">
         <v>204</v>
       </c>
-      <c r="M77" s="265">
+      <c r="M77" s="261">
         <v>2</v>
       </c>
       <c r="N77" s="195" t="s">
@@ -8364,16 +8364,16 @@
       <c r="O77" s="37" t="s">
         <v>216</v>
       </c>
-      <c r="P77" s="265" t="s">
+      <c r="P77" s="261" t="s">
         <v>199</v>
       </c>
-      <c r="Q77" s="265" t="s">
+      <c r="Q77" s="261" t="s">
         <v>136</v>
       </c>
-      <c r="R77" s="265" t="s">
+      <c r="R77" s="261" t="s">
         <v>33</v>
       </c>
-      <c r="S77" s="273" t="s">
+      <c r="S77" s="269" t="s">
         <v>657</v>
       </c>
       <c r="T77" s="140" t="s">
@@ -8382,24 +8382,24 @@
       <c r="U77" s="140" t="s">
         <v>150</v>
       </c>
-      <c r="V77" s="266"/>
-      <c r="W77" s="266"/>
-      <c r="X77" s="266"/>
-      <c r="Y77" s="266"/>
-      <c r="Z77" s="266"/>
-      <c r="AA77" s="266"/>
-      <c r="AB77" s="266"/>
-      <c r="AC77" s="266"/>
-      <c r="AD77" s="266"/>
-      <c r="AE77" s="266"/>
-      <c r="AF77" s="266"/>
-      <c r="AG77" s="266"/>
-      <c r="AH77" s="266"/>
-      <c r="AI77" s="266"/>
-      <c r="AJ77" s="266"/>
-      <c r="AK77" s="266"/>
-      <c r="AL77" s="266"/>
-      <c r="AM77" s="267"/>
+      <c r="V77" s="262"/>
+      <c r="W77" s="262"/>
+      <c r="X77" s="262"/>
+      <c r="Y77" s="262"/>
+      <c r="Z77" s="262"/>
+      <c r="AA77" s="262"/>
+      <c r="AB77" s="262"/>
+      <c r="AC77" s="262"/>
+      <c r="AD77" s="262"/>
+      <c r="AE77" s="262"/>
+      <c r="AF77" s="262"/>
+      <c r="AG77" s="262"/>
+      <c r="AH77" s="262"/>
+      <c r="AI77" s="262"/>
+      <c r="AJ77" s="262"/>
+      <c r="AK77" s="262"/>
+      <c r="AL77" s="262"/>
+      <c r="AM77" s="263"/>
     </row>
     <row r="78" spans="1:39" ht="17.7" customHeight="1">
       <c r="A78" s="165" t="s">
@@ -8551,19 +8551,19 @@
       <c r="G80" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="H80" s="269" t="s">
+      <c r="H80" s="265" t="s">
         <v>171</v>
       </c>
       <c r="I80" s="72" t="s">
         <v>227</v>
       </c>
-      <c r="J80" s="272" t="s">
+      <c r="J80" s="268" t="s">
         <v>222</v>
       </c>
-      <c r="K80" s="272" t="s">
+      <c r="K80" s="268" t="s">
         <v>161</v>
       </c>
-      <c r="L80" s="269" t="s">
+      <c r="L80" s="265" t="s">
         <v>204</v>
       </c>
       <c r="M80" s="72">
@@ -11117,13 +11117,13 @@
         <v>378</v>
       </c>
     </row>
-    <row r="120" spans="1:39" s="250" customFormat="1" ht="12.3">
-      <c r="A120" s="249" t="s">
+    <row r="120" spans="1:39" s="272" customFormat="1" ht="12.3">
+      <c r="A120" s="271" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="121" spans="1:39" s="250" customFormat="1" ht="12.3"/>
-    <row r="122" spans="1:39" s="250" customFormat="1" ht="12.3"/>
+    <row r="121" spans="1:39" s="272" customFormat="1" ht="12.3"/>
+    <row r="122" spans="1:39" s="272" customFormat="1" ht="12.3"/>
     <row r="123" spans="1:39" ht="15.75" customHeight="1">
       <c r="A123" s="165" t="s">
         <v>379</v>
@@ -11484,10 +11484,10 @@
       </c>
     </row>
     <row r="129" spans="1:39" s="224" customFormat="1" ht="12.3">
-      <c r="A129" s="252" t="s">
+      <c r="A129" s="274" t="s">
         <v>660</v>
       </c>
-      <c r="B129" s="252"/>
+      <c r="B129" s="274"/>
       <c r="C129" s="219"/>
       <c r="D129" s="219"/>
       <c r="E129" s="220"/>
@@ -11509,8 +11509,8 @@
       <c r="U129" s="219"/>
     </row>
     <row r="130" spans="1:39" s="224" customFormat="1" ht="12.3">
-      <c r="A130" s="252"/>
-      <c r="B130" s="252"/>
+      <c r="A130" s="274"/>
+      <c r="B130" s="274"/>
       <c r="C130" s="219"/>
       <c r="D130" s="219"/>
       <c r="E130" s="220"/>
@@ -11532,8 +11532,8 @@
       <c r="U130" s="219"/>
     </row>
     <row r="131" spans="1:39" s="224" customFormat="1" ht="12.3">
-      <c r="A131" s="252"/>
-      <c r="B131" s="252"/>
+      <c r="A131" s="274"/>
+      <c r="B131" s="274"/>
       <c r="C131" s="219"/>
       <c r="D131" s="219"/>
       <c r="E131" s="220"/>
@@ -12090,13 +12090,13 @@
       </c>
       <c r="U141" s="3"/>
     </row>
-    <row r="142" spans="1:39" s="251" customFormat="1" ht="12.3">
-      <c r="A142" s="251" t="s">
+    <row r="142" spans="1:39" s="273" customFormat="1" ht="12.3">
+      <c r="A142" s="273" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="143" spans="1:39" s="251" customFormat="1" ht="12.3"/>
-    <row r="144" spans="1:39" s="251" customFormat="1" ht="12.3"/>
+    <row r="143" spans="1:39" s="273" customFormat="1" ht="12.3"/>
+    <row r="144" spans="1:39" s="273" customFormat="1" ht="12.3"/>
     <row r="145" spans="1:39" ht="15.75" customHeight="1">
       <c r="A145" s="165" t="s">
         <v>418</v>
@@ -14080,13 +14080,13 @@
         <v>519</v>
       </c>
     </row>
-    <row r="178" spans="1:39" s="250" customFormat="1" ht="12.3">
-      <c r="A178" s="249" t="s">
+    <row r="178" spans="1:39" s="272" customFormat="1" ht="12.3">
+      <c r="A178" s="271" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="179" spans="1:39" s="250" customFormat="1" ht="12.3"/>
-    <row r="180" spans="1:39" s="250" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="179" spans="1:39" s="272" customFormat="1" ht="12.3"/>
+    <row r="180" spans="1:39" s="272" customFormat="1" ht="15.75" customHeight="1"/>
     <row r="181" spans="1:39" s="147" customFormat="1" ht="12.3">
       <c r="A181" s="155"/>
       <c r="B181" s="142"/>
@@ -35608,8 +35608,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E35F51-89D7-4D4E-9423-E5EB02F06689}">
   <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
@@ -35773,30 +35773,29 @@
       <c r="M4" s="188">
         <v>0.39</v>
       </c>
-      <c r="N4" s="108"/>
+      <c r="N4" s="152" t="s">
+        <v>29</v>
+      </c>
       <c r="O4" s="152" t="s">
-        <v>29</v>
-      </c>
-      <c r="P4" s="152" t="s">
         <v>629</v>
       </c>
+      <c r="P4" s="108" t="s">
+        <v>502</v>
+      </c>
       <c r="Q4" s="108" t="s">
-        <v>502</v>
+        <v>136</v>
       </c>
       <c r="R4" s="108" t="s">
-        <v>136</v>
+        <v>33</v>
       </c>
       <c r="S4" s="108" t="s">
-        <v>33</v>
-      </c>
-      <c r="T4" s="108" t="s">
         <v>639</v>
       </c>
-      <c r="U4" s="112" t="s">
+      <c r="T4" s="112" t="s">
         <v>224</v>
       </c>
-      <c r="V4" s="108"/>
-      <c r="W4" s="113" t="s">
+      <c r="U4" s="108"/>
+      <c r="V4" s="113" t="s">
         <v>530</v>
       </c>
     </row>
@@ -36332,8 +36331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3136F1D-A2E4-4CE7-8F50-95420C9B4A05}">
   <dimension ref="A2:X14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>

</xml_diff>

<commit_message>
new data acquired and new arduino daq
</commit_message>
<xml_diff>
--- a/data_25_01_14.xlsx
+++ b/data_25_01_14.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csuma-my.sharepoint.com/personal/toppenheim_csum_edu/Documents/Documents/GitHub/Strain-Sensor-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{CDA110EF-9F40-42E9-99F9-1FAEB6C9AEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{836B6EF5-D359-45F5-831F-F399A457CA70}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="13_ncr:1_{CDA110EF-9F40-42E9-99F9-1FAEB6C9AEC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A18D5B49-B807-4989-85A1-0B35C9C55B18}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all data" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4797" uniqueCount="688">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4832" uniqueCount="697">
   <si>
     <t>Sample Name</t>
   </si>
@@ -2130,6 +2130,33 @@
   </si>
   <si>
     <t xml:space="preserve">Circuit 0:  Below data tested on single first successully made sample.  A variety of circuits were tested.  Do NOT use these for analysis.  </t>
+  </si>
+  <si>
+    <t>5_5_25</t>
+  </si>
+  <si>
+    <t>Circuit 4: Volt. Div.  220 ohm and 0.5 gauge; LMC648 331x out strian gauge in+ , 2.048 ref to in-;  adc 2x 16 bit res.</t>
+  </si>
+  <si>
+    <t>1.86_static_v1_331x_test_5_5_25</t>
+  </si>
+  <si>
+    <t>Circuit 4: Volt. Div.  220 ohm and 0.5 gauge; LMC648 331x out strian gauge in+ , 2.048 ref to in-;  adc 4x 16 bit res ADS115</t>
+  </si>
+  <si>
+    <t>1.86_static_vADS1115_test_5_5_25</t>
+  </si>
+  <si>
+    <t>CSV Data/5_5_25/1.86_static_v1_331x_test_5_5_25.csv</t>
+  </si>
+  <si>
+    <t>LMC6481 331x gain + ADS115 4x gain+velcro  static re-test</t>
+  </si>
+  <si>
+    <t>LMC6481 331x gain + MCP3421 2x gain+velcro  static re-test</t>
+  </si>
+  <si>
+    <t>CSV Data/5_5_25/1.86_static_vADS1115_test_5_5_25.csv</t>
   </si>
 </sst>
 </file>
@@ -2528,7 +2555,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="275">
+  <cellXfs count="276">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3216,6 +3243,9 @@
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3236,6 +3266,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3441,9 +3475,9 @@
   </sheetPr>
   <dimension ref="A1:AM1008"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S1" sqref="S1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A178" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O209" sqref="O209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -15651,71 +15685,164 @@
         <v>594</v>
       </c>
     </row>
-    <row r="207" spans="1:39" ht="12.3">
-      <c r="A207" s="24"/>
-      <c r="B207" s="3"/>
-      <c r="C207" s="3"/>
-      <c r="D207" s="3"/>
-      <c r="E207" s="3"/>
-      <c r="F207" s="3"/>
-      <c r="G207" s="3"/>
-      <c r="H207" s="3"/>
-      <c r="I207" s="3"/>
-      <c r="J207" s="24"/>
-      <c r="K207" s="24"/>
-      <c r="L207" s="3"/>
-      <c r="M207" s="3"/>
-      <c r="N207" s="24"/>
-      <c r="O207" s="3"/>
-      <c r="P207" s="3"/>
-      <c r="Q207" s="3"/>
-      <c r="R207" s="3"/>
-      <c r="S207" s="3"/>
-      <c r="U207" s="3"/>
-    </row>
-    <row r="208" spans="1:39" ht="12.3">
-      <c r="A208" s="24"/>
-      <c r="B208" s="3"/>
-      <c r="C208" s="3"/>
-      <c r="D208" s="3"/>
-      <c r="E208" s="3"/>
-      <c r="F208" s="3"/>
-      <c r="G208" s="3"/>
-      <c r="H208" s="3"/>
-      <c r="I208" s="3"/>
-      <c r="J208" s="24"/>
-      <c r="K208" s="24"/>
-      <c r="L208" s="3"/>
-      <c r="M208" s="3"/>
-      <c r="N208" s="24"/>
-      <c r="O208" s="3"/>
-      <c r="P208" s="3"/>
-      <c r="Q208" s="3"/>
-      <c r="R208" s="3"/>
-      <c r="S208" s="3"/>
-      <c r="U208" s="3"/>
-    </row>
-    <row r="209" spans="1:21" ht="12.3">
-      <c r="A209" s="24"/>
-      <c r="B209" s="3"/>
-      <c r="C209" s="3"/>
-      <c r="D209" s="3"/>
-      <c r="E209" s="3"/>
-      <c r="F209" s="3"/>
-      <c r="G209" s="3"/>
-      <c r="H209" s="3"/>
-      <c r="I209" s="3"/>
-      <c r="J209" s="24"/>
-      <c r="K209" s="24"/>
-      <c r="L209" s="3"/>
-      <c r="M209" s="3"/>
-      <c r="N209" s="24"/>
-      <c r="O209" s="3"/>
-      <c r="P209" s="3"/>
-      <c r="Q209" s="3"/>
-      <c r="R209" s="3"/>
-      <c r="S209" s="3"/>
-      <c r="U209" s="3"/>
+    <row r="207" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A207" s="165" t="s">
+        <v>688</v>
+      </c>
+      <c r="B207" s="6"/>
+      <c r="C207" s="6"/>
+      <c r="D207" s="6"/>
+      <c r="E207" s="6"/>
+      <c r="F207" s="6"/>
+      <c r="G207" s="6"/>
+      <c r="H207" s="6"/>
+      <c r="I207" s="6"/>
+      <c r="J207" s="5"/>
+      <c r="K207" s="5"/>
+      <c r="L207" s="6"/>
+      <c r="M207" s="6"/>
+      <c r="N207" s="5"/>
+      <c r="O207" s="184"/>
+      <c r="P207" s="6"/>
+      <c r="Q207" s="6"/>
+      <c r="R207" s="6"/>
+      <c r="S207" s="6"/>
+      <c r="T207" s="7"/>
+      <c r="U207" s="6"/>
+      <c r="V207" s="7"/>
+      <c r="W207" s="7"/>
+      <c r="X207" s="7"/>
+      <c r="Y207" s="7"/>
+      <c r="Z207" s="7"/>
+      <c r="AA207" s="7"/>
+      <c r="AB207" s="7"/>
+      <c r="AC207" s="7"/>
+      <c r="AD207" s="7"/>
+      <c r="AE207" s="7"/>
+      <c r="AF207" s="7"/>
+      <c r="AG207" s="7"/>
+      <c r="AH207" s="7"/>
+      <c r="AI207" s="7"/>
+      <c r="AJ207" s="7"/>
+      <c r="AK207" s="7"/>
+      <c r="AL207" s="7"/>
+      <c r="AM207" s="7"/>
+    </row>
+    <row r="208" spans="1:39" s="107" customFormat="1" ht="12.3">
+      <c r="A208" s="275" t="s">
+        <v>690</v>
+      </c>
+      <c r="B208" s="101" t="s">
+        <v>695</v>
+      </c>
+      <c r="C208" s="101" t="s">
+        <v>339</v>
+      </c>
+      <c r="D208" s="101" t="s">
+        <v>581</v>
+      </c>
+      <c r="E208" s="101" t="s">
+        <v>220</v>
+      </c>
+      <c r="F208" s="101" t="s">
+        <v>130</v>
+      </c>
+      <c r="G208" s="101" t="s">
+        <v>472</v>
+      </c>
+      <c r="H208" s="101" t="s">
+        <v>277</v>
+      </c>
+      <c r="I208" s="101" t="s">
+        <v>231</v>
+      </c>
+      <c r="J208" s="154" t="s">
+        <v>275</v>
+      </c>
+      <c r="K208" s="154" t="s">
+        <v>590</v>
+      </c>
+      <c r="L208" s="190">
+        <v>0.4</v>
+      </c>
+      <c r="M208" s="101"/>
+      <c r="N208" s="154" t="s">
+        <v>29</v>
+      </c>
+      <c r="O208" s="101" t="s">
+        <v>693</v>
+      </c>
+      <c r="P208" s="101" t="s">
+        <v>688</v>
+      </c>
+      <c r="Q208" s="101" t="s">
+        <v>136</v>
+      </c>
+      <c r="R208" s="101" t="s">
+        <v>33</v>
+      </c>
+      <c r="S208" s="101" t="s">
+        <v>689</v>
+      </c>
+      <c r="U208" s="101"/>
+    </row>
+    <row r="209" spans="1:21" s="107" customFormat="1" ht="12.3">
+      <c r="A209" s="275" t="s">
+        <v>692</v>
+      </c>
+      <c r="B209" s="101" t="s">
+        <v>694</v>
+      </c>
+      <c r="C209" s="101" t="s">
+        <v>339</v>
+      </c>
+      <c r="D209" s="101" t="s">
+        <v>581</v>
+      </c>
+      <c r="E209" s="101" t="s">
+        <v>220</v>
+      </c>
+      <c r="F209" s="101" t="s">
+        <v>130</v>
+      </c>
+      <c r="G209" s="101" t="s">
+        <v>472</v>
+      </c>
+      <c r="H209" s="101" t="s">
+        <v>277</v>
+      </c>
+      <c r="I209" s="101" t="s">
+        <v>231</v>
+      </c>
+      <c r="J209" s="154" t="s">
+        <v>275</v>
+      </c>
+      <c r="K209" s="154" t="s">
+        <v>590</v>
+      </c>
+      <c r="L209" s="190">
+        <v>0.4</v>
+      </c>
+      <c r="M209" s="101"/>
+      <c r="N209" s="154" t="s">
+        <v>29</v>
+      </c>
+      <c r="O209" s="101" t="s">
+        <v>696</v>
+      </c>
+      <c r="P209" s="101" t="s">
+        <v>688</v>
+      </c>
+      <c r="Q209" s="101" t="s">
+        <v>136</v>
+      </c>
+      <c r="R209" s="101" t="s">
+        <v>33</v>
+      </c>
+      <c r="S209" s="101" t="s">
+        <v>691</v>
+      </c>
+      <c r="U209" s="101"/>
     </row>
     <row r="210" spans="1:21" ht="12.3">
       <c r="A210" s="24"/>
@@ -36331,7 +36458,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3136F1D-A2E4-4CE7-8F50-95420C9B4A05}">
   <dimension ref="A2:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
new data and data vs model analysis
</commit_message>
<xml_diff>
--- a/data_25_01_14.xlsx
+++ b/data_25_01_14.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csuma-my.sharepoint.com/personal/toppenheim_csum_edu/Documents/Documents/GitHub/Strain-Sensor-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="233" documentId="13_ncr:1_{9C3E2F24-F0BA-4ED0-966D-A349015366CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2029D67-06F5-405A-8BB1-3E262E1F824E}"/>
+  <xr:revisionPtr revIDLastSave="435" documentId="13_ncr:1_{9C3E2F24-F0BA-4ED0-966D-A349015366CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5ADDAF9-11CB-4835-B75D-5CDEC2DFECF2}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,6 +27,7 @@
     <sheet name="all_data_accuracy_TO_Old" sheetId="5" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5641" uniqueCount="817">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5829" uniqueCount="855">
   <si>
     <t>Sample Name</t>
   </si>
@@ -2519,12 +2520,126 @@
   <si>
     <t>2.1_static_v2_silpoxy_sam4_5_23_25</t>
   </si>
+  <si>
+    <t>CSV Data/5_23_25/2.1_static_v2_silpoxy_sam4_5_23_25.csv</t>
+  </si>
+  <si>
+    <t>6_2_25</t>
+  </si>
+  <si>
+    <t>CSV Data/6_2_25/2.1_static_v1_silpoxy_0.04_6_2_25.csv</t>
+  </si>
+  <si>
+    <t>...CAD Files/abs_lofted_insert/basic strain guage op03.ipt</t>
+  </si>
+  <si>
+    <t>Circuit 5: Volt. Div.  LT3092 75K:100  -&gt;0.4 ohm gauge; OPA333  831x out strian gauge in+ , 2.048 ref to in-;  MCP3421  adc 1x 16 bit res. (7.5 mA)</t>
+  </si>
+  <si>
+    <t>OPA333 831x gain + MCP3421 1x gain+LT3029 75K:100 ohm (7.5 mA)</t>
+  </si>
+  <si>
+    <t>CSV Data/6_2_25/2.1_static_v2_silpoxy_0.04_6_2_25.csv</t>
+  </si>
+  <si>
+    <t>data starts out very accurate and conssitent, and at 80 and 90 degree bend, very noisy</t>
+  </si>
+  <si>
+    <t>CSV Data/6_2_25/2.1_static_v4_silpoxy_0.04_6_2_25.csv</t>
+  </si>
+  <si>
+    <t>Data looks good minus a slight weird 90 deg data.   Generally good.  Turns out previous two not glued properly!</t>
+  </si>
+  <si>
+    <t>CSV Data/6_2_25/2.1_static_v5_silpoxy_0.04_6_2_25.csv</t>
+  </si>
+  <si>
+    <t>2.1_static_v1_silpoxy_0.03_6_2_25</t>
+  </si>
+  <si>
+    <t>2.1_static_v2_silpoxy_0.03_6_2_25</t>
+  </si>
+  <si>
+    <t>2.1_static_v4_silpoxy_0.03_6_2_25</t>
+  </si>
+  <si>
+    <t>2.1_static_v5_silpoxy_0.03_6_2_25</t>
+  </si>
+  <si>
+    <t>6_4_25</t>
+  </si>
+  <si>
+    <t>CSV Data/6_4_25/2.1_static_v1_silpoxy_0.04_6_4_25.csv</t>
+  </si>
+  <si>
+    <t>...CAD Files/abs_lofted_insert/basic strain guage op04.ipt</t>
+  </si>
+  <si>
+    <t>Slipping</t>
+  </si>
+  <si>
+    <t>0.125 in</t>
+  </si>
+  <si>
+    <t>CSV Data/6_4_25/2.1_static_v2_silpoxy_0.04_6_4_25.csv</t>
+  </si>
+  <si>
+    <t>2.1_static_v1_silpoxy_0.04_6_4_25</t>
+  </si>
+  <si>
+    <t>2.1_static_v2_silpoxy_0.04_6_4_25</t>
+  </si>
+  <si>
+    <t>2.1_static_v1_silpoxy_0.03_6_4_25</t>
+  </si>
+  <si>
+    <t>6_6_25</t>
+  </si>
+  <si>
+    <t>CSV Data/6_4_25/2.1_static_v2_silpoxy_0.03_6_4_25.csv</t>
+  </si>
+  <si>
+    <t>OPA333 (330 + 150)x gain + MCP3421 2x gain+LT3029 75K:100 ohm (7.5 mA)</t>
+  </si>
+  <si>
+    <t>0.23 in</t>
+  </si>
+  <si>
+    <t>CSV Data/6_6_25/2.1_static_v2_silpoxy_0.03_6_6_25.csv</t>
+  </si>
+  <si>
+    <t>Circuit 5: Volt. Div.  LT3092 75K:100  -&gt;0.4 ohm gauge; OPA333  (330 +150)x out strian gauge in+ , 2.048 ref to in-;  MCP3421  adc 2x 16 bit res. (7.5 mA)</t>
+  </si>
+  <si>
+    <t>Data looks perfect and fits model perfeectly except for some stray datapoints</t>
+  </si>
+  <si>
+    <t>0.02in x 0.02 in</t>
+  </si>
+  <si>
+    <t>0.03 in x 0.03 in</t>
+  </si>
+  <si>
+    <t>0.04 in x 0.04 in</t>
+  </si>
+  <si>
+    <t>CSV Data/6_6_25/2.1_static_v3_silpoxy_0.03_6_6_25.csv</t>
+  </si>
+  <si>
+    <t>Perfect</t>
+  </si>
+  <si>
+    <t>2.1_static_v2_silpoxy_0.03_6_6_25</t>
+  </si>
+  <si>
+    <t>2.1_static_v3_silpoxy_0.03_6_6_25</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -2629,6 +2744,12 @@
     </font>
     <font>
       <b/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -2916,7 +3037,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="279">
+  <cellXfs count="302">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -3604,6 +3725,42 @@
     <xf numFmtId="9" fontId="0" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="15" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="17" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -3616,6 +3773,35 @@
     <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="17" fillId="19" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3846,8 +4032,8 @@
   <dimension ref="A1:AM1008"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A228" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A255" sqref="A254:A255"/>
+      <pane ySplit="1" topLeftCell="A231" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A264" sqref="A264"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -3942,13 +4128,13 @@
       </c>
       <c r="W1" s="3"/>
     </row>
-    <row r="2" spans="1:39" s="276" customFormat="1" ht="12.3">
-      <c r="A2" s="275" t="s">
+    <row r="2" spans="1:39" s="288" customFormat="1" ht="12.3">
+      <c r="A2" s="287" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="3" spans="1:39" s="276" customFormat="1" ht="12.3"/>
-    <row r="4" spans="1:39" s="276" customFormat="1" ht="12.3"/>
+    <row r="3" spans="1:39" s="288" customFormat="1" ht="12.3"/>
+    <row r="4" spans="1:39" s="288" customFormat="1" ht="12.3"/>
     <row r="5" spans="1:39" ht="15.75" customHeight="1">
       <c r="A5" s="163" t="s">
         <v>18</v>
@@ -6976,13 +7162,13 @@
       <c r="AL49" s="262"/>
       <c r="AM49" s="263"/>
     </row>
-    <row r="50" spans="1:39" s="276" customFormat="1" ht="12.3">
-      <c r="A50" s="275" t="s">
+    <row r="50" spans="1:39" s="288" customFormat="1" ht="12.3">
+      <c r="A50" s="287" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="51" spans="1:39" s="276" customFormat="1" ht="12.3"/>
-    <row r="52" spans="1:39" s="276" customFormat="1" ht="12.3"/>
+    <row r="51" spans="1:39" s="288" customFormat="1" ht="12.3"/>
+    <row r="52" spans="1:39" s="288" customFormat="1" ht="12.3"/>
     <row r="53" spans="1:39" ht="15.75" customHeight="1">
       <c r="A53" s="166" t="s">
         <v>122</v>
@@ -11521,13 +11707,13 @@
         <v>378</v>
       </c>
     </row>
-    <row r="120" spans="1:39" s="276" customFormat="1" ht="12.3">
-      <c r="A120" s="275" t="s">
+    <row r="120" spans="1:39" s="288" customFormat="1" ht="12.3">
+      <c r="A120" s="287" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="121" spans="1:39" s="276" customFormat="1" ht="12.3"/>
-    <row r="122" spans="1:39" s="276" customFormat="1" ht="12.3"/>
+    <row r="121" spans="1:39" s="288" customFormat="1" ht="12.3"/>
+    <row r="122" spans="1:39" s="288" customFormat="1" ht="12.3"/>
     <row r="123" spans="1:39" ht="15.75" customHeight="1">
       <c r="A123" s="163" t="s">
         <v>379</v>
@@ -11888,10 +12074,10 @@
       </c>
     </row>
     <row r="129" spans="1:39" s="221" customFormat="1" ht="12.3">
-      <c r="A129" s="278" t="s">
+      <c r="A129" s="290" t="s">
         <v>660</v>
       </c>
-      <c r="B129" s="278"/>
+      <c r="B129" s="290"/>
       <c r="C129" s="217"/>
       <c r="D129" s="217"/>
       <c r="E129" s="218"/>
@@ -11913,8 +12099,8 @@
       <c r="U129" s="217"/>
     </row>
     <row r="130" spans="1:39" s="221" customFormat="1" ht="12.3">
-      <c r="A130" s="278"/>
-      <c r="B130" s="278"/>
+      <c r="A130" s="290"/>
+      <c r="B130" s="290"/>
       <c r="C130" s="217"/>
       <c r="D130" s="217"/>
       <c r="E130" s="218"/>
@@ -11936,8 +12122,8 @@
       <c r="U130" s="217"/>
     </row>
     <row r="131" spans="1:39" s="221" customFormat="1" ht="12.3">
-      <c r="A131" s="278"/>
-      <c r="B131" s="278"/>
+      <c r="A131" s="290"/>
+      <c r="B131" s="290"/>
       <c r="C131" s="217"/>
       <c r="D131" s="217"/>
       <c r="E131" s="218"/>
@@ -12494,13 +12680,13 @@
       </c>
       <c r="U141" s="3"/>
     </row>
-    <row r="142" spans="1:39" s="277" customFormat="1" ht="12.3">
-      <c r="A142" s="277" t="s">
+    <row r="142" spans="1:39" s="289" customFormat="1" ht="12.3">
+      <c r="A142" s="289" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="143" spans="1:39" s="277" customFormat="1" ht="12.3"/>
-    <row r="144" spans="1:39" s="277" customFormat="1" ht="12.3"/>
+    <row r="143" spans="1:39" s="289" customFormat="1" ht="12.3"/>
+    <row r="144" spans="1:39" s="289" customFormat="1" ht="12.3"/>
     <row r="145" spans="1:39" ht="15.75" customHeight="1">
       <c r="A145" s="163" t="s">
         <v>418</v>
@@ -14484,13 +14670,13 @@
         <v>519</v>
       </c>
     </row>
-    <row r="178" spans="1:39" s="276" customFormat="1" ht="12.3">
-      <c r="A178" s="275" t="s">
+    <row r="178" spans="1:39" s="288" customFormat="1" ht="12.3">
+      <c r="A178" s="287" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="179" spans="1:39" s="276" customFormat="1" ht="12.3"/>
-    <row r="180" spans="1:39" s="276" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="179" spans="1:39" s="288" customFormat="1" ht="12.3"/>
+    <row r="180" spans="1:39" s="288" customFormat="1" ht="15.75" customHeight="1"/>
     <row r="181" spans="1:39" s="145" customFormat="1" ht="12.3">
       <c r="A181" s="153"/>
       <c r="B181" s="140"/>
@@ -17871,13 +18057,13 @@
       </c>
       <c r="U237" s="107"/>
     </row>
-    <row r="238" spans="1:39" s="276" customFormat="1" ht="12.3">
-      <c r="A238" s="275" t="s">
+    <row r="238" spans="1:39" s="288" customFormat="1" ht="12.3">
+      <c r="A238" s="287" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="239" spans="1:39" s="276" customFormat="1" ht="12.3"/>
-    <row r="240" spans="1:39" s="276" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="239" spans="1:39" s="288" customFormat="1" ht="12.3"/>
+    <row r="240" spans="1:39" s="288" customFormat="1" ht="15.75" customHeight="1"/>
     <row r="241" spans="1:39" ht="15.75" customHeight="1">
       <c r="A241" s="163" t="s">
         <v>777</v>
@@ -18333,127 +18519,127 @@
       <c r="AL248" s="7"/>
       <c r="AM248" s="7"/>
     </row>
-    <row r="249" spans="1:39" s="145" customFormat="1" ht="12.3">
-      <c r="A249" s="153" t="s">
+    <row r="249" spans="1:39" s="106" customFormat="1" ht="12.3">
+      <c r="A249" s="152" t="s">
         <v>807</v>
       </c>
-      <c r="B249" s="140" t="s">
+      <c r="B249" s="100" t="s">
         <v>803</v>
       </c>
-      <c r="C249" s="140" t="s">
+      <c r="C249" s="100" t="s">
         <v>339</v>
       </c>
-      <c r="D249" s="140" t="s">
+      <c r="D249" s="100" t="s">
         <v>796</v>
       </c>
-      <c r="E249" s="140" t="s">
+      <c r="E249" s="100" t="s">
         <v>220</v>
       </c>
-      <c r="F249" s="140" t="s">
+      <c r="F249" s="100" t="s">
         <v>280</v>
       </c>
-      <c r="G249" s="140" t="s">
+      <c r="G249" s="100" t="s">
         <v>797</v>
       </c>
-      <c r="H249" s="140" t="s">
-        <v>798</v>
-      </c>
-      <c r="I249" s="140" t="s">
+      <c r="H249" s="100" t="s">
+        <v>848</v>
+      </c>
+      <c r="I249" s="100" t="s">
         <v>799</v>
       </c>
-      <c r="J249" s="153" t="s">
+      <c r="J249" s="152" t="s">
         <v>275</v>
       </c>
-      <c r="K249" s="153" t="s">
+      <c r="K249" s="152" t="s">
         <v>584</v>
       </c>
-      <c r="L249" s="184">
+      <c r="L249" s="188">
         <v>0.38</v>
       </c>
-      <c r="M249" s="140"/>
-      <c r="N249" s="153" t="s">
+      <c r="M249" s="100"/>
+      <c r="N249" s="152" t="s">
         <v>29</v>
       </c>
-      <c r="O249" s="140" t="s">
+      <c r="O249" s="100" t="s">
         <v>809</v>
       </c>
-      <c r="P249" s="140" t="s">
+      <c r="P249" s="100" t="s">
         <v>806</v>
       </c>
-      <c r="Q249" s="140" t="s">
+      <c r="Q249" s="100" t="s">
         <v>136</v>
       </c>
-      <c r="R249" s="140" t="s">
+      <c r="R249" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="S249" s="140" t="s">
+      <c r="S249" s="100" t="s">
         <v>805</v>
       </c>
-      <c r="T249" s="144" t="s">
+      <c r="T249" s="104" t="s">
         <v>224</v>
       </c>
-      <c r="U249" s="140"/>
-    </row>
-    <row r="250" spans="1:39" s="145" customFormat="1" ht="12.3">
-      <c r="A250" s="153" t="s">
+      <c r="U249" s="100"/>
+    </row>
+    <row r="250" spans="1:39" s="106" customFormat="1" ht="12.3">
+      <c r="A250" s="152" t="s">
         <v>808</v>
       </c>
-      <c r="B250" s="140" t="s">
+      <c r="B250" s="100" t="s">
         <v>803</v>
       </c>
-      <c r="C250" s="140" t="s">
+      <c r="C250" s="100" t="s">
         <v>339</v>
       </c>
-      <c r="D250" s="140" t="s">
+      <c r="D250" s="100" t="s">
         <v>796</v>
       </c>
-      <c r="E250" s="140" t="s">
+      <c r="E250" s="100" t="s">
         <v>220</v>
       </c>
-      <c r="F250" s="140" t="s">
+      <c r="F250" s="100" t="s">
         <v>130</v>
       </c>
-      <c r="G250" s="140" t="s">
+      <c r="G250" s="100" t="s">
         <v>797</v>
       </c>
-      <c r="H250" s="140" t="s">
-        <v>798</v>
-      </c>
-      <c r="I250" s="140" t="s">
+      <c r="H250" s="100" t="s">
+        <v>848</v>
+      </c>
+      <c r="I250" s="100" t="s">
         <v>799</v>
       </c>
-      <c r="J250" s="153" t="s">
+      <c r="J250" s="152" t="s">
         <v>275</v>
       </c>
-      <c r="K250" s="153" t="s">
+      <c r="K250" s="152" t="s">
         <v>584</v>
       </c>
-      <c r="L250" s="184">
+      <c r="L250" s="188">
         <v>0.38</v>
       </c>
-      <c r="M250" s="140"/>
-      <c r="N250" s="153" t="s">
+      <c r="M250" s="100"/>
+      <c r="N250" s="152" t="s">
         <v>29</v>
       </c>
-      <c r="O250" s="140" t="s">
+      <c r="O250" s="100" t="s">
         <v>810</v>
       </c>
-      <c r="P250" s="140" t="s">
+      <c r="P250" s="100" t="s">
         <v>806</v>
       </c>
-      <c r="Q250" s="140" t="s">
+      <c r="Q250" s="100" t="s">
         <v>136</v>
       </c>
-      <c r="R250" s="140" t="s">
+      <c r="R250" s="100" t="s">
         <v>33</v>
       </c>
-      <c r="S250" s="140" t="s">
+      <c r="S250" s="100" t="s">
         <v>805</v>
       </c>
-      <c r="T250" s="144" t="s">
+      <c r="T250" s="104" t="s">
         <v>224</v>
       </c>
-      <c r="U250" s="140"/>
+      <c r="U250" s="100"/>
     </row>
     <row r="251" spans="1:39" s="139" customFormat="1" ht="12.3">
       <c r="A251" s="154" t="s">
@@ -18477,8 +18663,8 @@
       <c r="G251" s="135" t="s">
         <v>797</v>
       </c>
-      <c r="H251" s="135" t="s">
-        <v>798</v>
+      <c r="H251" s="185" t="s">
+        <v>848</v>
       </c>
       <c r="I251" s="135" t="s">
         <v>799</v>
@@ -18522,290 +18708,759 @@
       <c r="A252" s="154" t="s">
         <v>816</v>
       </c>
-      <c r="C252" s="3"/>
-      <c r="D252" s="3"/>
-      <c r="E252" s="3"/>
-      <c r="F252" s="3"/>
-      <c r="G252" s="3"/>
-      <c r="H252" s="3"/>
-      <c r="I252" s="3"/>
-      <c r="J252" s="24"/>
-      <c r="K252" s="24"/>
-      <c r="L252" s="24"/>
+      <c r="B252" s="135" t="s">
+        <v>812</v>
+      </c>
+      <c r="C252" s="135" t="s">
+        <v>339</v>
+      </c>
+      <c r="D252" s="135" t="s">
+        <v>796</v>
+      </c>
+      <c r="E252" s="135" t="s">
+        <v>220</v>
+      </c>
+      <c r="F252" s="135" t="s">
+        <v>517</v>
+      </c>
+      <c r="G252" s="135" t="s">
+        <v>797</v>
+      </c>
+      <c r="H252" s="185" t="s">
+        <v>848</v>
+      </c>
+      <c r="I252" s="135" t="s">
+        <v>799</v>
+      </c>
+      <c r="J252" s="154" t="s">
+        <v>275</v>
+      </c>
+      <c r="K252" s="154" t="s">
+        <v>584</v>
+      </c>
+      <c r="L252" s="187">
+        <v>0.38</v>
+      </c>
       <c r="M252" s="3"/>
-      <c r="N252" s="24"/>
-      <c r="O252" s="3"/>
-      <c r="P252" s="3"/>
-      <c r="Q252" s="3"/>
-      <c r="R252" s="3"/>
-      <c r="S252" s="3"/>
+      <c r="N252" s="24" t="s">
+        <v>147</v>
+      </c>
+      <c r="O252" s="135" t="s">
+        <v>817</v>
+      </c>
+      <c r="P252" s="135" t="s">
+        <v>806</v>
+      </c>
+      <c r="Q252" s="135" t="s">
+        <v>136</v>
+      </c>
+      <c r="R252" s="135" t="s">
+        <v>33</v>
+      </c>
+      <c r="S252" s="135" t="s">
+        <v>814</v>
+      </c>
       <c r="U252" s="3"/>
     </row>
-    <row r="253" spans="1:39" ht="12.3">
-      <c r="A253" s="24"/>
-      <c r="B253" s="3"/>
-      <c r="C253" s="3"/>
-      <c r="D253" s="3"/>
-      <c r="E253" s="3"/>
-      <c r="F253" s="3"/>
-      <c r="G253" s="3"/>
-      <c r="H253" s="3"/>
-      <c r="I253" s="3"/>
-      <c r="J253" s="24"/>
-      <c r="K253" s="24"/>
-      <c r="L253" s="24"/>
-      <c r="M253" s="3"/>
-      <c r="N253" s="24"/>
-      <c r="O253" s="3"/>
-      <c r="P253" s="3"/>
-      <c r="Q253" s="3"/>
-      <c r="R253" s="3"/>
-      <c r="S253" s="3"/>
-      <c r="U253" s="3"/>
-    </row>
-    <row r="254" spans="1:39" ht="12.3">
-      <c r="A254" s="24"/>
-      <c r="B254" s="3"/>
-      <c r="C254" s="3"/>
-      <c r="D254" s="3"/>
-      <c r="E254" s="3"/>
-      <c r="F254" s="3"/>
-      <c r="G254" s="3"/>
-      <c r="H254" s="3"/>
-      <c r="I254" s="3"/>
-      <c r="J254" s="24"/>
-      <c r="K254" s="24"/>
-      <c r="L254" s="24"/>
-      <c r="M254" s="3"/>
-      <c r="N254" s="24"/>
-      <c r="O254" s="3"/>
-      <c r="P254" s="3"/>
-      <c r="Q254" s="3"/>
-      <c r="R254" s="3"/>
-      <c r="S254" s="3"/>
-      <c r="U254" s="3"/>
-    </row>
-    <row r="255" spans="1:39" ht="12.3">
-      <c r="A255" s="24"/>
-      <c r="B255" s="3"/>
-      <c r="C255" s="3"/>
-      <c r="D255" s="3"/>
-      <c r="E255" s="3"/>
-      <c r="F255" s="3"/>
-      <c r="G255" s="3"/>
-      <c r="H255" s="3"/>
-      <c r="I255" s="3"/>
-      <c r="J255" s="24"/>
-      <c r="K255" s="24"/>
-      <c r="L255" s="24"/>
-      <c r="M255" s="3"/>
-      <c r="N255" s="24"/>
-      <c r="O255" s="3"/>
-      <c r="P255" s="3"/>
-      <c r="Q255" s="3"/>
-      <c r="R255" s="3"/>
-      <c r="S255" s="3"/>
-      <c r="U255" s="3"/>
-    </row>
-    <row r="256" spans="1:39" ht="12.3">
-      <c r="A256" s="24"/>
-      <c r="B256" s="3"/>
-      <c r="C256" s="3"/>
-      <c r="D256" s="3"/>
-      <c r="E256" s="3"/>
-      <c r="F256" s="3"/>
-      <c r="G256" s="3"/>
-      <c r="H256" s="3"/>
-      <c r="I256" s="3"/>
-      <c r="J256" s="24"/>
-      <c r="K256" s="24"/>
-      <c r="L256" s="24"/>
-      <c r="M256" s="3"/>
-      <c r="N256" s="24"/>
-      <c r="O256" s="3"/>
-      <c r="P256" s="3"/>
-      <c r="Q256" s="3"/>
-      <c r="R256" s="3"/>
-      <c r="S256" s="3"/>
-      <c r="U256" s="3"/>
-    </row>
-    <row r="257" spans="1:21" ht="12.3">
-      <c r="A257" s="24"/>
-      <c r="B257" s="3"/>
-      <c r="C257" s="3"/>
-      <c r="D257" s="3"/>
-      <c r="E257" s="3"/>
-      <c r="F257" s="3"/>
-      <c r="G257" s="3"/>
-      <c r="H257" s="3"/>
-      <c r="I257" s="3"/>
-      <c r="J257" s="24"/>
-      <c r="K257" s="24"/>
-      <c r="L257" s="24"/>
-      <c r="M257" s="3"/>
-      <c r="N257" s="24"/>
-      <c r="O257" s="3"/>
-      <c r="P257" s="3"/>
-      <c r="Q257" s="3"/>
-      <c r="R257" s="3"/>
-      <c r="S257" s="3"/>
-      <c r="U257" s="3"/>
-    </row>
-    <row r="258" spans="1:21" ht="12.3">
-      <c r="A258" s="24"/>
-      <c r="B258" s="3"/>
-      <c r="C258" s="3"/>
-      <c r="D258" s="3"/>
-      <c r="E258" s="3"/>
-      <c r="F258" s="3"/>
-      <c r="G258" s="3"/>
-      <c r="H258" s="3"/>
-      <c r="I258" s="3"/>
-      <c r="J258" s="24"/>
-      <c r="K258" s="24"/>
-      <c r="L258" s="24"/>
-      <c r="M258" s="3"/>
-      <c r="N258" s="24"/>
-      <c r="O258" s="3"/>
-      <c r="P258" s="3"/>
-      <c r="Q258" s="3"/>
-      <c r="R258" s="3"/>
-      <c r="S258" s="3"/>
-      <c r="U258" s="3"/>
-    </row>
-    <row r="259" spans="1:21" ht="12.3">
-      <c r="A259" s="24"/>
-      <c r="B259" s="3"/>
-      <c r="C259" s="3"/>
-      <c r="D259" s="3"/>
-      <c r="E259" s="3"/>
-      <c r="F259" s="3"/>
-      <c r="G259" s="3"/>
-      <c r="H259" s="3"/>
-      <c r="I259" s="3"/>
-      <c r="J259" s="24"/>
-      <c r="K259" s="24"/>
-      <c r="L259" s="24"/>
-      <c r="M259" s="3"/>
-      <c r="N259" s="24"/>
-      <c r="O259" s="3"/>
-      <c r="P259" s="3"/>
-      <c r="Q259" s="3"/>
-      <c r="R259" s="3"/>
-      <c r="S259" s="3"/>
-      <c r="U259" s="3"/>
-    </row>
-    <row r="260" spans="1:21" ht="12.3">
-      <c r="A260" s="24"/>
-      <c r="B260" s="3"/>
-      <c r="C260" s="3"/>
-      <c r="D260" s="3"/>
-      <c r="E260" s="3"/>
-      <c r="F260" s="3"/>
-      <c r="G260" s="3"/>
-      <c r="H260" s="3"/>
-      <c r="I260" s="3"/>
-      <c r="J260" s="24"/>
-      <c r="K260" s="24"/>
-      <c r="L260" s="24"/>
-      <c r="M260" s="3"/>
-      <c r="N260" s="24"/>
-      <c r="O260" s="3"/>
-      <c r="P260" s="3"/>
-      <c r="Q260" s="3"/>
-      <c r="R260" s="3"/>
-      <c r="S260" s="3"/>
-      <c r="U260" s="3"/>
-    </row>
-    <row r="261" spans="1:21" ht="12.3">
-      <c r="A261" s="24"/>
-      <c r="B261" s="3"/>
-      <c r="C261" s="3"/>
-      <c r="D261" s="3"/>
-      <c r="E261" s="3"/>
-      <c r="F261" s="3"/>
-      <c r="G261" s="3"/>
-      <c r="H261" s="3"/>
-      <c r="I261" s="3"/>
-      <c r="J261" s="24"/>
-      <c r="K261" s="24"/>
-      <c r="L261" s="24"/>
-      <c r="M261" s="3"/>
-      <c r="N261" s="24"/>
-      <c r="O261" s="3"/>
-      <c r="P261" s="3"/>
-      <c r="Q261" s="3"/>
-      <c r="R261" s="3"/>
-      <c r="S261" s="3"/>
-      <c r="U261" s="3"/>
-    </row>
-    <row r="262" spans="1:21" ht="12.3">
-      <c r="A262" s="24"/>
-      <c r="B262" s="3"/>
-      <c r="C262" s="3"/>
-      <c r="D262" s="3"/>
-      <c r="E262" s="3"/>
-      <c r="F262" s="3"/>
-      <c r="G262" s="3"/>
-      <c r="H262" s="3"/>
-      <c r="I262" s="3"/>
-      <c r="J262" s="24"/>
-      <c r="K262" s="24"/>
-      <c r="L262" s="24"/>
-      <c r="M262" s="3"/>
-      <c r="N262" s="24"/>
-      <c r="O262" s="3"/>
-      <c r="P262" s="3"/>
-      <c r="Q262" s="3"/>
-      <c r="R262" s="3"/>
-      <c r="S262" s="3"/>
-      <c r="U262" s="3"/>
-    </row>
-    <row r="263" spans="1:21" ht="12.3">
-      <c r="A263" s="24"/>
-      <c r="B263" s="3"/>
-      <c r="C263" s="3"/>
-      <c r="D263" s="3"/>
-      <c r="E263" s="3"/>
-      <c r="F263" s="3"/>
-      <c r="G263" s="3"/>
-      <c r="H263" s="3"/>
-      <c r="I263" s="3"/>
-      <c r="J263" s="24"/>
-      <c r="K263" s="24"/>
-      <c r="L263" s="24"/>
-      <c r="M263" s="3"/>
-      <c r="N263" s="24"/>
-      <c r="O263" s="3"/>
-      <c r="P263" s="3"/>
-      <c r="Q263" s="3"/>
-      <c r="R263" s="3"/>
-      <c r="S263" s="3"/>
-      <c r="U263" s="3"/>
-    </row>
-    <row r="264" spans="1:21" ht="12.3">
-      <c r="A264" s="24"/>
-      <c r="B264" s="3"/>
-      <c r="C264" s="3"/>
-      <c r="D264" s="3"/>
-      <c r="E264" s="3"/>
-      <c r="F264" s="3"/>
-      <c r="G264" s="3"/>
-      <c r="H264" s="3"/>
-      <c r="I264" s="3"/>
-      <c r="J264" s="24"/>
-      <c r="K264" s="24"/>
-      <c r="L264" s="24"/>
-      <c r="M264" s="3"/>
-      <c r="N264" s="24"/>
-      <c r="O264" s="3"/>
-      <c r="P264" s="3"/>
-      <c r="Q264" s="3"/>
-      <c r="R264" s="3"/>
-      <c r="S264" s="3"/>
-      <c r="U264" s="3"/>
-    </row>
-    <row r="265" spans="1:21" ht="12.3">
+    <row r="253" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A253" s="163" t="s">
+        <v>818</v>
+      </c>
+      <c r="B253" s="6"/>
+      <c r="C253" s="6"/>
+      <c r="D253" s="6"/>
+      <c r="E253" s="6"/>
+      <c r="F253" s="6"/>
+      <c r="G253" s="6"/>
+      <c r="H253" s="6"/>
+      <c r="I253" s="6"/>
+      <c r="J253" s="5"/>
+      <c r="K253" s="5"/>
+      <c r="L253" s="5"/>
+      <c r="M253" s="6"/>
+      <c r="N253" s="5"/>
+      <c r="O253" s="182"/>
+      <c r="P253" s="6"/>
+      <c r="Q253" s="6"/>
+      <c r="R253" s="6"/>
+      <c r="S253" s="6"/>
+      <c r="T253" s="7"/>
+      <c r="U253" s="6"/>
+      <c r="V253" s="7"/>
+      <c r="W253" s="7"/>
+      <c r="X253" s="7"/>
+      <c r="Y253" s="7"/>
+      <c r="Z253" s="7"/>
+      <c r="AA253" s="7"/>
+      <c r="AB253" s="7"/>
+      <c r="AC253" s="7"/>
+      <c r="AD253" s="7"/>
+      <c r="AE253" s="7"/>
+      <c r="AF253" s="7"/>
+      <c r="AG253" s="7"/>
+      <c r="AH253" s="7"/>
+      <c r="AI253" s="7"/>
+      <c r="AJ253" s="7"/>
+      <c r="AK253" s="7"/>
+      <c r="AL253" s="7"/>
+      <c r="AM253" s="7"/>
+    </row>
+    <row r="254" spans="1:39" s="301" customFormat="1" ht="12.3">
+      <c r="A254" s="295" t="s">
+        <v>828</v>
+      </c>
+      <c r="B254" s="296" t="s">
+        <v>822</v>
+      </c>
+      <c r="C254" s="296" t="s">
+        <v>339</v>
+      </c>
+      <c r="D254" s="296" t="s">
+        <v>796</v>
+      </c>
+      <c r="E254" s="296" t="s">
+        <v>220</v>
+      </c>
+      <c r="F254" s="296" t="s">
+        <v>280</v>
+      </c>
+      <c r="G254" s="296" t="s">
+        <v>844</v>
+      </c>
+      <c r="H254" s="296" t="s">
+        <v>849</v>
+      </c>
+      <c r="I254" s="296" t="s">
+        <v>799</v>
+      </c>
+      <c r="J254" s="295" t="s">
+        <v>275</v>
+      </c>
+      <c r="K254" s="295" t="s">
+        <v>584</v>
+      </c>
+      <c r="L254" s="297">
+        <v>0.41</v>
+      </c>
+      <c r="M254" s="296"/>
+      <c r="N254" s="295" t="s">
+        <v>147</v>
+      </c>
+      <c r="O254" s="296" t="s">
+        <v>819</v>
+      </c>
+      <c r="P254" s="296" t="s">
+        <v>818</v>
+      </c>
+      <c r="Q254" s="296" t="s">
+        <v>136</v>
+      </c>
+      <c r="R254" s="296" t="s">
+        <v>33</v>
+      </c>
+      <c r="S254" s="296" t="s">
+        <v>821</v>
+      </c>
+      <c r="T254" s="299" t="s">
+        <v>820</v>
+      </c>
+      <c r="U254" s="296" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="255" spans="1:39" s="300" customFormat="1" ht="12.3">
+      <c r="A255" s="295" t="s">
+        <v>829</v>
+      </c>
+      <c r="B255" s="296" t="s">
+        <v>803</v>
+      </c>
+      <c r="C255" s="296" t="s">
+        <v>339</v>
+      </c>
+      <c r="D255" s="296" t="s">
+        <v>796</v>
+      </c>
+      <c r="E255" s="296" t="s">
+        <v>220</v>
+      </c>
+      <c r="F255" s="296" t="s">
+        <v>280</v>
+      </c>
+      <c r="G255" s="296" t="s">
+        <v>844</v>
+      </c>
+      <c r="H255" s="296" t="s">
+        <v>849</v>
+      </c>
+      <c r="I255" s="296" t="s">
+        <v>799</v>
+      </c>
+      <c r="J255" s="295" t="s">
+        <v>275</v>
+      </c>
+      <c r="K255" s="295" t="s">
+        <v>584</v>
+      </c>
+      <c r="L255" s="297">
+        <v>0.41</v>
+      </c>
+      <c r="M255" s="296"/>
+      <c r="N255" s="295" t="s">
+        <v>147</v>
+      </c>
+      <c r="O255" s="296" t="s">
+        <v>823</v>
+      </c>
+      <c r="P255" s="296" t="s">
+        <v>818</v>
+      </c>
+      <c r="Q255" s="296" t="s">
+        <v>136</v>
+      </c>
+      <c r="R255" s="296" t="s">
+        <v>33</v>
+      </c>
+      <c r="S255" s="296" t="s">
+        <v>805</v>
+      </c>
+      <c r="T255" s="299" t="s">
+        <v>820</v>
+      </c>
+      <c r="U255" s="296" t="s">
+        <v>824</v>
+      </c>
+      <c r="V255" s="301"/>
+      <c r="W255" s="301"/>
+      <c r="X255" s="301"/>
+      <c r="Y255" s="301"/>
+      <c r="Z255" s="301"/>
+      <c r="AA255" s="301"/>
+    </row>
+    <row r="256" spans="1:39" s="106" customFormat="1" ht="12.3">
+      <c r="A256" s="291" t="s">
+        <v>830</v>
+      </c>
+      <c r="B256" s="292" t="s">
+        <v>803</v>
+      </c>
+      <c r="C256" s="292" t="s">
+        <v>339</v>
+      </c>
+      <c r="D256" s="292" t="s">
+        <v>796</v>
+      </c>
+      <c r="E256" s="292" t="s">
+        <v>220</v>
+      </c>
+      <c r="F256" s="292" t="s">
+        <v>280</v>
+      </c>
+      <c r="G256" s="292" t="s">
+        <v>844</v>
+      </c>
+      <c r="H256" s="284" t="s">
+        <v>849</v>
+      </c>
+      <c r="I256" s="292" t="s">
+        <v>799</v>
+      </c>
+      <c r="J256" s="291" t="s">
+        <v>275</v>
+      </c>
+      <c r="K256" s="291" t="s">
+        <v>584</v>
+      </c>
+      <c r="L256" s="293">
+        <v>0.41</v>
+      </c>
+      <c r="M256" s="100"/>
+      <c r="N256" s="152" t="s">
+        <v>29</v>
+      </c>
+      <c r="O256" s="100" t="s">
+        <v>825</v>
+      </c>
+      <c r="P256" s="292" t="s">
+        <v>818</v>
+      </c>
+      <c r="Q256" s="292" t="s">
+        <v>136</v>
+      </c>
+      <c r="R256" s="292" t="s">
+        <v>33</v>
+      </c>
+      <c r="S256" s="292" t="s">
+        <v>805</v>
+      </c>
+      <c r="T256" s="294" t="s">
+        <v>820</v>
+      </c>
+      <c r="U256" s="100" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="257" spans="1:39" s="112" customFormat="1" ht="12.3">
+      <c r="A257" s="279" t="s">
+        <v>831</v>
+      </c>
+      <c r="B257" s="280" t="s">
+        <v>803</v>
+      </c>
+      <c r="C257" s="280" t="s">
+        <v>339</v>
+      </c>
+      <c r="D257" s="280" t="s">
+        <v>796</v>
+      </c>
+      <c r="E257" s="280" t="s">
+        <v>220</v>
+      </c>
+      <c r="F257" s="280" t="s">
+        <v>280</v>
+      </c>
+      <c r="G257" s="280" t="s">
+        <v>844</v>
+      </c>
+      <c r="H257" s="280" t="s">
+        <v>849</v>
+      </c>
+      <c r="I257" s="280" t="s">
+        <v>799</v>
+      </c>
+      <c r="J257" s="279" t="s">
+        <v>275</v>
+      </c>
+      <c r="K257" s="279" t="s">
+        <v>584</v>
+      </c>
+      <c r="L257" s="281">
+        <v>0.41</v>
+      </c>
+      <c r="M257" s="107"/>
+      <c r="N257" s="150" t="s">
+        <v>424</v>
+      </c>
+      <c r="O257" s="107" t="s">
+        <v>827</v>
+      </c>
+      <c r="P257" s="280" t="s">
+        <v>818</v>
+      </c>
+      <c r="Q257" s="280" t="s">
+        <v>136</v>
+      </c>
+      <c r="R257" s="280" t="s">
+        <v>33</v>
+      </c>
+      <c r="S257" s="280" t="s">
+        <v>805</v>
+      </c>
+      <c r="T257" s="282" t="s">
+        <v>820</v>
+      </c>
+      <c r="U257" s="107" t="s">
+        <v>826</v>
+      </c>
+    </row>
+    <row r="258" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A258" s="163" t="s">
+        <v>832</v>
+      </c>
+      <c r="B258" s="6"/>
+      <c r="C258" s="6"/>
+      <c r="D258" s="6"/>
+      <c r="E258" s="6"/>
+      <c r="F258" s="6"/>
+      <c r="G258" s="6"/>
+      <c r="H258" s="6"/>
+      <c r="I258" s="6"/>
+      <c r="J258" s="5"/>
+      <c r="K258" s="5"/>
+      <c r="L258" s="5"/>
+      <c r="M258" s="6"/>
+      <c r="N258" s="5"/>
+      <c r="O258" s="182"/>
+      <c r="P258" s="6"/>
+      <c r="Q258" s="6"/>
+      <c r="R258" s="6"/>
+      <c r="S258" s="6"/>
+      <c r="T258" s="7"/>
+      <c r="U258" s="6"/>
+      <c r="V258" s="7"/>
+      <c r="W258" s="7"/>
+      <c r="X258" s="7"/>
+      <c r="Y258" s="7"/>
+      <c r="Z258" s="7"/>
+      <c r="AA258" s="7"/>
+      <c r="AB258" s="7"/>
+      <c r="AC258" s="7"/>
+      <c r="AD258" s="7"/>
+      <c r="AE258" s="7"/>
+      <c r="AF258" s="7"/>
+      <c r="AG258" s="7"/>
+      <c r="AH258" s="7"/>
+      <c r="AI258" s="7"/>
+      <c r="AJ258" s="7"/>
+      <c r="AK258" s="7"/>
+      <c r="AL258" s="7"/>
+      <c r="AM258" s="7"/>
+    </row>
+    <row r="259" spans="1:39" s="300" customFormat="1" ht="12.3">
+      <c r="A259" s="295" t="s">
+        <v>838</v>
+      </c>
+      <c r="B259" s="296" t="s">
+        <v>803</v>
+      </c>
+      <c r="C259" s="296" t="s">
+        <v>339</v>
+      </c>
+      <c r="D259" s="296" t="s">
+        <v>796</v>
+      </c>
+      <c r="E259" s="296" t="s">
+        <v>220</v>
+      </c>
+      <c r="F259" s="296" t="s">
+        <v>280</v>
+      </c>
+      <c r="G259" s="296" t="s">
+        <v>836</v>
+      </c>
+      <c r="H259" s="185" t="s">
+        <v>850</v>
+      </c>
+      <c r="I259" s="296" t="s">
+        <v>799</v>
+      </c>
+      <c r="J259" s="295" t="s">
+        <v>275</v>
+      </c>
+      <c r="K259" s="295" t="s">
+        <v>584</v>
+      </c>
+      <c r="L259" s="297">
+        <v>0.41</v>
+      </c>
+      <c r="M259" s="185"/>
+      <c r="N259" s="298" t="s">
+        <v>147</v>
+      </c>
+      <c r="O259" s="185" t="s">
+        <v>833</v>
+      </c>
+      <c r="P259" s="185" t="s">
+        <v>832</v>
+      </c>
+      <c r="Q259" s="296" t="s">
+        <v>136</v>
+      </c>
+      <c r="R259" s="296" t="s">
+        <v>33</v>
+      </c>
+      <c r="S259" s="296" t="s">
+        <v>805</v>
+      </c>
+      <c r="T259" s="299" t="s">
+        <v>834</v>
+      </c>
+      <c r="U259" s="185" t="s">
+        <v>835</v>
+      </c>
+    </row>
+    <row r="260" spans="1:39" s="106" customFormat="1" ht="12.3">
+      <c r="A260" s="291" t="s">
+        <v>839</v>
+      </c>
+      <c r="B260" s="292" t="s">
+        <v>803</v>
+      </c>
+      <c r="C260" s="292" t="s">
+        <v>339</v>
+      </c>
+      <c r="D260" s="292" t="s">
+        <v>796</v>
+      </c>
+      <c r="E260" s="292" t="s">
+        <v>220</v>
+      </c>
+      <c r="F260" s="292" t="s">
+        <v>280</v>
+      </c>
+      <c r="G260" s="100" t="s">
+        <v>836</v>
+      </c>
+      <c r="H260" s="140" t="s">
+        <v>850</v>
+      </c>
+      <c r="I260" s="292" t="s">
+        <v>799</v>
+      </c>
+      <c r="J260" s="291" t="s">
+        <v>275</v>
+      </c>
+      <c r="K260" s="291" t="s">
+        <v>584</v>
+      </c>
+      <c r="L260" s="293">
+        <v>0.41</v>
+      </c>
+      <c r="M260" s="100"/>
+      <c r="N260" s="152" t="s">
+        <v>29</v>
+      </c>
+      <c r="O260" s="100" t="s">
+        <v>837</v>
+      </c>
+      <c r="P260" s="100" t="s">
+        <v>832</v>
+      </c>
+      <c r="Q260" s="292" t="s">
+        <v>136</v>
+      </c>
+      <c r="R260" s="292" t="s">
+        <v>33</v>
+      </c>
+      <c r="S260" s="292" t="s">
+        <v>805</v>
+      </c>
+      <c r="T260" s="294" t="s">
+        <v>834</v>
+      </c>
+      <c r="U260" s="100"/>
+    </row>
+    <row r="261" spans="1:39" s="139" customFormat="1" ht="12.3">
+      <c r="A261" s="275" t="s">
+        <v>840</v>
+      </c>
+      <c r="B261" s="276" t="s">
+        <v>803</v>
+      </c>
+      <c r="C261" s="276" t="s">
+        <v>339</v>
+      </c>
+      <c r="D261" s="276" t="s">
+        <v>796</v>
+      </c>
+      <c r="E261" s="276" t="s">
+        <v>220</v>
+      </c>
+      <c r="F261" s="276" t="s">
+        <v>280</v>
+      </c>
+      <c r="G261" s="276" t="s">
+        <v>844</v>
+      </c>
+      <c r="H261" s="135" t="s">
+        <v>849</v>
+      </c>
+      <c r="I261" s="276" t="s">
+        <v>799</v>
+      </c>
+      <c r="J261" s="275" t="s">
+        <v>275</v>
+      </c>
+      <c r="K261" s="275" t="s">
+        <v>584</v>
+      </c>
+      <c r="L261" s="277">
+        <v>0.41</v>
+      </c>
+      <c r="M261" s="135"/>
+      <c r="N261" s="154" t="s">
+        <v>147</v>
+      </c>
+      <c r="O261" s="135" t="s">
+        <v>842</v>
+      </c>
+      <c r="P261" s="135" t="s">
+        <v>832</v>
+      </c>
+      <c r="Q261" s="276" t="s">
+        <v>136</v>
+      </c>
+      <c r="R261" s="276" t="s">
+        <v>33</v>
+      </c>
+      <c r="S261" s="276" t="s">
+        <v>805</v>
+      </c>
+      <c r="T261" s="278" t="s">
+        <v>820</v>
+      </c>
+      <c r="U261" s="135"/>
+    </row>
+    <row r="262" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A262" s="163" t="s">
+        <v>841</v>
+      </c>
+      <c r="B262" s="6"/>
+      <c r="C262" s="6"/>
+      <c r="D262" s="6"/>
+      <c r="E262" s="6"/>
+      <c r="F262" s="6"/>
+      <c r="G262" s="6"/>
+      <c r="H262" s="6"/>
+      <c r="I262" s="6"/>
+      <c r="J262" s="5"/>
+      <c r="K262" s="5"/>
+      <c r="L262" s="5"/>
+      <c r="M262" s="6"/>
+      <c r="N262" s="5"/>
+      <c r="O262" s="182"/>
+      <c r="P262" s="6"/>
+      <c r="Q262" s="6"/>
+      <c r="R262" s="6"/>
+      <c r="S262" s="6"/>
+      <c r="T262" s="7"/>
+      <c r="U262" s="6"/>
+      <c r="V262" s="7"/>
+      <c r="W262" s="7"/>
+      <c r="X262" s="7"/>
+      <c r="Y262" s="7"/>
+      <c r="Z262" s="7"/>
+      <c r="AA262" s="7"/>
+      <c r="AB262" s="7"/>
+      <c r="AC262" s="7"/>
+      <c r="AD262" s="7"/>
+      <c r="AE262" s="7"/>
+      <c r="AF262" s="7"/>
+      <c r="AG262" s="7"/>
+      <c r="AH262" s="7"/>
+      <c r="AI262" s="7"/>
+      <c r="AJ262" s="7"/>
+      <c r="AK262" s="7"/>
+      <c r="AL262" s="7"/>
+      <c r="AM262" s="7"/>
+    </row>
+    <row r="263" spans="1:39" s="112" customFormat="1" ht="12.3">
+      <c r="A263" s="279" t="s">
+        <v>853</v>
+      </c>
+      <c r="B263" s="280" t="s">
+        <v>843</v>
+      </c>
+      <c r="C263" s="280" t="s">
+        <v>339</v>
+      </c>
+      <c r="D263" s="280" t="s">
+        <v>796</v>
+      </c>
+      <c r="E263" s="280" t="s">
+        <v>220</v>
+      </c>
+      <c r="F263" s="280" t="s">
+        <v>280</v>
+      </c>
+      <c r="G263" s="107" t="s">
+        <v>844</v>
+      </c>
+      <c r="H263" s="107" t="s">
+        <v>849</v>
+      </c>
+      <c r="I263" s="280" t="s">
+        <v>799</v>
+      </c>
+      <c r="J263" s="279" t="s">
+        <v>275</v>
+      </c>
+      <c r="K263" s="279" t="s">
+        <v>584</v>
+      </c>
+      <c r="L263" s="281">
+        <v>0.41</v>
+      </c>
+      <c r="M263" s="107"/>
+      <c r="N263" s="150" t="s">
+        <v>424</v>
+      </c>
+      <c r="O263" s="107" t="s">
+        <v>845</v>
+      </c>
+      <c r="P263" s="107" t="s">
+        <v>841</v>
+      </c>
+      <c r="Q263" s="280" t="s">
+        <v>136</v>
+      </c>
+      <c r="R263" s="280" t="s">
+        <v>33</v>
+      </c>
+      <c r="S263" s="280" t="s">
+        <v>846</v>
+      </c>
+      <c r="T263" s="282" t="s">
+        <v>820</v>
+      </c>
+      <c r="U263" s="107" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="264" spans="1:39" s="145" customFormat="1" ht="12.3">
+      <c r="A264" s="283" t="s">
+        <v>854</v>
+      </c>
+      <c r="B264" s="284" t="s">
+        <v>843</v>
+      </c>
+      <c r="C264" s="284" t="s">
+        <v>339</v>
+      </c>
+      <c r="D264" s="284" t="s">
+        <v>796</v>
+      </c>
+      <c r="E264" s="284" t="s">
+        <v>220</v>
+      </c>
+      <c r="F264" s="292" t="s">
+        <v>280</v>
+      </c>
+      <c r="G264" s="140" t="s">
+        <v>844</v>
+      </c>
+      <c r="H264" s="140" t="s">
+        <v>849</v>
+      </c>
+      <c r="I264" s="284" t="s">
+        <v>799</v>
+      </c>
+      <c r="J264" s="283" t="s">
+        <v>275</v>
+      </c>
+      <c r="K264" s="283" t="s">
+        <v>584</v>
+      </c>
+      <c r="L264" s="285">
+        <v>0.41</v>
+      </c>
+      <c r="M264" s="140"/>
+      <c r="N264" s="153" t="s">
+        <v>424</v>
+      </c>
+      <c r="O264" s="140" t="s">
+        <v>851</v>
+      </c>
+      <c r="P264" s="140" t="s">
+        <v>841</v>
+      </c>
+      <c r="Q264" s="284" t="s">
+        <v>136</v>
+      </c>
+      <c r="R264" s="284" t="s">
+        <v>33</v>
+      </c>
+      <c r="S264" s="284" t="s">
+        <v>846</v>
+      </c>
+      <c r="T264" s="286" t="s">
+        <v>820</v>
+      </c>
+      <c r="U264" s="140" t="s">
+        <v>852</v>
+      </c>
+    </row>
+    <row r="265" spans="1:39" ht="12.3">
       <c r="A265" s="24"/>
       <c r="B265" s="3"/>
       <c r="C265" s="3"/>
@@ -18827,7 +19482,7 @@
       <c r="S265" s="3"/>
       <c r="U265" s="3"/>
     </row>
-    <row r="266" spans="1:21" ht="12.3">
+    <row r="266" spans="1:39" ht="12.3">
       <c r="A266" s="24"/>
       <c r="B266" s="3"/>
       <c r="C266" s="3"/>
@@ -18849,7 +19504,7 @@
       <c r="S266" s="3"/>
       <c r="U266" s="3"/>
     </row>
-    <row r="267" spans="1:21" ht="12.3">
+    <row r="267" spans="1:39" ht="12.3">
       <c r="A267" s="24"/>
       <c r="B267" s="3"/>
       <c r="C267" s="3"/>
@@ -18871,7 +19526,7 @@
       <c r="S267" s="3"/>
       <c r="U267" s="3"/>
     </row>
-    <row r="268" spans="1:21" ht="12.3">
+    <row r="268" spans="1:39" ht="12.3">
       <c r="A268" s="24"/>
       <c r="B268" s="3"/>
       <c r="C268" s="3"/>
@@ -18893,7 +19548,7 @@
       <c r="S268" s="3"/>
       <c r="U268" s="3"/>
     </row>
-    <row r="269" spans="1:21" ht="12.3">
+    <row r="269" spans="1:39" ht="12.3">
       <c r="A269" s="24"/>
       <c r="B269" s="3"/>
       <c r="C269" s="3"/>
@@ -18915,7 +19570,7 @@
       <c r="S269" s="3"/>
       <c r="U269" s="3"/>
     </row>
-    <row r="270" spans="1:21" ht="12.3">
+    <row r="270" spans="1:39" ht="12.3">
       <c r="A270" s="24"/>
       <c r="B270" s="3"/>
       <c r="C270" s="3"/>
@@ -18937,7 +19592,7 @@
       <c r="S270" s="3"/>
       <c r="U270" s="3"/>
     </row>
-    <row r="271" spans="1:21" ht="12.3">
+    <row r="271" spans="1:39" ht="12.3">
       <c r="A271" s="24"/>
       <c r="B271" s="3"/>
       <c r="C271" s="3"/>
@@ -18959,7 +19614,7 @@
       <c r="S271" s="3"/>
       <c r="U271" s="3"/>
     </row>
-    <row r="272" spans="1:21" ht="12.3">
+    <row r="272" spans="1:39" ht="12.3">
       <c r="A272" s="24"/>
       <c r="B272" s="3"/>
       <c r="C272" s="3"/>

</xml_diff>

<commit_message>
updated model analysis notebook
</commit_message>
<xml_diff>
--- a/data_25_01_14.xlsx
+++ b/data_25_01_14.xlsx
@@ -8,26 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csuma-my.sharepoint.com/personal/toppenheim_csum_edu/Documents/Documents/GitHub/Strain-Sensor-/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="435" documentId="13_ncr:1_{9C3E2F24-F0BA-4ED0-966D-A349015366CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E5ADDAF9-11CB-4835-B75D-5CDEC2DFECF2}"/>
+  <xr:revisionPtr revIDLastSave="474" documentId="13_ncr:1_{9C3E2F24-F0BA-4ED0-966D-A349015366CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10E25A42-EF7D-4DBE-B306-0F48595BF7AB}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all data" sheetId="1" r:id="rId1"/>
-    <sheet name="TO_length_check_5_7_velcro" sheetId="12" r:id="rId2"/>
-    <sheet name="TO_length_accuracy_check_4_22" sheetId="9" r:id="rId3"/>
-    <sheet name="TO_misalignment_4_22" sheetId="11" r:id="rId4"/>
-    <sheet name="TO_reapplication_4_22" sheetId="10" r:id="rId5"/>
-    <sheet name="PK_data_accuracy_check" sheetId="8" r:id="rId6"/>
-    <sheet name="reapplication_Old_TO" sheetId="6" r:id="rId7"/>
-    <sheet name="misalignment_TO_Old" sheetId="3" r:id="rId8"/>
-    <sheet name="model comparison_TO_Old" sheetId="2" r:id="rId9"/>
-    <sheet name="abs_actual_dim_1_28_25" sheetId="7" r:id="rId10"/>
-    <sheet name=" dynamic autobending_TO_Old" sheetId="4" r:id="rId11"/>
-    <sheet name="all_data_accuracy_TO_Old" sheetId="5" r:id="rId12"/>
+    <sheet name="TO_model comparison" sheetId="13" r:id="rId2"/>
+    <sheet name="TO_length_check_5_7_velcro" sheetId="12" r:id="rId3"/>
+    <sheet name="TO_length_accuracy_check_4_22" sheetId="9" r:id="rId4"/>
+    <sheet name="TO_misalignment_4_22" sheetId="11" r:id="rId5"/>
+    <sheet name="TO_reapplication_4_22" sheetId="10" r:id="rId6"/>
+    <sheet name="PK_data_accuracy_check" sheetId="8" r:id="rId7"/>
+    <sheet name="reapplication_Old_TO" sheetId="6" r:id="rId8"/>
+    <sheet name="misalignment_TO_Old" sheetId="3" r:id="rId9"/>
+    <sheet name="model comparison_TO_Old" sheetId="2" r:id="rId10"/>
+    <sheet name="abs_actual_dim_1_28_25" sheetId="7" r:id="rId11"/>
+    <sheet name=" dynamic autobending_TO_Old" sheetId="4" r:id="rId12"/>
+    <sheet name="all_data_accuracy_TO_Old" sheetId="5" r:id="rId13"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5829" uniqueCount="855">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5906" uniqueCount="854">
   <si>
     <t>Sample Name</t>
   </si>
@@ -2462,9 +2462,6 @@
   </si>
   <si>
     <t>0.115 in</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>2.1 in</t>
@@ -3761,18 +3758,6 @@
     <xf numFmtId="0" fontId="17" fillId="17" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3802,6 +3787,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="17" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4031,9 +4028,9 @@
   </sheetPr>
   <dimension ref="A1:AM1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A231" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A264" sqref="A264"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A234" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H247" sqref="H247"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -4128,13 +4125,13 @@
       </c>
       <c r="W1" s="3"/>
     </row>
-    <row r="2" spans="1:39" s="288" customFormat="1" ht="12.3">
-      <c r="A2" s="287" t="s">
+    <row r="2" spans="1:39" s="299" customFormat="1" ht="12.3">
+      <c r="A2" s="298" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="3" spans="1:39" s="288" customFormat="1" ht="12.3"/>
-    <row r="4" spans="1:39" s="288" customFormat="1" ht="12.3"/>
+    <row r="3" spans="1:39" s="299" customFormat="1" ht="12.3"/>
+    <row r="4" spans="1:39" s="299" customFormat="1" ht="12.3"/>
     <row r="5" spans="1:39" ht="15.75" customHeight="1">
       <c r="A5" s="163" t="s">
         <v>18</v>
@@ -7162,13 +7159,13 @@
       <c r="AL49" s="262"/>
       <c r="AM49" s="263"/>
     </row>
-    <row r="50" spans="1:39" s="288" customFormat="1" ht="12.3">
-      <c r="A50" s="287" t="s">
+    <row r="50" spans="1:39" s="299" customFormat="1" ht="12.3">
+      <c r="A50" s="298" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="51" spans="1:39" s="288" customFormat="1" ht="12.3"/>
-    <row r="52" spans="1:39" s="288" customFormat="1" ht="12.3"/>
+    <row r="51" spans="1:39" s="299" customFormat="1" ht="12.3"/>
+    <row r="52" spans="1:39" s="299" customFormat="1" ht="12.3"/>
     <row r="53" spans="1:39" ht="15.75" customHeight="1">
       <c r="A53" s="166" t="s">
         <v>122</v>
@@ -11707,13 +11704,13 @@
         <v>378</v>
       </c>
     </row>
-    <row r="120" spans="1:39" s="288" customFormat="1" ht="12.3">
-      <c r="A120" s="287" t="s">
+    <row r="120" spans="1:39" s="299" customFormat="1" ht="12.3">
+      <c r="A120" s="298" t="s">
         <v>659</v>
       </c>
     </row>
-    <row r="121" spans="1:39" s="288" customFormat="1" ht="12.3"/>
-    <row r="122" spans="1:39" s="288" customFormat="1" ht="12.3"/>
+    <row r="121" spans="1:39" s="299" customFormat="1" ht="12.3"/>
+    <row r="122" spans="1:39" s="299" customFormat="1" ht="12.3"/>
     <row r="123" spans="1:39" ht="15.75" customHeight="1">
       <c r="A123" s="163" t="s">
         <v>379</v>
@@ -12074,10 +12071,10 @@
       </c>
     </row>
     <row r="129" spans="1:39" s="221" customFormat="1" ht="12.3">
-      <c r="A129" s="290" t="s">
+      <c r="A129" s="301" t="s">
         <v>660</v>
       </c>
-      <c r="B129" s="290"/>
+      <c r="B129" s="301"/>
       <c r="C129" s="217"/>
       <c r="D129" s="217"/>
       <c r="E129" s="218"/>
@@ -12099,8 +12096,8 @@
       <c r="U129" s="217"/>
     </row>
     <row r="130" spans="1:39" s="221" customFormat="1" ht="12.3">
-      <c r="A130" s="290"/>
-      <c r="B130" s="290"/>
+      <c r="A130" s="301"/>
+      <c r="B130" s="301"/>
       <c r="C130" s="217"/>
       <c r="D130" s="217"/>
       <c r="E130" s="218"/>
@@ -12122,8 +12119,8 @@
       <c r="U130" s="217"/>
     </row>
     <row r="131" spans="1:39" s="221" customFormat="1" ht="12.3">
-      <c r="A131" s="290"/>
-      <c r="B131" s="290"/>
+      <c r="A131" s="301"/>
+      <c r="B131" s="301"/>
       <c r="C131" s="217"/>
       <c r="D131" s="217"/>
       <c r="E131" s="218"/>
@@ -12680,13 +12677,13 @@
       </c>
       <c r="U141" s="3"/>
     </row>
-    <row r="142" spans="1:39" s="289" customFormat="1" ht="12.3">
-      <c r="A142" s="289" t="s">
+    <row r="142" spans="1:39" s="300" customFormat="1" ht="12.3">
+      <c r="A142" s="300" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="143" spans="1:39" s="289" customFormat="1" ht="12.3"/>
-    <row r="144" spans="1:39" s="289" customFormat="1" ht="12.3"/>
+    <row r="143" spans="1:39" s="300" customFormat="1" ht="12.3"/>
+    <row r="144" spans="1:39" s="300" customFormat="1" ht="12.3"/>
     <row r="145" spans="1:39" ht="15.75" customHeight="1">
       <c r="A145" s="163" t="s">
         <v>418</v>
@@ -14670,13 +14667,13 @@
         <v>519</v>
       </c>
     </row>
-    <row r="178" spans="1:39" s="288" customFormat="1" ht="12.3">
-      <c r="A178" s="287" t="s">
+    <row r="178" spans="1:39" s="299" customFormat="1" ht="12.3">
+      <c r="A178" s="298" t="s">
         <v>662</v>
       </c>
     </row>
-    <row r="179" spans="1:39" s="288" customFormat="1" ht="12.3"/>
-    <row r="180" spans="1:39" s="288" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="179" spans="1:39" s="299" customFormat="1" ht="12.3"/>
+    <row r="180" spans="1:39" s="299" customFormat="1" ht="15.75" customHeight="1"/>
     <row r="181" spans="1:39" s="145" customFormat="1" ht="12.3">
       <c r="A181" s="153"/>
       <c r="B181" s="140"/>
@@ -18057,13 +18054,13 @@
       </c>
       <c r="U237" s="107"/>
     </row>
-    <row r="238" spans="1:39" s="288" customFormat="1" ht="12.3">
-      <c r="A238" s="287" t="s">
+    <row r="238" spans="1:39" s="299" customFormat="1" ht="12.3">
+      <c r="A238" s="298" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="239" spans="1:39" s="288" customFormat="1" ht="12.3"/>
-    <row r="240" spans="1:39" s="288" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="239" spans="1:39" s="299" customFormat="1" ht="12.3"/>
+    <row r="240" spans="1:39" s="299" customFormat="1" ht="15.75" customHeight="1"/>
     <row r="241" spans="1:39" ht="15.75" customHeight="1">
       <c r="A241" s="163" t="s">
         <v>777</v>
@@ -18356,7 +18353,7 @@
     </row>
     <row r="246" spans="1:39" s="145" customFormat="1" ht="12.3">
       <c r="A246" s="153" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B246" s="140" t="s">
         <v>787</v>
@@ -18376,11 +18373,11 @@
       <c r="G246" s="140" t="s">
         <v>797</v>
       </c>
-      <c r="H246" s="140" t="s">
+      <c r="H246" s="100" t="s">
+        <v>847</v>
+      </c>
+      <c r="I246" s="140" t="s">
         <v>798</v>
-      </c>
-      <c r="I246" s="140" t="s">
-        <v>799</v>
       </c>
       <c r="J246" s="153" t="s">
         <v>275</v>
@@ -18396,7 +18393,7 @@
         <v>29</v>
       </c>
       <c r="O246" s="140" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="P246" s="140" t="s">
         <v>777</v>
@@ -18417,10 +18414,10 @@
     </row>
     <row r="247" spans="1:39" s="145" customFormat="1" ht="12.3">
       <c r="A247" s="153" t="s">
+        <v>801</v>
+      </c>
+      <c r="B247" s="140" t="s">
         <v>802</v>
-      </c>
-      <c r="B247" s="140" t="s">
-        <v>803</v>
       </c>
       <c r="C247" s="140" t="s">
         <v>339</v>
@@ -18437,11 +18434,11 @@
       <c r="G247" s="140" t="s">
         <v>797</v>
       </c>
-      <c r="H247" s="140" t="s">
+      <c r="H247" s="100" t="s">
+        <v>847</v>
+      </c>
+      <c r="I247" s="140" t="s">
         <v>798</v>
-      </c>
-      <c r="I247" s="140" t="s">
-        <v>799</v>
       </c>
       <c r="J247" s="153" t="s">
         <v>275</v>
@@ -18457,7 +18454,7 @@
         <v>29</v>
       </c>
       <c r="O247" s="140" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="P247" s="140" t="s">
         <v>777</v>
@@ -18469,7 +18466,7 @@
         <v>33</v>
       </c>
       <c r="S247" s="140" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="T247" s="144" t="s">
         <v>224</v>
@@ -18478,7 +18475,7 @@
     </row>
     <row r="248" spans="1:39" ht="15.75" customHeight="1">
       <c r="A248" s="163" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B248" s="6"/>
       <c r="C248" s="6"/>
@@ -18521,10 +18518,10 @@
     </row>
     <row r="249" spans="1:39" s="106" customFormat="1" ht="12.3">
       <c r="A249" s="152" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="B249" s="100" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C249" s="100" t="s">
         <v>339</v>
@@ -18542,10 +18539,10 @@
         <v>797</v>
       </c>
       <c r="H249" s="100" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="I249" s="100" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="J249" s="152" t="s">
         <v>275</v>
@@ -18561,10 +18558,10 @@
         <v>29</v>
       </c>
       <c r="O249" s="100" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="P249" s="100" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="Q249" s="100" t="s">
         <v>136</v>
@@ -18573,7 +18570,7 @@
         <v>33</v>
       </c>
       <c r="S249" s="100" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="T249" s="104" t="s">
         <v>224</v>
@@ -18582,10 +18579,10 @@
     </row>
     <row r="250" spans="1:39" s="106" customFormat="1" ht="12.3">
       <c r="A250" s="152" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="B250" s="100" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C250" s="100" t="s">
         <v>339</v>
@@ -18603,10 +18600,10 @@
         <v>797</v>
       </c>
       <c r="H250" s="100" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="I250" s="100" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="J250" s="152" t="s">
         <v>275</v>
@@ -18622,10 +18619,10 @@
         <v>29</v>
       </c>
       <c r="O250" s="100" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="P250" s="100" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="Q250" s="100" t="s">
         <v>136</v>
@@ -18634,7 +18631,7 @@
         <v>33</v>
       </c>
       <c r="S250" s="100" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="T250" s="104" t="s">
         <v>224</v>
@@ -18643,10 +18640,10 @@
     </row>
     <row r="251" spans="1:39" s="139" customFormat="1" ht="12.3">
       <c r="A251" s="154" t="s">
+        <v>810</v>
+      </c>
+      <c r="B251" s="135" t="s">
         <v>811</v>
-      </c>
-      <c r="B251" s="135" t="s">
-        <v>812</v>
       </c>
       <c r="C251" s="135" t="s">
         <v>339</v>
@@ -18664,10 +18661,10 @@
         <v>797</v>
       </c>
       <c r="H251" s="185" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="I251" s="135" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="J251" s="154" t="s">
         <v>275</v>
@@ -18683,10 +18680,10 @@
         <v>147</v>
       </c>
       <c r="O251" s="135" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="P251" s="135" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="Q251" s="135" t="s">
         <v>136</v>
@@ -18695,21 +18692,21 @@
         <v>33</v>
       </c>
       <c r="S251" s="135" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="T251" s="138" t="s">
         <v>224</v>
       </c>
       <c r="U251" s="135" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
     </row>
     <row r="252" spans="1:39" ht="12.3">
       <c r="A252" s="154" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="B252" s="135" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C252" s="135" t="s">
         <v>339</v>
@@ -18727,10 +18724,10 @@
         <v>797</v>
       </c>
       <c r="H252" s="185" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="I252" s="135" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="J252" s="154" t="s">
         <v>275</v>
@@ -18746,10 +18743,10 @@
         <v>147</v>
       </c>
       <c r="O252" s="135" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="P252" s="135" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="Q252" s="135" t="s">
         <v>136</v>
@@ -18758,13 +18755,13 @@
         <v>33</v>
       </c>
       <c r="S252" s="135" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="U252" s="3"/>
     </row>
     <row r="253" spans="1:39" ht="15.75" customHeight="1">
       <c r="A253" s="163" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="B253" s="6"/>
       <c r="C253" s="6"/>
@@ -18805,173 +18802,173 @@
       <c r="AL253" s="7"/>
       <c r="AM253" s="7"/>
     </row>
-    <row r="254" spans="1:39" s="301" customFormat="1" ht="12.3">
-      <c r="A254" s="295" t="s">
+    <row r="254" spans="1:39" s="297" customFormat="1" ht="12.3">
+      <c r="A254" s="291" t="s">
+        <v>827</v>
+      </c>
+      <c r="B254" s="292" t="s">
+        <v>821</v>
+      </c>
+      <c r="C254" s="292" t="s">
+        <v>339</v>
+      </c>
+      <c r="D254" s="292" t="s">
+        <v>796</v>
+      </c>
+      <c r="E254" s="292" t="s">
+        <v>220</v>
+      </c>
+      <c r="F254" s="292" t="s">
+        <v>280</v>
+      </c>
+      <c r="G254" s="292" t="s">
+        <v>843</v>
+      </c>
+      <c r="H254" s="292" t="s">
+        <v>848</v>
+      </c>
+      <c r="I254" s="292" t="s">
+        <v>798</v>
+      </c>
+      <c r="J254" s="291" t="s">
+        <v>275</v>
+      </c>
+      <c r="K254" s="291" t="s">
+        <v>584</v>
+      </c>
+      <c r="L254" s="293">
+        <v>0.41</v>
+      </c>
+      <c r="M254" s="292"/>
+      <c r="N254" s="291" t="s">
+        <v>147</v>
+      </c>
+      <c r="O254" s="292" t="s">
+        <v>818</v>
+      </c>
+      <c r="P254" s="292" t="s">
+        <v>817</v>
+      </c>
+      <c r="Q254" s="292" t="s">
+        <v>136</v>
+      </c>
+      <c r="R254" s="292" t="s">
+        <v>33</v>
+      </c>
+      <c r="S254" s="292" t="s">
+        <v>820</v>
+      </c>
+      <c r="T254" s="295" t="s">
+        <v>819</v>
+      </c>
+      <c r="U254" s="292" t="s">
+        <v>823</v>
+      </c>
+    </row>
+    <row r="255" spans="1:39" s="296" customFormat="1" ht="12.3">
+      <c r="A255" s="291" t="s">
         <v>828</v>
       </c>
-      <c r="B254" s="296" t="s">
+      <c r="B255" s="292" t="s">
+        <v>802</v>
+      </c>
+      <c r="C255" s="292" t="s">
+        <v>339</v>
+      </c>
+      <c r="D255" s="292" t="s">
+        <v>796</v>
+      </c>
+      <c r="E255" s="292" t="s">
+        <v>220</v>
+      </c>
+      <c r="F255" s="292" t="s">
+        <v>280</v>
+      </c>
+      <c r="G255" s="292" t="s">
+        <v>843</v>
+      </c>
+      <c r="H255" s="292" t="s">
+        <v>848</v>
+      </c>
+      <c r="I255" s="292" t="s">
+        <v>798</v>
+      </c>
+      <c r="J255" s="291" t="s">
+        <v>275</v>
+      </c>
+      <c r="K255" s="291" t="s">
+        <v>584</v>
+      </c>
+      <c r="L255" s="293">
+        <v>0.41</v>
+      </c>
+      <c r="M255" s="292"/>
+      <c r="N255" s="291" t="s">
+        <v>147</v>
+      </c>
+      <c r="O255" s="292" t="s">
         <v>822</v>
       </c>
-      <c r="C254" s="296" t="s">
+      <c r="P255" s="292" t="s">
+        <v>817</v>
+      </c>
+      <c r="Q255" s="292" t="s">
+        <v>136</v>
+      </c>
+      <c r="R255" s="292" t="s">
+        <v>33</v>
+      </c>
+      <c r="S255" s="292" t="s">
+        <v>804</v>
+      </c>
+      <c r="T255" s="295" t="s">
+        <v>819</v>
+      </c>
+      <c r="U255" s="292" t="s">
+        <v>823</v>
+      </c>
+      <c r="V255" s="297"/>
+      <c r="W255" s="297"/>
+      <c r="X255" s="297"/>
+      <c r="Y255" s="297"/>
+      <c r="Z255" s="297"/>
+      <c r="AA255" s="297"/>
+    </row>
+    <row r="256" spans="1:39" s="106" customFormat="1" ht="12.3">
+      <c r="A256" s="287" t="s">
+        <v>829</v>
+      </c>
+      <c r="B256" s="288" t="s">
+        <v>802</v>
+      </c>
+      <c r="C256" s="288" t="s">
         <v>339</v>
       </c>
-      <c r="D254" s="296" t="s">
+      <c r="D256" s="288" t="s">
         <v>796</v>
       </c>
-      <c r="E254" s="296" t="s">
+      <c r="E256" s="288" t="s">
         <v>220</v>
       </c>
-      <c r="F254" s="296" t="s">
+      <c r="F256" s="288" t="s">
         <v>280</v>
       </c>
-      <c r="G254" s="296" t="s">
-        <v>844</v>
-      </c>
-      <c r="H254" s="296" t="s">
-        <v>849</v>
-      </c>
-      <c r="I254" s="296" t="s">
-        <v>799</v>
-      </c>
-      <c r="J254" s="295" t="s">
+      <c r="G256" s="288" t="s">
+        <v>843</v>
+      </c>
+      <c r="H256" s="284" t="s">
+        <v>848</v>
+      </c>
+      <c r="I256" s="288" t="s">
+        <v>798</v>
+      </c>
+      <c r="J256" s="287" t="s">
         <v>275</v>
       </c>
-      <c r="K254" s="295" t="s">
+      <c r="K256" s="287" t="s">
         <v>584</v>
       </c>
-      <c r="L254" s="297">
-        <v>0.41</v>
-      </c>
-      <c r="M254" s="296"/>
-      <c r="N254" s="295" t="s">
-        <v>147</v>
-      </c>
-      <c r="O254" s="296" t="s">
-        <v>819</v>
-      </c>
-      <c r="P254" s="296" t="s">
-        <v>818</v>
-      </c>
-      <c r="Q254" s="296" t="s">
-        <v>136</v>
-      </c>
-      <c r="R254" s="296" t="s">
-        <v>33</v>
-      </c>
-      <c r="S254" s="296" t="s">
-        <v>821</v>
-      </c>
-      <c r="T254" s="299" t="s">
-        <v>820</v>
-      </c>
-      <c r="U254" s="296" t="s">
-        <v>824</v>
-      </c>
-    </row>
-    <row r="255" spans="1:39" s="300" customFormat="1" ht="12.3">
-      <c r="A255" s="295" t="s">
-        <v>829</v>
-      </c>
-      <c r="B255" s="296" t="s">
-        <v>803</v>
-      </c>
-      <c r="C255" s="296" t="s">
-        <v>339</v>
-      </c>
-      <c r="D255" s="296" t="s">
-        <v>796</v>
-      </c>
-      <c r="E255" s="296" t="s">
-        <v>220</v>
-      </c>
-      <c r="F255" s="296" t="s">
-        <v>280</v>
-      </c>
-      <c r="G255" s="296" t="s">
-        <v>844</v>
-      </c>
-      <c r="H255" s="296" t="s">
-        <v>849</v>
-      </c>
-      <c r="I255" s="296" t="s">
-        <v>799</v>
-      </c>
-      <c r="J255" s="295" t="s">
-        <v>275</v>
-      </c>
-      <c r="K255" s="295" t="s">
-        <v>584</v>
-      </c>
-      <c r="L255" s="297">
-        <v>0.41</v>
-      </c>
-      <c r="M255" s="296"/>
-      <c r="N255" s="295" t="s">
-        <v>147</v>
-      </c>
-      <c r="O255" s="296" t="s">
-        <v>823</v>
-      </c>
-      <c r="P255" s="296" t="s">
-        <v>818</v>
-      </c>
-      <c r="Q255" s="296" t="s">
-        <v>136</v>
-      </c>
-      <c r="R255" s="296" t="s">
-        <v>33</v>
-      </c>
-      <c r="S255" s="296" t="s">
-        <v>805</v>
-      </c>
-      <c r="T255" s="299" t="s">
-        <v>820</v>
-      </c>
-      <c r="U255" s="296" t="s">
-        <v>824</v>
-      </c>
-      <c r="V255" s="301"/>
-      <c r="W255" s="301"/>
-      <c r="X255" s="301"/>
-      <c r="Y255" s="301"/>
-      <c r="Z255" s="301"/>
-      <c r="AA255" s="301"/>
-    </row>
-    <row r="256" spans="1:39" s="106" customFormat="1" ht="12.3">
-      <c r="A256" s="291" t="s">
-        <v>830</v>
-      </c>
-      <c r="B256" s="292" t="s">
-        <v>803</v>
-      </c>
-      <c r="C256" s="292" t="s">
-        <v>339</v>
-      </c>
-      <c r="D256" s="292" t="s">
-        <v>796</v>
-      </c>
-      <c r="E256" s="292" t="s">
-        <v>220</v>
-      </c>
-      <c r="F256" s="292" t="s">
-        <v>280</v>
-      </c>
-      <c r="G256" s="292" t="s">
-        <v>844</v>
-      </c>
-      <c r="H256" s="284" t="s">
-        <v>849</v>
-      </c>
-      <c r="I256" s="292" t="s">
-        <v>799</v>
-      </c>
-      <c r="J256" s="291" t="s">
-        <v>275</v>
-      </c>
-      <c r="K256" s="291" t="s">
-        <v>584</v>
-      </c>
-      <c r="L256" s="293">
+      <c r="L256" s="289">
         <v>0.41</v>
       </c>
       <c r="M256" s="100"/>
@@ -18979,33 +18976,33 @@
         <v>29</v>
       </c>
       <c r="O256" s="100" t="s">
+        <v>824</v>
+      </c>
+      <c r="P256" s="288" t="s">
+        <v>817</v>
+      </c>
+      <c r="Q256" s="288" t="s">
+        <v>136</v>
+      </c>
+      <c r="R256" s="288" t="s">
+        <v>33</v>
+      </c>
+      <c r="S256" s="288" t="s">
+        <v>804</v>
+      </c>
+      <c r="T256" s="290" t="s">
+        <v>819</v>
+      </c>
+      <c r="U256" s="100" t="s">
         <v>825</v>
-      </c>
-      <c r="P256" s="292" t="s">
-        <v>818</v>
-      </c>
-      <c r="Q256" s="292" t="s">
-        <v>136</v>
-      </c>
-      <c r="R256" s="292" t="s">
-        <v>33</v>
-      </c>
-      <c r="S256" s="292" t="s">
-        <v>805</v>
-      </c>
-      <c r="T256" s="294" t="s">
-        <v>820</v>
-      </c>
-      <c r="U256" s="100" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="257" spans="1:39" s="112" customFormat="1" ht="12.3">
       <c r="A257" s="279" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="B257" s="280" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C257" s="280" t="s">
         <v>339</v>
@@ -19020,13 +19017,13 @@
         <v>280</v>
       </c>
       <c r="G257" s="280" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="H257" s="280" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="I257" s="280" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="J257" s="279" t="s">
         <v>275</v>
@@ -19042,10 +19039,10 @@
         <v>424</v>
       </c>
       <c r="O257" s="107" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="P257" s="280" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="Q257" s="280" t="s">
         <v>136</v>
@@ -19054,18 +19051,18 @@
         <v>33</v>
       </c>
       <c r="S257" s="280" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="T257" s="282" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="U257" s="107" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
     </row>
     <row r="258" spans="1:39" ht="15.75" customHeight="1">
       <c r="A258" s="163" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="B258" s="6"/>
       <c r="C258" s="6"/>
@@ -19106,104 +19103,104 @@
       <c r="AL258" s="7"/>
       <c r="AM258" s="7"/>
     </row>
-    <row r="259" spans="1:39" s="300" customFormat="1" ht="12.3">
-      <c r="A259" s="295" t="s">
+    <row r="259" spans="1:39" s="296" customFormat="1" ht="12.3">
+      <c r="A259" s="291" t="s">
+        <v>837</v>
+      </c>
+      <c r="B259" s="292" t="s">
+        <v>802</v>
+      </c>
+      <c r="C259" s="292" t="s">
+        <v>339</v>
+      </c>
+      <c r="D259" s="292" t="s">
+        <v>796</v>
+      </c>
+      <c r="E259" s="292" t="s">
+        <v>220</v>
+      </c>
+      <c r="F259" s="292" t="s">
+        <v>280</v>
+      </c>
+      <c r="G259" s="292" t="s">
+        <v>835</v>
+      </c>
+      <c r="H259" s="185" t="s">
+        <v>849</v>
+      </c>
+      <c r="I259" s="292" t="s">
+        <v>798</v>
+      </c>
+      <c r="J259" s="291" t="s">
+        <v>275</v>
+      </c>
+      <c r="K259" s="291" t="s">
+        <v>584</v>
+      </c>
+      <c r="L259" s="293">
+        <v>0.41</v>
+      </c>
+      <c r="M259" s="185"/>
+      <c r="N259" s="294" t="s">
+        <v>147</v>
+      </c>
+      <c r="O259" s="185" t="s">
+        <v>832</v>
+      </c>
+      <c r="P259" s="185" t="s">
+        <v>831</v>
+      </c>
+      <c r="Q259" s="292" t="s">
+        <v>136</v>
+      </c>
+      <c r="R259" s="292" t="s">
+        <v>33</v>
+      </c>
+      <c r="S259" s="292" t="s">
+        <v>804</v>
+      </c>
+      <c r="T259" s="295" t="s">
+        <v>833</v>
+      </c>
+      <c r="U259" s="185" t="s">
+        <v>834</v>
+      </c>
+    </row>
+    <row r="260" spans="1:39" s="106" customFormat="1" ht="12.3">
+      <c r="A260" s="287" t="s">
         <v>838</v>
       </c>
-      <c r="B259" s="296" t="s">
-        <v>803</v>
-      </c>
-      <c r="C259" s="296" t="s">
+      <c r="B260" s="288" t="s">
+        <v>802</v>
+      </c>
+      <c r="C260" s="288" t="s">
         <v>339</v>
       </c>
-      <c r="D259" s="296" t="s">
+      <c r="D260" s="288" t="s">
         <v>796</v>
       </c>
-      <c r="E259" s="296" t="s">
+      <c r="E260" s="288" t="s">
         <v>220</v>
       </c>
-      <c r="F259" s="296" t="s">
+      <c r="F260" s="288" t="s">
         <v>280</v>
       </c>
-      <c r="G259" s="296" t="s">
-        <v>836</v>
-      </c>
-      <c r="H259" s="185" t="s">
-        <v>850</v>
-      </c>
-      <c r="I259" s="296" t="s">
-        <v>799</v>
-      </c>
-      <c r="J259" s="295" t="s">
+      <c r="G260" s="100" t="s">
+        <v>835</v>
+      </c>
+      <c r="H260" s="140" t="s">
+        <v>849</v>
+      </c>
+      <c r="I260" s="288" t="s">
+        <v>798</v>
+      </c>
+      <c r="J260" s="287" t="s">
         <v>275</v>
       </c>
-      <c r="K259" s="295" t="s">
+      <c r="K260" s="287" t="s">
         <v>584</v>
       </c>
-      <c r="L259" s="297">
-        <v>0.41</v>
-      </c>
-      <c r="M259" s="185"/>
-      <c r="N259" s="298" t="s">
-        <v>147</v>
-      </c>
-      <c r="O259" s="185" t="s">
-        <v>833</v>
-      </c>
-      <c r="P259" s="185" t="s">
-        <v>832</v>
-      </c>
-      <c r="Q259" s="296" t="s">
-        <v>136</v>
-      </c>
-      <c r="R259" s="296" t="s">
-        <v>33</v>
-      </c>
-      <c r="S259" s="296" t="s">
-        <v>805</v>
-      </c>
-      <c r="T259" s="299" t="s">
-        <v>834</v>
-      </c>
-      <c r="U259" s="185" t="s">
-        <v>835</v>
-      </c>
-    </row>
-    <row r="260" spans="1:39" s="106" customFormat="1" ht="12.3">
-      <c r="A260" s="291" t="s">
-        <v>839</v>
-      </c>
-      <c r="B260" s="292" t="s">
-        <v>803</v>
-      </c>
-      <c r="C260" s="292" t="s">
-        <v>339</v>
-      </c>
-      <c r="D260" s="292" t="s">
-        <v>796</v>
-      </c>
-      <c r="E260" s="292" t="s">
-        <v>220</v>
-      </c>
-      <c r="F260" s="292" t="s">
-        <v>280</v>
-      </c>
-      <c r="G260" s="100" t="s">
-        <v>836</v>
-      </c>
-      <c r="H260" s="140" t="s">
-        <v>850</v>
-      </c>
-      <c r="I260" s="292" t="s">
-        <v>799</v>
-      </c>
-      <c r="J260" s="291" t="s">
-        <v>275</v>
-      </c>
-      <c r="K260" s="291" t="s">
-        <v>584</v>
-      </c>
-      <c r="L260" s="293">
+      <c r="L260" s="289">
         <v>0.41</v>
       </c>
       <c r="M260" s="100"/>
@@ -19211,31 +19208,31 @@
         <v>29</v>
       </c>
       <c r="O260" s="100" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="P260" s="100" t="s">
-        <v>832</v>
-      </c>
-      <c r="Q260" s="292" t="s">
+        <v>831</v>
+      </c>
+      <c r="Q260" s="288" t="s">
         <v>136</v>
       </c>
-      <c r="R260" s="292" t="s">
+      <c r="R260" s="288" t="s">
         <v>33</v>
       </c>
-      <c r="S260" s="292" t="s">
-        <v>805</v>
-      </c>
-      <c r="T260" s="294" t="s">
-        <v>834</v>
+      <c r="S260" s="288" t="s">
+        <v>804</v>
+      </c>
+      <c r="T260" s="290" t="s">
+        <v>833</v>
       </c>
       <c r="U260" s="100"/>
     </row>
     <row r="261" spans="1:39" s="139" customFormat="1" ht="12.3">
       <c r="A261" s="275" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="B261" s="276" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C261" s="276" t="s">
         <v>339</v>
@@ -19250,13 +19247,13 @@
         <v>280</v>
       </c>
       <c r="G261" s="276" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="H261" s="135" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="I261" s="276" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="J261" s="275" t="s">
         <v>275</v>
@@ -19272,10 +19269,10 @@
         <v>147</v>
       </c>
       <c r="O261" s="135" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="P261" s="135" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="Q261" s="276" t="s">
         <v>136</v>
@@ -19284,16 +19281,16 @@
         <v>33</v>
       </c>
       <c r="S261" s="276" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="T261" s="278" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="U261" s="135"/>
     </row>
     <row r="262" spans="1:39" ht="15.75" customHeight="1">
       <c r="A262" s="163" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="B262" s="6"/>
       <c r="C262" s="6"/>
@@ -19336,10 +19333,10 @@
     </row>
     <row r="263" spans="1:39" s="112" customFormat="1" ht="12.3">
       <c r="A263" s="279" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="B263" s="280" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C263" s="280" t="s">
         <v>339</v>
@@ -19354,13 +19351,13 @@
         <v>280</v>
       </c>
       <c r="G263" s="107" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="H263" s="107" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="I263" s="280" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="J263" s="279" t="s">
         <v>275</v>
@@ -19376,10 +19373,10 @@
         <v>424</v>
       </c>
       <c r="O263" s="107" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="P263" s="107" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="Q263" s="280" t="s">
         <v>136</v>
@@ -19388,21 +19385,21 @@
         <v>33</v>
       </c>
       <c r="S263" s="280" t="s">
+        <v>845</v>
+      </c>
+      <c r="T263" s="282" t="s">
+        <v>819</v>
+      </c>
+      <c r="U263" s="107" t="s">
         <v>846</v>
-      </c>
-      <c r="T263" s="282" t="s">
-        <v>820</v>
-      </c>
-      <c r="U263" s="107" t="s">
-        <v>847</v>
       </c>
     </row>
     <row r="264" spans="1:39" s="145" customFormat="1" ht="12.3">
       <c r="A264" s="283" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="B264" s="284" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C264" s="284" t="s">
         <v>339</v>
@@ -19413,17 +19410,17 @@
       <c r="E264" s="284" t="s">
         <v>220</v>
       </c>
-      <c r="F264" s="292" t="s">
+      <c r="F264" s="288" t="s">
         <v>280</v>
       </c>
       <c r="G264" s="140" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="H264" s="140" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="I264" s="284" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="J264" s="283" t="s">
         <v>275</v>
@@ -19439,10 +19436,10 @@
         <v>424</v>
       </c>
       <c r="O264" s="140" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="P264" s="140" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="Q264" s="284" t="s">
         <v>136</v>
@@ -19451,13 +19448,13 @@
         <v>33</v>
       </c>
       <c r="S264" s="284" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="T264" s="286" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="U264" s="140" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="265" spans="1:39" ht="12.3">
@@ -35844,6 +35841,1036 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:AM12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="15" max="15" width="87.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="30.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A1" s="74" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" s="75" t="s">
+        <v>169</v>
+      </c>
+      <c r="C1" s="75" t="s">
+        <v>170</v>
+      </c>
+      <c r="D1" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="75" t="s">
+        <v>22</v>
+      </c>
+      <c r="F1" s="75" t="s">
+        <v>130</v>
+      </c>
+      <c r="G1" s="75" t="s">
+        <v>131</v>
+      </c>
+      <c r="H1" s="75" t="s">
+        <v>171</v>
+      </c>
+      <c r="I1" s="75" t="s">
+        <v>172</v>
+      </c>
+      <c r="J1" s="76" t="s">
+        <v>173</v>
+      </c>
+      <c r="K1" s="76" t="s">
+        <v>161</v>
+      </c>
+      <c r="L1" s="77">
+        <v>0.39</v>
+      </c>
+      <c r="M1" s="75">
+        <v>1</v>
+      </c>
+      <c r="N1" s="78" t="s">
+        <v>29</v>
+      </c>
+      <c r="O1" s="78" t="s">
+        <v>174</v>
+      </c>
+      <c r="P1" s="75" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q1" s="75" t="s">
+        <v>136</v>
+      </c>
+      <c r="R1" s="75" t="s">
+        <v>33</v>
+      </c>
+      <c r="S1" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="T1" s="79" t="s">
+        <v>175</v>
+      </c>
+      <c r="U1" s="79" t="s">
+        <v>150</v>
+      </c>
+      <c r="V1" s="80" t="s">
+        <v>176</v>
+      </c>
+      <c r="W1" s="80"/>
+      <c r="X1" s="80"/>
+      <c r="Y1" s="80"/>
+      <c r="Z1" s="80"/>
+      <c r="AA1" s="80"/>
+      <c r="AB1" s="80"/>
+      <c r="AC1" s="80"/>
+      <c r="AD1" s="80"/>
+      <c r="AE1" s="80"/>
+      <c r="AF1" s="80"/>
+      <c r="AG1" s="80"/>
+      <c r="AH1" s="80"/>
+      <c r="AI1" s="80"/>
+      <c r="AJ1" s="80"/>
+      <c r="AK1" s="80"/>
+      <c r="AL1" s="80"/>
+      <c r="AM1" s="81"/>
+    </row>
+    <row r="2" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A2" s="82" t="s">
+        <v>181</v>
+      </c>
+      <c r="B2" s="58" t="s">
+        <v>169</v>
+      </c>
+      <c r="C2" s="58" t="s">
+        <v>182</v>
+      </c>
+      <c r="D2" s="58" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" s="58" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="58" t="s">
+        <v>130</v>
+      </c>
+      <c r="G2" s="58" t="s">
+        <v>131</v>
+      </c>
+      <c r="H2" s="75" t="s">
+        <v>171</v>
+      </c>
+      <c r="I2" s="58" t="s">
+        <v>183</v>
+      </c>
+      <c r="J2" s="76" t="s">
+        <v>173</v>
+      </c>
+      <c r="K2" s="76" t="s">
+        <v>161</v>
+      </c>
+      <c r="L2" s="77">
+        <v>0.39</v>
+      </c>
+      <c r="M2" s="58">
+        <v>1</v>
+      </c>
+      <c r="N2" s="83" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="83" t="s">
+        <v>184</v>
+      </c>
+      <c r="P2" s="58" t="s">
+        <v>159</v>
+      </c>
+      <c r="Q2" s="58" t="s">
+        <v>136</v>
+      </c>
+      <c r="R2" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="T2" s="79" t="s">
+        <v>175</v>
+      </c>
+      <c r="U2" s="79" t="s">
+        <v>150</v>
+      </c>
+      <c r="V2" s="84" t="s">
+        <v>185</v>
+      </c>
+      <c r="W2" s="84"/>
+      <c r="X2" s="84"/>
+      <c r="Y2" s="84"/>
+      <c r="Z2" s="84"/>
+      <c r="AA2" s="84"/>
+      <c r="AB2" s="84"/>
+      <c r="AC2" s="84"/>
+      <c r="AD2" s="84"/>
+      <c r="AE2" s="84"/>
+      <c r="AF2" s="84"/>
+      <c r="AG2" s="84"/>
+      <c r="AH2" s="84"/>
+      <c r="AI2" s="84"/>
+      <c r="AJ2" s="84"/>
+      <c r="AK2" s="84"/>
+      <c r="AL2" s="84"/>
+      <c r="AM2" s="85"/>
+    </row>
+    <row r="3" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A3" s="86" t="s">
+        <v>187</v>
+      </c>
+      <c r="B3" s="86" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" s="86" t="s">
+        <v>188</v>
+      </c>
+      <c r="D3" s="86" t="s">
+        <v>46</v>
+      </c>
+      <c r="E3" s="86" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="86" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" s="86" t="s">
+        <v>131</v>
+      </c>
+      <c r="H3" s="86" t="s">
+        <v>171</v>
+      </c>
+      <c r="I3" s="86" t="s">
+        <v>189</v>
+      </c>
+      <c r="J3" s="86" t="s">
+        <v>155</v>
+      </c>
+      <c r="K3" s="86" t="s">
+        <v>161</v>
+      </c>
+      <c r="L3" s="87">
+        <v>0.39</v>
+      </c>
+      <c r="M3" s="86">
+        <v>1</v>
+      </c>
+      <c r="N3" s="88" t="s">
+        <v>29</v>
+      </c>
+      <c r="O3" s="88" t="s">
+        <v>190</v>
+      </c>
+      <c r="P3" s="86" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q3" s="86" t="s">
+        <v>136</v>
+      </c>
+      <c r="R3" s="86" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="T3" s="79" t="s">
+        <v>191</v>
+      </c>
+      <c r="U3" s="79" t="s">
+        <v>150</v>
+      </c>
+      <c r="V3" s="89" t="s">
+        <v>192</v>
+      </c>
+      <c r="W3" s="89"/>
+      <c r="X3" s="89"/>
+      <c r="Y3" s="89"/>
+      <c r="Z3" s="89"/>
+      <c r="AA3" s="89"/>
+      <c r="AB3" s="89"/>
+      <c r="AC3" s="89"/>
+      <c r="AD3" s="89"/>
+      <c r="AE3" s="89"/>
+      <c r="AF3" s="89"/>
+      <c r="AG3" s="89"/>
+      <c r="AH3" s="89"/>
+      <c r="AI3" s="89"/>
+      <c r="AJ3" s="89"/>
+      <c r="AK3" s="89"/>
+      <c r="AL3" s="89"/>
+      <c r="AM3" s="89"/>
+    </row>
+    <row r="4" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A4" s="76" t="s">
+        <v>187</v>
+      </c>
+      <c r="B4" s="76" t="s">
+        <v>193</v>
+      </c>
+      <c r="C4" s="76" t="s">
+        <v>194</v>
+      </c>
+      <c r="D4" s="76" t="s">
+        <v>46</v>
+      </c>
+      <c r="E4" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="F4" s="76" t="s">
+        <v>130</v>
+      </c>
+      <c r="G4" s="76" t="s">
+        <v>131</v>
+      </c>
+      <c r="H4" s="75" t="s">
+        <v>171</v>
+      </c>
+      <c r="I4" s="76" t="s">
+        <v>189</v>
+      </c>
+      <c r="J4" s="76" t="s">
+        <v>155</v>
+      </c>
+      <c r="K4" s="76" t="s">
+        <v>161</v>
+      </c>
+      <c r="L4" s="77">
+        <v>0.39</v>
+      </c>
+      <c r="M4" s="76">
+        <v>2</v>
+      </c>
+      <c r="N4" s="90" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" s="90" t="s">
+        <v>195</v>
+      </c>
+      <c r="P4" s="76" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q4" s="76" t="s">
+        <v>136</v>
+      </c>
+      <c r="R4" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="T4" s="79" t="s">
+        <v>191</v>
+      </c>
+      <c r="U4" s="79" t="s">
+        <v>150</v>
+      </c>
+      <c r="V4" s="91"/>
+      <c r="W4" s="91"/>
+      <c r="X4" s="91"/>
+      <c r="Y4" s="91"/>
+      <c r="Z4" s="91"/>
+      <c r="AA4" s="91"/>
+      <c r="AB4" s="91"/>
+      <c r="AC4" s="91"/>
+      <c r="AD4" s="91"/>
+      <c r="AE4" s="91"/>
+      <c r="AF4" s="91"/>
+      <c r="AG4" s="91"/>
+      <c r="AH4" s="91"/>
+      <c r="AI4" s="91"/>
+      <c r="AJ4" s="91"/>
+      <c r="AK4" s="91"/>
+      <c r="AL4" s="91"/>
+      <c r="AM4" s="91"/>
+    </row>
+    <row r="5" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A5" s="76" t="s">
+        <v>187</v>
+      </c>
+      <c r="B5" s="76" t="s">
+        <v>193</v>
+      </c>
+      <c r="C5" s="76" t="s">
+        <v>194</v>
+      </c>
+      <c r="D5" s="76" t="s">
+        <v>46</v>
+      </c>
+      <c r="E5" s="76" t="s">
+        <v>196</v>
+      </c>
+      <c r="F5" s="76" t="s">
+        <v>130</v>
+      </c>
+      <c r="G5" s="76" t="s">
+        <v>131</v>
+      </c>
+      <c r="H5" s="75" t="s">
+        <v>171</v>
+      </c>
+      <c r="I5" s="76" t="s">
+        <v>189</v>
+      </c>
+      <c r="J5" s="76" t="s">
+        <v>155</v>
+      </c>
+      <c r="K5" s="76" t="s">
+        <v>161</v>
+      </c>
+      <c r="L5" s="77">
+        <v>0.39</v>
+      </c>
+      <c r="M5" s="76">
+        <v>3</v>
+      </c>
+      <c r="N5" s="90" t="s">
+        <v>29</v>
+      </c>
+      <c r="O5" s="90" t="s">
+        <v>197</v>
+      </c>
+      <c r="P5" s="76" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q5" s="76" t="s">
+        <v>136</v>
+      </c>
+      <c r="R5" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="S5" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="T5" s="79" t="s">
+        <v>191</v>
+      </c>
+      <c r="U5" s="79" t="s">
+        <v>150</v>
+      </c>
+      <c r="V5" s="91"/>
+      <c r="W5" s="91"/>
+      <c r="X5" s="91"/>
+      <c r="Y5" s="91"/>
+      <c r="Z5" s="91"/>
+      <c r="AA5" s="91"/>
+      <c r="AB5" s="91"/>
+      <c r="AC5" s="91"/>
+      <c r="AD5" s="91"/>
+      <c r="AE5" s="91"/>
+      <c r="AF5" s="91"/>
+      <c r="AG5" s="91"/>
+      <c r="AH5" s="91"/>
+      <c r="AI5" s="91"/>
+      <c r="AJ5" s="91"/>
+      <c r="AK5" s="91"/>
+      <c r="AL5" s="91"/>
+      <c r="AM5" s="91"/>
+    </row>
+    <row r="6" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A6" s="76" t="s">
+        <v>187</v>
+      </c>
+      <c r="B6" s="76" t="s">
+        <v>193</v>
+      </c>
+      <c r="C6" s="76" t="s">
+        <v>194</v>
+      </c>
+      <c r="D6" s="76" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="76" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="76" t="s">
+        <v>130</v>
+      </c>
+      <c r="G6" s="76" t="s">
+        <v>131</v>
+      </c>
+      <c r="H6" s="75" t="s">
+        <v>171</v>
+      </c>
+      <c r="I6" s="76" t="s">
+        <v>189</v>
+      </c>
+      <c r="J6" s="76" t="s">
+        <v>155</v>
+      </c>
+      <c r="K6" s="76" t="s">
+        <v>161</v>
+      </c>
+      <c r="L6" s="77">
+        <v>0.39</v>
+      </c>
+      <c r="M6" s="76">
+        <v>4</v>
+      </c>
+      <c r="N6" s="90" t="s">
+        <v>29</v>
+      </c>
+      <c r="O6" s="90" t="s">
+        <v>198</v>
+      </c>
+      <c r="P6" s="76" t="s">
+        <v>186</v>
+      </c>
+      <c r="Q6" s="76" t="s">
+        <v>136</v>
+      </c>
+      <c r="R6" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="S6" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="T6" s="79" t="s">
+        <v>191</v>
+      </c>
+      <c r="U6" s="79" t="s">
+        <v>150</v>
+      </c>
+      <c r="V6" s="91"/>
+      <c r="W6" s="91"/>
+      <c r="X6" s="91"/>
+      <c r="Y6" s="91"/>
+      <c r="Z6" s="91"/>
+      <c r="AA6" s="91"/>
+      <c r="AB6" s="91"/>
+      <c r="AC6" s="91"/>
+      <c r="AD6" s="91"/>
+      <c r="AE6" s="91"/>
+      <c r="AF6" s="91"/>
+      <c r="AG6" s="91"/>
+      <c r="AH6" s="91"/>
+      <c r="AI6" s="91"/>
+      <c r="AJ6" s="91"/>
+      <c r="AK6" s="91"/>
+      <c r="AL6" s="91"/>
+      <c r="AM6" s="91"/>
+    </row>
+    <row r="7" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A7" s="82" t="s">
+        <v>218</v>
+      </c>
+      <c r="B7" s="58" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" s="58" t="s">
+        <v>219</v>
+      </c>
+      <c r="D7" s="92" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="76" t="s">
+        <v>220</v>
+      </c>
+      <c r="F7" s="92" t="s">
+        <v>130</v>
+      </c>
+      <c r="G7" s="58" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="75" t="s">
+        <v>171</v>
+      </c>
+      <c r="I7" s="58" t="s">
+        <v>221</v>
+      </c>
+      <c r="J7" s="76" t="s">
+        <v>222</v>
+      </c>
+      <c r="K7" s="76" t="s">
+        <v>161</v>
+      </c>
+      <c r="L7" s="77">
+        <v>0.39</v>
+      </c>
+      <c r="M7" s="58">
+        <v>1</v>
+      </c>
+      <c r="N7" s="83" t="s">
+        <v>29</v>
+      </c>
+      <c r="O7" s="83" t="s">
+        <v>223</v>
+      </c>
+      <c r="P7" s="58" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q7" s="58" t="s">
+        <v>136</v>
+      </c>
+      <c r="R7" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="S7" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="T7" s="79" t="s">
+        <v>224</v>
+      </c>
+      <c r="U7" s="79" t="s">
+        <v>150</v>
+      </c>
+      <c r="V7" s="84" t="s">
+        <v>225</v>
+      </c>
+      <c r="W7" s="84"/>
+      <c r="X7" s="84"/>
+      <c r="Y7" s="84"/>
+      <c r="Z7" s="84"/>
+      <c r="AA7" s="84"/>
+      <c r="AB7" s="84"/>
+      <c r="AC7" s="84"/>
+      <c r="AD7" s="84"/>
+      <c r="AE7" s="84"/>
+      <c r="AF7" s="84"/>
+      <c r="AG7" s="84"/>
+      <c r="AH7" s="84"/>
+      <c r="AI7" s="84"/>
+      <c r="AJ7" s="84"/>
+      <c r="AK7" s="84"/>
+      <c r="AL7" s="84"/>
+      <c r="AM7" s="85"/>
+    </row>
+    <row r="8" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A8" s="76" t="s">
+        <v>230</v>
+      </c>
+      <c r="B8" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="C8" s="75" t="s">
+        <v>219</v>
+      </c>
+      <c r="D8" s="92" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="76" t="s">
+        <v>220</v>
+      </c>
+      <c r="F8" s="75" t="s">
+        <v>130</v>
+      </c>
+      <c r="G8" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" s="75" t="s">
+        <v>171</v>
+      </c>
+      <c r="I8" s="76" t="s">
+        <v>231</v>
+      </c>
+      <c r="J8" s="76" t="s">
+        <v>222</v>
+      </c>
+      <c r="K8" s="76" t="s">
+        <v>161</v>
+      </c>
+      <c r="L8" s="77">
+        <v>0.39</v>
+      </c>
+      <c r="M8" s="76">
+        <v>1</v>
+      </c>
+      <c r="N8" s="90" t="s">
+        <v>29</v>
+      </c>
+      <c r="O8" s="90" t="s">
+        <v>232</v>
+      </c>
+      <c r="P8" s="76" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q8" s="76" t="s">
+        <v>136</v>
+      </c>
+      <c r="R8" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="S8" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="T8" s="79" t="s">
+        <v>224</v>
+      </c>
+      <c r="U8" s="79" t="s">
+        <v>150</v>
+      </c>
+      <c r="V8" s="91" t="s">
+        <v>233</v>
+      </c>
+      <c r="W8" s="91"/>
+      <c r="X8" s="91"/>
+      <c r="Y8" s="91"/>
+      <c r="Z8" s="91"/>
+      <c r="AA8" s="91"/>
+      <c r="AB8" s="91"/>
+      <c r="AC8" s="91"/>
+      <c r="AD8" s="91"/>
+      <c r="AE8" s="91"/>
+      <c r="AF8" s="91"/>
+      <c r="AG8" s="91"/>
+      <c r="AH8" s="91"/>
+      <c r="AI8" s="91"/>
+      <c r="AJ8" s="91"/>
+      <c r="AK8" s="91"/>
+      <c r="AL8" s="91"/>
+      <c r="AM8" s="91"/>
+    </row>
+    <row r="9" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A9" s="76" t="s">
+        <v>234</v>
+      </c>
+      <c r="B9" s="92" t="s">
+        <v>169</v>
+      </c>
+      <c r="C9" s="92" t="s">
+        <v>219</v>
+      </c>
+      <c r="D9" s="92" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9" s="76" t="s">
+        <v>220</v>
+      </c>
+      <c r="F9" s="92" t="s">
+        <v>130</v>
+      </c>
+      <c r="G9" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" s="75" t="s">
+        <v>171</v>
+      </c>
+      <c r="I9" s="76" t="s">
+        <v>231</v>
+      </c>
+      <c r="J9" s="76" t="s">
+        <v>222</v>
+      </c>
+      <c r="K9" s="76" t="s">
+        <v>161</v>
+      </c>
+      <c r="L9" s="77">
+        <v>0.39</v>
+      </c>
+      <c r="M9" s="76">
+        <v>2</v>
+      </c>
+      <c r="N9" s="90" t="s">
+        <v>29</v>
+      </c>
+      <c r="O9" s="90" t="s">
+        <v>235</v>
+      </c>
+      <c r="P9" s="76" t="s">
+        <v>217</v>
+      </c>
+      <c r="Q9" s="76" t="s">
+        <v>136</v>
+      </c>
+      <c r="R9" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="S9" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="T9" s="79" t="s">
+        <v>224</v>
+      </c>
+      <c r="U9" s="79" t="s">
+        <v>150</v>
+      </c>
+      <c r="V9" s="91" t="s">
+        <v>236</v>
+      </c>
+      <c r="W9" s="91"/>
+      <c r="X9" s="91"/>
+      <c r="Y9" s="91"/>
+      <c r="Z9" s="91"/>
+      <c r="AA9" s="91"/>
+      <c r="AB9" s="91"/>
+      <c r="AC9" s="91"/>
+      <c r="AD9" s="91"/>
+      <c r="AE9" s="91"/>
+      <c r="AF9" s="91"/>
+      <c r="AG9" s="91"/>
+      <c r="AH9" s="91"/>
+      <c r="AI9" s="91"/>
+      <c r="AJ9" s="91"/>
+      <c r="AK9" s="91"/>
+      <c r="AL9" s="91"/>
+      <c r="AM9" s="91"/>
+    </row>
+    <row r="10" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A10" s="76" t="s">
+        <v>242</v>
+      </c>
+      <c r="B10" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="C10" s="76" t="s">
+        <v>243</v>
+      </c>
+      <c r="D10" s="76" t="s">
+        <v>202</v>
+      </c>
+      <c r="E10" s="76" t="s">
+        <v>220</v>
+      </c>
+      <c r="F10" s="76" t="s">
+        <v>130</v>
+      </c>
+      <c r="G10" s="76" t="s">
+        <v>244</v>
+      </c>
+      <c r="H10" s="75" t="s">
+        <v>171</v>
+      </c>
+      <c r="I10" s="76" t="s">
+        <v>245</v>
+      </c>
+      <c r="J10" s="76" t="s">
+        <v>222</v>
+      </c>
+      <c r="K10" s="76" t="s">
+        <v>161</v>
+      </c>
+      <c r="L10" s="77">
+        <v>0.39</v>
+      </c>
+      <c r="M10" s="76">
+        <v>1</v>
+      </c>
+      <c r="N10" s="90" t="s">
+        <v>29</v>
+      </c>
+      <c r="O10" s="90" t="s">
+        <v>246</v>
+      </c>
+      <c r="P10" s="76" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q10" s="76" t="s">
+        <v>136</v>
+      </c>
+      <c r="R10" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="S10" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="T10" s="79" t="s">
+        <v>224</v>
+      </c>
+      <c r="U10" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="V10" s="91"/>
+      <c r="W10" s="91"/>
+      <c r="X10" s="91"/>
+      <c r="Y10" s="91"/>
+      <c r="Z10" s="91"/>
+      <c r="AA10" s="91"/>
+      <c r="AB10" s="91"/>
+      <c r="AC10" s="91"/>
+      <c r="AD10" s="91"/>
+      <c r="AE10" s="91"/>
+      <c r="AF10" s="91"/>
+      <c r="AG10" s="91"/>
+      <c r="AH10" s="91"/>
+      <c r="AI10" s="91"/>
+      <c r="AJ10" s="91"/>
+      <c r="AK10" s="91"/>
+      <c r="AL10" s="91"/>
+      <c r="AM10" s="91"/>
+    </row>
+    <row r="11" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A11" s="76" t="s">
+        <v>248</v>
+      </c>
+      <c r="B11" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="C11" s="76" t="s">
+        <v>243</v>
+      </c>
+      <c r="D11" s="76" t="s">
+        <v>202</v>
+      </c>
+      <c r="E11" s="76" t="s">
+        <v>220</v>
+      </c>
+      <c r="F11" s="76" t="s">
+        <v>130</v>
+      </c>
+      <c r="G11" s="76" t="s">
+        <v>244</v>
+      </c>
+      <c r="H11" s="75" t="s">
+        <v>171</v>
+      </c>
+      <c r="I11" s="76" t="s">
+        <v>245</v>
+      </c>
+      <c r="J11" s="76" t="s">
+        <v>222</v>
+      </c>
+      <c r="K11" s="76" t="s">
+        <v>161</v>
+      </c>
+      <c r="L11" s="77">
+        <v>0.39</v>
+      </c>
+      <c r="M11" s="76">
+        <v>1</v>
+      </c>
+      <c r="N11" s="90" t="s">
+        <v>29</v>
+      </c>
+      <c r="O11" s="90" t="s">
+        <v>249</v>
+      </c>
+      <c r="P11" s="76" t="s">
+        <v>241</v>
+      </c>
+      <c r="Q11" s="76" t="s">
+        <v>136</v>
+      </c>
+      <c r="R11" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="S11" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="T11" s="79" t="s">
+        <v>224</v>
+      </c>
+      <c r="U11" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="V11" s="91"/>
+      <c r="W11" s="91"/>
+      <c r="X11" s="91"/>
+      <c r="Y11" s="91"/>
+      <c r="Z11" s="91"/>
+      <c r="AA11" s="91"/>
+      <c r="AB11" s="91"/>
+      <c r="AC11" s="91"/>
+      <c r="AD11" s="91"/>
+      <c r="AE11" s="91"/>
+      <c r="AF11" s="91"/>
+      <c r="AG11" s="91"/>
+      <c r="AH11" s="91"/>
+      <c r="AI11" s="91"/>
+      <c r="AJ11" s="91"/>
+      <c r="AK11" s="91"/>
+      <c r="AL11" s="91"/>
+      <c r="AM11" s="91"/>
+    </row>
+    <row r="12" spans="1:39" ht="15.75" customHeight="1">
+      <c r="A12" s="76" t="s">
+        <v>258</v>
+      </c>
+      <c r="B12" s="76" t="s">
+        <v>169</v>
+      </c>
+      <c r="C12" s="76" t="s">
+        <v>259</v>
+      </c>
+      <c r="D12" s="76" t="s">
+        <v>202</v>
+      </c>
+      <c r="E12" s="76" t="s">
+        <v>220</v>
+      </c>
+      <c r="F12" s="76" t="s">
+        <v>130</v>
+      </c>
+      <c r="G12" s="76" t="s">
+        <v>254</v>
+      </c>
+      <c r="H12" s="75" t="s">
+        <v>171</v>
+      </c>
+      <c r="I12" s="76" t="s">
+        <v>255</v>
+      </c>
+      <c r="J12" s="76" t="s">
+        <v>222</v>
+      </c>
+      <c r="K12" s="76" t="s">
+        <v>161</v>
+      </c>
+      <c r="L12" s="77">
+        <v>0.39</v>
+      </c>
+      <c r="M12" s="76">
+        <v>1</v>
+      </c>
+      <c r="N12" s="90" t="s">
+        <v>29</v>
+      </c>
+      <c r="O12" s="90" t="s">
+        <v>260</v>
+      </c>
+      <c r="P12" s="76" t="s">
+        <v>250</v>
+      </c>
+      <c r="Q12" s="76" t="s">
+        <v>136</v>
+      </c>
+      <c r="R12" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="S12" s="58" t="s">
+        <v>125</v>
+      </c>
+      <c r="T12" s="79" t="s">
+        <v>224</v>
+      </c>
+      <c r="U12" s="79" t="s">
+        <v>150</v>
+      </c>
+      <c r="V12" s="91"/>
+      <c r="W12" s="91"/>
+      <c r="X12" s="91"/>
+      <c r="Y12" s="91"/>
+      <c r="Z12" s="91"/>
+      <c r="AA12" s="91"/>
+      <c r="AB12" s="91"/>
+      <c r="AC12" s="91"/>
+      <c r="AD12" s="91"/>
+      <c r="AE12" s="91"/>
+      <c r="AF12" s="91"/>
+      <c r="AG12" s="91"/>
+      <c r="AH12" s="91"/>
+      <c r="AI12" s="91"/>
+      <c r="AJ12" s="91"/>
+      <c r="AK12" s="91"/>
+      <c r="AL12" s="91"/>
+      <c r="AM12" s="91"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:K26"/>
   <sheetViews>
@@ -36164,7 +37191,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -36354,7 +37381,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -37389,6 +38416,296 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3377A13-D0DE-4E13-9840-63DCC917F2F0}">
+  <dimension ref="A1:W4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.3"/>
+  <cols>
+    <col min="1" max="1" width="29.38671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.609375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.77734375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.0546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="4.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="47.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.38671875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="125.27734375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="46.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.71875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" ht="15.75" customHeight="1">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>303</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>664</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="3"/>
+    </row>
+    <row r="2" spans="1:23" s="145" customFormat="1">
+      <c r="A2" s="153" t="s">
+        <v>801</v>
+      </c>
+      <c r="B2" s="140" t="s">
+        <v>802</v>
+      </c>
+      <c r="C2" s="140" t="s">
+        <v>339</v>
+      </c>
+      <c r="D2" s="140" t="s">
+        <v>796</v>
+      </c>
+      <c r="E2" s="140" t="s">
+        <v>220</v>
+      </c>
+      <c r="F2" s="140" t="s">
+        <v>280</v>
+      </c>
+      <c r="G2" s="140" t="s">
+        <v>797</v>
+      </c>
+      <c r="H2" s="140" t="s">
+        <v>171</v>
+      </c>
+      <c r="I2" s="140" t="s">
+        <v>798</v>
+      </c>
+      <c r="J2" s="153" t="s">
+        <v>275</v>
+      </c>
+      <c r="K2" s="153" t="s">
+        <v>584</v>
+      </c>
+      <c r="L2" s="184">
+        <v>0.38</v>
+      </c>
+      <c r="M2" s="140"/>
+      <c r="N2" s="153" t="s">
+        <v>29</v>
+      </c>
+      <c r="O2" s="140" t="s">
+        <v>803</v>
+      </c>
+      <c r="P2" s="140" t="s">
+        <v>777</v>
+      </c>
+      <c r="Q2" s="140" t="s">
+        <v>136</v>
+      </c>
+      <c r="R2" s="140" t="s">
+        <v>33</v>
+      </c>
+      <c r="S2" s="140" t="s">
+        <v>804</v>
+      </c>
+      <c r="T2" s="144" t="s">
+        <v>224</v>
+      </c>
+      <c r="U2" s="140"/>
+    </row>
+    <row r="3" spans="1:23" s="145" customFormat="1">
+      <c r="A3" s="283" t="s">
+        <v>853</v>
+      </c>
+      <c r="B3" s="284" t="s">
+        <v>842</v>
+      </c>
+      <c r="C3" s="284" t="s">
+        <v>339</v>
+      </c>
+      <c r="D3" s="284" t="s">
+        <v>796</v>
+      </c>
+      <c r="E3" s="284" t="s">
+        <v>220</v>
+      </c>
+      <c r="F3" s="288" t="s">
+        <v>280</v>
+      </c>
+      <c r="G3" s="140" t="s">
+        <v>843</v>
+      </c>
+      <c r="H3" s="140" t="s">
+        <v>848</v>
+      </c>
+      <c r="I3" s="284" t="s">
+        <v>798</v>
+      </c>
+      <c r="J3" s="283" t="s">
+        <v>275</v>
+      </c>
+      <c r="K3" s="283" t="s">
+        <v>584</v>
+      </c>
+      <c r="L3" s="285">
+        <v>0.41</v>
+      </c>
+      <c r="M3" s="140"/>
+      <c r="N3" s="153" t="s">
+        <v>424</v>
+      </c>
+      <c r="O3" s="140" t="s">
+        <v>850</v>
+      </c>
+      <c r="P3" s="140" t="s">
+        <v>840</v>
+      </c>
+      <c r="Q3" s="284" t="s">
+        <v>136</v>
+      </c>
+      <c r="R3" s="284" t="s">
+        <v>33</v>
+      </c>
+      <c r="S3" s="284" t="s">
+        <v>845</v>
+      </c>
+      <c r="T3" s="286" t="s">
+        <v>819</v>
+      </c>
+      <c r="U3" s="140" t="s">
+        <v>851</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" s="106" customFormat="1">
+      <c r="A4" s="287" t="s">
+        <v>838</v>
+      </c>
+      <c r="B4" s="288" t="s">
+        <v>802</v>
+      </c>
+      <c r="C4" s="288" t="s">
+        <v>339</v>
+      </c>
+      <c r="D4" s="288" t="s">
+        <v>796</v>
+      </c>
+      <c r="E4" s="288" t="s">
+        <v>220</v>
+      </c>
+      <c r="F4" s="288" t="s">
+        <v>280</v>
+      </c>
+      <c r="G4" s="100" t="s">
+        <v>835</v>
+      </c>
+      <c r="H4" s="140" t="s">
+        <v>849</v>
+      </c>
+      <c r="I4" s="288" t="s">
+        <v>798</v>
+      </c>
+      <c r="J4" s="287" t="s">
+        <v>275</v>
+      </c>
+      <c r="K4" s="287" t="s">
+        <v>584</v>
+      </c>
+      <c r="L4" s="289">
+        <v>0.41</v>
+      </c>
+      <c r="M4" s="100"/>
+      <c r="N4" s="152" t="s">
+        <v>29</v>
+      </c>
+      <c r="O4" s="100" t="s">
+        <v>836</v>
+      </c>
+      <c r="P4" s="100" t="s">
+        <v>831</v>
+      </c>
+      <c r="Q4" s="288" t="s">
+        <v>136</v>
+      </c>
+      <c r="R4" s="288" t="s">
+        <v>33</v>
+      </c>
+      <c r="S4" s="288" t="s">
+        <v>804</v>
+      </c>
+      <c r="T4" s="290" t="s">
+        <v>833</v>
+      </c>
+      <c r="U4" s="100"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40195B12-F772-4F2E-B8F1-2C039FF19123}">
   <dimension ref="A1:W11"/>
   <sheetViews>
@@ -38074,7 +39391,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C55639-70D8-4772-A7C7-0A253515BD91}">
   <dimension ref="A1:AM17"/>
   <sheetViews>
@@ -39145,7 +40462,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1E35F51-89D7-4D4E-9423-E5EB02F06689}">
   <dimension ref="A1:W14"/>
   <sheetViews>
@@ -39868,7 +41185,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3136F1D-A2E4-4CE7-8F50-95420C9B4A05}">
   <dimension ref="A2:X14"/>
   <sheetViews>
@@ -40595,7 +41912,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C6FF399-B898-9B4D-9BEA-88752D6153C6}">
   <dimension ref="A1:AM16"/>
   <sheetViews>
@@ -41539,7 +42856,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AM14"/>
   <sheetViews>
@@ -42470,7 +43787,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -43205,1034 +44522,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:AM12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
-  <cols>
-    <col min="15" max="15" width="87.6640625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="30.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A1" s="74" t="s">
-        <v>168</v>
-      </c>
-      <c r="B1" s="75" t="s">
-        <v>169</v>
-      </c>
-      <c r="C1" s="75" t="s">
-        <v>170</v>
-      </c>
-      <c r="D1" s="75" t="s">
-        <v>46</v>
-      </c>
-      <c r="E1" s="75" t="s">
-        <v>22</v>
-      </c>
-      <c r="F1" s="75" t="s">
-        <v>130</v>
-      </c>
-      <c r="G1" s="75" t="s">
-        <v>131</v>
-      </c>
-      <c r="H1" s="75" t="s">
-        <v>171</v>
-      </c>
-      <c r="I1" s="75" t="s">
-        <v>172</v>
-      </c>
-      <c r="J1" s="76" t="s">
-        <v>173</v>
-      </c>
-      <c r="K1" s="76" t="s">
-        <v>161</v>
-      </c>
-      <c r="L1" s="77">
-        <v>0.39</v>
-      </c>
-      <c r="M1" s="75">
-        <v>1</v>
-      </c>
-      <c r="N1" s="78" t="s">
-        <v>29</v>
-      </c>
-      <c r="O1" s="78" t="s">
-        <v>174</v>
-      </c>
-      <c r="P1" s="75" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q1" s="75" t="s">
-        <v>136</v>
-      </c>
-      <c r="R1" s="75" t="s">
-        <v>33</v>
-      </c>
-      <c r="S1" s="58" t="s">
-        <v>125</v>
-      </c>
-      <c r="T1" s="79" t="s">
-        <v>175</v>
-      </c>
-      <c r="U1" s="79" t="s">
-        <v>150</v>
-      </c>
-      <c r="V1" s="80" t="s">
-        <v>176</v>
-      </c>
-      <c r="W1" s="80"/>
-      <c r="X1" s="80"/>
-      <c r="Y1" s="80"/>
-      <c r="Z1" s="80"/>
-      <c r="AA1" s="80"/>
-      <c r="AB1" s="80"/>
-      <c r="AC1" s="80"/>
-      <c r="AD1" s="80"/>
-      <c r="AE1" s="80"/>
-      <c r="AF1" s="80"/>
-      <c r="AG1" s="80"/>
-      <c r="AH1" s="80"/>
-      <c r="AI1" s="80"/>
-      <c r="AJ1" s="80"/>
-      <c r="AK1" s="80"/>
-      <c r="AL1" s="80"/>
-      <c r="AM1" s="81"/>
-    </row>
-    <row r="2" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A2" s="82" t="s">
-        <v>181</v>
-      </c>
-      <c r="B2" s="58" t="s">
-        <v>169</v>
-      </c>
-      <c r="C2" s="58" t="s">
-        <v>182</v>
-      </c>
-      <c r="D2" s="58" t="s">
-        <v>38</v>
-      </c>
-      <c r="E2" s="58" t="s">
-        <v>22</v>
-      </c>
-      <c r="F2" s="58" t="s">
-        <v>130</v>
-      </c>
-      <c r="G2" s="58" t="s">
-        <v>131</v>
-      </c>
-      <c r="H2" s="75" t="s">
-        <v>171</v>
-      </c>
-      <c r="I2" s="58" t="s">
-        <v>183</v>
-      </c>
-      <c r="J2" s="76" t="s">
-        <v>173</v>
-      </c>
-      <c r="K2" s="76" t="s">
-        <v>161</v>
-      </c>
-      <c r="L2" s="77">
-        <v>0.39</v>
-      </c>
-      <c r="M2" s="58">
-        <v>1</v>
-      </c>
-      <c r="N2" s="83" t="s">
-        <v>29</v>
-      </c>
-      <c r="O2" s="83" t="s">
-        <v>184</v>
-      </c>
-      <c r="P2" s="58" t="s">
-        <v>159</v>
-      </c>
-      <c r="Q2" s="58" t="s">
-        <v>136</v>
-      </c>
-      <c r="R2" s="58" t="s">
-        <v>33</v>
-      </c>
-      <c r="S2" s="58" t="s">
-        <v>125</v>
-      </c>
-      <c r="T2" s="79" t="s">
-        <v>175</v>
-      </c>
-      <c r="U2" s="79" t="s">
-        <v>150</v>
-      </c>
-      <c r="V2" s="84" t="s">
-        <v>185</v>
-      </c>
-      <c r="W2" s="84"/>
-      <c r="X2" s="84"/>
-      <c r="Y2" s="84"/>
-      <c r="Z2" s="84"/>
-      <c r="AA2" s="84"/>
-      <c r="AB2" s="84"/>
-      <c r="AC2" s="84"/>
-      <c r="AD2" s="84"/>
-      <c r="AE2" s="84"/>
-      <c r="AF2" s="84"/>
-      <c r="AG2" s="84"/>
-      <c r="AH2" s="84"/>
-      <c r="AI2" s="84"/>
-      <c r="AJ2" s="84"/>
-      <c r="AK2" s="84"/>
-      <c r="AL2" s="84"/>
-      <c r="AM2" s="85"/>
-    </row>
-    <row r="3" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A3" s="86" t="s">
-        <v>187</v>
-      </c>
-      <c r="B3" s="86" t="s">
-        <v>177</v>
-      </c>
-      <c r="C3" s="86" t="s">
-        <v>188</v>
-      </c>
-      <c r="D3" s="86" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="86" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" s="86" t="s">
-        <v>130</v>
-      </c>
-      <c r="G3" s="86" t="s">
-        <v>131</v>
-      </c>
-      <c r="H3" s="86" t="s">
-        <v>171</v>
-      </c>
-      <c r="I3" s="86" t="s">
-        <v>189</v>
-      </c>
-      <c r="J3" s="86" t="s">
-        <v>155</v>
-      </c>
-      <c r="K3" s="86" t="s">
-        <v>161</v>
-      </c>
-      <c r="L3" s="87">
-        <v>0.39</v>
-      </c>
-      <c r="M3" s="86">
-        <v>1</v>
-      </c>
-      <c r="N3" s="88" t="s">
-        <v>29</v>
-      </c>
-      <c r="O3" s="88" t="s">
-        <v>190</v>
-      </c>
-      <c r="P3" s="86" t="s">
-        <v>186</v>
-      </c>
-      <c r="Q3" s="86" t="s">
-        <v>136</v>
-      </c>
-      <c r="R3" s="86" t="s">
-        <v>33</v>
-      </c>
-      <c r="S3" s="44" t="s">
-        <v>125</v>
-      </c>
-      <c r="T3" s="79" t="s">
-        <v>191</v>
-      </c>
-      <c r="U3" s="79" t="s">
-        <v>150</v>
-      </c>
-      <c r="V3" s="89" t="s">
-        <v>192</v>
-      </c>
-      <c r="W3" s="89"/>
-      <c r="X3" s="89"/>
-      <c r="Y3" s="89"/>
-      <c r="Z3" s="89"/>
-      <c r="AA3" s="89"/>
-      <c r="AB3" s="89"/>
-      <c r="AC3" s="89"/>
-      <c r="AD3" s="89"/>
-      <c r="AE3" s="89"/>
-      <c r="AF3" s="89"/>
-      <c r="AG3" s="89"/>
-      <c r="AH3" s="89"/>
-      <c r="AI3" s="89"/>
-      <c r="AJ3" s="89"/>
-      <c r="AK3" s="89"/>
-      <c r="AL3" s="89"/>
-      <c r="AM3" s="89"/>
-    </row>
-    <row r="4" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A4" s="76" t="s">
-        <v>187</v>
-      </c>
-      <c r="B4" s="76" t="s">
-        <v>193</v>
-      </c>
-      <c r="C4" s="76" t="s">
-        <v>194</v>
-      </c>
-      <c r="D4" s="76" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="76" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="76" t="s">
-        <v>130</v>
-      </c>
-      <c r="G4" s="76" t="s">
-        <v>131</v>
-      </c>
-      <c r="H4" s="75" t="s">
-        <v>171</v>
-      </c>
-      <c r="I4" s="76" t="s">
-        <v>189</v>
-      </c>
-      <c r="J4" s="76" t="s">
-        <v>155</v>
-      </c>
-      <c r="K4" s="76" t="s">
-        <v>161</v>
-      </c>
-      <c r="L4" s="77">
-        <v>0.39</v>
-      </c>
-      <c r="M4" s="76">
-        <v>2</v>
-      </c>
-      <c r="N4" s="90" t="s">
-        <v>29</v>
-      </c>
-      <c r="O4" s="90" t="s">
-        <v>195</v>
-      </c>
-      <c r="P4" s="76" t="s">
-        <v>186</v>
-      </c>
-      <c r="Q4" s="76" t="s">
-        <v>136</v>
-      </c>
-      <c r="R4" s="76" t="s">
-        <v>33</v>
-      </c>
-      <c r="S4" s="58" t="s">
-        <v>125</v>
-      </c>
-      <c r="T4" s="79" t="s">
-        <v>191</v>
-      </c>
-      <c r="U4" s="79" t="s">
-        <v>150</v>
-      </c>
-      <c r="V4" s="91"/>
-      <c r="W4" s="91"/>
-      <c r="X4" s="91"/>
-      <c r="Y4" s="91"/>
-      <c r="Z4" s="91"/>
-      <c r="AA4" s="91"/>
-      <c r="AB4" s="91"/>
-      <c r="AC4" s="91"/>
-      <c r="AD4" s="91"/>
-      <c r="AE4" s="91"/>
-      <c r="AF4" s="91"/>
-      <c r="AG4" s="91"/>
-      <c r="AH4" s="91"/>
-      <c r="AI4" s="91"/>
-      <c r="AJ4" s="91"/>
-      <c r="AK4" s="91"/>
-      <c r="AL4" s="91"/>
-      <c r="AM4" s="91"/>
-    </row>
-    <row r="5" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A5" s="76" t="s">
-        <v>187</v>
-      </c>
-      <c r="B5" s="76" t="s">
-        <v>193</v>
-      </c>
-      <c r="C5" s="76" t="s">
-        <v>194</v>
-      </c>
-      <c r="D5" s="76" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="76" t="s">
-        <v>196</v>
-      </c>
-      <c r="F5" s="76" t="s">
-        <v>130</v>
-      </c>
-      <c r="G5" s="76" t="s">
-        <v>131</v>
-      </c>
-      <c r="H5" s="75" t="s">
-        <v>171</v>
-      </c>
-      <c r="I5" s="76" t="s">
-        <v>189</v>
-      </c>
-      <c r="J5" s="76" t="s">
-        <v>155</v>
-      </c>
-      <c r="K5" s="76" t="s">
-        <v>161</v>
-      </c>
-      <c r="L5" s="77">
-        <v>0.39</v>
-      </c>
-      <c r="M5" s="76">
-        <v>3</v>
-      </c>
-      <c r="N5" s="90" t="s">
-        <v>29</v>
-      </c>
-      <c r="O5" s="90" t="s">
-        <v>197</v>
-      </c>
-      <c r="P5" s="76" t="s">
-        <v>186</v>
-      </c>
-      <c r="Q5" s="76" t="s">
-        <v>136</v>
-      </c>
-      <c r="R5" s="76" t="s">
-        <v>33</v>
-      </c>
-      <c r="S5" s="58" t="s">
-        <v>125</v>
-      </c>
-      <c r="T5" s="79" t="s">
-        <v>191</v>
-      </c>
-      <c r="U5" s="79" t="s">
-        <v>150</v>
-      </c>
-      <c r="V5" s="91"/>
-      <c r="W5" s="91"/>
-      <c r="X5" s="91"/>
-      <c r="Y5" s="91"/>
-      <c r="Z5" s="91"/>
-      <c r="AA5" s="91"/>
-      <c r="AB5" s="91"/>
-      <c r="AC5" s="91"/>
-      <c r="AD5" s="91"/>
-      <c r="AE5" s="91"/>
-      <c r="AF5" s="91"/>
-      <c r="AG5" s="91"/>
-      <c r="AH5" s="91"/>
-      <c r="AI5" s="91"/>
-      <c r="AJ5" s="91"/>
-      <c r="AK5" s="91"/>
-      <c r="AL5" s="91"/>
-      <c r="AM5" s="91"/>
-    </row>
-    <row r="6" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A6" s="76" t="s">
-        <v>187</v>
-      </c>
-      <c r="B6" s="76" t="s">
-        <v>193</v>
-      </c>
-      <c r="C6" s="76" t="s">
-        <v>194</v>
-      </c>
-      <c r="D6" s="76" t="s">
-        <v>46</v>
-      </c>
-      <c r="E6" s="76" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="76" t="s">
-        <v>130</v>
-      </c>
-      <c r="G6" s="76" t="s">
-        <v>131</v>
-      </c>
-      <c r="H6" s="75" t="s">
-        <v>171</v>
-      </c>
-      <c r="I6" s="76" t="s">
-        <v>189</v>
-      </c>
-      <c r="J6" s="76" t="s">
-        <v>155</v>
-      </c>
-      <c r="K6" s="76" t="s">
-        <v>161</v>
-      </c>
-      <c r="L6" s="77">
-        <v>0.39</v>
-      </c>
-      <c r="M6" s="76">
-        <v>4</v>
-      </c>
-      <c r="N6" s="90" t="s">
-        <v>29</v>
-      </c>
-      <c r="O6" s="90" t="s">
-        <v>198</v>
-      </c>
-      <c r="P6" s="76" t="s">
-        <v>186</v>
-      </c>
-      <c r="Q6" s="76" t="s">
-        <v>136</v>
-      </c>
-      <c r="R6" s="76" t="s">
-        <v>33</v>
-      </c>
-      <c r="S6" s="58" t="s">
-        <v>125</v>
-      </c>
-      <c r="T6" s="79" t="s">
-        <v>191</v>
-      </c>
-      <c r="U6" s="79" t="s">
-        <v>150</v>
-      </c>
-      <c r="V6" s="91"/>
-      <c r="W6" s="91"/>
-      <c r="X6" s="91"/>
-      <c r="Y6" s="91"/>
-      <c r="Z6" s="91"/>
-      <c r="AA6" s="91"/>
-      <c r="AB6" s="91"/>
-      <c r="AC6" s="91"/>
-      <c r="AD6" s="91"/>
-      <c r="AE6" s="91"/>
-      <c r="AF6" s="91"/>
-      <c r="AG6" s="91"/>
-      <c r="AH6" s="91"/>
-      <c r="AI6" s="91"/>
-      <c r="AJ6" s="91"/>
-      <c r="AK6" s="91"/>
-      <c r="AL6" s="91"/>
-      <c r="AM6" s="91"/>
-    </row>
-    <row r="7" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A7" s="82" t="s">
-        <v>218</v>
-      </c>
-      <c r="B7" s="58" t="s">
-        <v>169</v>
-      </c>
-      <c r="C7" s="58" t="s">
-        <v>219</v>
-      </c>
-      <c r="D7" s="92" t="s">
-        <v>38</v>
-      </c>
-      <c r="E7" s="76" t="s">
-        <v>220</v>
-      </c>
-      <c r="F7" s="92" t="s">
-        <v>130</v>
-      </c>
-      <c r="G7" s="58" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="75" t="s">
-        <v>171</v>
-      </c>
-      <c r="I7" s="58" t="s">
-        <v>221</v>
-      </c>
-      <c r="J7" s="76" t="s">
-        <v>222</v>
-      </c>
-      <c r="K7" s="76" t="s">
-        <v>161</v>
-      </c>
-      <c r="L7" s="77">
-        <v>0.39</v>
-      </c>
-      <c r="M7" s="58">
-        <v>1</v>
-      </c>
-      <c r="N7" s="83" t="s">
-        <v>29</v>
-      </c>
-      <c r="O7" s="83" t="s">
-        <v>223</v>
-      </c>
-      <c r="P7" s="58" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q7" s="58" t="s">
-        <v>136</v>
-      </c>
-      <c r="R7" s="58" t="s">
-        <v>33</v>
-      </c>
-      <c r="S7" s="58" t="s">
-        <v>125</v>
-      </c>
-      <c r="T7" s="79" t="s">
-        <v>224</v>
-      </c>
-      <c r="U7" s="79" t="s">
-        <v>150</v>
-      </c>
-      <c r="V7" s="84" t="s">
-        <v>225</v>
-      </c>
-      <c r="W7" s="84"/>
-      <c r="X7" s="84"/>
-      <c r="Y7" s="84"/>
-      <c r="Z7" s="84"/>
-      <c r="AA7" s="84"/>
-      <c r="AB7" s="84"/>
-      <c r="AC7" s="84"/>
-      <c r="AD7" s="84"/>
-      <c r="AE7" s="84"/>
-      <c r="AF7" s="84"/>
-      <c r="AG7" s="84"/>
-      <c r="AH7" s="84"/>
-      <c r="AI7" s="84"/>
-      <c r="AJ7" s="84"/>
-      <c r="AK7" s="84"/>
-      <c r="AL7" s="84"/>
-      <c r="AM7" s="85"/>
-    </row>
-    <row r="8" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A8" s="76" t="s">
-        <v>230</v>
-      </c>
-      <c r="B8" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="C8" s="75" t="s">
-        <v>219</v>
-      </c>
-      <c r="D8" s="92" t="s">
-        <v>38</v>
-      </c>
-      <c r="E8" s="76" t="s">
-        <v>220</v>
-      </c>
-      <c r="F8" s="75" t="s">
-        <v>130</v>
-      </c>
-      <c r="G8" s="76" t="s">
-        <v>24</v>
-      </c>
-      <c r="H8" s="75" t="s">
-        <v>171</v>
-      </c>
-      <c r="I8" s="76" t="s">
-        <v>231</v>
-      </c>
-      <c r="J8" s="76" t="s">
-        <v>222</v>
-      </c>
-      <c r="K8" s="76" t="s">
-        <v>161</v>
-      </c>
-      <c r="L8" s="77">
-        <v>0.39</v>
-      </c>
-      <c r="M8" s="76">
-        <v>1</v>
-      </c>
-      <c r="N8" s="90" t="s">
-        <v>29</v>
-      </c>
-      <c r="O8" s="90" t="s">
-        <v>232</v>
-      </c>
-      <c r="P8" s="76" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q8" s="76" t="s">
-        <v>136</v>
-      </c>
-      <c r="R8" s="76" t="s">
-        <v>33</v>
-      </c>
-      <c r="S8" s="58" t="s">
-        <v>125</v>
-      </c>
-      <c r="T8" s="79" t="s">
-        <v>224</v>
-      </c>
-      <c r="U8" s="79" t="s">
-        <v>150</v>
-      </c>
-      <c r="V8" s="91" t="s">
-        <v>233</v>
-      </c>
-      <c r="W8" s="91"/>
-      <c r="X8" s="91"/>
-      <c r="Y8" s="91"/>
-      <c r="Z8" s="91"/>
-      <c r="AA8" s="91"/>
-      <c r="AB8" s="91"/>
-      <c r="AC8" s="91"/>
-      <c r="AD8" s="91"/>
-      <c r="AE8" s="91"/>
-      <c r="AF8" s="91"/>
-      <c r="AG8" s="91"/>
-      <c r="AH8" s="91"/>
-      <c r="AI8" s="91"/>
-      <c r="AJ8" s="91"/>
-      <c r="AK8" s="91"/>
-      <c r="AL8" s="91"/>
-      <c r="AM8" s="91"/>
-    </row>
-    <row r="9" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A9" s="76" t="s">
-        <v>234</v>
-      </c>
-      <c r="B9" s="92" t="s">
-        <v>169</v>
-      </c>
-      <c r="C9" s="92" t="s">
-        <v>219</v>
-      </c>
-      <c r="D9" s="92" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="76" t="s">
-        <v>220</v>
-      </c>
-      <c r="F9" s="92" t="s">
-        <v>130</v>
-      </c>
-      <c r="G9" s="76" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="75" t="s">
-        <v>171</v>
-      </c>
-      <c r="I9" s="76" t="s">
-        <v>231</v>
-      </c>
-      <c r="J9" s="76" t="s">
-        <v>222</v>
-      </c>
-      <c r="K9" s="76" t="s">
-        <v>161</v>
-      </c>
-      <c r="L9" s="77">
-        <v>0.39</v>
-      </c>
-      <c r="M9" s="76">
-        <v>2</v>
-      </c>
-      <c r="N9" s="90" t="s">
-        <v>29</v>
-      </c>
-      <c r="O9" s="90" t="s">
-        <v>235</v>
-      </c>
-      <c r="P9" s="76" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q9" s="76" t="s">
-        <v>136</v>
-      </c>
-      <c r="R9" s="76" t="s">
-        <v>33</v>
-      </c>
-      <c r="S9" s="58" t="s">
-        <v>125</v>
-      </c>
-      <c r="T9" s="79" t="s">
-        <v>224</v>
-      </c>
-      <c r="U9" s="79" t="s">
-        <v>150</v>
-      </c>
-      <c r="V9" s="91" t="s">
-        <v>236</v>
-      </c>
-      <c r="W9" s="91"/>
-      <c r="X9" s="91"/>
-      <c r="Y9" s="91"/>
-      <c r="Z9" s="91"/>
-      <c r="AA9" s="91"/>
-      <c r="AB9" s="91"/>
-      <c r="AC9" s="91"/>
-      <c r="AD9" s="91"/>
-      <c r="AE9" s="91"/>
-      <c r="AF9" s="91"/>
-      <c r="AG9" s="91"/>
-      <c r="AH9" s="91"/>
-      <c r="AI9" s="91"/>
-      <c r="AJ9" s="91"/>
-      <c r="AK9" s="91"/>
-      <c r="AL9" s="91"/>
-      <c r="AM9" s="91"/>
-    </row>
-    <row r="10" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A10" s="76" t="s">
-        <v>242</v>
-      </c>
-      <c r="B10" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="C10" s="76" t="s">
-        <v>243</v>
-      </c>
-      <c r="D10" s="76" t="s">
-        <v>202</v>
-      </c>
-      <c r="E10" s="76" t="s">
-        <v>220</v>
-      </c>
-      <c r="F10" s="76" t="s">
-        <v>130</v>
-      </c>
-      <c r="G10" s="76" t="s">
-        <v>244</v>
-      </c>
-      <c r="H10" s="75" t="s">
-        <v>171</v>
-      </c>
-      <c r="I10" s="76" t="s">
-        <v>245</v>
-      </c>
-      <c r="J10" s="76" t="s">
-        <v>222</v>
-      </c>
-      <c r="K10" s="76" t="s">
-        <v>161</v>
-      </c>
-      <c r="L10" s="77">
-        <v>0.39</v>
-      </c>
-      <c r="M10" s="76">
-        <v>1</v>
-      </c>
-      <c r="N10" s="90" t="s">
-        <v>29</v>
-      </c>
-      <c r="O10" s="90" t="s">
-        <v>246</v>
-      </c>
-      <c r="P10" s="76" t="s">
-        <v>241</v>
-      </c>
-      <c r="Q10" s="76" t="s">
-        <v>136</v>
-      </c>
-      <c r="R10" s="76" t="s">
-        <v>33</v>
-      </c>
-      <c r="S10" s="58" t="s">
-        <v>125</v>
-      </c>
-      <c r="T10" s="79" t="s">
-        <v>224</v>
-      </c>
-      <c r="U10" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="V10" s="91"/>
-      <c r="W10" s="91"/>
-      <c r="X10" s="91"/>
-      <c r="Y10" s="91"/>
-      <c r="Z10" s="91"/>
-      <c r="AA10" s="91"/>
-      <c r="AB10" s="91"/>
-      <c r="AC10" s="91"/>
-      <c r="AD10" s="91"/>
-      <c r="AE10" s="91"/>
-      <c r="AF10" s="91"/>
-      <c r="AG10" s="91"/>
-      <c r="AH10" s="91"/>
-      <c r="AI10" s="91"/>
-      <c r="AJ10" s="91"/>
-      <c r="AK10" s="91"/>
-      <c r="AL10" s="91"/>
-      <c r="AM10" s="91"/>
-    </row>
-    <row r="11" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A11" s="76" t="s">
-        <v>248</v>
-      </c>
-      <c r="B11" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="C11" s="76" t="s">
-        <v>243</v>
-      </c>
-      <c r="D11" s="76" t="s">
-        <v>202</v>
-      </c>
-      <c r="E11" s="76" t="s">
-        <v>220</v>
-      </c>
-      <c r="F11" s="76" t="s">
-        <v>130</v>
-      </c>
-      <c r="G11" s="76" t="s">
-        <v>244</v>
-      </c>
-      <c r="H11" s="75" t="s">
-        <v>171</v>
-      </c>
-      <c r="I11" s="76" t="s">
-        <v>245</v>
-      </c>
-      <c r="J11" s="76" t="s">
-        <v>222</v>
-      </c>
-      <c r="K11" s="76" t="s">
-        <v>161</v>
-      </c>
-      <c r="L11" s="77">
-        <v>0.39</v>
-      </c>
-      <c r="M11" s="76">
-        <v>1</v>
-      </c>
-      <c r="N11" s="90" t="s">
-        <v>29</v>
-      </c>
-      <c r="O11" s="90" t="s">
-        <v>249</v>
-      </c>
-      <c r="P11" s="76" t="s">
-        <v>241</v>
-      </c>
-      <c r="Q11" s="76" t="s">
-        <v>136</v>
-      </c>
-      <c r="R11" s="76" t="s">
-        <v>33</v>
-      </c>
-      <c r="S11" s="58" t="s">
-        <v>125</v>
-      </c>
-      <c r="T11" s="79" t="s">
-        <v>224</v>
-      </c>
-      <c r="U11" s="9" t="s">
-        <v>247</v>
-      </c>
-      <c r="V11" s="91"/>
-      <c r="W11" s="91"/>
-      <c r="X11" s="91"/>
-      <c r="Y11" s="91"/>
-      <c r="Z11" s="91"/>
-      <c r="AA11" s="91"/>
-      <c r="AB11" s="91"/>
-      <c r="AC11" s="91"/>
-      <c r="AD11" s="91"/>
-      <c r="AE11" s="91"/>
-      <c r="AF11" s="91"/>
-      <c r="AG11" s="91"/>
-      <c r="AH11" s="91"/>
-      <c r="AI11" s="91"/>
-      <c r="AJ11" s="91"/>
-      <c r="AK11" s="91"/>
-      <c r="AL11" s="91"/>
-      <c r="AM11" s="91"/>
-    </row>
-    <row r="12" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A12" s="76" t="s">
-        <v>258</v>
-      </c>
-      <c r="B12" s="76" t="s">
-        <v>169</v>
-      </c>
-      <c r="C12" s="76" t="s">
-        <v>259</v>
-      </c>
-      <c r="D12" s="76" t="s">
-        <v>202</v>
-      </c>
-      <c r="E12" s="76" t="s">
-        <v>220</v>
-      </c>
-      <c r="F12" s="76" t="s">
-        <v>130</v>
-      </c>
-      <c r="G12" s="76" t="s">
-        <v>254</v>
-      </c>
-      <c r="H12" s="75" t="s">
-        <v>171</v>
-      </c>
-      <c r="I12" s="76" t="s">
-        <v>255</v>
-      </c>
-      <c r="J12" s="76" t="s">
-        <v>222</v>
-      </c>
-      <c r="K12" s="76" t="s">
-        <v>161</v>
-      </c>
-      <c r="L12" s="77">
-        <v>0.39</v>
-      </c>
-      <c r="M12" s="76">
-        <v>1</v>
-      </c>
-      <c r="N12" s="90" t="s">
-        <v>29</v>
-      </c>
-      <c r="O12" s="90" t="s">
-        <v>260</v>
-      </c>
-      <c r="P12" s="76" t="s">
-        <v>250</v>
-      </c>
-      <c r="Q12" s="76" t="s">
-        <v>136</v>
-      </c>
-      <c r="R12" s="76" t="s">
-        <v>33</v>
-      </c>
-      <c r="S12" s="58" t="s">
-        <v>125</v>
-      </c>
-      <c r="T12" s="79" t="s">
-        <v>224</v>
-      </c>
-      <c r="U12" s="79" t="s">
-        <v>150</v>
-      </c>
-      <c r="V12" s="91"/>
-      <c r="W12" s="91"/>
-      <c r="X12" s="91"/>
-      <c r="Y12" s="91"/>
-      <c r="Z12" s="91"/>
-      <c r="AA12" s="91"/>
-      <c r="AB12" s="91"/>
-      <c r="AC12" s="91"/>
-      <c r="AD12" s="91"/>
-      <c r="AE12" s="91"/>
-      <c r="AF12" s="91"/>
-      <c r="AG12" s="91"/>
-      <c r="AH12" s="91"/>
-      <c r="AI12" s="91"/>
-      <c r="AJ12" s="91"/>
-      <c r="AK12" s="91"/>
-      <c r="AL12" s="91"/>
-      <c r="AM12" s="91"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
added calibration plot to fig 2
</commit_message>
<xml_diff>
--- a/data_25_01_14.xlsx
+++ b/data_25_01_14.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="474" documentId="13_ncr:1_{9C3E2F24-F0BA-4ED0-966D-A349015366CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10E25A42-EF7D-4DBE-B306-0F48595BF7AB}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all data" sheetId="1" r:id="rId1"/>
@@ -3821,10 +3821,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
@@ -4028,9 +4024,9 @@
   </sheetPr>
   <dimension ref="A1:AM1008"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A234" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H247" sqref="H247"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A210" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B246" sqref="B246"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -38710,7 +38706,7 @@
   <dimension ref="A1:W11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>
@@ -39395,8 +39391,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15C55639-70D8-4772-A7C7-0A253515BD91}">
   <dimension ref="A1:AM17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.3"/>

</xml_diff>